<commit_message>
update response list to properly output data
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -591,252 +591,252 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '87797664', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5d/ba/ea/1026649594.jpg', 'externalReference': 'BCN05285', 'numPhotos': 52, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 170.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3863885, 'longitude': 2.1622455, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/87797664/', 'distance': '636', 'description': 'Magnífica vivienda de obra nueva con terraza en Eixample Esquerra. Espectacular vivienda de obra nueva en finca modernista rehabilitada con ascensor, situada junto a la histórica Universidad de Barcelona. Se trata de una ubicación perfecta en pleno centro de la ciudad, con los mejores servicios y comunicaciones, a tan solo 3 calles de Plaza Catalunya y el Paseo de Gracia. El piso dispone de 130 m2 construidos interiores más 40 m2 de terraza, que le da un gran valor, un patio de 8 m2 y un balcón de 3 m2. La zona de día consta de salón-comedor con balcón hacia la calle, cocina independiente con electrodomésticos y galería con lavadero. La zona de noche se compone de dos habitaciones en suite con cuarto de baño propio: la principal tiene vestidor y acceso a la terraza, orientada hacia el patio de manzana inrterior; y la otra es interior y tiene acceso a un patio de 8 m2. Además, hay un aseo de cortesía. El edificio tiene además un terrado comunitario para disfrutar del aire libre. El piso goza de una reforma de alta calidad y diseño de la mano del prestigioso interiorista Jaime Beriestain. Está equipado con sistema hibrido de aerotermia de la casa Mintsubishi con integración de Hidrokit, fancoils por conductos y suelo radiante (controlado por domótica), suelos de piedra natural, armarios empotrados y cristales Climalit.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4988.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '87797664', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5d/ba/ea/1026649594.jpg', 'externalReference': 'BCN05285', 'numPhotos': 52, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 170.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3863885, 'longitude': 2.1622455, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/87797664/', 'distance': '636', 'description': 'Magnífica vivienda de obra nueva con terraza en Eixample Esquerra. Espectacular vivienda de obra nueva en finca modernista rehabilitada con ascensor, situada junto a la histórica Universidad de Barcelona. Se trata de una ubicación perfecta en pleno centro de la ciudad, con los mejores servicios y comunicaciones, a tan solo 3 calles de Plaza Catalunya y el Paseo de Gracia. El piso dispone de 130 m2 construidos interiores más 40 m2 de terraza, que le da un gran valor, un patio de 8 m2 y un balcón de 3 m2. La zona de día consta de salón-comedor con balcón hacia la calle, cocina independiente con electrodomésticos y galería con lavadero. La zona de noche se compone de dos habitaciones en suite con cuarto de baño propio: la principal tiene vestidor y acceso a la terraza, orientada hacia el patio de manzana inrterior; y la otra es interior y tiene acceso a un patio de 8 m2. Además, hay un aseo de cortesía. El edificio tiene además un terrado comunitario para disfrutar del aire libre. El piso goza de una reforma de alta calidad y diseño de la mano del prestigioso interiorista Jaime Beriestain. Está equipado con sistema hibrido de aerotermia de la casa Mintsubishi con integración de Hidrokit, fancoils por conductos y suelo radiante (controlado por domótica), suelos de piedra natural, armarios empotrados y cristales Climalit.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4988.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98351591', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/d2/66/bf/1009058214.jpg', 'externalReference': 'VB2207038', 'numPhotos': 29, 'floor': '3', 'price': 359000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 63.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Pi i Margall', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': "El Camp d'En Grassot i Gràcia Nova", 'latitude': 41.4096591, 'longitude': 2.1622433, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98351591/', 'distance': '2545', 'description': 'Piso reformado de dos habitaciones en venta en Gràcia Nova Fantástico piso reformado con dos habitaciones y balcón en Gràcia Nova En plena Gràcia Nova, a pocos metros del Mercat del Estrella, entre las paradas de metro Alfons X y Joanic, en uno de los futuros ejes verdes de la ciudad, encontramos este bonito apartamento totalmente reformado y a estrenar, listo para entrar a vivir. Luminosidad, buen gusto, distribución de espacios muy bien pensada y una reforma de calidad, es lo que describe mejor esta propiedad. la vivienda tiene una superficie de 60 m2 aprox que se distribuyen de forma muy lógica, al entrar en la vivienda encontramos el recibidor y el baño de cortesía, avanzamos en el pasillo y encontramos una primera habitación doble con baño completo en suite, avanzando un poco más llegamos a la habitación individual. Al final del pasillo se encuentra la amplia sala con cocina abierta totalmente equipada y con salida a un agradable balcón con vistas a un patio de manzana muy tranquilo y soleado por la tarde. La vivienda cuenta con aire acondicionado / calefacción por conductos, los suelos de parqué natural dan una calidez ideal a toda la vivienda. El edificio de los años 1963 cuenta con ascensor. ¡Sin duda, hablamos de una excelente oportunidad en la zona!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5698.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "El Camp d'En Grassot i Gràcia Nova, Barcelona", 'title': 'Piso en Calle de Pi i Margall'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98351591', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/d2/66/bf/1009058214.jpg', 'externalReference': 'VB2207038', 'numPhotos': 29, 'floor': '3', 'price': 359000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 63.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Pi i Margall', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': "El Camp d'En Grassot i Gràcia Nova", 'latitude': 41.4096591, 'longitude': 2.1622433, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98351591/', 'distance': '2545', 'description': 'Piso reformado de dos habitaciones en venta en Gràcia Nova Fantástico piso reformado con dos habitaciones y balcón en Gràcia Nova En plena Gràcia Nova, a pocos metros del Mercat del Estrella, entre las paradas de metro Alfons X y Joanic, en uno de los futuros ejes verdes de la ciudad, encontramos este bonito apartamento totalmente reformado y a estrenar, listo para entrar a vivir. Luminosidad, buen gusto, distribución de espacios muy bien pensada y una reforma de calidad, es lo que describe mejor esta propiedad. la vivienda tiene una superficie de 60 m2 aprox que se distribuyen de forma muy lógica, al entrar en la vivienda encontramos el recibidor y el baño de cortesía, avanzamos en el pasillo y encontramos una primera habitación doble con baño completo en suite, avanzando un poco más llegamos a la habitación individual. Al final del pasillo se encuentra la amplia sala con cocina abierta totalmente equipada y con salida a un agradable balcón con vistas a un patio de manzana muy tranquilo y soleado por la tarde. La vivienda cuenta con aire acondicionado / calefacción por conductos, los suelos de parqué natural dan una calidez ideal a toda la vivienda. El edificio de los años 1963 cuenta con ascensor. ¡Sin duda, hablamos de una excelente oportunidad en la zona!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5698.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "El Camp d'En Grassot i Gràcia Nova, Barcelona", 'title': 'Piso en Calle de Pi i Margall'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99349576', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b0/f6/f4/1041061889.jpg', 'externalReference': 'S-35432', 'numPhotos': 36, 'floor': '2', 'price': 229000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 68.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Ronda de Sant Pau', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'Sant Antoni', 'latitude': 41.375152, 'longitude': 2.1633305, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99349576/', 'distance': '1470', 'description': 'PLAÇA JOSEP MARIA FOLCH I TORRES Acogedora vivienda situada en uno de los barrios más emblemáticos de la ciudad condal junto a la Ronda Sant Pau y los Jardines de la Plaça Josep María Floch i Torres. Consta de 2 dormitorios (originalmente 3), luminoso comedor, baño con bañera y cocina con salida a lavadero. Toda la vivienda se encuentra en perfecto estado de conservación, con acabados de calidad. Suelo de mármol, puertas de madera noble, carpintería exterior de aluminio con persianas integradas y puerta de entrada de seguridad. Piso muy luminoso y tranquilo. Edificio de obra vista con ascensor.  En FINCAS Gp somos una empresa especializada en servicios inmobiliarios en la ciudad de Barcelona desde 1993. Los precios indicados no incluyen gastos e impuestos de escrituración ni de financiación. Venta y alquiler de apartamentos y locales comerciales. Encuentre más en nuestro sitio web.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3368.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Antoni, Barcelona', 'title': 'Piso en Ronda de Sant Pau'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99349576', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b0/f6/f4/1041061889.jpg', 'externalReference': 'S-35432', 'numPhotos': 36, 'floor': '2', 'price': 229000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 68.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Ronda de Sant Pau', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'Sant Antoni', 'latitude': 41.375152, 'longitude': 2.1633305, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99349576/', 'distance': '1470', 'description': 'PLAÇA JOSEP MARIA FOLCH I TORRES Acogedora vivienda situada en uno de los barrios más emblemáticos de la ciudad condal junto a la Ronda Sant Pau y los Jardines de la Plaça Josep María Floch i Torres. Consta de 2 dormitorios (originalmente 3), luminoso comedor, baño con bañera y cocina con salida a lavadero. Toda la vivienda se encuentra en perfecto estado de conservación, con acabados de calidad. Suelo de mármol, puertas de madera noble, carpintería exterior de aluminio con persianas integradas y puerta de entrada de seguridad. Piso muy luminoso y tranquilo. Edificio de obra vista con ascensor.  En FINCAS Gp somos una empresa especializada en servicios inmobiliarios en la ciudad de Barcelona desde 1993. Los precios indicados no incluyen gastos e impuestos de escrituración ni de financiación. Venta y alquiler de apartamentos y locales comerciales. Encuentre más en nuestro sitio web.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3368.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Antoni, Barcelona', 'title': 'Piso en Ronda de Sant Pau'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98840562', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/0e/a9/0e/1025701609.jpg', 'externalReference': 'BCNP4881', 'numPhotos': 24, 'price': 1100000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 125.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio Sant Pere - Santa Caterina i la Ribera', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3832064, 'longitude': 2.1829743, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98840562/', 'distance': '1201', 'description': 'El impacto directo de este excepcional apartamento hace que se distinga de otros en el mercado desde el primer momento en que se cruza la puerta. Encontrará techos altos, cinco grandes y originales puertas balconeras de tres orientaciones que ofrecen una inmensa luz natural, y vistas a la terraza privada con un verde jardín vertical. La cocina abierta de alta gama y totalmente equipada en la zona de estar ha sido hecha a medida desde Italia y da una agradable elegancia al apartamento con sus colores oscuros. La carpintería ha sido igualmente hecha a medida desde Italia para el apartamento y equilibra bien un espacio de oficina abierto con el primer dormitorio en suite. También hay un cuarto de baño para invitados justo al lado del segundo dormitorio. El suelo es de parquet natural y el apartamento dispone de radiadores para la calefacción. Pero la joya de la propiedad es sin duda la terraza de 28 m2 que conecta con el salón y el segundo dormitorio. Ofrece un hermoso jardín vertical y el lujo de la tranquilidad en el corazón de El Born. Escondido en el jardín vertical hay un acceso a un trastero que también se utiliza como lavadero. La micro ubicación del apartamento es otro importante punto de venta de la propiedad, ya que está rodeado de algunas de las mejores plazas y restaurantes de la zona. Además, a pocos minutos a pie se encuentra también el Parque de la Ciutadella, el puerto Port-Vell y la playa de la Barceloneta. En definitiva, estamos hablando de una auténtica oportunidad en uno de los barrios más populares de Barcelona. Si hay un lugar de moda tanto para turistas como locales, es el dinámico barrio de El Born con su particular mercado, ahora convertido en museo, tras conseguir unas fantásticas ruinas romanas durante su remodelación. Es hogar de artistas, artesanos y bohemios, con infinidad de tiendas curiosas y únicas. Aún más famosos son sus \xa0variados restaurantes, tantos como para descubrir uno nuevo cada día. El mercado de Santa Caterina con su techo inspirado en la piel del dragón de Sant Jordi es por sí mismo una obra para admirar. La Basílica de Santa María del Mar, El Palau de la Música, y el pulmón verde de La Ciutadella son algunos de los referentes importantes de este barrio. Es un barrio para vivir y conocer. Sus edificios continúan el patrón irregular de El Barrio Gótico, y sus calles aunque por momentos más despejadas, también son angostas. En los bajos de los edificios puede encontrar bares de autor, galerías de arte, talleres de artesanos y un sinfín de pequeños y curiosos negocios. Este barrio le interesará si le gusta el estilo de vida bohemio, convivir con los\xa0 múltiples artesanos, el tapeo y buen comer, y vivir en un barrio que le sorprenda con tiendas y rincones nuevos. Es una buena ubicación para invertir en un pied-à-terre.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 8800.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98840562', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/0e/a9/0e/1025701609.jpg', 'externalReference': 'BCNP4881', 'numPhotos': 24, 'price': 1100000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 125.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio Sant Pere - Santa Caterina i la Ribera', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3832064, 'longitude': 2.1829743, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98840562/', 'distance': '1201', 'description': 'El impacto directo de este excepcional apartamento hace que se distinga de otros en el mercado desde el primer momento en que se cruza la puerta. Encontrará techos altos, cinco grandes y originales puertas balconeras de tres orientaciones que ofrecen una inmensa luz natural, y vistas a la terraza privada con un verde jardín vertical. La cocina abierta de alta gama y totalmente equipada en la zona de estar ha sido hecha a medida desde Italia y da una agradable elegancia al apartamento con sus colores oscuros. La carpintería ha sido igualmente hecha a medida desde Italia para el apartamento y equilibra bien un espacio de oficina abierto con el primer dormitorio en suite. También hay un cuarto de baño para invitados justo al lado del segundo dormitorio. El suelo es de parquet natural y el apartamento dispone de radiadores para la calefacción. Pero la joya de la propiedad es sin duda la terraza de 28 m2 que conecta con el salón y el segundo dormitorio. Ofrece un hermoso jardín vertical y el lujo de la tranquilidad en el corazón de El Born. Escondido en el jardín vertical hay un acceso a un trastero que también se utiliza como lavadero. La micro ubicación del apartamento es otro importante punto de venta de la propiedad, ya que está rodeado de algunas de las mejores plazas y restaurantes de la zona. Además, a pocos minutos a pie se encuentra también el Parque de la Ciutadella, el puerto Port-Vell y la playa de la Barceloneta. En definitiva, estamos hablando de una auténtica oportunidad en uno de los barrios más populares de Barcelona. Si hay un lugar de moda tanto para turistas como locales, es el dinámico barrio de El Born con su particular mercado, ahora convertido en museo, tras conseguir unas fantásticas ruinas romanas durante su remodelación. Es hogar de artistas, artesanos y bohemios, con infinidad de tiendas curiosas y únicas. Aún más famosos son sus \xa0variados restaurantes, tantos como para descubrir uno nuevo cada día. El mercado de Santa Caterina con su techo inspirado en la piel del dragón de Sant Jordi es por sí mismo una obra para admirar. La Basílica de Santa María del Mar, El Palau de la Música, y el pulmón verde de La Ciutadella son algunos de los referentes importantes de este barrio. Es un barrio para vivir y conocer. Sus edificios continúan el patrón irregular de El Barrio Gótico, y sus calles aunque por momentos más despejadas, también son angostas. En los bajos de los edificios puede encontrar bares de autor, galerías de arte, talleres de artesanos y un sinfín de pequeños y curiosos negocios. Este barrio le interesará si le gusta el estilo de vida bohemio, convivir con los\xa0 múltiples artesanos, el tapeo y buen comer, y vivir en un barrio que le sorprenda con tiendas y rincones nuevos. Es una buena ubicación para invertir en un pied-à-terre.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 8800.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98382386', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a8/9e/34/1022400721.jpg', 'externalReference': 'BCNP4798', 'numPhotos': 27, 'price': 690000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 85.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3905269, 'longitude': 2.1644133, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98382386/', 'distance': '559', 'description': 'Maravilloso piso en venta en el corazón del Ensanche Derecho de Barcelona, a la vuelta de la esquina de la elegante Rambla de Catalunya conocida por sus lujosos comercios y conocida aun más por sus restaurantes con terraza ideales para disfrutar del buen tiempo de la ciudad condal. El piso es una auténtica maravilla. Los acabados que se han utilizado en la reforma es de auténtico lujo, como por ejemplo los suelos de madera noble de roble americano, la cocina de muy buena calidad con vinoteca y nevera Liebherr, baños y grifería de diseño, radiadores de alta gamma, armarios empotrados realizados a medida, panelados de madera en las paredes y papel decorativo de alta calidad, además de un sistema de filtro osmosis para mejorar el agua de toda la vivienda. El piso no solo dispone de maravillosos acabados, sino que además dispone de características arquitectónicas de la época, como los techos altos y artesonados, la chimenea original y marcos decorativos. El piso consta de un agradable salón comedor con salida a una terraza muy disfrutable de aproximadamente unos 8m2 orientada hacia el sudeste, una cocina totalmente equipada, un lavadero muy práctico, un dormitorio doble “en suite” también con salida a la terraza, y otro dormitorio individual con su propio baño. La finca es también un espectáculo, ya que se trata de un edificio regio del 1900, completamente reformada y actualizada con acceso directo al ascensor y además un excelente servicio de conserjería. En resumen una propiedad para gozar desde el primer instante que reúne todo lo que se buscaría en la mejor zona de Barcelona. La Dreta de L’Eixample se inicia en Plaça de Catalunya y su eje central gira en torno al Passeig de Gràcia y el Cuadrat d’Or. Se delimita desde la transitada Calle Balmes hasta el renovado Passeig de Sant Joan y desde la comercial Ronda Sant Pere hasta la conveniente Avinguda Diagonal. Es uno de los barrios, junto con Pedralbes y Sarrià-Sant Gervasi, más caros y exclusivos de Barcelona ciudad. Es imposible no hacer referencia al lujo del Paseo de Gràcia, con las boutiques de las marcas más exclusivas del mundo, o a los comercios de La Rambla de Catalunya. Sin embargo, el resto de sus calles son tanto o más interesantes. En ellas residía parte de la burguesía textilera catalana de principios del siglo XX, la cual ha dejado huella en las espectaculares fincas regias y casas modernistas diseñadas por los arquitectos más famosos de la época, como la Pedrera o la Casa Batlló del gran Antoni Gaudí. En consecuencia, las viviendas características de este barrio son apartamentos amplios, de techos elevados, molduras, elaborados pavimentos y balcones. Muchos edificios y pisos conservan esta herencia arquitectónica original artesanal y es posible encontrar apartamentos remodelados recientemente, áticos, lofts e incluso estudios, que reviven estos elementos, así como pisos con mucho potencial para ser reformados. Este lado de L’Eixample está dotado de todo tipo de servicios y comercios, centros educativos -principalmente escuelas concertadas y privadas-. Le resultará muy fácil moverse andando o desplazarse a través de las conexiones de transporte público hasta las tiendas y restaurantes más caros y en vogue de la ciudad. Este es el mejor barrio si quiere admirar y vivir en la zona noble del fascinante modernismo catalán, residir en una de sus características fincas regias, y convivir en perfecto equilibrio con la vibrante y lujosa vida comercial. Es ideal si desea caminar cada día por sus calles anchas y ordenadas, con fáciles conexiones de transporte, disponer de todo tipo de servicios y equipamientos incluidas escuelas concertadas o privadas, y disfrutar del ambiente más chic, cultural y cosmopolita de Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8118.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98382386', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a8/9e/34/1022400721.jpg', 'externalReference': 'BCNP4798', 'numPhotos': 27, 'price': 690000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 85.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3905269, 'longitude': 2.1644133, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98382386/', 'distance': '559', 'description': 'Maravilloso piso en venta en el corazón del Ensanche Derecho de Barcelona, a la vuelta de la esquina de la elegante Rambla de Catalunya conocida por sus lujosos comercios y conocida aun más por sus restaurantes con terraza ideales para disfrutar del buen tiempo de la ciudad condal. El piso es una auténtica maravilla. Los acabados que se han utilizado en la reforma es de auténtico lujo, como por ejemplo los suelos de madera noble de roble americano, la cocina de muy buena calidad con vinoteca y nevera Liebherr, baños y grifería de diseño, radiadores de alta gamma, armarios empotrados realizados a medida, panelados de madera en las paredes y papel decorativo de alta calidad, además de un sistema de filtro osmosis para mejorar el agua de toda la vivienda. El piso no solo dispone de maravillosos acabados, sino que además dispone de características arquitectónicas de la época, como los techos altos y artesonados, la chimenea original y marcos decorativos. El piso consta de un agradable salón comedor con salida a una terraza muy disfrutable de aproximadamente unos 8m2 orientada hacia el sudeste, una cocina totalmente equipada, un lavadero muy práctico, un dormitorio doble “en suite” también con salida a la terraza, y otro dormitorio individual con su propio baño. La finca es también un espectáculo, ya que se trata de un edificio regio del 1900, completamente reformada y actualizada con acceso directo al ascensor y además un excelente servicio de conserjería. En resumen una propiedad para gozar desde el primer instante que reúne todo lo que se buscaría en la mejor zona de Barcelona. La Dreta de L’Eixample se inicia en Plaça de Catalunya y su eje central gira en torno al Passeig de Gràcia y el Cuadrat d’Or. Se delimita desde la transitada Calle Balmes hasta el renovado Passeig de Sant Joan y desde la comercial Ronda Sant Pere hasta la conveniente Avinguda Diagonal. Es uno de los barrios, junto con Pedralbes y Sarrià-Sant Gervasi, más caros y exclusivos de Barcelona ciudad. Es imposible no hacer referencia al lujo del Paseo de Gràcia, con las boutiques de las marcas más exclusivas del mundo, o a los comercios de La Rambla de Catalunya. Sin embargo, el resto de sus calles son tanto o más interesantes. En ellas residía parte de la burguesía textilera catalana de principios del siglo XX, la cual ha dejado huella en las espectaculares fincas regias y casas modernistas diseñadas por los arquitectos más famosos de la época, como la Pedrera o la Casa Batlló del gran Antoni Gaudí. En consecuencia, las viviendas características de este barrio son apartamentos amplios, de techos elevados, molduras, elaborados pavimentos y balcones. Muchos edificios y pisos conservan esta herencia arquitectónica original artesanal y es posible encontrar apartamentos remodelados recientemente, áticos, lofts e incluso estudios, que reviven estos elementos, así como pisos con mucho potencial para ser reformados. Este lado de L’Eixample está dotado de todo tipo de servicios y comercios, centros educativos -principalmente escuelas concertadas y privadas-. Le resultará muy fácil moverse andando o desplazarse a través de las conexiones de transporte público hasta las tiendas y restaurantes más caros y en vogue de la ciudad. Este es el mejor barrio si quiere admirar y vivir en la zona noble del fascinante modernismo catalán, residir en una de sus características fincas regias, y convivir en perfecto equilibrio con la vibrante y lujosa vida comercial. Es ideal si desea caminar cada día por sus calles anchas y ordenadas, con fáciles conexiones de transporte, disponer de todo tipo de servicios y equipamientos incluidas escuelas concertadas o privadas, y disfrutar del ambiente más chic, cultural y cosmopolita de Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8118.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98378398', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/af/08/1c/1027086647.jpg', 'externalReference': '3000', 'numPhotos': 22, 'floor': '2', 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 90.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Petritxol', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3822216, 'longitude': 2.1741355, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98378398/', 'distance': '689', 'description': 'Fabulosa propiedad situada en el corazón del Barrio Gótico, en la emblemática Calle Petritxol, a escasos metros de la Plaza del Pi y Las Ramblas. Se trata de un elegante piso exterior de 90 m2 ubicada en una finca regia del año 1780.    La propiedad ha sido completamente renovada manteniendo y respetando elementos originales como las vigas de madera de los techos y los suelos de mosaico originales combinados con parquet de madera y hormigón pulido en la cocina y baños.     El resultado es un hogar elegante, moderno y acogedor. El edificio, que cuenta con un ascensor recientemente instalado, data de 1780. Ha pasado la ITE (inspección técnica del edificio) y ha sido rehabilitado recientemente.    Cocina abierta con electrodomésticos de alta calidad, integrados junto al salón comedor muy agradable que disfruta de dos grandes balcones orientados a la calle Petritxol.    Es un piso ideal tanto para vivir como para invertir, ya que alquilado, tiene una alta rentabilidad.  El piso, gracias a su rehabilitación integral de todo el edificio, combina las ventajas de una construcción nueva con elementos originales, lo que sin duda hacen de está vivienda una pieza única.    Una gran oportunidad de adquirir una vivienda única con amplias estancias y mucha luz en una de las zonas más demandadas del barrio Gótico.    La zona disfruta de todos los servicios, colegios, mercados como La Boquería o Santa Catalina, comercios y locales de ocio. La zona también está muy bien comunicada por transporte público, cercana a las líneas de metro L1 y L3, y líneas de autobús que atraviesan la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5389.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso en Calle de Petritxol'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98378398', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/af/08/1c/1027086647.jpg', 'externalReference': '3000', 'numPhotos': 22, 'floor': '2', 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 90.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Petritxol', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3822216, 'longitude': 2.1741355, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98378398/', 'distance': '689', 'description': 'Fabulosa propiedad situada en el corazón del Barrio Gótico, en la emblemática Calle Petritxol, a escasos metros de la Plaza del Pi y Las Ramblas. Se trata de un elegante piso exterior de 90 m2 ubicada en una finca regia del año 1780.    La propiedad ha sido completamente renovada manteniendo y respetando elementos originales como las vigas de madera de los techos y los suelos de mosaico originales combinados con parquet de madera y hormigón pulido en la cocina y baños.     El resultado es un hogar elegante, moderno y acogedor. El edificio, que cuenta con un ascensor recientemente instalado, data de 1780. Ha pasado la ITE (inspección técnica del edificio) y ha sido rehabilitado recientemente.    Cocina abierta con electrodomésticos de alta calidad, integrados junto al salón comedor muy agradable que disfruta de dos grandes balcones orientados a la calle Petritxol.    Es un piso ideal tanto para vivir como para invertir, ya que alquilado, tiene una alta rentabilidad.  El piso, gracias a su rehabilitación integral de todo el edificio, combina las ventajas de una construcción nueva con elementos originales, lo que sin duda hacen de está vivienda una pieza única.    Una gran oportunidad de adquirir una vivienda única con amplias estancias y mucha luz en una de las zonas más demandadas del barrio Gótico.    La zona disfruta de todos los servicios, colegios, mercados como La Boquería o Santa Catalina, comercios y locales de ocio. La zona también está muy bien comunicada por transporte público, cercana a las líneas de metro L1 y L3, y líneas de autobús que atraviesan la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5389.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso en Calle de Petritxol'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98264311', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b9/b6/8a/1006013108.jpg', 'externalReference': '3855V_6', 'numPhotos': 46, 'floor': '6', 'price': 2650000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 195.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3919731, 'longitude': 2.1693451, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98264311/', 'distance': '501', 'description': 'Este espectacular y exclusivo ático de 101m2 construidos y 94m2 de terraza viene distribuido en un amplio y luminoso salón comedor con salida a la magnifíca terraza con doble altura. El suelo es de madera flotante que proporciona una sensación de relajación gracias a sus zonas ajardinadas. Con posbilidades de amueblar con una zona chill out o un agradable comedor exterior donde disfrutar las tardes de verano. Las increíbles vistas que proporciona no te dejarán indiferente.  La cocina es abierta al comedor con isleta y barra de desayuno. Viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr) y tiene acceso a la zona de aguas independiente. La zona de noche consta de un dormitorio máster suite con salida a un amplio balcón, un vestidor y un baño con bañera ovalada y plato de ducha.  El segundo dormitorio también en suite y con salida al balcón. Ambos dormitorios cuentan con armarios empotrados. Todas las estancias disponen de aire acondicionado y calefacción por conductos, domótica, suelos de parqué, carpintería de aluminio y cristales dobles. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 13590.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Ático en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98264311', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b9/b6/8a/1006013108.jpg', 'externalReference': '3855V_6', 'numPhotos': 46, 'floor': '6', 'price': 2650000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 195.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3919731, 'longitude': 2.1693451, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98264311/', 'distance': '501', 'description': 'Este espectacular y exclusivo ático de 101m2 construidos y 94m2 de terraza viene distribuido en un amplio y luminoso salón comedor con salida a la magnifíca terraza con doble altura. El suelo es de madera flotante que proporciona una sensación de relajación gracias a sus zonas ajardinadas. Con posbilidades de amueblar con una zona chill out o un agradable comedor exterior donde disfrutar las tardes de verano. Las increíbles vistas que proporciona no te dejarán indiferente.  La cocina es abierta al comedor con isleta y barra de desayuno. Viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr) y tiene acceso a la zona de aguas independiente. La zona de noche consta de un dormitorio máster suite con salida a un amplio balcón, un vestidor y un baño con bañera ovalada y plato de ducha.  El segundo dormitorio también en suite y con salida al balcón. Ambos dormitorios cuentan con armarios empotrados. Todas las estancias disponen de aire acondicionado y calefacción por conductos, domótica, suelos de parqué, carpintería de aluminio y cristales dobles. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 13590.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Ático en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98261311', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f2/8a/bd/1005921523.jpg', 'externalReference': '3855V_3', 'numPhotos': 42, 'floor': '1', 'price': 1925000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 168.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3890208, 'longitude': 2.1642732, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98261311/', 'distance': '487', 'description': 'Exclusiva vivienda de 143m2 construidos y 23m2 de terraza, distribuidos en un luminoso salón comedor con salida a dos agradables balcones. La cocina es abierta y viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr). A través del distribuidor accedemos a la zona de noche, donde encontraremos la habitación master suite con salida a la espectacular terraza, este dormitorio dispone de un amplio vestidor y un baño completo con plato de ducha. La segunda habitación también es doble y tiene justo en frente un baño completo con bañera. Ambas habitaciones tienen armarios empotrados y vienen diseñadas con materiales de alta calidad. Todas las estancias disponen de aire acondicionado y calefacción por conductos, domótica, suelos de parqué, carpintería de aluminio y cristales dobles. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Ubicada en el corazón de Barcelona, Paseo de Gracia es la avenida más elegante y señorial de la ciudad, y en una de las ubicaciones más buscadas para los negocios. Una propuesta comercial muy atractiva. Ofrece una vida muy cómoda, con todos los servicios al alcance de su mano. Vivir en esta avenida significa disfrutar de exclusividad en el mismo centro de la ciudad. Disfruta de la exquisita arquitectura de sus edificios modernistas como son la Casa Batlló, la Casa Milá o la Casa Lleó Morera, mezclados con edificios del estilo moderno, clásico y neoclásico.  Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 11458.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98261311', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f2/8a/bd/1005921523.jpg', 'externalReference': '3855V_3', 'numPhotos': 42, 'floor': '1', 'price': 1925000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 168.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3890208, 'longitude': 2.1642732, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98261311/', 'distance': '487', 'description': 'Exclusiva vivienda de 143m2 construidos y 23m2 de terraza, distribuidos en un luminoso salón comedor con salida a dos agradables balcones. La cocina es abierta y viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr). A través del distribuidor accedemos a la zona de noche, donde encontraremos la habitación master suite con salida a la espectacular terraza, este dormitorio dispone de un amplio vestidor y un baño completo con plato de ducha. La segunda habitación también es doble y tiene justo en frente un baño completo con bañera. Ambas habitaciones tienen armarios empotrados y vienen diseñadas con materiales de alta calidad. Todas las estancias disponen de aire acondicionado y calefacción por conductos, domótica, suelos de parqué, carpintería de aluminio y cristales dobles. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Ubicada en el corazón de Barcelona, Paseo de Gracia es la avenida más elegante y señorial de la ciudad, y en una de las ubicaciones más buscadas para los negocios. Una propuesta comercial muy atractiva. Ofrece una vida muy cómoda, con todos los servicios al alcance de su mano. Vivir en esta avenida significa disfrutar de exclusividad en el mismo centro de la ciudad. Disfruta de la exquisita arquitectura de sus edificios modernistas como son la Casa Batlló, la Casa Milá o la Casa Lleó Morera, mezclados con edificios del estilo moderno, clásico y neoclásico.  Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 11458.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98256266', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f3/cf/34/1005719750.jpg', 'externalReference': '3855V_2', 'numPhotos': 43, 'floor': '5', 'price': 2680000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 157.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3924731, 'longitude': 2.1675451, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98256266/', 'distance': '585', 'description': 'Piso a estrenar con Piscina en Paseo de Gracia, Barcelona Exclusiva vivienda de 157m2 construidos, distribuidos en un amplio salón comedor. La cocina es abierta con isleta y barra de desayuno y viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr). La zona de noche dispone de 2 habitaciones; una doble y otra doble en suite con bañera ovalada y plato de ducha. Ambas disponen de armarios empotrado. Otro baño completo con plato de ducha por donde se accede al lavadero. En el recibidor encontramos un cómodo baño de cortesía y un armario empotrado. Todas las estancias disponen de suelo radiante, aire acondicionado y calefacción, domótica, suelos de roble, carpintería de madera y doble acristalamiento. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Ubicada en el corazón de Barcelona, Paseo de Gracia es la avenida más elegante y señorial de la ciudad, y en una de las ubicaciones más buscadas para los negocios. Una propuesta comercial muy atractiva. Ofrece una vida muy cómoda, con todos los servicios al alcance de su mano. Vivir en esta avenida significa disfrutar de exclusividad en el mismo centro de la ciudad. Disfruta de la exquisita arquitectura de sus edificios modernistas como son la Casa Batlló, la Casa Milá o la Casa Lleó Morera, mezclados con edificios del estilo moderno, clásico y neoclásico.  Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas. En total, la finca presenta 21 viviendas únicas, una azotea con piscina y zona chill out, un patio vegetal interior, mirador y zonas comunes. Distribuidos en 5 plantas más ático, viviendas de 1, 2 o 4 dormitorios, algunos con balcón y otros con agradables terrazas. El exclusivo ático, de un dormitorio y salida a una impresionante terraza con vistas inmejorables, el mejor producto para nuestros clientes más exigentes.  Cada tipología de vivienda tiene su personalidad, diferente distribución y distintas superficies, todas construidas con materiales de alta calidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 17070.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98256266', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f3/cf/34/1005719750.jpg', 'externalReference': '3855V_2', 'numPhotos': 43, 'floor': '5', 'price': 2680000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 157.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3924731, 'longitude': 2.1675451, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98256266/', 'distance': '585', 'description': 'Piso a estrenar con Piscina en Paseo de Gracia, Barcelona Exclusiva vivienda de 157m2 construidos, distribuidos en un amplio salón comedor. La cocina es abierta con isleta y barra de desayuno y viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr). La zona de noche dispone de 2 habitaciones; una doble y otra doble en suite con bañera ovalada y plato de ducha. Ambas disponen de armarios empotrado. Otro baño completo con plato de ducha por donde se accede al lavadero. En el recibidor encontramos un cómodo baño de cortesía y un armario empotrado. Todas las estancias disponen de suelo radiante, aire acondicionado y calefacción, domótica, suelos de roble, carpintería de madera y doble acristalamiento. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Ubicada en el corazón de Barcelona, Paseo de Gracia es la avenida más elegante y señorial de la ciudad, y en una de las ubicaciones más buscadas para los negocios. Una propuesta comercial muy atractiva. Ofrece una vida muy cómoda, con todos los servicios al alcance de su mano. Vivir en esta avenida significa disfrutar de exclusividad en el mismo centro de la ciudad. Disfruta de la exquisita arquitectura de sus edificios modernistas como son la Casa Batlló, la Casa Milá o la Casa Lleó Morera, mezclados con edificios del estilo moderno, clásico y neoclásico.  Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas. En total, la finca presenta 21 viviendas únicas, una azotea con piscina y zona chill out, un patio vegetal interior, mirador y zonas comunes. Distribuidos en 5 plantas más ático, viviendas de 1, 2 o 4 dormitorios, algunos con balcón y otros con agradables terrazas. El exclusivo ático, de un dormitorio y salida a una impresionante terraza con vistas inmejorables, el mejor producto para nuestros clientes más exigentes.  Cada tipología de vivienda tiene su personalidad, diferente distribución y distintas superficies, todas construidas con materiales de alta calidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 17070.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98000858', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8b/d9/71/997711176.jpg', 'externalReference': '3835V', 'numPhotos': 36, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 114.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3902528, 'longitude': 2.1608339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98000858/', 'distance': '804', 'description': 'Espectacular y exclusiva vivienda de 114m2, distribuida en un amplio recibidor con paredes de ladrillo visto que conducen a una luminosa habitación doble con armarios empotrados y acceso a una pequeña salida exterior. Un baño completo con plato de ducha. La cocina es abierta y viene completamente equipada con electrodomésticos y placas de inducción. El suelo es hidráulico. Dispone de zona de aguas independiente. Un amplio y luminoso comedor con dos grandes ventanales y vistas al patio del Eixample. El dormitorio principal con baño en suite; con plato de ducha, bañera de hidromasaje y suelos de microcemento. Orientado al exterior y también con armarios empotrados. El piso incluye sistema de ósmosis en la cocina, aire acodicionado, calefacción, suelos de parqué y persianas eléctricas. Ubicado en Rambla Catalunya, una de las calles más exclusivas de la ciudad, en una 5º planta de una magnífica finca regia con servicio de consejería y ascensir. La vivienda goza de mucha tranquilidad a pesar de su ubicación tan céntrica. Con VISITA SEGURA de Walter Haus podrás seguir alquilando y vendiendo tu piso con total seguridad. Nuestras viviendas y las visitas que realizamos están libres de Covid-19 gracias al protocolo que hemos desarrollado: •Visitas Virtuales •Desinfección con ozono •Kit de seguridad •Firma digital Todo para que puedas seguir alquilando y vendiendo tu piso con total normalidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 7719.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98000858', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8b/d9/71/997711176.jpg', 'externalReference': '3835V', 'numPhotos': 36, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 114.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3902528, 'longitude': 2.1608339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98000858/', 'distance': '804', 'description': 'Espectacular y exclusiva vivienda de 114m2, distribuida en un amplio recibidor con paredes de ladrillo visto que conducen a una luminosa habitación doble con armarios empotrados y acceso a una pequeña salida exterior. Un baño completo con plato de ducha. La cocina es abierta y viene completamente equipada con electrodomésticos y placas de inducción. El suelo es hidráulico. Dispone de zona de aguas independiente. Un amplio y luminoso comedor con dos grandes ventanales y vistas al patio del Eixample. El dormitorio principal con baño en suite; con plato de ducha, bañera de hidromasaje y suelos de microcemento. Orientado al exterior y también con armarios empotrados. El piso incluye sistema de ósmosis en la cocina, aire acodicionado, calefacción, suelos de parqué y persianas eléctricas. Ubicado en Rambla Catalunya, una de las calles más exclusivas de la ciudad, en una 5º planta de una magnífica finca regia con servicio de consejería y ascensir. La vivienda goza de mucha tranquilidad a pesar de su ubicación tan céntrica. Con VISITA SEGURA de Walter Haus podrás seguir alquilando y vendiendo tu piso con total seguridad. Nuestras viviendas y las visitas que realizamos están libres de Covid-19 gracias al protocolo que hemos desarrollado: •Visitas Virtuales •Desinfección con ozono •Kit de seguridad •Firma digital Todo para que puedas seguir alquilando y vendiendo tu piso con total normalidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 7719.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98676867', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5d/9f/10/1052038319.jpg', 'externalReference': 'KB1508', 'numPhotos': 25, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 132.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3904528, 'longitude': 2.1637339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98676867/', 'distance': '600', 'description': 'Excelente propiedad en la quinta planta de un edificio histórico de Rambla Catalunya, una de las mejores calles de Barcelona. En una de las zonas más lujosas nos encontramos con esta exclusiva propiedad que ofrece todas las comodidades de un moderno apartamento en un entorno único y con uno acabados interiores excelentes. Exterior a patio de manzana, dispone de grandes ventanales que inundan de luz sus estancias. Su entrada está perfectamente trabajada y nos ofrece calidez mediante sus preciosos ventanales y sus paredes originales. La moderna cocina, abierta al salón conjuga un precioso diseño con una excelente funcionalidad y su ubicación facilita mucho la accesibilidad al salón. El suelo es de madera natural. Una de las habitaciones con armarios empotrados, tiene salida a una terraza y goza de mucha luminosidad. Encontramos un baño completo con ducha y baldosas hidráulicas. La habitación principal es suite con armarios empotrados y dispone también de un enorme y luminoso baño con bañera de hidromasaje con cascada y amplia ducha. La habitación tiene amplios ventanales también que le dan luz y vistas despejadas.  El inmueble ha sido recientemente renovado con acabados de máxima calidad e insonorizado en su totalidad, dispone de persianas eléctricas, aire acondicionado por conductos y calefacción por gas natural. El edificio dispone de conserje a jornada completa y ascensor. La ubicación es excelente, cerca del transporte público, en el cuadrado de oro de Barcelona, en una de las mejores calles y a escasos pasos de Passeig de gràcia o Plaza Catalunya. Un pedazo de la historia de Barcelona en una de las mejore ubicaciones de la ciudad. Estaremos encantados de poder mostrarselo.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6667.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98676867', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5d/9f/10/1052038319.jpg', 'externalReference': 'KB1508', 'numPhotos': 25, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 132.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3904528, 'longitude': 2.1637339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98676867/', 'distance': '600', 'description': 'Excelente propiedad en la quinta planta de un edificio histórico de Rambla Catalunya, una de las mejores calles de Barcelona. En una de las zonas más lujosas nos encontramos con esta exclusiva propiedad que ofrece todas las comodidades de un moderno apartamento en un entorno único y con uno acabados interiores excelentes. Exterior a patio de manzana, dispone de grandes ventanales que inundan de luz sus estancias. Su entrada está perfectamente trabajada y nos ofrece calidez mediante sus preciosos ventanales y sus paredes originales. La moderna cocina, abierta al salón conjuga un precioso diseño con una excelente funcionalidad y su ubicación facilita mucho la accesibilidad al salón. El suelo es de madera natural. Una de las habitaciones con armarios empotrados, tiene salida a una terraza y goza de mucha luminosidad. Encontramos un baño completo con ducha y baldosas hidráulicas. La habitación principal es suite con armarios empotrados y dispone también de un enorme y luminoso baño con bañera de hidromasaje con cascada y amplia ducha. La habitación tiene amplios ventanales también que le dan luz y vistas despejadas.  El inmueble ha sido recientemente renovado con acabados de máxima calidad e insonorizado en su totalidad, dispone de persianas eléctricas, aire acondicionado por conductos y calefacción por gas natural. El edificio dispone de conserje a jornada completa y ascensor. La ubicación es excelente, cerca del transporte público, en el cuadrado de oro de Barcelona, en una de las mejores calles y a escasos pasos de Passeig de gràcia o Plaza Catalunya. Un pedazo de la historia de Barcelona en una de las mejore ubicaciones de la ciudad. Estaremos encantados de poder mostrarselo.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6667.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99119853', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/fd/90/38/1034166911.jpg', 'externalReference': 'PBARDE 39', 'numPhotos': 51, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 170.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3873408, 'longitude': 2.1621522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99119853/', 'distance': '633', 'description': 'Terraza soleada de 40 metros orientada al mar, en una propiedad de obra nueva que da a las 2 fachadas, con acabados de altísima calidad, suelos radiantes, hidrotermia, domótica, reguladores de la intensidad de la luz, y todo el glamour que caracteriza a este barrio del Eixample de Barcelona.  La vivienda está ubicada a 100 metros de Plaza Universidad, en una finca completamente rehabilitada con ascensor.  A la entrada a la izquierda encontramos una elegante y moderna cocina abierta al salón comedor, con salida a un balcón que discurre por la calle Diputació. En esta zona también se halla un aseo de cortesía, el equipo de hidrotermia y el dispositivo táctil para la domótica de la casa.  En la parte posterior del piso se encuentran las dos habitaciones dobles, ambas con baños completos en suite, armarios con iluminación led interior, y mucha luz y sol.  A continuación del dormitorio principal encontramos la joya de la corona, su gran terraza. De la misma solo podemos añadir que, si a la funcionalidad y elegancia de unas magníficas reformas de alto standing, sumamos el hecho de tener este espacio exterior con sol todo el año, en el barrio seguramente con más Flow de Barcelona, podemos considerar que nos encontramos ante una vivienda única, difícilmente superable. Cabe señalar que es un piso con amplias estancias, se trata de 130 metros construidos para tres ambientes principales, salón y dos habitaciones dobles, con lo cual nos ofrece mucha versatilidad: salón comedor en la zona de los balcones que dan a la calle, como está distribuido ahora, o salón comedor hacia la terraza. Como hablamos de un solo piso por rellano, las dimensiones de la estancia trasera y la delantera son idénticas, o sea, que sin demasiado cambio se podría distribuir según nuestras preferencias. El barrio y esa calle en concreto se caracteriza por su encanto, con bares de moda, estilo, buen rollo y ese encanto urbanita de sus comercios y tiendas siempre a la vanguardia. Casi en los bajos del edificio encontramos una estación de Bicing, por si somos de los que prefieren moverse de esta forma por la ciudad.  Le invitamos a visitar este magnífico inmueble con QUATRECASES, y disfrutar de la experiencia.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4988.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99119853', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/fd/90/38/1034166911.jpg', 'externalReference': 'PBARDE 39', 'numPhotos': 51, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 170.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3873408, 'longitude': 2.1621522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99119853/', 'distance': '633', 'description': 'Terraza soleada de 40 metros orientada al mar, en una propiedad de obra nueva que da a las 2 fachadas, con acabados de altísima calidad, suelos radiantes, hidrotermia, domótica, reguladores de la intensidad de la luz, y todo el glamour que caracteriza a este barrio del Eixample de Barcelona.  La vivienda está ubicada a 100 metros de Plaza Universidad, en una finca completamente rehabilitada con ascensor.  A la entrada a la izquierda encontramos una elegante y moderna cocina abierta al salón comedor, con salida a un balcón que discurre por la calle Diputació. En esta zona también se halla un aseo de cortesía, el equipo de hidrotermia y el dispositivo táctil para la domótica de la casa.  En la parte posterior del piso se encuentran las dos habitaciones dobles, ambas con baños completos en suite, armarios con iluminación led interior, y mucha luz y sol.  A continuación del dormitorio principal encontramos la joya de la corona, su gran terraza. De la misma solo podemos añadir que, si a la funcionalidad y elegancia de unas magníficas reformas de alto standing, sumamos el hecho de tener este espacio exterior con sol todo el año, en el barrio seguramente con más Flow de Barcelona, podemos considerar que nos encontramos ante una vivienda única, difícilmente superable. Cabe señalar que es un piso con amplias estancias, se trata de 130 metros construidos para tres ambientes principales, salón y dos habitaciones dobles, con lo cual nos ofrece mucha versatilidad: salón comedor en la zona de los balcones que dan a la calle, como está distribuido ahora, o salón comedor hacia la terraza. Como hablamos de un solo piso por rellano, las dimensiones de la estancia trasera y la delantera son idénticas, o sea, que sin demasiado cambio se podría distribuir según nuestras preferencias. El barrio y esa calle en concreto se caracteriza por su encanto, con bares de moda, estilo, buen rollo y ese encanto urbanita de sus comercios y tiendas siempre a la vanguardia. Casi en los bajos del edificio encontramos una estación de Bicing, por si somos de los que prefieren moverse de esta forma por la ciudad.  Le invitamos a visitar este magnífico inmueble con QUATRECASES, y disfrutar de la experiencia.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4988.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98192535', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/eb/3a/00/1003587995.jpg', 'externalReference': 'W-02I8M0', 'numPhotos': 31, 'floor': '5', 'price': 1619000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 207.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle del Tenor Viñas', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sarrià-Sant Gervasi', 'country': 'es', 'neighborhood': 'Sant Gervasi - Galvany', 'latitude': 41.3937255, 'longitude': 2.1418776, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98192535/', 'distance': '2426', 'description': 'Espectacular ático con terraza en Turó Parc En una de las mejores fincas de la zona se sitúa este ático con una espectacular terraza de 135 metros. Se trata de un piso de 142 metros cuadrados, reformado, en el que antiguamente tenía 4 dormitorios, y ahora con la reforma tiene 2 grandes suites. El piso tiene un bonito recibidor que nos conduce a la zona de día, una bonita cocina con una zona de lavadero y al esplendido salón comedor con chimenea de mármol y salida directa a la terraza. En el pasillo encontramos un aseo de cortesía y la zona de noche con las 2 magníficas suites también con acceso a la terraza. La terraza tiene forma de L pudiendo crear en ella diferentes ambientes.  Se trata de una finca de lujo, con servicio de portería, 2 ascensores y posibilidad de alquilar parking en la misma finca. El Turó Parc es una de las zonas más demandadas de la ciudad. La elegancia y el prestigio son las características que definen tanto sus edificios como sus habitantes. Se trata de una zona muy segura, con todo tipo de comercios, servicios y ocio. El Turó Parc es la esencia del espíritu más sofisticado de Barcelona, sin perder al mismo tiempo la dimensión más pura y la calidez del barrio.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 7821.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': 'Sant Gervasi - Galvany, Barcelona', 'title': 'Ático en Calle del Tenor Viñas'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98192535', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/eb/3a/00/1003587995.jpg', 'externalReference': 'W-02I8M0', 'numPhotos': 31, 'floor': '5', 'price': 1619000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 207.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle del Tenor Viñas', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sarrià-Sant Gervasi', 'country': 'es', 'neighborhood': 'Sant Gervasi - Galvany', 'latitude': 41.3937255, 'longitude': 2.1418776, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98192535/', 'distance': '2426', 'description': 'Espectacular ático con terraza en Turó Parc En una de las mejores fincas de la zona se sitúa este ático con una espectacular terraza de 135 metros. Se trata de un piso de 142 metros cuadrados, reformado, en el que antiguamente tenía 4 dormitorios, y ahora con la reforma tiene 2 grandes suites. El piso tiene un bonito recibidor que nos conduce a la zona de día, una bonita cocina con una zona de lavadero y al esplendido salón comedor con chimenea de mármol y salida directa a la terraza. En el pasillo encontramos un aseo de cortesía y la zona de noche con las 2 magníficas suites también con acceso a la terraza. La terraza tiene forma de L pudiendo crear en ella diferentes ambientes.  Se trata de una finca de lujo, con servicio de portería, 2 ascensores y posibilidad de alquilar parking en la misma finca. El Turó Parc es una de las zonas más demandadas de la ciudad. La elegancia y el prestigio son las características que definen tanto sus edificios como sus habitantes. Se trata de una zona muy segura, con todo tipo de comercios, servicios y ocio. El Turó Parc es la esencia del espíritu más sofisticado de Barcelona, sin perder al mismo tiempo la dimensión más pura y la calidez del barrio.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 7821.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': 'Sant Gervasi - Galvany, Barcelona', 'title': 'Ático en Calle del Tenor Viñas'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '89103723', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b0/f6/f1/976630614.jpg', 'externalReference': '019264', 'numPhotos': 31, 'price': 768000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 149.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3874885, 'longitude': 2.1594455, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/89103723/', 'distance': '859', 'description': 'Exclusivo piso de diseño y obra nueva a estrenar de 149m² situado en calle Diputació, junto la calle Muntaner. Dispone de un amplio y luminoso salón comedor con cocina independiente, 1 espacioso recibidor, 2 habitaciones dobles suite (25m² y 14m² respectivamente), 2 baños completos y 1 aseo de cortesía. Excelentes acabados. Cuenta con suelos de mármol, aire acondicionado (frío - calor), calefacción a gas y carpintería exterior de aluminio. Exterior y soleado. Ubicado en una finca regia de 1886 rehabilitada que dispone de una gran terraza comunitaria, un espacio de 60m² con zona “chill out” y unas preciosas vistas de Barcelona. En la rehabilitación se han utilizado los mejores materiales con un diseño muy elegante, creando espacios actuales y acogedores. El proyecto de reforma ha sido realizado por Jaime Beriestain Studio, que cuenta con reconocimiento de nivel mundial. Muy bien comunicado con transporte público, autobuses y metro (parada- Universitat). Una magnífica oportunidad para adquirir una lujosa vivienda a estrenar en el corazón de Barcelona. "Contacte con nosotros para solicitar más información o visitar el inmueble".', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5154.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '89103723', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b0/f6/f1/976630614.jpg', 'externalReference': '019264', 'numPhotos': 31, 'price': 768000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 149.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3874885, 'longitude': 2.1594455, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/89103723/', 'distance': '859', 'description': 'Exclusivo piso de diseño y obra nueva a estrenar de 149m² situado en calle Diputació, junto la calle Muntaner. Dispone de un amplio y luminoso salón comedor con cocina independiente, 1 espacioso recibidor, 2 habitaciones dobles suite (25m² y 14m² respectivamente), 2 baños completos y 1 aseo de cortesía. Excelentes acabados. Cuenta con suelos de mármol, aire acondicionado (frío - calor), calefacción a gas y carpintería exterior de aluminio. Exterior y soleado. Ubicado en una finca regia de 1886 rehabilitada que dispone de una gran terraza comunitaria, un espacio de 60m² con zona “chill out” y unas preciosas vistas de Barcelona. En la rehabilitación se han utilizado los mejores materiales con un diseño muy elegante, creando espacios actuales y acogedores. El proyecto de reforma ha sido realizado por Jaime Beriestain Studio, que cuenta con reconocimiento de nivel mundial. Muy bien comunicado con transporte público, autobuses y metro (parada- Universitat). Una magnífica oportunidad para adquirir una lujosa vivienda a estrenar en el corazón de Barcelona. "Contacte con nosotros para solicitar más información o visitar el inmueble".', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5154.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98269623', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a3/9c/10/1006157929.jpg', 'externalReference': 'VB2112040-1', 'numPhotos': 28, 'floor': 'en', 'price': 369000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 70.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "Calle d'Aribau", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3948237, 'longitude': 2.1524215, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98269623/', 'distance': '1660', 'description': 'Piso con terraza en venta en Calle Aribau Esta vivienda está ubicada en la Calle Aribau, cerca de la Diagonal y Enric Granados. Es un entresuelo, de 63m2 construidos, tiene una excelente ubicación en una finca clásica que conserva los elementos originales de la época, con ascensor y terrado comunitario. La zona de día consta de un amplio salón-comedor con salida a una terraza de 14m2, muy disfrutable, soleada y tranquila. Dispone de dos armarios para lavadora y secadora. Cocina equipada independiente, con la posibilidad de poderse abrir al salón-comedor. La zona de noche tiene un dormitorio principal y un baño completo en suite, un segundo dormitorio/despacho adjunto, con salida a la terraza. Tiene también baño completo con ducha. Suelos de parqué, aire acondicionado (frío/calor) calefacción, acumulador de agua, gran equipamiento de armarios, toldo eléctrico. ITE del edificio pasada.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 5271.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': "Piso en Calle d'Aribau"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98269623', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a3/9c/10/1006157929.jpg', 'externalReference': 'VB2112040-1', 'numPhotos': 28, 'floor': 'en', 'price': 369000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 70.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "Calle d'Aribau", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3948237, 'longitude': 2.1524215, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98269623/', 'distance': '1660', 'description': 'Piso con terraza en venta en Calle Aribau Esta vivienda está ubicada en la Calle Aribau, cerca de la Diagonal y Enric Granados. Es un entresuelo, de 63m2 construidos, tiene una excelente ubicación en una finca clásica que conserva los elementos originales de la época, con ascensor y terrado comunitario. La zona de día consta de un amplio salón-comedor con salida a una terraza de 14m2, muy disfrutable, soleada y tranquila. Dispone de dos armarios para lavadora y secadora. Cocina equipada independiente, con la posibilidad de poderse abrir al salón-comedor. La zona de noche tiene un dormitorio principal y un baño completo en suite, un segundo dormitorio/despacho adjunto, con salida a la terraza. Tiene también baño completo con ducha. Suelos de parqué, aire acondicionado (frío/calor) calefacción, acumulador de agua, gran equipamiento de armarios, toldo eléctrico. ITE del edificio pasada.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 5271.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': "Piso en Calle d'Aribau"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99268088', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/1d/34/d4/1038618419.jpg', 'externalReference': 'VB2210039', 'numPhotos': 28, 'floor': '3', 'price': 299000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 62.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de la Riereta', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3778121, 'longitude': 2.1688796, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99268088/', 'distance': '1076', 'description': 'Piso reformado con terraza en venta en la calle Riereta Preciosa vivienda totalmente reformada en 2019 situada a escasos metros de la Rambla del Raval y muy bien ubicada en el centro de Barcelona. La calle Riereta es una calle muy tranquila en la que se combinan edificios clásicos y edificios de recién construcción. El piso se encuentra en una tercera planta real en una finca de 1860 SIN ASCENSOR, rehabilitada y en muy buen estado de conservación, con terrado comunitario practicable con estupendas vistas a la ciudad de Barcelona y a la montaña de Montjuic. Se distribuye de la siguiente forma: dos habitaciones dobles exteriores a calle, baño completo, zona de aguas, cocina abierta al comedor, salón independiente con salida a terraza a nivel que orienta a un tranquilo y amplio patio de manzana. Doble orientación NE y SO. La propiedad se reformó en 2019. Los suelos son de gres imitación madera. Cerramientos de doble cristal en todas las estancias, aire acondicionado y calefacción por splits, puerta blindada, cocina equipada con todos los electrodomésticos, volta catalana y vigas vistas de madera, termo de agua caliente de 100L y alarma de Securitas Direct. Es un piso ideal como piso vacacional o como inversión por su alta rentabilidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 4823.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de la Riereta'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99268088', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/1d/34/d4/1038618419.jpg', 'externalReference': 'VB2210039', 'numPhotos': 28, 'floor': '3', 'price': 299000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 62.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de la Riereta', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3778121, 'longitude': 2.1688796, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99268088/', 'distance': '1076', 'description': 'Piso reformado con terraza en venta en la calle Riereta Preciosa vivienda totalmente reformada en 2019 situada a escasos metros de la Rambla del Raval y muy bien ubicada en el centro de Barcelona. La calle Riereta es una calle muy tranquila en la que se combinan edificios clásicos y edificios de recién construcción. El piso se encuentra en una tercera planta real en una finca de 1860 SIN ASCENSOR, rehabilitada y en muy buen estado de conservación, con terrado comunitario practicable con estupendas vistas a la ciudad de Barcelona y a la montaña de Montjuic. Se distribuye de la siguiente forma: dos habitaciones dobles exteriores a calle, baño completo, zona de aguas, cocina abierta al comedor, salón independiente con salida a terraza a nivel que orienta a un tranquilo y amplio patio de manzana. Doble orientación NE y SO. La propiedad se reformó en 2019. Los suelos son de gres imitación madera. Cerramientos de doble cristal en todas las estancias, aire acondicionado y calefacción por splits, puerta blindada, cocina equipada con todos los electrodomésticos, volta catalana y vigas vistas de madera, termo de agua caliente de 100L y alarma de Securitas Direct. Es un piso ideal como piso vacacional o como inversión por su alta rentabilidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 4823.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de la Riereta'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98985637', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/2d/73/6b/1030519082.jpg', 'externalReference': 'VB2209039', 'numPhotos': 27, 'floor': 'en', 'price': 325000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 69.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de Ribes', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'El Fort Pienc', 'latitude': 41.4015389, 'longitude': 2.1846789, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98985637/', 'distance': '1999', 'description': 'Piso en venta frente al Auditori y al Teatre Nacional En el barrio de Fortpienc, frente al Teatre Nacional y al Auditori de Barcelona, muy cerca dels Encants nous y de la Plaça de les Glòries, encontramos esta propiedad, situada en una finca clásica de 1890, en muy buen estado de conservación, con ascensor y con doble orientación. El piso se reformó en 2004 y actualmente su estado de conservación es muy bueno. Se vende completamente equipado y amueblado. Consta de 69m2 construidos, 57m2 útiles y dos balcones, el que da a calle de 2m2 y el que está en la habitación de 3,25m2. Se distribuye de la siguiente manera: salón independiente exterior a la calle Ribes, con salida directa a balcón, con orientación sur. Cocina abierta al comedor. Baño completo con ventilación natural. Dormitorio individual amplio con ventana a patio interior de la finca. Dormitorio doble con salida a balcón. La zona de aguas se encuentra en el balcón al lado de la habitación de matrimonio. Termo de agua caliente eléctrico, ventanas de aluminio, splits de aire frío y caliente. Cocina equipada con vitro, campana extractora, horno, lavaplatos y nevera-congelador. La ubicación de esta vivienda es inmejorable, cerca de todos los servicios, bien comunicado, con aparcamiento público frente al edificio, el centro comercial Glòries a 10 minutos caminando, transporte público (bus, metro, tranvía), comercios y restaurantes. ¡No dudes en contactar con nosotros para ver esta magnífica propiedad!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4710.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Fort Pienc, Barcelona', 'title': 'Piso en Calle de Ribes'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98985637', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/2d/73/6b/1030519082.jpg', 'externalReference': 'VB2209039', 'numPhotos': 27, 'floor': 'en', 'price': 325000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 69.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de Ribes', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'El Fort Pienc', 'latitude': 41.4015389, 'longitude': 2.1846789, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98985637/', 'distance': '1999', 'description': 'Piso en venta frente al Auditori y al Teatre Nacional En el barrio de Fortpienc, frente al Teatre Nacional y al Auditori de Barcelona, muy cerca dels Encants nous y de la Plaça de les Glòries, encontramos esta propiedad, situada en una finca clásica de 1890, en muy buen estado de conservación, con ascensor y con doble orientación. El piso se reformó en 2004 y actualmente su estado de conservación es muy bueno. Se vende completamente equipado y amueblado. Consta de 69m2 construidos, 57m2 útiles y dos balcones, el que da a calle de 2m2 y el que está en la habitación de 3,25m2. Se distribuye de la siguiente manera: salón independiente exterior a la calle Ribes, con salida directa a balcón, con orientación sur. Cocina abierta al comedor. Baño completo con ventilación natural. Dormitorio individual amplio con ventana a patio interior de la finca. Dormitorio doble con salida a balcón. La zona de aguas se encuentra en el balcón al lado de la habitación de matrimonio. Termo de agua caliente eléctrico, ventanas de aluminio, splits de aire frío y caliente. Cocina equipada con vitro, campana extractora, horno, lavaplatos y nevera-congelador. La ubicación de esta vivienda es inmejorable, cerca de todos los servicios, bien comunicado, con aparcamiento público frente al edificio, el centro comercial Glòries a 10 minutos caminando, transporte público (bus, metro, tranvía), comercios y restaurantes. ¡No dudes en contactar con nosotros para ver esta magnífica propiedad!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4710.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Fort Pienc, Barcelona', 'title': 'Piso en Calle de Ribes'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98374038', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/4a/c7/58/1009839184.jpg', 'externalReference': 'VB2207045', 'numPhotos': 47, 'floor': '3', 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 77.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Riereta', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3791652, 'longitude': 2.1708504, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98374038/', 'distance': '928', 'description': 'Loft de Obra Nueva con jardín y piscina en el centro histórico de Barcelona  Preciosa vivienda en edificio de obra nueva del 2021 en el centro de Barcelona. Se trata de una rehabilitación integral de una antigua fábrica textil de 1833, creando unas viviendas únicas de estilo neoyorquino con grande ventanales y techos de doble altura con vigas de madera y paredes de ladrillo visto. El piso estilo loft se encuentra en la planta tercera, tiene una superficie de 74 m2, más una terraza cubierta de 6 m2 que da a las zonas comunitarias. Los materiales utilizados son de la más alta calidad y además consta de algunos elementos recuperados. Se compone de cocina totalmente equipada, salón, comedor, un dormitorio doble con baño en suite, y otro baño completo. Además, se ha aprovechado de la altura de los techos para realizar un altillo de 12 m2 donde ahora se ubica otro dormitorio doble. El edificio cuenta con zonas comunes que incluyen piscina y solárium con impresionantes vistas a la ciudad, huertos urbanos, jardines verticales, sistema de climatización por Aerotermia, servicio conserjería, video vigilancia 24h, reciclaje de aguas pluviales, parking para bicicletas y un atrio en medio del complejo lleno de tragaluces y árboles. Una oportunidad única para vivir una nueva experiencia en la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6299.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de la Riereta'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98374038', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/4a/c7/58/1009839184.jpg', 'externalReference': 'VB2207045', 'numPhotos': 47, 'floor': '3', 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 77.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Riereta', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3791652, 'longitude': 2.1708504, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98374038/', 'distance': '928', 'description': 'Loft de Obra Nueva con jardín y piscina en el centro histórico de Barcelona  Preciosa vivienda en edificio de obra nueva del 2021 en el centro de Barcelona. Se trata de una rehabilitación integral de una antigua fábrica textil de 1833, creando unas viviendas únicas de estilo neoyorquino con grande ventanales y techos de doble altura con vigas de madera y paredes de ladrillo visto. El piso estilo loft se encuentra en la planta tercera, tiene una superficie de 74 m2, más una terraza cubierta de 6 m2 que da a las zonas comunitarias. Los materiales utilizados son de la más alta calidad y además consta de algunos elementos recuperados. Se compone de cocina totalmente equipada, salón, comedor, un dormitorio doble con baño en suite, y otro baño completo. Además, se ha aprovechado de la altura de los techos para realizar un altillo de 12 m2 donde ahora se ubica otro dormitorio doble. El edificio cuenta con zonas comunes que incluyen piscina y solárium con impresionantes vistas a la ciudad, huertos urbanos, jardines verticales, sistema de climatización por Aerotermia, servicio conserjería, video vigilancia 24h, reciclaje de aguas pluviales, parking para bicicletas y un atrio en medio del complejo lleno de tragaluces y árboles. Una oportunidad única para vivir una nueva experiencia en la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6299.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de la Riereta'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98272281', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/df/38/a0/1006238408.jpg', 'externalReference': 'VB2206060', 'numPhotos': 29, 'floor': 'en', 'price': 345000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 63.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle d'Enric Granados", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3923655, 'longitude': 2.1573188, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98272281/', 'distance': '1170', 'description': 'Piso reformado de 2 habitaciones en la Calle Enric Granados Situado en una de las calles más emblemáticas de Barcelona i del Eixample Esquerra, rodeado de todo tipo de servicios, restaurantes, cafeterías y muy bien comunicado, se encuentra este bonito, reformado y práctico piso ubicado en una finca Regia con estilo del 1900. La vivienda, de 63 m2, está para entrar a vivir y se encuentra en una planta baja por lo que disfruta de una agradable terraza, muy agradable y tranquila orientada a Noreste de 12 m2. El piso dispone de dos habitaciones dobles, y una de ellas tiene una galería con vistas a la terraza, ideal para ubicar un despacho, por ejemplo. La segunda, interior y con salida a patio de luces, completa Completa este práctico piso la cocina / salón desde donde también se accede a la terraza, que permite disfrutar del sol y el aire libre en un espacio alegre. Ven a visitar este bonito y céntrico piso en Barcelona!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5476.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': "Piso en Calle d'Enric Granados"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98272281', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/df/38/a0/1006238408.jpg', 'externalReference': 'VB2206060', 'numPhotos': 29, 'floor': 'en', 'price': 345000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 63.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle d'Enric Granados", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3923655, 'longitude': 2.1573188, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98272281/', 'distance': '1170', 'description': 'Piso reformado de 2 habitaciones en la Calle Enric Granados Situado en una de las calles más emblemáticas de Barcelona i del Eixample Esquerra, rodeado de todo tipo de servicios, restaurantes, cafeterías y muy bien comunicado, se encuentra este bonito, reformado y práctico piso ubicado en una finca Regia con estilo del 1900. La vivienda, de 63 m2, está para entrar a vivir y se encuentra en una planta baja por lo que disfruta de una agradable terraza, muy agradable y tranquila orientada a Noreste de 12 m2. El piso dispone de dos habitaciones dobles, y una de ellas tiene una galería con vistas a la terraza, ideal para ubicar un despacho, por ejemplo. La segunda, interior y con salida a patio de luces, completa Completa este práctico piso la cocina / salón desde donde también se accede a la terraza, que permite disfrutar del sol y el aire libre en un espacio alegre. Ven a visitar este bonito y céntrico piso en Barcelona!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5476.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': "Piso en Calle d'Enric Granados"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98271905', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/e5/49/6f/1006228158.jpg', 'externalReference': 'VB2206005', 'numPhotos': 41, 'floor': 'bj', 'price': 480000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 139.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "Calle d'en Carabassa", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3811984, 'longitude': 2.1775831, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98271905/', 'distance': '956', 'description': 'Piso en venta reformado con bodega de 47m2 al lado de la Iglesia de la Mercè A escasos pasos de la Basílica de la Mercè y del Moll de la Fusta, en el pleno centro del barrio Gótico con más historia de la ciudad, encontramos este apartamento de 92m2 construidos totalmente rehabilitado, situado en la primera planta de una finca de 1890 con ascensor, orientación Sur. El piso, gracias a su rehabilitación integral de todo el edificio, combina las ventajas de una construcción nueva con elementos originales, lo que sin duda hacen de está vivienda una pieza única. A destacar las zonas comunes con el terrado de uso comunitario con vistas a la ciudad y totalmente acondicionado con barbacoa, baño y sala de reuniones. Zona de parking para bicicletas en la entrada de la vivienda, y un largo etc. Sus 139m2 están compuestos de una bodega en la planta –1 de 47m2 totalmente habilitada y el piso de 92m2 que consta dde un amplio salón comedor con una cocina totalmente integrada y equipada, una suite con baño, una habitación semi doble y un baño completo. La zona de aguas está contigua a la cocina. Las ventanas del piso son de aluminio con rotura de puente térmico y doble cristal, para garantizar un aislamiento térmico y acústico. Sistema de eficiencia energética mediante aerotermia, los suelos están pavimentados con parquet en madera y los baños con gres porcelánico. Terrado de uso comunitario con vistas a la ciudad y totalmente acondicionado con barbacoa, baño y sala de reuniones. Si quiere vivir en el barrio gótico, no dudes en pedirnos visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3453.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': "Piso en Calle d'en Carabassa"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98271905', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/e5/49/6f/1006228158.jpg', 'externalReference': 'VB2206005', 'numPhotos': 41, 'floor': 'bj', 'price': 480000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 139.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "Calle d'en Carabassa", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3811984, 'longitude': 2.1775831, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98271905/', 'distance': '956', 'description': 'Piso en venta reformado con bodega de 47m2 al lado de la Iglesia de la Mercè A escasos pasos de la Basílica de la Mercè y del Moll de la Fusta, en el pleno centro del barrio Gótico con más historia de la ciudad, encontramos este apartamento de 92m2 construidos totalmente rehabilitado, situado en la primera planta de una finca de 1890 con ascensor, orientación Sur. El piso, gracias a su rehabilitación integral de todo el edificio, combina las ventajas de una construcción nueva con elementos originales, lo que sin duda hacen de está vivienda una pieza única. A destacar las zonas comunes con el terrado de uso comunitario con vistas a la ciudad y totalmente acondicionado con barbacoa, baño y sala de reuniones. Zona de parking para bicicletas en la entrada de la vivienda, y un largo etc. Sus 139m2 están compuestos de una bodega en la planta –1 de 47m2 totalmente habilitada y el piso de 92m2 que consta dde un amplio salón comedor con una cocina totalmente integrada y equipada, una suite con baño, una habitación semi doble y un baño completo. La zona de aguas está contigua a la cocina. Las ventanas del piso son de aluminio con rotura de puente térmico y doble cristal, para garantizar un aislamiento térmico y acústico. Sistema de eficiencia energética mediante aerotermia, los suelos están pavimentados con parquet en madera y los baños con gres porcelánico. Terrado de uso comunitario con vistas a la ciudad y totalmente acondicionado con barbacoa, baño y sala de reuniones. Si quiere vivir en el barrio gótico, no dudes en pedirnos visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3453.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': "Piso en Calle d'en Carabassa"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98271257', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f4/c7/a6/1006207841.jpg', 'externalReference': 'VB2203084-1', 'numPhotos': 34, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 110.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3928528, 'longitude': 2.1615339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98271257/', 'distance': '909', 'description': 'Piso de diseño en venta en Rambla Catalunya En la Rambla Catalunya, una de las calles más exclusivas de la ciudad encontramos esta magnífica vivienda en una preciosa finca regia con servicio de conserjería y ascensor. El piso consta de 110m2 y gracias a su altura y orientación, goza de mucha tranquilidad a pesar de su ubicación tan céntrica. Al entrar, un amplio pasillo con pared de ladrillo visto nos conduce a un dormitorio doble con armario empotrado y salida a una pequeña terraza. Sus puertas cristaleras confieren al piso una sensación maravillosa de espacio y luz. En la habitación contigua el lavadero con armario empotrado y en frente un baño completo con ducha. A continuación, la moderna cocina office, equipada con electrodomésticos de primera categoría y con espacio para mesa de 6 comensales. Seguidamente accedemos al amplio salón que gracias a su grandes ventanales y orientación a bonito patio de manzana goza de muchísima luz natural. El segundo dormitorio es el principal, orientado al exterior, con armarios empotrados y con baño completo con ducha y bañera de hidromasaje en suite. El piso dispone de suelos de parquet, calefacción por radiadores, aire acondicionado por conductos y ventanas con doble acristalamiento. ¡Contacta con nosotros hoy para visitar esta propiedad única en la zona más exclusiva de L’Eixample!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8000.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98271257', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f4/c7/a6/1006207841.jpg', 'externalReference': 'VB2203084-1', 'numPhotos': 34, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 110.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3928528, 'longitude': 2.1615339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98271257/', 'distance': '909', 'description': 'Piso de diseño en venta en Rambla Catalunya En la Rambla Catalunya, una de las calles más exclusivas de la ciudad encontramos esta magnífica vivienda en una preciosa finca regia con servicio de conserjería y ascensor. El piso consta de 110m2 y gracias a su altura y orientación, goza de mucha tranquilidad a pesar de su ubicación tan céntrica. Al entrar, un amplio pasillo con pared de ladrillo visto nos conduce a un dormitorio doble con armario empotrado y salida a una pequeña terraza. Sus puertas cristaleras confieren al piso una sensación maravillosa de espacio y luz. En la habitación contigua el lavadero con armario empotrado y en frente un baño completo con ducha. A continuación, la moderna cocina office, equipada con electrodomésticos de primera categoría y con espacio para mesa de 6 comensales. Seguidamente accedemos al amplio salón que gracias a su grandes ventanales y orientación a bonito patio de manzana goza de muchísima luz natural. El segundo dormitorio es el principal, orientado al exterior, con armarios empotrados y con baño completo con ducha y bañera de hidromasaje en suite. El piso dispone de suelos de parquet, calefacción por radiadores, aire acondicionado por conductos y ventanas con doble acristalamiento. ¡Contacta con nosotros hoy para visitar esta propiedad única en la zona más exclusiva de L’Eixample!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8000.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98269646', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/0e/44/3a/1006158045.jpg', 'externalReference': 'VB2112041-1', 'numPhotos': 34, 'floor': '1', 'price': 750000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 140.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de les Jonqueres', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3867007, 'longitude': 2.1744305, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98269646/', 'distance': '400', 'description': 'Piso tipo Loft en venta en la calle Jonqueres Este loft está situado en Born, muy cerca del Palau de la Musica, en un edificio original del 1870 que había sido un antiguo convento y se rehabilitó íntegramente en el año 1997. En la entrada del edificio hay un amplio recibidor que da acceso a la escalera y al ascensor. En el primer piso encontramos una zona comunitaria ajardinada central donde se ubicaba en el antiguo claustro, que da acceso a la propiedad. La vivienda es toda exterior, con amplios ventanales al tranquilo y silencioso espacio central del edificio. El loft se reformó hace unos 13 años y mantiene ese encanto bohemio tan característico de la zona. En la entrada encontramos el recibidor abierto al amplio salón-comedor con cocina abierta. Está rodeado de grandes ventanales con mucha luz. Tiene acceso a una amplia terraza de 40m2, una zona muy tranquila y luminosa. En la misma planta hay un dormitorio doble con baño completo y en la zona del altillo (planta escriturada) se encuentra el segundo dormitorio abierto al espacio del salón, también dispone de un baño completo en suite. El techo mide 4.50mts de alto y tiene bonitas vigas de madera, el suelo es de parque macizo (se pulirá a gusto del comprador). Además, la vivienda dispone de screens, aire acondicionado frío-calor por Split y calefacción individual por radiadores. La propiedad no dispone de parking en finca, pero existe la posibilidad de alquilar una plaza de aparcamiento en la misma manzana..', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5357.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso en Calle de les Jonqueres'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98269646', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/0e/44/3a/1006158045.jpg', 'externalReference': 'VB2112041-1', 'numPhotos': 34, 'floor': '1', 'price': 750000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 140.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de les Jonqueres', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3867007, 'longitude': 2.1744305, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98269646/', 'distance': '400', 'description': 'Piso tipo Loft en venta en la calle Jonqueres Este loft está situado en Born, muy cerca del Palau de la Musica, en un edificio original del 1870 que había sido un antiguo convento y se rehabilitó íntegramente en el año 1997. En la entrada del edificio hay un amplio recibidor que da acceso a la escalera y al ascensor. En el primer piso encontramos una zona comunitaria ajardinada central donde se ubicaba en el antiguo claustro, que da acceso a la propiedad. La vivienda es toda exterior, con amplios ventanales al tranquilo y silencioso espacio central del edificio. El loft se reformó hace unos 13 años y mantiene ese encanto bohemio tan característico de la zona. En la entrada encontramos el recibidor abierto al amplio salón-comedor con cocina abierta. Está rodeado de grandes ventanales con mucha luz. Tiene acceso a una amplia terraza de 40m2, una zona muy tranquila y luminosa. En la misma planta hay un dormitorio doble con baño completo y en la zona del altillo (planta escriturada) se encuentra el segundo dormitorio abierto al espacio del salón, también dispone de un baño completo en suite. El techo mide 4.50mts de alto y tiene bonitas vigas de madera, el suelo es de parque macizo (se pulirá a gusto del comprador). Además, la vivienda dispone de screens, aire acondicionado frío-calor por Split y calefacción individual por radiadores. La propiedad no dispone de parking en finca, pero existe la posibilidad de alquilar una plaza de aparcamiento en la misma manzana..', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5357.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso en Calle de les Jonqueres'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '91592832', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/72/64/da/925378429.jpg', 'externalReference': 'W-02JZPS', 'numPhotos': 40, 'floor': '2', 'price': 818000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 87.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3949048, 'longitude': 2.167361, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/91592832/', 'distance': '850', 'description': 'Finca regia renovada cerca de Paseo de Gracia\r Estamos encantados de ofrecer este impresionante apartamento de 2 dormitorios en un edificio histórico completamente renovado con 10 pisos impecables, ubicado justo al lado de la famosa avenida comercial de Paseo de Gracia de Barcelona.\r Cada hogar ha sido diseñado por expertos en estilo y funcionalidad. Mientras que las características arquitectónicas clásicas de Barcelona se han restaurado para impartir la esencia de la historia del edificio como una "finca regia".\r Un vestíbulo de cristal le da la bienvenida a la casa antes de entrar en la cocina de diseño contemporáneo que se abre a la sala de estar. Con dos balcones, esta casa está bien iluminada y tiene un sentido de conexión con la ciudad, ya que todas las habitaciones dan al exterior.\r Las zonas separadas de día y de noche imparten amplitud y privacidad, y en la parte trasera del apartamento encontramos la suite principal. Los amplios pisos de tablones de madera de roble alargan el espacio. Los armarios están inteligentemente integrados en todas partes. Los amplios baños están equipados con accesorios de primera calidad.\r Los detalles arquitectónicos restaurados incluyen las fachadas del edificio, los techos abovedados catalanes, la entrada y la escalera del edificio, además de integrar pisos hidráulicos originales en los baños.\r La propiedad cuenta con marcas de primera calidad y materiales de construcción para maximizar el confort: electrodomésticos Miele, aerotermia Mitsubishi, cocinas Bulthaup, electrodomésticos Duravit y más. Se han tomado medidas específicas para maximizar la privacidad y el control del sonido, como las nuevas ventanas de doble acristalamiento y los sustratos de piso reforzado.\r El elegante barrio del Eixample se caracteriza por su arquitectura visionaria modernista, tiendas independientes, boutiques elegantes y cultura del café.\r La propiedad está situada en el corazón del Eixample Quadrat d’Or (‘Square Golden Square’), a solo una cuadra de la avenida arbolada del Passeig de Gràcia.\r Barcelona se ha transformado desde los Juegos Olímpicos de 1992, y la capital catalana se ha convertido en la meca de los creativos y emprendedores de todo el mundo gracias a su creciente reputación como un importante centro de nuevas empresas e innovación tecnológica.\r La segunda ciudad de España continúa liderando la cocina internacional de vanguardia y actualmente alberga más de 30 restaurantes con estrellas Michelin. Una de las ciudades "inteligentes" líderes en Europa, sus credenciales incluyen 500 kilómetros de fibra óptica, WiFi gratis a través de su alumbrado público y sensores para monitorear la calidad del aire. La propiedad tiene una gran demanda, particularmente en los barrios principales del casco antiguo de Barcelona y el Eixample, el núcleo cultural y vibrante de la ciudad.\r En la década de 1900, este codiciado barrio fue construido por la burguesía de Barcelona, que compitió para crear las casas más estéticamente refinadas. En los últimos años, esta área ha experimentado un gran renacimiento y se ha convertido en un imán para los compradores internacionales, especialmente con la concentración de una serie de desarrollos de lujo.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 9402.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '91592832', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/72/64/da/925378429.jpg', 'externalReference': 'W-02JZPS', 'numPhotos': 40, 'floor': '2', 'price': 818000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 87.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3949048, 'longitude': 2.167361, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/91592832/', 'distance': '850', 'description': 'Finca regia renovada cerca de Paseo de Gracia\r Estamos encantados de ofrecer este impresionante apartamento de 2 dormitorios en un edificio histórico completamente renovado con 10 pisos impecables, ubicado justo al lado de la famosa avenida comercial de Paseo de Gracia de Barcelona.\r Cada hogar ha sido diseñado por expertos en estilo y funcionalidad. Mientras que las características arquitectónicas clásicas de Barcelona se han restaurado para impartir la esencia de la historia del edificio como una "finca regia".\r Un vestíbulo de cristal le da la bienvenida a la casa antes de entrar en la cocina de diseño contemporáneo que se abre a la sala de estar. Con dos balcones, esta casa está bien iluminada y tiene un sentido de conexión con la ciudad, ya que todas las habitaciones dan al exterior.\r Las zonas separadas de día y de noche imparten amplitud y privacidad, y en la parte trasera del apartamento encontramos la suite principal. Los amplios pisos de tablones de madera de roble alargan el espacio. Los armarios están inteligentemente integrados en todas partes. Los amplios baños están equipados con accesorios de primera calidad.\r Los detalles arquitectónicos restaurados incluyen las fachadas del edificio, los techos abovedados catalanes, la entrada y la escalera del edificio, además de integrar pisos hidráulicos originales en los baños.\r La propiedad cuenta con marcas de primera calidad y materiales de construcción para maximizar el confort: electrodomésticos Miele, aerotermia Mitsubishi, cocinas Bulthaup, electrodomésticos Duravit y más. Se han tomado medidas específicas para maximizar la privacidad y el control del sonido, como las nuevas ventanas de doble acristalamiento y los sustratos de piso reforzado.\r El elegante barrio del Eixample se caracteriza por su arquitectura visionaria modernista, tiendas independientes, boutiques elegantes y cultura del café.\r La propiedad está situada en el corazón del Eixample Quadrat d’Or (‘Square Golden Square’), a solo una cuadra de la avenida arbolada del Passeig de Gràcia.\r Barcelona se ha transformado desde los Juegos Olímpicos de 1992, y la capital catalana se ha convertido en la meca de los creativos y emprendedores de todo el mundo gracias a su creciente reputación como un importante centro de nuevas empresas e innovación tecnológica.\r La segunda ciudad de España continúa liderando la cocina internacional de vanguardia y actualmente alberga más de 30 restaurantes con estrellas Michelin. Una de las ciudades "inteligentes" líderes en Europa, sus credenciales incluyen 500 kilómetros de fibra óptica, WiFi gratis a través de su alumbrado público y sensores para monitorear la calidad del aire. La propiedad tiene una gran demanda, particularmente en los barrios principales del casco antiguo de Barcelona y el Eixample, el núcleo cultural y vibrante de la ciudad.\r En la década de 1900, este codiciado barrio fue construido por la burguesía de Barcelona, que compitió para crear las casas más estéticamente refinadas. En los últimos años, esta área ha experimentado un gran renacimiento y se ha convertido en un imán para los compradores internacionales, especialmente con la concentración de una serie de desarrollos de lujo.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 9402.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '96603203', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/99/69/76/951332285.jpg', 'externalReference': 'BHHS-004107', 'numPhotos': 40, 'floor': '6', 'price': 560000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 62.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3967221, 'longitude': 2.1548047, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96603203/', 'distance': '1615', 'description': 'PISO ALTO Y SOLEADO EN FINCA MODERNA DE LA PARTE ALTA DEL EIXAMPLE EL PISO IDEAL EN FINCA MODERNA BERKSHIRE\xa0HATHAWAY\xa0HomeServices\xa0Barcelona, consultora especializada en la comercialización de propiedades exclusivas en las mejores zonas de Barcelona, les ofrece este fantástico piso, situado en la parte alta del barrio del Eixample de Barcelona, junto a la Rambla Catalunya. Según entramos en el piso, nos encontramos con la barra baja que separa el hall de la\xa0cocina\xa0la izquierda. Al frente\xa0nos dirigimos\xa0al salón comedor con salida al gran ventanal exterior a la calle, con vistas y muy soleado durante todo el día. También tiene un estrecho balcón, por el que se mueven las persianas correderas. El salón está orientado a Sur, y es exterior a la calle\xa0Córsega, que es de poquísimo tránsito en este\xa0tramo, ya que\xa0su acceso se inicia desde la adyacente Rambla de\xa0Catalunya. La cocina está equipada con electrodomésticos y cruzando una puerta se accede al lavadero con espacio para lavadora, secadora y lavabo. Los muebles de diseño, y electrodomésticos que ven en las fotografías, no están incluidos en el precio. Desde el salón, a través de una puerta que separa la zona de día de la zona de noche, accedemos a un distribuidor con un baño completo al frente, con bañera, y las dos habitaciones, una a cada lado, son dobles y tienen armarios empotrados. Una es exterior al pequeño balcón que da a la calle, y la otra da al vestíbulo privado de vecinos de la planta. El piso tiene calefacción por radiadores, caldera y acumulador, aire acondicionado por conductos a todas las estancias, suelos de parquet... \xa0Además, \xa0está muy bien distribuido, con muy buen gusto, y sin espacios perdidos. Esta finca fue construida en el 1967, y en el 2007\xa0Metrovacesa\xa0la adaptó para tener viviendas cómodas y accesibles, además con buen gusto y diseño, como se puede apreciar en las fotografías de la misma. Se completa con un vestíbulo muy acogedor, donde recibe, el que posiblemente sea, el mejor conserje de Barcelona. Para más información no dude en contactar con Berkshire Hathaway\xa0HomeServices\xa0Barcelona, especialistas en inmuebles de alto standing en Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 9032.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '96603203', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/99/69/76/951332285.jpg', 'externalReference': 'BHHS-004107', 'numPhotos': 40, 'floor': '6', 'price': 560000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 62.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3967221, 'longitude': 2.1548047, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96603203/', 'distance': '1615', 'description': 'PISO ALTO Y SOLEADO EN FINCA MODERNA DE LA PARTE ALTA DEL EIXAMPLE EL PISO IDEAL EN FINCA MODERNA BERKSHIRE\xa0HATHAWAY\xa0HomeServices\xa0Barcelona, consultora especializada en la comercialización de propiedades exclusivas en las mejores zonas de Barcelona, les ofrece este fantástico piso, situado en la parte alta del barrio del Eixample de Barcelona, junto a la Rambla Catalunya. Según entramos en el piso, nos encontramos con la barra baja que separa el hall de la\xa0cocina\xa0la izquierda. Al frente\xa0nos dirigimos\xa0al salón comedor con salida al gran ventanal exterior a la calle, con vistas y muy soleado durante todo el día. También tiene un estrecho balcón, por el que se mueven las persianas correderas. El salón está orientado a Sur, y es exterior a la calle\xa0Córsega, que es de poquísimo tránsito en este\xa0tramo, ya que\xa0su acceso se inicia desde la adyacente Rambla de\xa0Catalunya. La cocina está equipada con electrodomésticos y cruzando una puerta se accede al lavadero con espacio para lavadora, secadora y lavabo. Los muebles de diseño, y electrodomésticos que ven en las fotografías, no están incluidos en el precio. Desde el salón, a través de una puerta que separa la zona de día de la zona de noche, accedemos a un distribuidor con un baño completo al frente, con bañera, y las dos habitaciones, una a cada lado, son dobles y tienen armarios empotrados. Una es exterior al pequeño balcón que da a la calle, y la otra da al vestíbulo privado de vecinos de la planta. El piso tiene calefacción por radiadores, caldera y acumulador, aire acondicionado por conductos a todas las estancias, suelos de parquet... \xa0Además, \xa0está muy bien distribuido, con muy buen gusto, y sin espacios perdidos. Esta finca fue construida en el 1967, y en el 2007\xa0Metrovacesa\xa0la adaptó para tener viviendas cómodas y accesibles, además con buen gusto y diseño, como se puede apreciar en las fotografías de la misma. Se completa con un vestíbulo muy acogedor, donde recibe, el que posiblemente sea, el mejor conserje de Barcelona. Para más información no dude en contactar con Berkshire Hathaway\xa0HomeServices\xa0Barcelona, especialistas en inmuebles de alto standing en Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 9032.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99671987', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ef/7d/5e/1050814553.jpg', 'externalReference': 'BCN38016', 'numPhotos': 33, 'price': 500000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 66.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3940703, 'longitude': 2.1510348, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99671987/', 'distance': '1724', 'description': 'Lucas Fox presenta esta propiedad reformada ubicada a pocos pasos de la Avenida Diagonal y de la plaza de Francesc Macià.  Está situada en la planta principal del edificio, por lo que dispone de techos altos.  En la zona de día, encontramos una cocina americana totalmente equipada. \xa0El salón comedor es exterior y tiene un pequeño balcón donde colocar una mesa y dos sillas para disfrutar del sol de tarde. \xa0Además, tiene suelos hidráulicos y una bonita pared de obra vista en uno de sus laterales.  Por otro lado, un pequeño pasillo conduce a la otra parte de la vivienda. Aquí, vemos el dormitorio principal doble equipado con armario y un aseo y un segundo dormitorio también doble y con un armario muy espacioso. Ambos dormitorios son interiores, por lo que son muy tranquilos. Finalmente, entre los dormitorios encontramos el baño principal con ducha. El piso cuenta con unos altillos muy prácticos que se pueden aprovechar para almacenaje, aire acondicionado, calefacción por conductos y suelos de parquet en parte de la casa e hidráulicos en otra. Asimismo, los vecinos del edificio pueden disfrutar de la terraza comunitaria.  Póngase en contacto con nosotros para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 7576.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99671987', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ef/7d/5e/1050814553.jpg', 'externalReference': 'BCN38016', 'numPhotos': 33, 'price': 500000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 66.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3940703, 'longitude': 2.1510348, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99671987/', 'distance': '1724', 'description': 'Lucas Fox presenta esta propiedad reformada ubicada a pocos pasos de la Avenida Diagonal y de la plaza de Francesc Macià.  Está situada en la planta principal del edificio, por lo que dispone de techos altos.  En la zona de día, encontramos una cocina americana totalmente equipada. \xa0El salón comedor es exterior y tiene un pequeño balcón donde colocar una mesa y dos sillas para disfrutar del sol de tarde. \xa0Además, tiene suelos hidráulicos y una bonita pared de obra vista en uno de sus laterales.  Por otro lado, un pequeño pasillo conduce a la otra parte de la vivienda. Aquí, vemos el dormitorio principal doble equipado con armario y un aseo y un segundo dormitorio también doble y con un armario muy espacioso. Ambos dormitorios son interiores, por lo que son muy tranquilos. Finalmente, entre los dormitorios encontramos el baño principal con ducha. El piso cuenta con unos altillos muy prácticos que se pueden aprovechar para almacenaje, aire acondicionado, calefacción por conductos y suelos de parquet en parte de la casa e hidráulicos en otra. Asimismo, los vecinos del edificio pueden disfrutar de la terraza comunitaria.  Póngase en contacto con nosotros para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 7576.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99602294', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/e5/3c/c0/1048891671.jpg', 'externalReference': 'BCN37037', 'numPhotos': 37, 'price': 649000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 102.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Gòtic', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3858046, 'longitude': 2.1752293, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99602294/', 'distance': '493', 'description': "Situado en el Barrio Gótico, a un paso de Portal de l'Àngel, Plaza de Catalunya y de la Catedral de Barcelona, Lucas Fox presenta este piso recién reformado y totalmente amueblado a estrenar.  La reforma ha terminado recientemente y el piso está listo para entrar a vivir.  Tiene doble orientación y al estar en una planta alta, goza de abundante luz natural que entra por grandes ventanales.  Al entrar en el piso nos encontramos con un amplio hall de entrada, con espacio de almacenamiento adicional, que nos da acceso a la zona de día. A nuestra derecha tenemos el salón-comedor de 32m2 con salida a dos balcones con bonitas vistas a edificios monumentales. A nuestra izquierda tenemos un baño y el cuarto lavadero.  A través de la cocina totalmente equipada, que alberga otro espacio de comedor/zona de trabajo, accedemos a la zona de noche que consta de dos dormitorios dobles con armarios y el segundo baño. \xa0Ambos dormitorios dan a un tranquilo patio interior.  Este excelente piso cuenta con todas las instalaciones nuevas: fontanería, gas, electricidad, ventilación, aire acondicionado por conductos en la zona de día, splits en la zona de noche y calefacción eléctrica independiente en todas partes.  Consta con suelos y baldosas de madera nuevos, una cocina hecha a medida con electrodomésticos de marcas de alta calidad, muebles de diseño, lámparas y fotografías de lugares emblemáticos de Barcelona, como se muestra en las imágenes.  Los residentes del edificio pueden disfrutar de la terraza comunitaria con vistas al casco antiguo.  Póngase en contacto con nosotros para concertar una visita.  Características básicas:  - 102 m² construidos  - 2 dormitorios dobles  - 2 baños  - Terraza  - Armarios  Edificio  - Exterior/interior  -\xa0Construido en 1836  Equipamiento  - Aire acondicionado (conductos/splits)  - Calefacción independiente.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 6363.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99602294', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/e5/3c/c0/1048891671.jpg', 'externalReference': 'BCN37037', 'numPhotos': 37, 'price': 649000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 102.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Gòtic', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3858046, 'longitude': 2.1752293, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99602294/', 'distance': '493', 'description': "Situado en el Barrio Gótico, a un paso de Portal de l'Àngel, Plaza de Catalunya y de la Catedral de Barcelona, Lucas Fox presenta este piso recién reformado y totalmente amueblado a estrenar.  La reforma ha terminado recientemente y el piso está listo para entrar a vivir.  Tiene doble orientación y al estar en una planta alta, goza de abundante luz natural que entra por grandes ventanales.  Al entrar en el piso nos encontramos con un amplio hall de entrada, con espacio de almacenamiento adicional, que nos da acceso a la zona de día. A nuestra derecha tenemos el salón-comedor de 32m2 con salida a dos balcones con bonitas vistas a edificios monumentales. A nuestra izquierda tenemos un baño y el cuarto lavadero.  A través de la cocina totalmente equipada, que alberga otro espacio de comedor/zona de trabajo, accedemos a la zona de noche que consta de dos dormitorios dobles con armarios y el segundo baño. \xa0Ambos dormitorios dan a un tranquilo patio interior.  Este excelente piso cuenta con todas las instalaciones nuevas: fontanería, gas, electricidad, ventilación, aire acondicionado por conductos en la zona de día, splits en la zona de noche y calefacción eléctrica independiente en todas partes.  Consta con suelos y baldosas de madera nuevos, una cocina hecha a medida con electrodomésticos de marcas de alta calidad, muebles de diseño, lámparas y fotografías de lugares emblemáticos de Barcelona, como se muestra en las imágenes.  Los residentes del edificio pueden disfrutar de la terraza comunitaria con vistas al casco antiguo.  Póngase en contacto con nosotros para concertar una visita.  Características básicas:  - 102 m² construidos  - 2 dormitorios dobles  - 2 baños  - Terraza  - Armarios  Edificio  - Exterior/interior  -\xa0Construido en 1836  Equipamiento  - Aire acondicionado (conductos/splits)  - Calefacción independiente.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 6363.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99484200', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/49/bd/6f/1045894352.jpg', 'externalReference': 'BCNP4955', 'numPhotos': 30, 'price': 990000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 126.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Gòtic', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3837041, 'longitude': 2.1717083, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99484200/', 'distance': '449', 'description': 'Céntrico y alto apartamento con detalles de la época en el barrio Gótico. Los apartamentos esquineros suelen ser los más demandados en el centro de Barcelona. Esta preciosa finca con ascensor en el barrio Gótico, queda a 15 minutos caminando de Paseo de Gracia, haciendo ruta por el Portal de Ángel. Un magnífico paseo a lo largo del barrio histórico de la ciudad condal. Destaca en esta propiedad la reforma integral realizada en el año 2021 preservando el carácter modernista visto en sus suelos hidráulicos, techos altos y el detalle de dar nueva vida a la pared original de la finca del año 1900. El apartamento está distribuido en dos dormitorios dobles y dos baños. Uno de los dormitorios dispone de un walking closet que en el caso de necesidad podría hacer función de un tercer dormitorio. Amplio y luminoso salón comedor y cocina americana con cuatro balcones. Excelentes materiales y acabados. Solo disponible con Sotheby’s International Realty. El Barrio Gótico es el núcleo más antiguo de la ciudad. Está delimitado por Las Ramblas, La Vía Laietana, el Paseo Colón y la Plaza de Catalunya, cada uno de estos puntos por sí solos tiene su propia importancia e historia. De calles angostas y estructura irregular, varios de sus edificios han sido construidos sobre los restos románicos de la ciudad, así que puede hacerse con algún apartamento en el que al menos una pared date de la época romana o medieval. Es el barrio turístico por excelencia por lo que representa una inversión asegurada, sobretodo si está cerca de alguno de sus atractivos como La Catedral, la Plaza Sant Jaume con el Ayuntamiento y el Palacio de la Generalitat, la Plaza Real, Las famosas Rambas, y el Museo de Historia de la ciudad. Este podría ser su barrio si busca hacer una inversión rentable o adquirir un excelente piet-à-terre en un barrio con gran historia, edificaciones particulares, de interés turístico y con todo tipo de negocios a mano, buena gastronomía, y múltiples rincones mágicos para descubrir y recorrer.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 7857.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99484200', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/49/bd/6f/1045894352.jpg', 'externalReference': 'BCNP4955', 'numPhotos': 30, 'price': 990000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 126.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Gòtic', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3837041, 'longitude': 2.1717083, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99484200/', 'distance': '449', 'description': 'Céntrico y alto apartamento con detalles de la época en el barrio Gótico. Los apartamentos esquineros suelen ser los más demandados en el centro de Barcelona. Esta preciosa finca con ascensor en el barrio Gótico, queda a 15 minutos caminando de Paseo de Gracia, haciendo ruta por el Portal de Ángel. Un magnífico paseo a lo largo del barrio histórico de la ciudad condal. Destaca en esta propiedad la reforma integral realizada en el año 2021 preservando el carácter modernista visto en sus suelos hidráulicos, techos altos y el detalle de dar nueva vida a la pared original de la finca del año 1900. El apartamento está distribuido en dos dormitorios dobles y dos baños. Uno de los dormitorios dispone de un walking closet que en el caso de necesidad podría hacer función de un tercer dormitorio. Amplio y luminoso salón comedor y cocina americana con cuatro balcones. Excelentes materiales y acabados. Solo disponible con Sotheby’s International Realty. El Barrio Gótico es el núcleo más antiguo de la ciudad. Está delimitado por Las Ramblas, La Vía Laietana, el Paseo Colón y la Plaza de Catalunya, cada uno de estos puntos por sí solos tiene su propia importancia e historia. De calles angostas y estructura irregular, varios de sus edificios han sido construidos sobre los restos románicos de la ciudad, así que puede hacerse con algún apartamento en el que al menos una pared date de la época romana o medieval. Es el barrio turístico por excelencia por lo que representa una inversión asegurada, sobretodo si está cerca de alguno de sus atractivos como La Catedral, la Plaza Sant Jaume con el Ayuntamiento y el Palacio de la Generalitat, la Plaza Real, Las famosas Rambas, y el Museo de Historia de la ciudad. Este podría ser su barrio si busca hacer una inversión rentable o adquirir un excelente piet-à-terre en un barrio con gran historia, edificaciones particulares, de interés turístico y con todo tipo de negocios a mano, buena gastronomía, y múltiples rincones mágicos para descubrir y recorrer.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 7857.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97472923', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/9d/de/31/980489261.jpg', 'externalReference': 'B83', 'numPhotos': 32, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 180.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3864408, 'longitude': 2.1600522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97472923/', 'distance': '816', 'description': 'Magnífico piso de lujo reformado a estrenar, con calidades muy altas y grandes espacios, pensado para personas que quieran estar en el centro de la ciudad, sin estar en zona turística. Estas son sus características principales: 2 grandes habitaciones suites. Una de las habitaciones da hacia el patio interior con armarios empotrados e iluminación y maderas nobles, también se encuentra una pequeña zona de estudio y un baño incorporado completo con ducha y sanitario. Master suite con espacio para cama king size con salida a terraza amplia una zona tranquila. Armarios empotrados. Baño completo espacioso y doble lavabo, luz natural que da hacia la terraza y armarios incorporados. Ducha amplia con sanitario separado. Cocina pequeña, pensada para uso básico y disfrutar de la zona gourmet de Barcelona. Enchufes con USB. Maderas nobles. Electrodomésticos integrados, nevera americana de alta calidad. Sistema de domótica para la iluminación. Sistema de calefacción y aire acondicionado última generación. Edificio reformado recientemente.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4711.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97472923', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/9d/de/31/980489261.jpg', 'externalReference': 'B83', 'numPhotos': 32, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 180.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3864408, 'longitude': 2.1600522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97472923/', 'distance': '816', 'description': 'Magnífico piso de lujo reformado a estrenar, con calidades muy altas y grandes espacios, pensado para personas que quieran estar en el centro de la ciudad, sin estar en zona turística. Estas son sus características principales: 2 grandes habitaciones suites. Una de las habitaciones da hacia el patio interior con armarios empotrados e iluminación y maderas nobles, también se encuentra una pequeña zona de estudio y un baño incorporado completo con ducha y sanitario. Master suite con espacio para cama king size con salida a terraza amplia una zona tranquila. Armarios empotrados. Baño completo espacioso y doble lavabo, luz natural que da hacia la terraza y armarios incorporados. Ducha amplia con sanitario separado. Cocina pequeña, pensada para uso básico y disfrutar de la zona gourmet de Barcelona. Enchufes con USB. Maderas nobles. Electrodomésticos integrados, nevera americana de alta calidad. Sistema de domótica para la iluminación. Sistema de calefacción y aire acondicionado última generación. Edificio reformado recientemente.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4711.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99440277', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/02/5b/41/1044037924.jpg', 'externalReference': '4919', 'numPhotos': 42, 'floor': '5', 'price': 345000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 64.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Mallorca', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3831025, 'longitude': 2.1528715, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99440277/', 'distance': '1488', 'description': 'Excelente vivienda en la Nova Esquerra del Eixample reformado para entrar a vivir ¡ Luminoso y muy tranquilo orientado a patio de manzana, con amplio salón comedor, cocina equipada, 2 habitaciones (1 doble y 1 individual), baño completo con plato de ducha. climatizado mediante aire acondicionado y calefaccion de gas natural, suelos de parquet. Anteriormente distribido en cuatro habitaciones. 5ª planta con ascensor en finca del año 1.964. No cobramos honorarios al comprador. Impuestos, gastos de notaría y gestoría no incluidos en el precio de compra de la vivienda.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5391.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Mallorca'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99440277', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/02/5b/41/1044037924.jpg', 'externalReference': '4919', 'numPhotos': 42, 'floor': '5', 'price': 345000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 64.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Mallorca', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3831025, 'longitude': 2.1528715, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99440277/', 'distance': '1488', 'description': 'Excelente vivienda en la Nova Esquerra del Eixample reformado para entrar a vivir ¡ Luminoso y muy tranquilo orientado a patio de manzana, con amplio salón comedor, cocina equipada, 2 habitaciones (1 doble y 1 individual), baño completo con plato de ducha. climatizado mediante aire acondicionado y calefaccion de gas natural, suelos de parquet. Anteriormente distribido en cuatro habitaciones. 5ª planta con ascensor en finca del año 1.964. No cobramos honorarios al comprador. Impuestos, gastos de notaría y gestoría no incluidos en el precio de compra de la vivienda.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5391.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Mallorca'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '96745288', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5f/9b/9b/955352422.jpg', 'externalReference': 'BCN23896', 'numPhotos': 42, 'price': 1200000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 187.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3849911, 'longitude': 2.1546049, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96745288/', 'distance': '1292', 'description': 'En un edificio del año 2000, en perfectas condiciones y con ascensor, encontramos este magnífico ático de 160 m², totalmente reformado, muy amplio y con mucha luz gracias a los grandes ventanales de suelo a techo que hay en prácticamente toda la vivienda.  El piso consta de un agradable salón-comedor con cocina abierta con mucha luz y bonitas vistas a la ciudad, dos dormitorios dobles, uno de ellos con vestidor y baño privado, así como un baño completo extra con zona de aguas integrada.  En la planta superior, accesible desde la escalera comunitaria, encontramos un espacio exterior de más de 150 m² escriturado junto con nuestra vivienda.  En este espacio se consolidó una construcción de 69 m² que actualmente alberga un gran salón con la cocina abierta y un baño completo. Un espacio ideal para celebrar reuniones, fiestas o simplemente relajarse. Este espacio tiene salida a una soleada terraza de más de 85 m² con zona de barbacoa y un trastero.  En el precio se incluyen dos plazas de aparcamiento de tamaño grande en la misma finca, donde pueden caber dos coches grandes y una moto.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6417.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Ático'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '96745288', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5f/9b/9b/955352422.jpg', 'externalReference': 'BCN23896', 'numPhotos': 42, 'price': 1200000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 187.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3849911, 'longitude': 2.1546049, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96745288/', 'distance': '1292', 'description': 'En un edificio del año 2000, en perfectas condiciones y con ascensor, encontramos este magnífico ático de 160 m², totalmente reformado, muy amplio y con mucha luz gracias a los grandes ventanales de suelo a techo que hay en prácticamente toda la vivienda.  El piso consta de un agradable salón-comedor con cocina abierta con mucha luz y bonitas vistas a la ciudad, dos dormitorios dobles, uno de ellos con vestidor y baño privado, así como un baño completo extra con zona de aguas integrada.  En la planta superior, accesible desde la escalera comunitaria, encontramos un espacio exterior de más de 150 m² escriturado junto con nuestra vivienda.  En este espacio se consolidó una construcción de 69 m² que actualmente alberga un gran salón con la cocina abierta y un baño completo. Un espacio ideal para celebrar reuniones, fiestas o simplemente relajarse. Este espacio tiene salida a una soleada terraza de más de 85 m² con zona de barbacoa y un trastero.  En el precio se incluyen dos plazas de aparcamiento de tamaño grande en la misma finca, donde pueden caber dos coches grandes y una moto.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6417.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Ático'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '94496557', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ae/e9/5e/890458989.jpg', 'externalReference': 'BCN28118', 'numPhotos': 36, 'floor': '6', 'price': 1500000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 139.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3901548, 'longitude': 2.1655207, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/94496557/', 'distance': '461', 'description': 'Lucas Fox presenta este piso en venta reformado a estrenar y totalmente amueblado en una ubicación Prime de Barcelona, entre Paseo de Gracia y Rambla Catalunya.  Está situado en la última planta de una finca regia del 1.890 con ascensor, que ha pasado favorablemente la Inspección Técnica de Edificios.  Todos los espacios de la vivienda son amplios y gozan de abundante entrada de luz natural. Al entrar en la vivienda, a mano izquierda encontramos la zona de día compuesta por el salón-comedor con balcón exterior a la calle y con una chimenea de bioetanol. A continuación, se dispone la elegante cocina de la firma italiana Modulnova, equipada con vinoteca y electrodomésticos de marca.  A través de un amplio pasillo con armarios empotrados, accedemos a la zona de noche compuesta por dos dormitorios dobles, uno de ellos con baño privado. Ambos dormitorios disponen de amplios armarios empotrados y salida a una terraza orientada a sureste. Esta zona se completa con un baño con ducha.  El piso está equipado por calefacción por radiadores de gas (que se puede controlar mediante Wifi), aire acondicionado por conductos con bomba para frío y calor, suelos de parqué y además dispone de un trastero en el terrado de la finca.  La reforma se ha realizada de la mano de un reconocido estudio de arquitectura de interiores, con grandes calidades y creando ambientes elegantes, cálidos y con carácter.  Póngase en contacto con nosotros para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 10791.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '94496557', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ae/e9/5e/890458989.jpg', 'externalReference': 'BCN28118', 'numPhotos': 36, 'floor': '6', 'price': 1500000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 139.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3901548, 'longitude': 2.1655207, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/94496557/', 'distance': '461', 'description': 'Lucas Fox presenta este piso en venta reformado a estrenar y totalmente amueblado en una ubicación Prime de Barcelona, entre Paseo de Gracia y Rambla Catalunya.  Está situado en la última planta de una finca regia del 1.890 con ascensor, que ha pasado favorablemente la Inspección Técnica de Edificios.  Todos los espacios de la vivienda son amplios y gozan de abundante entrada de luz natural. Al entrar en la vivienda, a mano izquierda encontramos la zona de día compuesta por el salón-comedor con balcón exterior a la calle y con una chimenea de bioetanol. A continuación, se dispone la elegante cocina de la firma italiana Modulnova, equipada con vinoteca y electrodomésticos de marca.  A través de un amplio pasillo con armarios empotrados, accedemos a la zona de noche compuesta por dos dormitorios dobles, uno de ellos con baño privado. Ambos dormitorios disponen de amplios armarios empotrados y salida a una terraza orientada a sureste. Esta zona se completa con un baño con ducha.  El piso está equipado por calefacción por radiadores de gas (que se puede controlar mediante Wifi), aire acondicionado por conductos con bomba para frío y calor, suelos de parqué y además dispone de un trastero en el terrado de la finca.  La reforma se ha realizada de la mano de un reconocido estudio de arquitectura de interiores, con grandes calidades y creando ambientes elegantes, cálidos y con carácter.  Póngase en contacto con nosotros para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 10791.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97637906', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/77/0d/ef/985947670.jpg', 'externalReference': '4392', 'numPhotos': 71, 'floor': 'en', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 190.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3860408, 'longitude': 2.1633522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97637906/', 'distance': '556', 'description': 'Viviendas de Lujo en Ensanche Izquierdo. Viviendas a estrenar en exclusiva finca clásica. Situada en el Ensanche Izquierdo, está ubicada en la calle Diputación cerca de Plaza Universidad y a escasos minutos de la Rambla de Catalunya y el Paseo de Gracia. Terraza privada de 41m2. Ademas podrá disfrutar de una gran terraza comunitaria, un espacio de 60 m² con zona “chill out” y unas preciosas vistas de Barcelona. Exclusiva finca con sólo 4 vecinos, ha sido totalmente rehabilitada teniendo todas las zonas comunes, ascensor y terrado nuevos. El proyecto de esta fantástica vivienda ha sido realizado por Jaime Beriestain Studio, se han utilizado los mejores materiales con un diseño muy elegante creando espacios actuales y acogedores. Vivienda de alto standing con todo tipo de detalles, distribuida en:  - Recibidor. - Salón de unos 26m2 independiente y exterior a la calle. - Cocina independiente cerrada con puertas correderas, lo que nos facilita la sensación de cocina abierta. - Zona de lavado. - Aseo de cortesía. - Zona de noche con dos dormitorios ambos dobles y en suite, uno de ellos de 13m2 con armarios empotrados, estudio y con un baño de 8m2 con plato de ducha. El dormitorio principal tiene una superficie de 25m2, consta de vestidor y de un baño de 13m2 con plato de ducha y bañera, también tiene acceso a la terraza de 42m2. Zona comercial con todo tipo de servicios y muy bien comunicada con transporte público. Oportunidad inmejorable para adquirir una vivienda a estrenar en el corazón de Barcelona. Disponemos de más pisos a la venta en la misma finca: 1° de 130m2 a 768.000€  2° de 130m2 a 816.000€  Local de 165m2 a 576.000€ Posibilidad de comprar edificio completo. Aincasa Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4463.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97637906', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/77/0d/ef/985947670.jpg', 'externalReference': '4392', 'numPhotos': 71, 'floor': 'en', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 190.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3860408, 'longitude': 2.1633522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97637906/', 'distance': '556', 'description': 'Viviendas de Lujo en Ensanche Izquierdo. Viviendas a estrenar en exclusiva finca clásica. Situada en el Ensanche Izquierdo, está ubicada en la calle Diputación cerca de Plaza Universidad y a escasos minutos de la Rambla de Catalunya y el Paseo de Gracia. Terraza privada de 41m2. Ademas podrá disfrutar de una gran terraza comunitaria, un espacio de 60 m² con zona “chill out” y unas preciosas vistas de Barcelona. Exclusiva finca con sólo 4 vecinos, ha sido totalmente rehabilitada teniendo todas las zonas comunes, ascensor y terrado nuevos. El proyecto de esta fantástica vivienda ha sido realizado por Jaime Beriestain Studio, se han utilizado los mejores materiales con un diseño muy elegante creando espacios actuales y acogedores. Vivienda de alto standing con todo tipo de detalles, distribuida en:  - Recibidor. - Salón de unos 26m2 independiente y exterior a la calle. - Cocina independiente cerrada con puertas correderas, lo que nos facilita la sensación de cocina abierta. - Zona de lavado. - Aseo de cortesía. - Zona de noche con dos dormitorios ambos dobles y en suite, uno de ellos de 13m2 con armarios empotrados, estudio y con un baño de 8m2 con plato de ducha. El dormitorio principal tiene una superficie de 25m2, consta de vestidor y de un baño de 13m2 con plato de ducha y bañera, también tiene acceso a la terraza de 42m2. Zona comercial con todo tipo de servicios y muy bien comunicada con transporte público. Oportunidad inmejorable para adquirir una vivienda a estrenar en el corazón de Barcelona. Disponemos de más pisos a la venta en la misma finca: 1° de 130m2 a 768.000€  2° de 130m2 a 816.000€  Local de 165m2 a 576.000€ Posibilidad de comprar edificio completo. Aincasa Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4463.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99794526', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/14/7c/63/1054779399.jpg', 'externalReference': '2809', 'numPhotos': 26, 'floor': '2', 'price': 490000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 71.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de París', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3887258, 'longitude': 2.1473163, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99794526/', 'distance': '1876', 'description': 'Vivienda de 71m2 en edificio de 2011. En excelente estado, exterior y funcional. Salón comedor esquinero, dos habitaciones dobles. Cocina americana equipada. Un baño completo. Armarios empotrados. Calefacción y aire acondicionado por conductos. Excelentes cerramientos Technal con doble cristal. Persianas mecanizadas. Terraza comunitaria en la cubierta del edificio. Plaza de garaje grande y trastero de 14m2. Garaje con vigilancia 24 horas. Dos ascensores. Gastos e impuestos no incluidos en el precio del anuncio.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': True}, 'priceByArea': 6901.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de París'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99794526', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/14/7c/63/1054779399.jpg', 'externalReference': '2809', 'numPhotos': 26, 'floor': '2', 'price': 490000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 71.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de París', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3887258, 'longitude': 2.1473163, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99794526/', 'distance': '1876', 'description': 'Vivienda de 71m2 en edificio de 2011. En excelente estado, exterior y funcional. Salón comedor esquinero, dos habitaciones dobles. Cocina americana equipada. Un baño completo. Armarios empotrados. Calefacción y aire acondicionado por conductos. Excelentes cerramientos Technal con doble cristal. Persianas mecanizadas. Terraza comunitaria en la cubierta del edificio. Plaza de garaje grande y trastero de 14m2. Garaje con vigilancia 24 horas. Dos ascensores. Gastos e impuestos no incluidos en el precio del anuncio.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': True}, 'priceByArea': 6901.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de París'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97534780', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/3e/ee/b3/982449385.jpg', 'externalReference': 'BCN-Carrera Bajos2', 'numPhotos': 31, 'floor': 'bj', 'price': 510000.0, 'propertyType': 'duplex', 'operation': 'sale', 'size': 86.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Carrera', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'El Poble Sec - Parc de Montjuïc', 'latitude': 41.372431, 'longitude': 2.1760547, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97534780/', 'distance': '1753', 'description': 'Fabulosa planta baja dúplex de 86 m2, muy luminosa, con soleado patio de 59m2. La vivienda se distribuye en planta baja (recibidor, aseo de cortesía, cocina abierta, salón comedor con salida al patio de 59m2) y planta piso (2 habitaciones a patio de manzana y 2 baños). Finca con ascensor y con una ubicación privilegiada. Disponemos de plazas de parking en la misma finca, así como otros pisos en diferentes alturas. Nuestras viviendas se encuentran en la calle Carrera, justo delante de los Jardines de Walter Benjamin y la Plaça de les Drassanes, frente al Puerto de Barcelona. Justo al lado de la famosa Avda del Paral. lel con sus teatros y todo tipo de comercios. A un paso del Mirador del Poble Sec, disfrute de los paseos por Montjuïc y por sus amplias zonas ajardinadas ideales para hacer deporte al aire libre. Aproveche el buen clima de nuestra ciudad en las playas de alrededor. Muy bien comunicado con toda la ciudad con Lineas de Metro y autobuses. deportes al aire libre. Aproveche el buen clima de nuestra ciudad en las playas de alrededor. Muy bien comunicado con toda la ciudad con Líneas de Metro y autobuses.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': True}, 'priceByArea': 5930.0, 'detailedType': {'typology': 'flat', 'subTypology': 'duplex'}, 'suggestedTexts': {'subtitle': 'El Poble Sec - Parc de Montjuïc, Barcelona', 'title': 'Dúplex en Carrera'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97534780', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/3e/ee/b3/982449385.jpg', 'externalReference': 'BCN-Carrera Bajos2', 'numPhotos': 31, 'floor': 'bj', 'price': 510000.0, 'propertyType': 'duplex', 'operation': 'sale', 'size': 86.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Carrera', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'El Poble Sec - Parc de Montjuïc', 'latitude': 41.372431, 'longitude': 2.1760547, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97534780/', 'distance': '1753', 'description': 'Fabulosa planta baja dúplex de 86 m2, muy luminosa, con soleado patio de 59m2. La vivienda se distribuye en planta baja (recibidor, aseo de cortesía, cocina abierta, salón comedor con salida al patio de 59m2) y planta piso (2 habitaciones a patio de manzana y 2 baños). Finca con ascensor y con una ubicación privilegiada. Disponemos de plazas de parking en la misma finca, así como otros pisos en diferentes alturas. Nuestras viviendas se encuentran en la calle Carrera, justo delante de los Jardines de Walter Benjamin y la Plaça de les Drassanes, frente al Puerto de Barcelona. Justo al lado de la famosa Avda del Paral. lel con sus teatros y todo tipo de comercios. A un paso del Mirador del Poble Sec, disfrute de los paseos por Montjuïc y por sus amplias zonas ajardinadas ideales para hacer deporte al aire libre. Aproveche el buen clima de nuestra ciudad en las playas de alrededor. Muy bien comunicado con toda la ciudad con Lineas de Metro y autobuses. deportes al aire libre. Aproveche el buen clima de nuestra ciudad en las playas de alrededor. Muy bien comunicado con toda la ciudad con Líneas de Metro y autobuses.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': True}, 'priceByArea': 5930.0, 'detailedType': {'typology': 'flat', 'subTypology': 'duplex'}, 'suggestedTexts': {'subtitle': 'El Poble Sec - Parc de Montjuïc, Barcelona', 'title': 'Dúplex en Carrera'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99348106', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a6/63/11/962649051.jpg', 'externalReference': 'B34', 'numPhotos': 23, 'floor': '2', 'price': 579000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 70.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de París', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3899266, 'longitude': 2.1499647, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99348106/', 'distance': '1672', 'description': 'Un piso único con bóveda catalana 70 m2 1 dormitorio doble en suite con baño abierto con ducha, con armario grande 1 dormitorio individual con sofa-cama y armario 1 sala de estar Cocina con comedor, con isla, totalmente equipada (lavadora, lavaplatos, placa de inducción, campana, nevera, horno, tostadora, hervidor…) 1 baño separado con una bañera y WC  1 Balcón Aire acondicionado split (frio/calor) Caldera de gas nueva Hay plancha, aspiradora, secador de pelo Parquet de madera buena calidad, gres en la cocina Orientación Sur.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8271.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de París'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99348106', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a6/63/11/962649051.jpg', 'externalReference': 'B34', 'numPhotos': 23, 'floor': '2', 'price': 579000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 70.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de París', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3899266, 'longitude': 2.1499647, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99348106/', 'distance': '1672', 'description': 'Un piso único con bóveda catalana 70 m2 1 dormitorio doble en suite con baño abierto con ducha, con armario grande 1 dormitorio individual con sofa-cama y armario 1 sala de estar Cocina con comedor, con isla, totalmente equipada (lavadora, lavaplatos, placa de inducción, campana, nevera, horno, tostadora, hervidor…) 1 baño separado con una bañera y WC  1 Balcón Aire acondicionado split (frio/calor) Caldera de gas nueva Hay plancha, aspiradora, secador de pelo Parquet de madera buena calidad, gres en la cocina Orientación Sur.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8271.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de París'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '91626925', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8c/85/9a/958647886.jpg', 'externalReference': 'V2084-R', 'numPhotos': 28, 'floor': '3', 'price': 256000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 67.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Princesa', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3879197, 'longitude': 2.1811329, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/91626925/', 'distance': '951', 'description': 'Vivienda de 67 m2 con doble orientación a calle Princesa y Assaonadors, con sol todo el día, que ocupa la tercera planta de un edificio de 1880, sin ascensor.   Distribuye 2 dormitorios, uno doble con balcón a calle Princesa y otro individual (habitación ciega), vestidor, baño completo con bañera, cocina abierta al comedor y salón.   Ventilación cruzada, cerramientos de aluminio, suelos de parquet laminado y de gres en baño, climatización en la estancia con más incidencia solar. El dormitorio individual y vestidor ventilan al actual dormitorio doble.  La distribución actual puede modificarse cambiando el dormitorio doble por el salón, sin obras. No hay posibilidad de instalar ascensor en la finca.   El Born, con comercio de proximidad y servicios, pero también una amplia oferta gastronómica y un envidiable entorno histórico de la evolución de la ciudad.   Los honorarios son a cargo del vendedor. El precio no incluye los impuestos, ni gastos de notaría ni de gestoría de la compraventa.  Eurofincas International Real Estate | Referencia V2084.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 3821.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso en Princesa'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '91626925', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8c/85/9a/958647886.jpg', 'externalReference': 'V2084-R', 'numPhotos': 28, 'floor': '3', 'price': 256000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 67.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Princesa', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3879197, 'longitude': 2.1811329, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/91626925/', 'distance': '951', 'description': 'Vivienda de 67 m2 con doble orientación a calle Princesa y Assaonadors, con sol todo el día, que ocupa la tercera planta de un edificio de 1880, sin ascensor.   Distribuye 2 dormitorios, uno doble con balcón a calle Princesa y otro individual (habitación ciega), vestidor, baño completo con bañera, cocina abierta al comedor y salón.   Ventilación cruzada, cerramientos de aluminio, suelos de parquet laminado y de gres en baño, climatización en la estancia con más incidencia solar. El dormitorio individual y vestidor ventilan al actual dormitorio doble.  La distribución actual puede modificarse cambiando el dormitorio doble por el salón, sin obras. No hay posibilidad de instalar ascensor en la finca.   El Born, con comercio de proximidad y servicios, pero también una amplia oferta gastronómica y un envidiable entorno histórico de la evolución de la ciudad.   Los honorarios son a cargo del vendedor. El precio no incluye los impuestos, ni gastos de notaría ni de gestoría de la compraventa.  Eurofincas International Real Estate | Referencia V2084.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 3821.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso en Princesa'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98124798', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/45/91/16/1001891426.jpg', 'externalReference': '4400', 'numPhotos': 37, 'floor': 'bj', 'price': 350000.0, 'propertyType': 'duplex', 'operation': 'sale', 'size': 147.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle de l'Olivera", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'El Poble Sec - Parc de Montjuïc', 'latitude': 41.3715925, 'longitude': 2.1592743, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98124798/', 'distance': '1969', 'description': 'Planta baja reformada con mucho encanto. En una calle muy tranquila junto a la Plaza de Santa Madrona encontramos esta planta baja con mucho encanto. Se accede al interior por una entrada independiente, encontramos una vez en su interior a un amplio espacio para poder guardar bicicletas así como espacio polivalente para almacenaje, a continuación accedemos a un amplio comedor con cocina abierta, desde ahí podemos acceder a la planta altillo mediante unas escaleras de hierro forjado incrustadas en la pared de piedra natural o al fondo del comedor un pasillo nos daría paso a u baño con ducha seguido de un agradable patio con luz natural seguido de un cuarto de máquinas y al final un amplio espacio que hace de sala y zona polivalente con salida a una pequeña terraza con mucha luminosidad. destacar el microclima que se respira y el silencio que se respira. ! Si lo que realmente buscas es luz y tranquilidad dejaras de seguir buscando ¡ En la planta duplex o altillo encontramos un amplio espacio con zona de armarios actualmente la propiedad lo utiliza como una zona de trabajo con la posibilidad de poder hacer otro dormitorio con otro baño (preparado para ejecutar la obra, se puede ver en el plano adjunto, al fondo un pequeño pasillo nos daría paso a un segundo dormitorio con zona de vestidor con posibilidad de hacer otro baño (preparado para ejecutar la obra, se puede ver en el plano adjunto). Dispone de calefacción de gas, ventilador de techo, cocina equipada con electrodomésticos. Aincasa Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 2381.0, 'detailedType': {'typology': 'flat', 'subTypology': 'duplex'}, 'suggestedTexts': {'subtitle': 'El Poble Sec - Parc de Montjuïc, Barcelona', 'title': "Dúplex en Calle de l'Olivera"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98124798', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/45/91/16/1001891426.jpg', 'externalReference': '4400', 'numPhotos': 37, 'floor': 'bj', 'price': 350000.0, 'propertyType': 'duplex', 'operation': 'sale', 'size': 147.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle de l'Olivera", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'El Poble Sec - Parc de Montjuïc', 'latitude': 41.3715925, 'longitude': 2.1592743, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98124798/', 'distance': '1969', 'description': 'Planta baja reformada con mucho encanto. En una calle muy tranquila junto a la Plaza de Santa Madrona encontramos esta planta baja con mucho encanto. Se accede al interior por una entrada independiente, encontramos una vez en su interior a un amplio espacio para poder guardar bicicletas así como espacio polivalente para almacenaje, a continuación accedemos a un amplio comedor con cocina abierta, desde ahí podemos acceder a la planta altillo mediante unas escaleras de hierro forjado incrustadas en la pared de piedra natural o al fondo del comedor un pasillo nos daría paso a u baño con ducha seguido de un agradable patio con luz natural seguido de un cuarto de máquinas y al final un amplio espacio que hace de sala y zona polivalente con salida a una pequeña terraza con mucha luminosidad. destacar el microclima que se respira y el silencio que se respira. ! Si lo que realmente buscas es luz y tranquilidad dejaras de seguir buscando ¡ En la planta duplex o altillo encontramos un amplio espacio con zona de armarios actualmente la propiedad lo utiliza como una zona de trabajo con la posibilidad de poder hacer otro dormitorio con otro baño (preparado para ejecutar la obra, se puede ver en el plano adjunto, al fondo un pequeño pasillo nos daría paso a un segundo dormitorio con zona de vestidor con posibilidad de hacer otro baño (preparado para ejecutar la obra, se puede ver en el plano adjunto). Dispone de calefacción de gas, ventilador de techo, cocina equipada con electrodomésticos. Aincasa Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 2381.0, 'detailedType': {'typology': 'flat', 'subTypology': 'duplex'}, 'suggestedTexts': {'subtitle': 'El Poble Sec - Parc de Montjuïc, Barcelona', 'title': "Dúplex en Calle de l'Olivera"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AM2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97501131', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/6b/f9/3d/981296577.jpg', 'externalReference': 'V220429', 'numPhotos': 20, 'floor': '1', 'price': 384000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 78.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle Balmes', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3925976, 'longitude': 2.1616804, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97501131/', 'distance': '881', 'description': 'Cafur les presenta, en la céntrica calle Balmes, en el corazón de la Barcelona tradicional, esta maravillosa propiedad en finca regia del año 1909 con ascensor. La vivienda, que destaca por la altura de los techos, la sensación de confort y la luminosidad da al patio de manzana, por lo que no tendrás que sufrir por los ruidos del tráfico rodado. Cuenta con la siguiente distribución: amplio y luminoso salón comedor gracias a su conexión con la galería, ideal para poner una zona de lectura o un pequeño estudio; cocina independiente para actualizar; 2 dormitorios; 1 baño completo de tres piezas con bañera; y pasillo distribuidor. Está ubicado a sólo unos metros de la emblemática Rambla Catalunya y Passeig de Gràcia, donde encontrarás tiendas de primeras marcas. Además estarás rodeado de todos los servicios que puedas necesitar y de una amplia red de transporte público.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4923.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle Balmes'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97501131', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/6b/f9/3d/981296577.jpg', 'externalReference': 'V220429', 'numPhotos': 20, 'floor': '1', 'price': 384000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 78.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle Balmes', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3925976, 'longitude': 2.1616804, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97501131/', 'distance': '881', 'description': 'Cafur les presenta, en la céntrica calle Balmes, en el corazón de la Barcelona tradicional, esta maravillosa propiedad en finca regia del año 1909 con ascensor. La vivienda, que destaca por la altura de los techos, la sensación de confort y la luminosidad da al patio de manzana, por lo que no tendrás que sufrir por los ruidos del tráfico rodado. Cuenta con la siguiente distribución: amplio y luminoso salón comedor gracias a su conexión con la galería, ideal para poner una zona de lectura o un pequeño estudio; cocina independiente para actualizar; 2 dormitorios; 1 baño completo de tres piezas con bañera; y pasillo distribuidor. Está ubicado a sólo unos metros de la emblemática Rambla Catalunya y Passeig de Gràcia, donde encontrarás tiendas de primeras marcas. Además estarás rodeado de todos los servicios que puedas necesitar y de una amplia red de transporte público.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4923.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle Balmes'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AN2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '96967469', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/21/cc/9b/961770545.jpg', 'externalReference': '4382', 'numPhotos': 39, 'floor': 'bj', 'price': 249000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 80.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de Sant Antoni Abat', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3780021, 'longitude': 2.1625679, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96967469/', 'distance': '1211', 'description': 'A escasos metros del Mercado de Sant Antoni y Ronda Sant Antoni. Reforma de Lujo. Planta baja reformada integralmente, paredes recuperadas de piedra, techos altos con bóveda catalana y vigas de madera, en el acceso nos encontramos con una doble entrada con pared de piedra ideal par dejar bicicleta o moto protegidas. Al acceder al interior tenemos un amplio salón-comedor, cocina independiente totalmente equipada, dos dormitorios dobles, ambos con baño en suite mas un tercer baño con ducha, el dormitorio principal tiene salida a un patio por el que entra luz natural. Dispone de aire acondicionado con bomba de calor. Con mucho encanto, reforma cuidada hasta el ultimo detalle. En los gastos de comunidad está incluido el suministro del agua. Zona con todo tipo de servicios, comercios y restaurantes, a 200 metros del Mercado de Sant Antoni. El precio no incluye los impuestos, ni los gastos de Notaria, Registro y Gestoría. Aincasa Aicat número 2677. Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 3113.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de Sant Antoni Abat'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '96967469', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/21/cc/9b/961770545.jpg', 'externalReference': '4382', 'numPhotos': 39, 'floor': 'bj', 'price': 249000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 80.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de Sant Antoni Abat', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3780021, 'longitude': 2.1625679, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96967469/', 'distance': '1211', 'description': 'A escasos metros del Mercado de Sant Antoni y Ronda Sant Antoni. Reforma de Lujo. Planta baja reformada integralmente, paredes recuperadas de piedra, techos altos con bóveda catalana y vigas de madera, en el acceso nos encontramos con una doble entrada con pared de piedra ideal par dejar bicicleta o moto protegidas. Al acceder al interior tenemos un amplio salón-comedor, cocina independiente totalmente equipada, dos dormitorios dobles, ambos con baño en suite mas un tercer baño con ducha, el dormitorio principal tiene salida a un patio por el que entra luz natural. Dispone de aire acondicionado con bomba de calor. Con mucho encanto, reforma cuidada hasta el ultimo detalle. En los gastos de comunidad está incluido el suministro del agua. Zona con todo tipo de servicios, comercios y restaurantes, a 200 metros del Mercado de Sant Antoni. El precio no incluye los impuestos, ni los gastos de Notaria, Registro y Gestoría. Aincasa Aicat número 2677. Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 3113.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de Sant Antoni Abat'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AO2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '94041284', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/cd/c0/bb/888738711.jpg', 'externalReference': '4340', 'numPhotos': 27, 'floor': '4', 'price': 360000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle de l'Oli", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3833513, 'longitude': 2.1766716, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/94041284/', 'distance': '737', 'description': "A escasos metros de La Catedral de Barcelona y Mercado de Santa Caterina. En el Barrio de La Ribera- Borne se encuentra esta fabulosa vivienda, con mucho encanto, al acceder a la vivienda dos zonas dividen la zona de día y de noche, en la zona de día encontramos un amplio salón-comedor con luz a raudales y bonitas vistas a terrazas ajardinadas, la cocina comunica con una ventana que permite el paso con el comedor para compartir momentos con familia y amigos, en frente se encuentra el baño con ducha, un amplio pasillo nos da paso a los dormitorios (2) dobles y muy soleados, el dormitorio principal tiene salida a un pequeño balcón con vistas a la misma calle de L'Oli, destacar los detalles como las vigas vistas, la contraventanas tienen aislamiento térmico con poco uso, calefacción. La finca dispone de ascensor, se accede subiendo un tramo de escaleras. El edificio cuenta con dos terrazas de uso comunitario con unas vistas únicas para poder disfrutar de las puestas de sol, en el terrado también se encuentra un amplio trastero para uso comunitario. El Born es un barrio a la última caracterizado por sus callejas medievales. De día, es posible disfrutar de cafeterías y boutiques de diseñadores, mientras que las coctelerías y la samba protagonizan sus noches. La basílica de Santa María del Mar exhibe ornamentales vidrieras. En el famoso museo Picasso se exponen muchas de las obras maestras del artista. El Born Centre de Cultura i Memoria es un centro polivalente que ocupa el edificio de un antiguo mercado y conserva en su interior un yacimiento arqueológico. El Born se encuentra entre la Via Laietana y la Barceloneta y tiene un buen servicio de transporte, con las paradas del metro Barceloneta y Jaume 1 en la misma línea. No obstante, a Las Ramblas y al centro de la ciudad puedes llegar caminando en sólo 10 minutos. La playa también está a unos 10 minutos caminando, lo que significa que podrás disfrutar de unas vacaciones en la playa y descansar de la ciudad al mismo tiempo. Además, el Born está bastante cerca del Parque de la Ciutadella: un pulmón de la ciudad condal, un lugar tranquilo para relajarte y pasear. Aincasa Un sueño una realidad.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4337.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': "Piso en Calle de l'Oli"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '94041284', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/cd/c0/bb/888738711.jpg', 'externalReference': '4340', 'numPhotos': 27, 'floor': '4', 'price': 360000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle de l'Oli", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3833513, 'longitude': 2.1766716, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/94041284/', 'distance': '737', 'description': "A escasos metros de La Catedral de Barcelona y Mercado de Santa Caterina. En el Barrio de La Ribera- Borne se encuentra esta fabulosa vivienda, con mucho encanto, al acceder a la vivienda dos zonas dividen la zona de día y de noche, en la zona de día encontramos un amplio salón-comedor con luz a raudales y bonitas vistas a terrazas ajardinadas, la cocina comunica con una ventana que permite el paso con el comedor para compartir momentos con familia y amigos, en frente se encuentra el baño con ducha, un amplio pasillo nos da paso a los dormitorios (2) dobles y muy soleados, el dormitorio principal tiene salida a un pequeño balcón con vistas a la misma calle de L'Oli, destacar los detalles como las vigas vistas, la contraventanas tienen aislamiento térmico con poco uso, calefacción. La finca dispone de ascensor, se accede subiendo un tramo de escaleras. El edificio cuenta con dos terrazas de uso comunitario con unas vistas únicas para poder disfrutar de las puestas de sol, en el terrado también se encuentra un amplio trastero para uso comunitario. El Born es un barrio a la última caracterizado por sus callejas medievales. De día, es posible disfrutar de cafeterías y boutiques de diseñadores, mientras que las coctelerías y la samba protagonizan sus noches. La basílica de Santa María del Mar exhibe ornamentales vidrieras. En el famoso museo Picasso se exponen muchas de las obras maestras del artista. El Born Centre de Cultura i Memoria es un centro polivalente que ocupa el edificio de un antiguo mercado y conserva en su interior un yacimiento arqueológico. El Born se encuentra entre la Via Laietana y la Barceloneta y tiene un buen servicio de transporte, con las paradas del metro Barceloneta y Jaume 1 en la misma línea. No obstante, a Las Ramblas y al centro de la ciudad puedes llegar caminando en sólo 10 minutos. La playa también está a unos 10 minutos caminando, lo que significa que podrás disfrutar de unas vacaciones en la playa y descansar de la ciudad al mismo tiempo. Además, el Born está bastante cerca del Parque de la Ciutadella: un pulmón de la ciudad condal, un lugar tranquilo para relajarte y pasear. Aincasa Un sueño una realidad.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4337.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': "Piso en Calle de l'Oli"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AP2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98793896', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ce/23/f6/1024006628.jpg', 'externalReference': '11650', 'numPhotos': 28, 'floor': '3', 'price': 574000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 86.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio Vila de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'Vila de Gràcia', 'latitude': 41.4110641, 'longitude': 2.1580262, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98793896/', 'distance': '2799', 'description': "Situado en una finca moderna, nos encontramos con este coqueto y acogedor ático dúplex de 86\u202fm construidos más 20\u202fm de trza. Con vistas totalmente despejadas al Icónico Tenis, la Salut y al Tibidabo, muy luminoso y con sol de tarde. La vivienda está muy bien conservado. Se distribuye en un amplio y agradable salón comedor con vistas al tenis, y con cocina americana, práctica y funcional, totalmente equipada y amueblada. En esta planta también nos encontramos con una habitación individual exterior al tenis. Un baño completo con ducha y un armario amplio que nos puede hacer la función de trastero. Accedemos a la primera planta a través de una amplia y cómoda escalera que nos da paso, a la Suite, con un espacioso baño. Y a la agradable terraza. Dicha terraza nos induce a disfrutarla durante el día, al sol para, relajarse, leer o hacer actividades, y a sus atardeceres que se prestan a tomar una copa con la tranquilidad y la calma. Al igual que al anochecer que nos invita al disfrute de cenas y veladas bajo las estrellas y a la luz de la luna. Rodeada de plantas y flores que nos pueden transportar a un pequeño Edén, en la ciudad. Observaciones: plaza de parking opcional por 25.000, calefacción a gas, aire centralizado, armarios empotrados. Suelos de parquet, etc. En definitiva, una excelente calidad de vida. Gracia es un barrio informal con calles estrechas y plazas acogedoras lleno de tiendas de comestibles ecológicos, espacios de trabajo compartido modernos y estudios de artistas. La zona está muy bien comunicada a todos los niveles. Pocos distritos de Barcelona están rodeados de tanta simbología como el de Gràcia. El casco antiguo del barrio que le da nombre no ha dejado nunca de reivindicar con orgullo su pasado como municipio independiente (se agregó a la ciudad en 1897) La urbanización del barrio de la Salut-Gracia Nova, comenzó, en la segunda mitad del siglo XIX, alrededor de la iglesia, que tomo el nombre de Nuestra Señora de la Salut cuyas inmediaciones creció el barrio a lo largo de los años. En sus inicios la actividad más importante de la zona era agrícola, hallándose importantes masías como Can Xipreret, Can Tusquets, Can Muntaner y Ca l'Alegre de Dalt, pero progresivamente fueron convirtiéndose en zona residencial de veraneo de la burguesía barcelonesa y de la antigua villa de Gracia. También se halla en el barrio el reconocidísimo tenis la Salut, la entidad fue constituida como Salud Sport Club el 8 de junio de 1902, por un grupo de deportistas a partir del Club Social La Salud, fundado en 1899. Eusebio Güell, conde de Güell, fue nombrado presidente honorífico. Para construir sus instalaciones lograron unos terrenos de la masía de Can Xipreret. En el ámbito de la raqueta, destaca la creación de la primera escuela de tenis de España, en 1959. En ella se han formado algunos de los principales tenistas españoles de la historia como Manuel Orantes, Beto Martín, Conchita Martínez o Àlex Corretja. La Salut es el único club del mundo con dos campeones de la Copa Másters de Tenis, los citados Orantes y Corretja.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': False, 'parkingSpacePrice': 25000.0}, 'priceByArea': 6674.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': 'Vila de Gràcia, Barcelona', 'title': 'Ático'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98793896', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ce/23/f6/1024006628.jpg', 'externalReference': '11650', 'numPhotos': 28, 'floor': '3', 'price': 574000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 86.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio Vila de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'Vila de Gràcia', 'latitude': 41.4110641, 'longitude': 2.1580262, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98793896/', 'distance': '2799', 'description': "Situado en una finca moderna, nos encontramos con este coqueto y acogedor ático dúplex de 86\u202fm construidos más 20\u202fm de trza. Con vistas totalmente despejadas al Icónico Tenis, la Salut y al Tibidabo, muy luminoso y con sol de tarde. La vivienda está muy bien conservado. Se distribuye en un amplio y agradable salón comedor con vistas al tenis, y con cocina americana, práctica y funcional, totalmente equipada y amueblada. En esta planta también nos encontramos con una habitación individual exterior al tenis. Un baño completo con ducha y un armario amplio que nos puede hacer la función de trastero. Accedemos a la primera planta a través de una amplia y cómoda escalera que nos da paso, a la Suite, con un espacioso baño. Y a la agradable terraza. Dicha terraza nos induce a disfrutarla durante el día, al sol para, relajarse, leer o hacer actividades, y a sus atardeceres que se prestan a tomar una copa con la tranquilidad y la calma. Al igual que al anochecer que nos invita al disfrute de cenas y veladas bajo las estrellas y a la luz de la luna. Rodeada de plantas y flores que nos pueden transportar a un pequeño Edén, en la ciudad. Observaciones: plaza de parking opcional por 25.000, calefacción a gas, aire centralizado, armarios empotrados. Suelos de parquet, etc. En definitiva, una excelente calidad de vida. Gracia es un barrio informal con calles estrechas y plazas acogedoras lleno de tiendas de comestibles ecológicos, espacios de trabajo compartido modernos y estudios de artistas. La zona está muy bien comunicada a todos los niveles. Pocos distritos de Barcelona están rodeados de tanta simbología como el de Gràcia. El casco antiguo del barrio que le da nombre no ha dejado nunca de reivindicar con orgullo su pasado como municipio independiente (se agregó a la ciudad en 1897) La urbanización del barrio de la Salut-Gracia Nova, comenzó, en la segunda mitad del siglo XIX, alrededor de la iglesia, que tomo el nombre de Nuestra Señora de la Salut cuyas inmediaciones creció el barrio a lo largo de los años. En sus inicios la actividad más importante de la zona era agrícola, hallándose importantes masías como Can Xipreret, Can Tusquets, Can Muntaner y Ca l'Alegre de Dalt, pero progresivamente fueron convirtiéndose en zona residencial de veraneo de la burguesía barcelonesa y de la antigua villa de Gracia. También se halla en el barrio el reconocidísimo tenis la Salut, la entidad fue constituida como Salud Sport Club el 8 de junio de 1902, por un grupo de deportistas a partir del Club Social La Salud, fundado en 1899. Eusebio Güell, conde de Güell, fue nombrado presidente honorífico. Para construir sus instalaciones lograron unos terrenos de la masía de Can Xipreret. En el ámbito de la raqueta, destaca la creación de la primera escuela de tenis de España, en 1959. En ella se han formado algunos de los principales tenistas españoles de la historia como Manuel Orantes, Beto Martín, Conchita Martínez o Àlex Corretja. La Salut es el único club del mundo con dos campeones de la Copa Másters de Tenis, los citados Orantes y Corretja.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': False, 'parkingSpacePrice': 25000.0}, 'priceByArea': 6674.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': 'Vila de Gràcia, Barcelona', 'title': 'Ático'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AQ2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98508998', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/19/98/bb/1014756994.jpg', 'externalReference': '4740X', 'numPhotos': 17, 'floor': '5', 'price': 385000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle del Rosselló', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3858287, 'longitude': 2.148551, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98508998/', 'distance': '1777', 'description': "Este piso se encuentra en la zona del La Nova Esquerra de l'Eixample, en la quinta planta.  En el área hay todo tipo de servicios como ocio y restauración, colegios, sanidad, transporte público, etc.  La vivienda tiene dos dormitorios, uno de ellos es doble exterior y el otro es individual con ventana a un patio interior.  Tiene un baño en perfecto estado que es completo con ducha y se ubica en el centro del piso. El piso tiene un amplio y luminosos salón, estilo diáfano, con dos ambientes comunicados para el comedor y otro para el salón. En el mismo hay una salida directa a un perfecto balcón.  La cocina es estilo americana y se encuentra en perfecto estado. Para más información o programar una visita pueden dejar un WhatsApp en el 681 38 77 03 Encuentra más en.", 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4639.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle del Rosselló'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98508998', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/19/98/bb/1014756994.jpg', 'externalReference': '4740X', 'numPhotos': 17, 'floor': '5', 'price': 385000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle del Rosselló', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3858287, 'longitude': 2.148551, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98508998/', 'distance': '1777', 'description': "Este piso se encuentra en la zona del La Nova Esquerra de l'Eixample, en la quinta planta.  En el área hay todo tipo de servicios como ocio y restauración, colegios, sanidad, transporte público, etc.  La vivienda tiene dos dormitorios, uno de ellos es doble exterior y el otro es individual con ventana a un patio interior.  Tiene un baño en perfecto estado que es completo con ducha y se ubica en el centro del piso. El piso tiene un amplio y luminosos salón, estilo diáfano, con dos ambientes comunicados para el comedor y otro para el salón. En el mismo hay una salida directa a un perfecto balcón.  La cocina es estilo americana y se encuentra en perfecto estado. Para más información o programar una visita pueden dejar un WhatsApp en el 681 38 77 03 Encuentra más en.", 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4639.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle del Rosselló'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AR2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98145102', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/94/3e/d6/1002492446.jpg', 'externalReference': '101217', 'numPhotos': 35, 'floor': 'en', 'price': 420000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 101.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Sant Pau', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3776106, 'longitude': 2.172716, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98145102/', 'distance': '1124', 'description': 'PISAZO DE 100M2 + 58M2 DE TERRAZA, EN FINCA DEL AÑO 1850 COMPLETAMENTE REHABILITADA. La propiedad en venta actualmente está dividida físicamente (no segregada) en dos apartamentos completos e independientes, que comparten luz, agua y gas. Cada apartamento tiene su propio acceso independiente con llave, y constan de un dormitorio doble, cocina totalmente equipada, sala de estar/comedor y baño completo. La vivienda está situada en la amplia plaza Salvador Seguí, delante de la Filmoteca, en el Raval, a tres minutos de les Ramblas. La finca es del año 1850, ha sido completamente rehabilitada, cuenta con cámaras de seguridad en la entrada y en cada rellano, tiene la ITE pasada con su correspondiente Certificado de Aptitud del año 2020, y no tiene derramas pendientes. El acceso a la finca es a través de un código numérico, llave física o interfono preparado con videocámara.  La propiedad está en una primera planta real sin ascensor y tiene caja de llaves digital. Al entrar por la puerta principal, tenemos un distribuidor con cámara de vigilancia y los contadores generales del inmueble, desde aquí accedemos a mano derecha al apartamento exterior a la calle, que da a la plaza Salvador Seguí, que consta de un salón comedor exterior con dos ventanas y un gran ventanal con balcón, con orientación noroeste, cocina totalmente equipada, un dormitorio doble que le entra luz por unas ventanas que dan al salón, y un baño completo. Techos altos de unos cuatro metros. Tiene luz todo el día y sol por las tardes.  El otro apartamento consta de un amplio salón comedor que goza de mucha luz natural gracias a su gran ventanal orientado al sudeste por donde entra luz todo el día y sol directo toda la mañana y mediodía, que da a una terraza de 50 metros cuadrados, privada, amueblada, con toldo retraible y de uso exclusivo. La terraza está en un patio interior de manzana absolutamente silencioso. Techos altos a más de cuatro metros con volta catalana. Consta de una habitación doble, baño completo, y cocina totalmente equipada. Ambos apartamentos gozan de carpintería de aluminio con doble cristal acústico, aire acondicionado y bomba de calor por conductos en todas las habitaciones, calefacción de radiadores y agua caliente ilimitada por caldera de gas centralizada. Actualmente, cada apartamento tiene un contrato de alquiler a largo plazo. Por lo tanto, esta propiedad genera dos alquileres que conjuntamente suman 2.150€ brutos al mes, o 25,800€ anuales. En una configuración de alquiler vacacional puro (contratos mensuales, el apartamento no tiene licencia turística) el bruto anual incrementa un 35% hasta los 35,000€, aproximadamente. A pesar de los contratos de largo plazo actuales, los apartamentos están diseñados para alquileres de temporada o vacacionales e incluyen en el precio de venta todo lo necesario para entrar a vivir inmediatamente: cubertería, ropa de cama, etc. Los apartamentos están separados por anchas paredes de piedra y fibra acústica en ambos lados, justamente para que no se molesten acústicamente. Cada apartamento tiene su llave privada y una cámara de seguridad en el pasillo interior que los une. Así, sería posible alquilar un apartamento en régimen vacacional y otro a largo plazo, por ejemplo. La flexibilidad es total. El propietario ha alquilado la propiedad como un solo apartamento y como dos apartamentos independientes. Ha alquilado a largo plazo, por temporada y como apartamentos vacacionales. Los apartamentos se han diseñado como hogares de alto standing. El precio de venta incluye todos los muebles y objetos de decoración tal y como se ven en las fotografías, menos los cuadros. Destaco: dos sofás cama (uno de ellos un Chesterfield original, importado de Inglaterra, de cuero rojo), dos camas dobles, dos mesas y sus sillas de comedor, los muebles de terraza (sofás de exterior, alfombra, plantas y tumbonas de madera). Gracias a los sofás cama, cada apart.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 4158.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de Sant Pau'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98145102', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/94/3e/d6/1002492446.jpg', 'externalReference': '101217', 'numPhotos': 35, 'floor': 'en', 'price': 420000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 101.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Sant Pau', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3776106, 'longitude': 2.172716, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98145102/', 'distance': '1124', 'description': 'PISAZO DE 100M2 + 58M2 DE TERRAZA, EN FINCA DEL AÑO 1850 COMPLETAMENTE REHABILITADA. La propiedad en venta actualmente está dividida físicamente (no segregada) en dos apartamentos completos e independientes, que comparten luz, agua y gas. Cada apartamento tiene su propio acceso independiente con llave, y constan de un dormitorio doble, cocina totalmente equipada, sala de estar/comedor y baño completo. La vivienda está situada en la amplia plaza Salvador Seguí, delante de la Filmoteca, en el Raval, a tres minutos de les Ramblas. La finca es del año 1850, ha sido completamente rehabilitada, cuenta con cámaras de seguridad en la entrada y en cada rellano, tiene la ITE pasada con su correspondiente Certificado de Aptitud del año 2020, y no tiene derramas pendientes. El acceso a la finca es a través de un código numérico, llave física o interfono preparado con videocámara.  La propiedad está en una primera planta real sin ascensor y tiene caja de llaves digital. Al entrar por la puerta principal, tenemos un distribuidor con cámara de vigilancia y los contadores generales del inmueble, desde aquí accedemos a mano derecha al apartamento exterior a la calle, que da a la plaza Salvador Seguí, que consta de un salón comedor exterior con dos ventanas y un gran ventanal con balcón, con orientación noroeste, cocina totalmente equipada, un dormitorio doble que le entra luz por unas ventanas que dan al salón, y un baño completo. Techos altos de unos cuatro metros. Tiene luz todo el día y sol por las tardes.  El otro apartamento consta de un amplio salón comedor que goza de mucha luz natural gracias a su gran ventanal orientado al sudeste por donde entra luz todo el día y sol directo toda la mañana y mediodía, que da a una terraza de 50 metros cuadrados, privada, amueblada, con toldo retraible y de uso exclusivo. La terraza está en un patio interior de manzana absolutamente silencioso. Techos altos a más de cuatro metros con volta catalana. Consta de una habitación doble, baño completo, y cocina totalmente equipada. Ambos apartamentos gozan de carpintería de aluminio con doble cristal acústico, aire acondicionado y bomba de calor por conductos en todas las habitaciones, calefacción de radiadores y agua caliente ilimitada por caldera de gas centralizada. Actualmente, cada apartamento tiene un contrato de alquiler a largo plazo. Por lo tanto, esta propiedad genera dos alquileres que conjuntamente suman 2.150€ brutos al mes, o 25,800€ anuales. En una configuración de alquiler vacacional puro (contratos mensuales, el apartamento no tiene licencia turística) el bruto anual incrementa un 35% hasta los 35,000€, aproximadamente. A pesar de los contratos de largo plazo actuales, los apartamentos están diseñados para alquileres de temporada o vacacionales e incluyen en el precio de venta todo lo necesario para entrar a vivir inmediatamente: cubertería, ropa de cama, etc. Los apartamentos están separados por anchas paredes de piedra y fibra acústica en ambos lados, justamente para que no se molesten acústicamente. Cada apartamento tiene su llave privada y una cámara de seguridad en el pasillo interior que los une. Así, sería posible alquilar un apartamento en régimen vacacional y otro a largo plazo, por ejemplo. La flexibilidad es total. El propietario ha alquilado la propiedad como un solo apartamento y como dos apartamentos independientes. Ha alquilado a largo plazo, por temporada y como apartamentos vacacionales. Los apartamentos se han diseñado como hogares de alto standing. El precio de venta incluye todos los muebles y objetos de decoración tal y como se ven en las fotografías, menos los cuadros. Destaco: dos sofás cama (uno de ellos un Chesterfield original, importado de Inglaterra, de cuero rojo), dos camas dobles, dos mesas y sus sillas de comedor, los muebles de terraza (sofás de exterior, alfombra, plantas y tumbonas de madera). Gracias a los sofás cama, cada apart.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 4158.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de Sant Pau'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AS2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97933192', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/11/01/9b/995459861.jpg', 'externalReference': '261437', 'numPhotos': 16, 'floor': '1', 'price': 768000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 130.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3858408, 'longitude': 2.1603522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97933192/', 'distance': '804', 'description': 'DIPUTACIO - ARIBAU impresionante piso de diseño nuevo a estrenar en finca regia tiene 148 m² según referencia catastral, dispone de 2 habitaciones tipos suite, gran vestidor. La vivienda muy bien distribuida y bien diferenciada la zona de día de la de noche, al entrar encontramos un gran hall que da acceso a la cómoda cocina completamente equipada con electrodomésticos de alta gama y al magnífico salón comedor exterior a la calle con balcón, dispone de sistema de domótica de luz y persianas, carpintería de aluminio, aire acondicionado en todas las estancias y radiadores. En la zona de noche encontramos los dos dormitorios suitte uno de ellos con vestidor. La finca regia es preciosa, muy elegante, cuidada. Está ubicado en uno de los barrios más elegantes y de mayor comercio de Barcelona y una zona muy demandada debido a su enclave privilegiado. Se encuentra cerca de las principales vías de entrada y salida de la ciudad, cerca del exclusivo Paseo de Gracia y rodeada de transporte publico para acceder a cualquier parte de Barcelona. Este barrio cuenta con todos los servicios y tiendas especializadas que usted necesite. Desde las tiendas más exclusivas de la ciudad y famosas internacionalmente tanto moda y complementos como tiendas gourmet, parques, oficinas etc. Zona prime en pleno centro de Barcelona. Zona Ciutat Vella. ( El PVP indicado no incluye impuestos ni gastos de Escritura ).  PARA PROPIETARIOS:  1. ¿Necesitas vender para comprar? donpiso puede comprar tu casa entregándote el 10% en 48 horas y el resto ante Notario.  2. ¿Problemas económicos? Te ayudamos entregándote una cantidad pactada cada mes mientras vendemos tu casa. Sin gastos de ningún tipo.  3. ¿Vendes un piso con hipoteca? mientras gestionamos la venta, te adelantamos la cuota mensual.  4. ¿Reformas? al mejor precio y te las financiamos dentro de la hipoteca.  5. ¿La mejor hipoteca? en donpiso la encuentras y con condiciones preferentes.  6. ¿Herencias y divorcios? te ayudamos y coordinamos todo.  Infórmate: 93 306 90 90 -.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5908.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': False, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97933192', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/11/01/9b/995459861.jpg', 'externalReference': '261437', 'numPhotos': 16, 'floor': '1', 'price': 768000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 130.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3858408, 'longitude': 2.1603522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97933192/', 'distance': '804', 'description': 'DIPUTACIO - ARIBAU impresionante piso de diseño nuevo a estrenar en finca regia tiene 148 m² según referencia catastral, dispone de 2 habitaciones tipos suite, gran vestidor. La vivienda muy bien distribuida y bien diferenciada la zona de día de la de noche, al entrar encontramos un gran hall que da acceso a la cómoda cocina completamente equipada con electrodomésticos de alta gama y al magnífico salón comedor exterior a la calle con balcón, dispone de sistema de domótica de luz y persianas, carpintería de aluminio, aire acondicionado en todas las estancias y radiadores. En la zona de noche encontramos los dos dormitorios suitte uno de ellos con vestidor. La finca regia es preciosa, muy elegante, cuidada. Está ubicado en uno de los barrios más elegantes y de mayor comercio de Barcelona y una zona muy demandada debido a su enclave privilegiado. Se encuentra cerca de las principales vías de entrada y salida de la ciudad, cerca del exclusivo Paseo de Gracia y rodeada de transporte publico para acceder a cualquier parte de Barcelona. Este barrio cuenta con todos los servicios y tiendas especializadas que usted necesite. Desde las tiendas más exclusivas de la ciudad y famosas internacionalmente tanto moda y complementos como tiendas gourmet, parques, oficinas etc. Zona prime en pleno centro de Barcelona. Zona Ciutat Vella. ( El PVP indicado no incluye impuestos ni gastos de Escritura ).  PARA PROPIETARIOS:  1. ¿Necesitas vender para comprar? donpiso puede comprar tu casa entregándote el 10% en 48 horas y el resto ante Notario.  2. ¿Problemas económicos? Te ayudamos entregándote una cantidad pactada cada mes mientras vendemos tu casa. Sin gastos de ningún tipo.  3. ¿Vendes un piso con hipoteca? mientras gestionamos la venta, te adelantamos la cuota mensual.  4. ¿Reformas? al mejor precio y te las financiamos dentro de la hipoteca.  5. ¿La mejor hipoteca? en donpiso la encuentras y con condiciones preferentes.  6. ¿Herencias y divorcios? te ayudamos y coordinamos todo.  Infórmate: 93 306 90 90 -.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5908.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': False, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AT2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97661362', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/27/af/fc/1031239714.jpg', 'externalReference': '236620', 'numPhotos': 19, 'floor': 'bj', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 149.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3843408, 'longitude': 2.1626522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97661362/', 'distance': '686', 'description': 'DIPUTACIO - ARIBAU Impresionante piso de diseño con terraza nuevo a estrenar en finca regia tiene 148 m² según referencia catastral, dispone de 2 habitaciones de las cuales dos son suite, gran vestidor. La vivienda muy bien distribuida y bien diferenciada la zona de día de la de noche, al entrar encontramos un gran hall que da acceso a la cómoda cocina completamente equipada con electrodomésticos de alta gama y al magnífico salón comedor exterior a la calle con balcón, dispone de sistema de domótica de luz y persianas, carpintería de aluminio, aire acondicionado en todas las estancias y radiadores. En la zona de noche encontramos los dos dormitorios suitte uno de ellos con vestidor y con salia a la magnífica terraza de 41 m². La finca regia es preciosa, muy elegante, cuidada. Está ubicado en uno de los barrios más elegantes y de mayor comercio de Barcelona y una zona muy demandada debido a su enclave privilegiado. Se encuentra cerca de las principales vías de entrada y salida de la ciudad, cerca del exclusivo Paseo de Gracia y rodeada de transporte publico para acceder a cualquier parte de Barcelona. Este barrio cuenta con todos los servicios y tiendas especializadas que usted necesite. Desde las tiendas más exclusivas de la ciudad y famosas internacionalmente tanto moda y complementos como tiendas gourmet, parques, oficinas etc. Zona prime en pleno centro de Barcelona. Zona Ciutat Vella. ( El PVP indicado no incluye impuestos ni gastos de Escritura ).  PARA PROPIETARIOS:  1. ¿Necesitas vender para comprar? donpiso puede comprar tu casa entregándote el 10% en 48 horas y el resto ante Notario.  2. ¿Problemas económicos? Te ayudamos entregándote una cantidad pactada cada mes mientras vendemos tu casa. Sin gastos de ningún tipo.  3. ¿Vendes un piso con hipoteca? mientras gestionamos la venta, te adelantamos la cuota mensual.  4. ¿Reformas? al mejor precio y te las financiamos dentro de la hipoteca.  5. ¿La mejor hipoteca? en donpiso la encuentras y con condiciones preferentes.  6. ¿Herencias y divorcios? te ayudamos y coordinamos todo.  Infórmate: 93 306 90 90 -.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5691.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': False, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97661362', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/27/af/fc/1031239714.jpg', 'externalReference': '236620', 'numPhotos': 19, 'floor': 'bj', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 149.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3843408, 'longitude': 2.1626522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97661362/', 'distance': '686', 'description': 'DIPUTACIO - ARIBAU Impresionante piso de diseño con terraza nuevo a estrenar en finca regia tiene 148 m² según referencia catastral, dispone de 2 habitaciones de las cuales dos son suite, gran vestidor. La vivienda muy bien distribuida y bien diferenciada la zona de día de la de noche, al entrar encontramos un gran hall que da acceso a la cómoda cocina completamente equipada con electrodomésticos de alta gama y al magnífico salón comedor exterior a la calle con balcón, dispone de sistema de domótica de luz y persianas, carpintería de aluminio, aire acondicionado en todas las estancias y radiadores. En la zona de noche encontramos los dos dormitorios suitte uno de ellos con vestidor y con salia a la magnífica terraza de 41 m². La finca regia es preciosa, muy elegante, cuidada. Está ubicado en uno de los barrios más elegantes y de mayor comercio de Barcelona y una zona muy demandada debido a su enclave privilegiado. Se encuentra cerca de las principales vías de entrada y salida de la ciudad, cerca del exclusivo Paseo de Gracia y rodeada de transporte publico para acceder a cualquier parte de Barcelona. Este barrio cuenta con todos los servicios y tiendas especializadas que usted necesite. Desde las tiendas más exclusivas de la ciudad y famosas internacionalmente tanto moda y complementos como tiendas gourmet, parques, oficinas etc. Zona prime en pleno centro de Barcelona. Zona Ciutat Vella. ( El PVP indicado no incluye impuestos ni gastos de Escritura ).  PARA PROPIETARIOS:  1. ¿Necesitas vender para comprar? donpiso puede comprar tu casa entregándote el 10% en 48 horas y el resto ante Notario.  2. ¿Problemas económicos? Te ayudamos entregándote una cantidad pactada cada mes mientras vendemos tu casa. Sin gastos de ningún tipo.  3. ¿Vendes un piso con hipoteca? mientras gestionamos la venta, te adelantamos la cuota mensual.  4. ¿Reformas? al mejor precio y te las financiamos dentro de la hipoteca.  5. ¿La mejor hipoteca? en donpiso la encuentras y con condiciones preferentes.  6. ¿Herencias y divorcios? te ayudamos y coordinamos todo.  Infórmate: 93 306 90 90 -.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5691.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': False, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AU2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '95993558', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8a/45/92/933783157.jpg', 'externalReference': 'W-02NAXU', 'numPhotos': 31, 'price': 275000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 88.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle del Moianès', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'Hostafrancs', 'latitude': 41.3748961, 'longitude': 2.1433843, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/95993558/', 'distance': '2605', 'description': 'Pis a reformar con cédula Engel &amp; Völkers presenta una oportunidad de inversión en un amplio piso con vistas despejadas en Carrer de Moianès. Se compone de una vivienda de 88m2 construidos con cédula de habitabilidad, en una finca con ascensor, que hasta el momento se utilizaba como oficina, por tanto, tenemos un gran espacio diáfano con dos habitaciones y un baño que se puede reconvertir al piso que desees. Una quinta planta real. Entrando por la puerta accedemos a un pequeño pasillo con una amplia habitación y cocina a la izquierda y, a la derecha, otra pequeña con el baño. A continuación vemos el gran espacio diáfano con grandes ventanales que dejan entrar muchísima luz. Piso de grandes dimensiones para hacerlo completamente al gusto. La propiedad está estratégicamente ubicada en la mejor zona del barrio de Hostafrancs (Sants). La proximidad de la vivienda a la Plaza España, uno de los centros neurálgicos de Barcelona, así como también a la Estación de Sants, situándose en calle Moianès, representa la comodidad de tenerlo todo a solo dos minutos, supermercados, comercios varios, bancos, gimnasios, escuelas. Contando además con todos los medios de transporte urbano (FGC, Metro Líneas 1 y 3, Aerobús A1 y A2, más de 10 líneas de buses) y el desplazamiento directo a pie de la Fira de Barcelona. Es una ubicación ideal para familias, turistas, y personas que necesiten un "pied a terre" en Barcelona, facilitando los desplazamientos y viajes por trabajo. Sants, La Bordeta y Hostafrancs, son el símbolo de la Barcelona turística y cosmopolita, pero también de las tradiciones de los barrios más céntricos de la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3125.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Hostafrancs, Barcelona', 'title': 'Piso en Calle del Moianès'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': True, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '95993558', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8a/45/92/933783157.jpg', 'externalReference': 'W-02NAXU', 'numPhotos': 31, 'price': 275000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 88.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle del Moianès', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'Hostafrancs', 'latitude': 41.3748961, 'longitude': 2.1433843, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/95993558/', 'distance': '2605', 'description': 'Pis a reformar con cédula Engel &amp; Völkers presenta una oportunidad de inversión en un amplio piso con vistas despejadas en Carrer de Moianès. Se compone de una vivienda de 88m2 construidos con cédula de habitabilidad, en una finca con ascensor, que hasta el momento se utilizaba como oficina, por tanto, tenemos un gran espacio diáfano con dos habitaciones y un baño que se puede reconvertir al piso que desees. Una quinta planta real. Entrando por la puerta accedemos a un pequeño pasillo con una amplia habitación y cocina a la izquierda y, a la derecha, otra pequeña con el baño. A continuación vemos el gran espacio diáfano con grandes ventanales que dejan entrar muchísima luz. Piso de grandes dimensiones para hacerlo completamente al gusto. La propiedad está estratégicamente ubicada en la mejor zona del barrio de Hostafrancs (Sants). La proximidad de la vivienda a la Plaza España, uno de los centros neurálgicos de Barcelona, así como también a la Estación de Sants, situándose en calle Moianès, representa la comodidad de tenerlo todo a solo dos minutos, supermercados, comercios varios, bancos, gimnasios, escuelas. Contando además con todos los medios de transporte urbano (FGC, Metro Líneas 1 y 3, Aerobús A1 y A2, más de 10 líneas de buses) y el desplazamiento directo a pie de la Fira de Barcelona. Es una ubicación ideal para familias, turistas, y personas que necesiten un "pied a terre" en Barcelona, facilitando los desplazamientos y viajes por trabajo. Sants, La Bordeta y Hostafrancs, son el símbolo de la Barcelona turística y cosmopolita, pero también de las tradiciones de los barrios más céntricos de la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3125.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Hostafrancs, Barcelona', 'title': 'Piso en Calle del Moianès'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': True, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AV2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97340498', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/80/e6/98/1046925847.jpg', 'externalReference': 'FloridaFranç', 'numPhotos': 23, 'floor': '2', 'price': 315000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de Floridablanca', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'Sant Antoni', 'latitude': 41.3766483, 'longitude': 2.1541467, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97340498/', 'distance': '1772', 'description': 'Piso totalmente reformado conservando de manera cuidadosa los elementos originales tales como techos de bóveda catalana y puerta originales de madera recuperada, todo combinado con una reforma integral con materiales de muy buena calidad de un gusto excepcional. El piso tiene una superficie construida de 83 metros y una superficie útil de 75 metros, el piso tiene 2 habitaciones, baño completo cocina equipada y salón con balcón. Es una segunda planta real con ASCENSOR, en una finca Regia. No esperes más y ven a visitar este piso con nosotros. Valoramos tu casa Encuentra más en.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3795.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Antoni, Barcelona', 'title': 'Piso en Calle de Floridablanca'}, 'hasPlan': False, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97340498', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/80/e6/98/1046925847.jpg', 'externalReference': 'FloridaFranç', 'numPhotos': 23, 'floor': '2', 'price': 315000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de Floridablanca', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'Sant Antoni', 'latitude': 41.3766483, 'longitude': 2.1541467, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97340498/', 'distance': '1772', 'description': 'Piso totalmente reformado conservando de manera cuidadosa los elementos originales tales como techos de bóveda catalana y puerta originales de madera recuperada, todo combinado con una reforma integral con materiales de muy buena calidad de un gusto excepcional. El piso tiene una superficie construida de 83 metros y una superficie útil de 75 metros, el piso tiene 2 habitaciones, baño completo cocina equipada y salón con balcón. Es una segunda planta real con ASCENSOR, en una finca Regia. No esperes más y ven a visitar este piso con nosotros. Valoramos tu casa Encuentra más en.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3795.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Antoni, Barcelona', 'title': 'Piso en Calle de Floridablanca'}, 'hasPlan': False, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AW2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99079881', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/9e/74/a7/1032868162.jpg', 'externalReference': 'VB2210011', 'numPhotos': 45, 'floor': 'bj', 'price': 890000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 137.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Fraternitat', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'Vila de Gràcia', 'latitude': 41.3991723, 'longitude': 2.158972, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99079881/', 'distance': '1581', 'description': 'Vivienda exclusiva con jardín en el corazón de Vila de Gràcia \xa0 En pleno corazón de la Vila de Gràcia, cerca de la plaza de la revolución y a cinco minutos caminando del metro Diagonal, encontramos esta vivienda exclusiva reformada en 2018 con todos los materiales de la mejor calidad. Este piso sorprende por sus detalles Arquitectónicos, Al entrar en la vivienda encontramos un recibidor con armarios y ventanas hacia el exterior y detrás de ello un sorprendente doble nivel donde la zona de abajo se convierte en una habitación totalmente cerrada y la parte de arriba puede ser un estudio o una sala de estar. A continuación, encontramos la cocina abierta y la sala de estar con mucha luz natural y vistas hacia el patio / jardín. con los techos altos en bóveda catalana toda la vivienda tiene una gran sensación de amplitud. Y después de la sala encontramos un pasillo con techos ventanas que dejan pasar totalmente la luz del día. Este pasillo puede quedar totalmente abierto en patio ya que la separación con el propio patio es con unos grandes ventanales tipo paneles japoneses y se pueden abrir totalmente para dejar un espacio muy grande donde se puede instalar mesa y sillas para hacer comidas en verano. En este mismo pasillo encontramos una pared entera de armarios para poder almacenar todo lo necesario en la vivienda. En la última parte a continuación del pasillo, encontramos en el antiguo lavadero una habitación doble en suite con su propio baño. Desde el patio interior podemos acceder a través de unas escaleras a un espacio extra, un jardín con vegetación y toldo, ideal para comidas y cenas y disfrutar de un espacio exterior despejado. La vivienda cuenta con una reforma de la mejor calidad, y ha conservado los detalles originales como las bóvedas catalanas, las paredes de piedras, y añadiendo materiales cálidos como los suelos de Madera. La finca tiene pasado la ITE y ha obtenido el certificado de aptitud. Disponemos de planos. No dudes en pedirnos visita en esta vivienda espectacular! \xa0 \xa0.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6496.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Vila de Gràcia, Barcelona', 'title': 'Piso en Calle de la Fraternitat'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': True, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99079881', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/9e/74/a7/1032868162.jpg', 'externalReference': 'VB2210011', 'numPhotos': 45, 'floor': 'bj', 'price': 890000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 137.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Fraternitat', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'Vila de Gràcia', 'latitude': 41.3991723, 'longitude': 2.158972, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99079881/', 'distance': '1581', 'description': 'Vivienda exclusiva con jardín en el corazón de Vila de Gràcia \xa0 En pleno corazón de la Vila de Gràcia, cerca de la plaza de la revolución y a cinco minutos caminando del metro Diagonal, encontramos esta vivienda exclusiva reformada en 2018 con todos los materiales de la mejor calidad. Este piso sorprende por sus detalles Arquitectónicos, Al entrar en la vivienda encontramos un recibidor con armarios y ventanas hacia el exterior y detrás de ello un sorprendente doble nivel donde la zona de abajo se convierte en una habitación totalmente cerrada y la parte de arriba puede ser un estudio o una sala de estar. A continuación, encontramos la cocina abierta y la sala de estar con mucha luz natural y vistas hacia el patio / jardín. con los techos altos en bóveda catalana toda la vivienda tiene una gran sensación de amplitud. Y después de la sala encontramos un pasillo con techos ventanas que dejan pasar totalmente la luz del día. Este pasillo puede quedar totalmente abierto en patio ya que la separación con el propio patio es con unos grandes ventanales tipo paneles japoneses y se pueden abrir totalmente para dejar un espacio muy grande donde se puede instalar mesa y sillas para hacer comidas en verano. En este mismo pasillo encontramos una pared entera de armarios para poder almacenar todo lo necesario en la vivienda. En la última parte a continuación del pasillo, encontramos en el antiguo lavadero una habitación doble en suite con su propio baño. Desde el patio interior podemos acceder a través de unas escaleras a un espacio extra, un jardín con vegetación y toldo, ideal para comidas y cenas y disfrutar de un espacio exterior despejado. La vivienda cuenta con una reforma de la mejor calidad, y ha conservado los detalles originales como las bóvedas catalanas, las paredes de piedras, y añadiendo materiales cálidos como los suelos de Madera. La finca tiene pasado la ITE y ha obtenido el certificado de aptitud. Disponemos de planos. No dudes en pedirnos visita en esta vivienda espectacular! \xa0 \xa0.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6496.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Vila de Gràcia, Barcelona', 'title': 'Piso en Calle de la Fraternitat'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': True, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AX2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99791140', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/de/1c/b1/1054580932.jpg', 'externalReference': 'BCN38000', 'numPhotos': 32, 'price': 575000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 103.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio La Salut', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'La Salut', 'latitude': 41.4073525, 'longitude': 2.1502985, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99791140/', 'distance': '2741', 'description': 'Propiedad en venta en perfecto estado impecable, con dos dormitorios dobles (uno en suite) y 2 baños con una bonita distribución abierta. Se han utilizado materiales de alta calidad con la renovación, lo que resultó en esta propiedad luminosa y lista para entrar. El estilo es contemporáneo y de buen gusto; el lienzo en blanco perfecto para que el nuevo propietario entre y lo complete con su propio toque personal.  El apartamento se encuentra en el sexto piso real del edificio y cuenta con una terraza soleada con espacio para comer al aire libre. También en el edificio existe la posibilidad de alquilar o comprar una plaza de aparcamiento; un detalle que se agradecerá mucho en un barrio donde escasea el aparcamiento.  La propiedad viene completamente equipada con aire acondicionado central por conductos, y la propiedad cuenta con pisos de madera real, una cocina totalmente equipada y muebles flexibles.  El edificio dispone de servicio de conserjería para mayor comodidad.  La ubicación es en Gracia, al lado del transporte público, restaurantes, etc. pero también cerca de parques para tener un entorno verde.  No dude en ponerse en contacto con nosotros para obtener más información o para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5583.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'La Salut, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99791140', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/de/1c/b1/1054580932.jpg', 'externalReference': 'BCN38000', 'numPhotos': 32, 'price': 575000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 103.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio La Salut', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'La Salut', 'latitude': 41.4073525, 'longitude': 2.1502985, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99791140/', 'distance': '2741', 'description': 'Propiedad en venta en perfecto estado impecable, con dos dormitorios dobles (uno en suite) y 2 baños con una bonita distribución abierta. Se han utilizado materiales de alta calidad con la renovación, lo que resultó en esta propiedad luminosa y lista para entrar. El estilo es contemporáneo y de buen gusto; el lienzo en blanco perfecto para que el nuevo propietario entre y lo complete con su propio toque personal.  El apartamento se encuentra en el sexto piso real del edificio y cuenta con una terraza soleada con espacio para comer al aire libre. También en el edificio existe la posibilidad de alquilar o comprar una plaza de aparcamiento; un detalle que se agradecerá mucho en un barrio donde escasea el aparcamiento.  La propiedad viene completamente equipada con aire acondicionado central por conductos, y la propiedad cuenta con pisos de madera real, una cocina totalmente equipada y muebles flexibles.  El edificio dispone de servicio de conserjería para mayor comodidad.  La ubicación es en Gracia, al lado del transporte público, restaurantes, etc. pero también cerca de parques para tener un entorno verde.  No dude en ponerse en contacto con nosotros para obtener más información o para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5583.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'La Salut, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AY2" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99766521', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/29/1b/91/1053990542.jpg', 'externalReference': 'BCN37642', 'numPhotos': 27, 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 80.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Raval', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3763632, 'longitude': 2.1674975, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99766521/', 'distance': '1249', 'description': 'Nos encontramos ante una obra nueva a partir de la rehabilitación de una antigua fábrica textil de los años 30. Se han mantenido muchos de sus elementos originales, y se han creado\xa0lofts modernos de estilo industrial y con mucha luz, grandes ventanales y zonas comunes como piscina, sala social, terrazas y jardines.  La propiedad en venta es un apartamento muy diáfano que consta de salón comedor cocina con acceso a una bonita terraza cubierta orientada a las zonas comunes del complejo. También tenemos una habitación doble con baño en suite, otro baño completo y una segunda habitación doble en un mezzanine construido gracias a la altura de los techos.  El apartamento está en perfecto estado y cuenta con vigas vistas de madera, cerramientos de aluminio de suelo a techo de grandes dimensiones, aire acondicionado, bomba de calor por splits, paredes de ladrillo visto y suelos de parquet, entre otros aspectos.  Se trata así de un pequeño oasis en el centro del casco antiguo de Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6063.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99766521', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/29/1b/91/1053990542.jpg', 'externalReference': 'BCN37642', 'numPhotos': 27, 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 80.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Raval', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3763632, 'longitude': 2.1674975, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99766521/', 'distance': '1249', 'description': 'Nos encontramos ante una obra nueva a partir de la rehabilitación de una antigua fábrica textil de los años 30. Se han mantenido muchos de sus elementos originales, y se han creado\xa0lofts modernos de estilo industrial y con mucha luz, grandes ventanales y zonas comunes como piscina, sala social, terrazas y jardines.  La propiedad en venta es un apartamento muy diáfano que consta de salón comedor cocina con acceso a una bonita terraza cubierta orientada a las zonas comunes del complejo. También tenemos una habitación doble con baño en suite, otro baño completo y una segunda habitación doble en un mezzanine construido gracias a la altura de los techos.  El apartamento está en perfecto estado y cuenta con vigas vistas de madera, cerramientos de aluminio de suelo a techo de grandes dimensiones, aire acondicionado, bomba de calor por splits, paredes de ladrillo visto y suelos de parquet, entre otros aspectos.  Se trata así de un pequeño oasis en el centro del casco antiguo de Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6063.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
     </row>
@@ -1356,252 +1356,252 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '87797664', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5d/ba/ea/1026649594.jpg', 'externalReference': 'BCN05285', 'numPhotos': 52, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 170.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3863885, 'longitude': 2.1622455, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/87797664/', 'distance': '636', 'description': 'Magnífica vivienda de obra nueva con terraza en Eixample Esquerra. Espectacular vivienda de obra nueva en finca modernista rehabilitada con ascensor, situada junto a la histórica Universidad de Barcelona. Se trata de una ubicación perfecta en pleno centro de la ciudad, con los mejores servicios y comunicaciones, a tan solo 3 calles de Plaza Catalunya y el Paseo de Gracia. El piso dispone de 130 m2 construidos interiores más 40 m2 de terraza, que le da un gran valor, un patio de 8 m2 y un balcón de 3 m2. La zona de día consta de salón-comedor con balcón hacia la calle, cocina independiente con electrodomésticos y galería con lavadero. La zona de noche se compone de dos habitaciones en suite con cuarto de baño propio: la principal tiene vestidor y acceso a la terraza, orientada hacia el patio de manzana inrterior; y la otra es interior y tiene acceso a un patio de 8 m2. Además, hay un aseo de cortesía. El edificio tiene además un terrado comunitario para disfrutar del aire libre. El piso goza de una reforma de alta calidad y diseño de la mano del prestigioso interiorista Jaime Beriestain. Está equipado con sistema hibrido de aerotermia de la casa Mintsubishi con integración de Hidrokit, fancoils por conductos y suelo radiante (controlado por domótica), suelos de piedra natural, armarios empotrados y cristales Climalit.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4988.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '87797664', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5d/ba/ea/1026649594.jpg', 'externalReference': 'BCN05285', 'numPhotos': 52, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 170.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3863885, 'longitude': 2.1622455, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/87797664/', 'distance': '636', 'description': 'Magnífica vivienda de obra nueva con terraza en Eixample Esquerra. Espectacular vivienda de obra nueva en finca modernista rehabilitada con ascensor, situada junto a la histórica Universidad de Barcelona. Se trata de una ubicación perfecta en pleno centro de la ciudad, con los mejores servicios y comunicaciones, a tan solo 3 calles de Plaza Catalunya y el Paseo de Gracia. El piso dispone de 130 m2 construidos interiores más 40 m2 de terraza, que le da un gran valor, un patio de 8 m2 y un balcón de 3 m2. La zona de día consta de salón-comedor con balcón hacia la calle, cocina independiente con electrodomésticos y galería con lavadero. La zona de noche se compone de dos habitaciones en suite con cuarto de baño propio: la principal tiene vestidor y acceso a la terraza, orientada hacia el patio de manzana inrterior; y la otra es interior y tiene acceso a un patio de 8 m2. Además, hay un aseo de cortesía. El edificio tiene además un terrado comunitario para disfrutar del aire libre. El piso goza de una reforma de alta calidad y diseño de la mano del prestigioso interiorista Jaime Beriestain. Está equipado con sistema hibrido de aerotermia de la casa Mintsubishi con integración de Hidrokit, fancoils por conductos y suelo radiante (controlado por domótica), suelos de piedra natural, armarios empotrados y cristales Climalit.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4988.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98351591', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/d2/66/bf/1009058214.jpg', 'externalReference': 'VB2207038', 'numPhotos': 29, 'floor': '3', 'price': 359000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 63.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Pi i Margall', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': "El Camp d'En Grassot i Gràcia Nova", 'latitude': 41.4096591, 'longitude': 2.1622433, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98351591/', 'distance': '2545', 'description': 'Piso reformado de dos habitaciones en venta en Gràcia Nova Fantástico piso reformado con dos habitaciones y balcón en Gràcia Nova En plena Gràcia Nova, a pocos metros del Mercat del Estrella, entre las paradas de metro Alfons X y Joanic, en uno de los futuros ejes verdes de la ciudad, encontramos este bonito apartamento totalmente reformado y a estrenar, listo para entrar a vivir. Luminosidad, buen gusto, distribución de espacios muy bien pensada y una reforma de calidad, es lo que describe mejor esta propiedad. la vivienda tiene una superficie de 60 m2 aprox que se distribuyen de forma muy lógica, al entrar en la vivienda encontramos el recibidor y el baño de cortesía, avanzamos en el pasillo y encontramos una primera habitación doble con baño completo en suite, avanzando un poco más llegamos a la habitación individual. Al final del pasillo se encuentra la amplia sala con cocina abierta totalmente equipada y con salida a un agradable balcón con vistas a un patio de manzana muy tranquilo y soleado por la tarde. La vivienda cuenta con aire acondicionado / calefacción por conductos, los suelos de parqué natural dan una calidez ideal a toda la vivienda. El edificio de los años 1963 cuenta con ascensor. ¡Sin duda, hablamos de una excelente oportunidad en la zona!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5698.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "El Camp d'En Grassot i Gràcia Nova, Barcelona", 'title': 'Piso en Calle de Pi i Margall'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98351591', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/d2/66/bf/1009058214.jpg', 'externalReference': 'VB2207038', 'numPhotos': 29, 'floor': '3', 'price': 359000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 63.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Pi i Margall', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': "El Camp d'En Grassot i Gràcia Nova", 'latitude': 41.4096591, 'longitude': 2.1622433, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98351591/', 'distance': '2545', 'description': 'Piso reformado de dos habitaciones en venta en Gràcia Nova Fantástico piso reformado con dos habitaciones y balcón en Gràcia Nova En plena Gràcia Nova, a pocos metros del Mercat del Estrella, entre las paradas de metro Alfons X y Joanic, en uno de los futuros ejes verdes de la ciudad, encontramos este bonito apartamento totalmente reformado y a estrenar, listo para entrar a vivir. Luminosidad, buen gusto, distribución de espacios muy bien pensada y una reforma de calidad, es lo que describe mejor esta propiedad. la vivienda tiene una superficie de 60 m2 aprox que se distribuyen de forma muy lógica, al entrar en la vivienda encontramos el recibidor y el baño de cortesía, avanzamos en el pasillo y encontramos una primera habitación doble con baño completo en suite, avanzando un poco más llegamos a la habitación individual. Al final del pasillo se encuentra la amplia sala con cocina abierta totalmente equipada y con salida a un agradable balcón con vistas a un patio de manzana muy tranquilo y soleado por la tarde. La vivienda cuenta con aire acondicionado / calefacción por conductos, los suelos de parqué natural dan una calidez ideal a toda la vivienda. El edificio de los años 1963 cuenta con ascensor. ¡Sin duda, hablamos de una excelente oportunidad en la zona!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5698.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "El Camp d'En Grassot i Gràcia Nova, Barcelona", 'title': 'Piso en Calle de Pi i Margall'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99349576', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b0/f6/f4/1041061889.jpg', 'externalReference': 'S-35432', 'numPhotos': 36, 'floor': '2', 'price': 229000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 68.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Ronda de Sant Pau', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'Sant Antoni', 'latitude': 41.375152, 'longitude': 2.1633305, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99349576/', 'distance': '1470', 'description': 'PLAÇA JOSEP MARIA FOLCH I TORRES Acogedora vivienda situada en uno de los barrios más emblemáticos de la ciudad condal junto a la Ronda Sant Pau y los Jardines de la Plaça Josep María Floch i Torres. Consta de 2 dormitorios (originalmente 3), luminoso comedor, baño con bañera y cocina con salida a lavadero. Toda la vivienda se encuentra en perfecto estado de conservación, con acabados de calidad. Suelo de mármol, puertas de madera noble, carpintería exterior de aluminio con persianas integradas y puerta de entrada de seguridad. Piso muy luminoso y tranquilo. Edificio de obra vista con ascensor.  En FINCAS Gp somos una empresa especializada en servicios inmobiliarios en la ciudad de Barcelona desde 1993. Los precios indicados no incluyen gastos e impuestos de escrituración ni de financiación. Venta y alquiler de apartamentos y locales comerciales. Encuentre más en nuestro sitio web.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3368.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Antoni, Barcelona', 'title': 'Piso en Ronda de Sant Pau'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '99349576', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b0/f6/f4/1041061889.jpg', 'externalReference': 'S-35432', 'numPhotos': 36, 'floor': '2', 'price': 229000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 68.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Ronda de Sant Pau', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'Sant Antoni', 'latitude': 41.375152, 'longitude': 2.1633305, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99349576/', 'distance': '1470', 'description': 'PLAÇA JOSEP MARIA FOLCH I TORRES Acogedora vivienda situada en uno de los barrios más emblemáticos de la ciudad condal junto a la Ronda Sant Pau y los Jardines de la Plaça Josep María Floch i Torres. Consta de 2 dormitorios (originalmente 3), luminoso comedor, baño con bañera y cocina con salida a lavadero. Toda la vivienda se encuentra en perfecto estado de conservación, con acabados de calidad. Suelo de mármol, puertas de madera noble, carpintería exterior de aluminio con persianas integradas y puerta de entrada de seguridad. Piso muy luminoso y tranquilo. Edificio de obra vista con ascensor.  En FINCAS Gp somos una empresa especializada en servicios inmobiliarios en la ciudad de Barcelona desde 1993. Los precios indicados no incluyen gastos e impuestos de escrituración ni de financiación. Venta y alquiler de apartamentos y locales comerciales. Encuentre más en nuestro sitio web.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3368.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Antoni, Barcelona', 'title': 'Piso en Ronda de Sant Pau'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98840562', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/0e/a9/0e/1025701609.jpg', 'externalReference': 'BCNP4881', 'numPhotos': 24, 'price': 1100000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 125.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio Sant Pere - Santa Caterina i la Ribera', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3832064, 'longitude': 2.1829743, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98840562/', 'distance': '1201', 'description': 'El impacto directo de este excepcional apartamento hace que se distinga de otros en el mercado desde el primer momento en que se cruza la puerta. Encontrará techos altos, cinco grandes y originales puertas balconeras de tres orientaciones que ofrecen una inmensa luz natural, y vistas a la terraza privada con un verde jardín vertical. La cocina abierta de alta gama y totalmente equipada en la zona de estar ha sido hecha a medida desde Italia y da una agradable elegancia al apartamento con sus colores oscuros. La carpintería ha sido igualmente hecha a medida desde Italia para el apartamento y equilibra bien un espacio de oficina abierto con el primer dormitorio en suite. También hay un cuarto de baño para invitados justo al lado del segundo dormitorio. El suelo es de parquet natural y el apartamento dispone de radiadores para la calefacción. Pero la joya de la propiedad es sin duda la terraza de 28 m2 que conecta con el salón y el segundo dormitorio. Ofrece un hermoso jardín vertical y el lujo de la tranquilidad en el corazón de El Born. Escondido en el jardín vertical hay un acceso a un trastero que también se utiliza como lavadero. La micro ubicación del apartamento es otro importante punto de venta de la propiedad, ya que está rodeado de algunas de las mejores plazas y restaurantes de la zona. Además, a pocos minutos a pie se encuentra también el Parque de la Ciutadella, el puerto Port-Vell y la playa de la Barceloneta. En definitiva, estamos hablando de una auténtica oportunidad en uno de los barrios más populares de Barcelona. Si hay un lugar de moda tanto para turistas como locales, es el dinámico barrio de El Born con su particular mercado, ahora convertido en museo, tras conseguir unas fantásticas ruinas romanas durante su remodelación. Es hogar de artistas, artesanos y bohemios, con infinidad de tiendas curiosas y únicas. Aún más famosos son sus \xa0variados restaurantes, tantos como para descubrir uno nuevo cada día. El mercado de Santa Caterina con su techo inspirado en la piel del dragón de Sant Jordi es por sí mismo una obra para admirar. La Basílica de Santa María del Mar, El Palau de la Música, y el pulmón verde de La Ciutadella son algunos de los referentes importantes de este barrio. Es un barrio para vivir y conocer. Sus edificios continúan el patrón irregular de El Barrio Gótico, y sus calles aunque por momentos más despejadas, también son angostas. En los bajos de los edificios puede encontrar bares de autor, galerías de arte, talleres de artesanos y un sinfín de pequeños y curiosos negocios. Este barrio le interesará si le gusta el estilo de vida bohemio, convivir con los\xa0 múltiples artesanos, el tapeo y buen comer, y vivir en un barrio que le sorprenda con tiendas y rincones nuevos. Es una buena ubicación para invertir en un pied-à-terre.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 8800.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98840562', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/0e/a9/0e/1025701609.jpg', 'externalReference': 'BCNP4881', 'numPhotos': 24, 'price': 1100000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 125.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio Sant Pere - Santa Caterina i la Ribera', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3832064, 'longitude': 2.1829743, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98840562/', 'distance': '1201', 'description': 'El impacto directo de este excepcional apartamento hace que se distinga de otros en el mercado desde el primer momento en que se cruza la puerta. Encontrará techos altos, cinco grandes y originales puertas balconeras de tres orientaciones que ofrecen una inmensa luz natural, y vistas a la terraza privada con un verde jardín vertical. La cocina abierta de alta gama y totalmente equipada en la zona de estar ha sido hecha a medida desde Italia y da una agradable elegancia al apartamento con sus colores oscuros. La carpintería ha sido igualmente hecha a medida desde Italia para el apartamento y equilibra bien un espacio de oficina abierto con el primer dormitorio en suite. También hay un cuarto de baño para invitados justo al lado del segundo dormitorio. El suelo es de parquet natural y el apartamento dispone de radiadores para la calefacción. Pero la joya de la propiedad es sin duda la terraza de 28 m2 que conecta con el salón y el segundo dormitorio. Ofrece un hermoso jardín vertical y el lujo de la tranquilidad en el corazón de El Born. Escondido en el jardín vertical hay un acceso a un trastero que también se utiliza como lavadero. La micro ubicación del apartamento es otro importante punto de venta de la propiedad, ya que está rodeado de algunas de las mejores plazas y restaurantes de la zona. Además, a pocos minutos a pie se encuentra también el Parque de la Ciutadella, el puerto Port-Vell y la playa de la Barceloneta. En definitiva, estamos hablando de una auténtica oportunidad en uno de los barrios más populares de Barcelona. Si hay un lugar de moda tanto para turistas como locales, es el dinámico barrio de El Born con su particular mercado, ahora convertido en museo, tras conseguir unas fantásticas ruinas romanas durante su remodelación. Es hogar de artistas, artesanos y bohemios, con infinidad de tiendas curiosas y únicas. Aún más famosos son sus \xa0variados restaurantes, tantos como para descubrir uno nuevo cada día. El mercado de Santa Caterina con su techo inspirado en la piel del dragón de Sant Jordi es por sí mismo una obra para admirar. La Basílica de Santa María del Mar, El Palau de la Música, y el pulmón verde de La Ciutadella son algunos de los referentes importantes de este barrio. Es un barrio para vivir y conocer. Sus edificios continúan el patrón irregular de El Barrio Gótico, y sus calles aunque por momentos más despejadas, también son angostas. En los bajos de los edificios puede encontrar bares de autor, galerías de arte, talleres de artesanos y un sinfín de pequeños y curiosos negocios. Este barrio le interesará si le gusta el estilo de vida bohemio, convivir con los\xa0 múltiples artesanos, el tapeo y buen comer, y vivir en un barrio que le sorprenda con tiendas y rincones nuevos. Es una buena ubicación para invertir en un pied-à-terre.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 8800.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98382386', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a8/9e/34/1022400721.jpg', 'externalReference': 'BCNP4798', 'numPhotos': 27, 'price': 690000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 85.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3905269, 'longitude': 2.1644133, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98382386/', 'distance': '559', 'description': 'Maravilloso piso en venta en el corazón del Ensanche Derecho de Barcelona, a la vuelta de la esquina de la elegante Rambla de Catalunya conocida por sus lujosos comercios y conocida aun más por sus restaurantes con terraza ideales para disfrutar del buen tiempo de la ciudad condal. El piso es una auténtica maravilla. Los acabados que se han utilizado en la reforma es de auténtico lujo, como por ejemplo los suelos de madera noble de roble americano, la cocina de muy buena calidad con vinoteca y nevera Liebherr, baños y grifería de diseño, radiadores de alta gamma, armarios empotrados realizados a medida, panelados de madera en las paredes y papel decorativo de alta calidad, además de un sistema de filtro osmosis para mejorar el agua de toda la vivienda. El piso no solo dispone de maravillosos acabados, sino que además dispone de características arquitectónicas de la época, como los techos altos y artesonados, la chimenea original y marcos decorativos. El piso consta de un agradable salón comedor con salida a una terraza muy disfrutable de aproximadamente unos 8m2 orientada hacia el sudeste, una cocina totalmente equipada, un lavadero muy práctico, un dormitorio doble “en suite” también con salida a la terraza, y otro dormitorio individual con su propio baño. La finca es también un espectáculo, ya que se trata de un edificio regio del 1900, completamente reformada y actualizada con acceso directo al ascensor y además un excelente servicio de conserjería. En resumen una propiedad para gozar desde el primer instante que reúne todo lo que se buscaría en la mejor zona de Barcelona. La Dreta de L’Eixample se inicia en Plaça de Catalunya y su eje central gira en torno al Passeig de Gràcia y el Cuadrat d’Or. Se delimita desde la transitada Calle Balmes hasta el renovado Passeig de Sant Joan y desde la comercial Ronda Sant Pere hasta la conveniente Avinguda Diagonal. Es uno de los barrios, junto con Pedralbes y Sarrià-Sant Gervasi, más caros y exclusivos de Barcelona ciudad. Es imposible no hacer referencia al lujo del Paseo de Gràcia, con las boutiques de las marcas más exclusivas del mundo, o a los comercios de La Rambla de Catalunya. Sin embargo, el resto de sus calles son tanto o más interesantes. En ellas residía parte de la burguesía textilera catalana de principios del siglo XX, la cual ha dejado huella en las espectaculares fincas regias y casas modernistas diseñadas por los arquitectos más famosos de la época, como la Pedrera o la Casa Batlló del gran Antoni Gaudí. En consecuencia, las viviendas características de este barrio son apartamentos amplios, de techos elevados, molduras, elaborados pavimentos y balcones. Muchos edificios y pisos conservan esta herencia arquitectónica original artesanal y es posible encontrar apartamentos remodelados recientemente, áticos, lofts e incluso estudios, que reviven estos elementos, así como pisos con mucho potencial para ser reformados. Este lado de L’Eixample está dotado de todo tipo de servicios y comercios, centros educativos -principalmente escuelas concertadas y privadas-. Le resultará muy fácil moverse andando o desplazarse a través de las conexiones de transporte público hasta las tiendas y restaurantes más caros y en vogue de la ciudad. Este es el mejor barrio si quiere admirar y vivir en la zona noble del fascinante modernismo catalán, residir en una de sus características fincas regias, y convivir en perfecto equilibrio con la vibrante y lujosa vida comercial. Es ideal si desea caminar cada día por sus calles anchas y ordenadas, con fáciles conexiones de transporte, disponer de todo tipo de servicios y equipamientos incluidas escuelas concertadas o privadas, y disfrutar del ambiente más chic, cultural y cosmopolita de Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8118.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98382386', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a8/9e/34/1022400721.jpg', 'externalReference': 'BCNP4798', 'numPhotos': 27, 'price': 690000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 85.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3905269, 'longitude': 2.1644133, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98382386/', 'distance': '559', 'description': 'Maravilloso piso en venta en el corazón del Ensanche Derecho de Barcelona, a la vuelta de la esquina de la elegante Rambla de Catalunya conocida por sus lujosos comercios y conocida aun más por sus restaurantes con terraza ideales para disfrutar del buen tiempo de la ciudad condal. El piso es una auténtica maravilla. Los acabados que se han utilizado en la reforma es de auténtico lujo, como por ejemplo los suelos de madera noble de roble americano, la cocina de muy buena calidad con vinoteca y nevera Liebherr, baños y grifería de diseño, radiadores de alta gamma, armarios empotrados realizados a medida, panelados de madera en las paredes y papel decorativo de alta calidad, además de un sistema de filtro osmosis para mejorar el agua de toda la vivienda. El piso no solo dispone de maravillosos acabados, sino que además dispone de características arquitectónicas de la época, como los techos altos y artesonados, la chimenea original y marcos decorativos. El piso consta de un agradable salón comedor con salida a una terraza muy disfrutable de aproximadamente unos 8m2 orientada hacia el sudeste, una cocina totalmente equipada, un lavadero muy práctico, un dormitorio doble “en suite” también con salida a la terraza, y otro dormitorio individual con su propio baño. La finca es también un espectáculo, ya que se trata de un edificio regio del 1900, completamente reformada y actualizada con acceso directo al ascensor y además un excelente servicio de conserjería. En resumen una propiedad para gozar desde el primer instante que reúne todo lo que se buscaría en la mejor zona de Barcelona. La Dreta de L’Eixample se inicia en Plaça de Catalunya y su eje central gira en torno al Passeig de Gràcia y el Cuadrat d’Or. Se delimita desde la transitada Calle Balmes hasta el renovado Passeig de Sant Joan y desde la comercial Ronda Sant Pere hasta la conveniente Avinguda Diagonal. Es uno de los barrios, junto con Pedralbes y Sarrià-Sant Gervasi, más caros y exclusivos de Barcelona ciudad. Es imposible no hacer referencia al lujo del Paseo de Gràcia, con las boutiques de las marcas más exclusivas del mundo, o a los comercios de La Rambla de Catalunya. Sin embargo, el resto de sus calles son tanto o más interesantes. En ellas residía parte de la burguesía textilera catalana de principios del siglo XX, la cual ha dejado huella en las espectaculares fincas regias y casas modernistas diseñadas por los arquitectos más famosos de la época, como la Pedrera o la Casa Batlló del gran Antoni Gaudí. En consecuencia, las viviendas características de este barrio son apartamentos amplios, de techos elevados, molduras, elaborados pavimentos y balcones. Muchos edificios y pisos conservan esta herencia arquitectónica original artesanal y es posible encontrar apartamentos remodelados recientemente, áticos, lofts e incluso estudios, que reviven estos elementos, así como pisos con mucho potencial para ser reformados. Este lado de L’Eixample está dotado de todo tipo de servicios y comercios, centros educativos -principalmente escuelas concertadas y privadas-. Le resultará muy fácil moverse andando o desplazarse a través de las conexiones de transporte público hasta las tiendas y restaurantes más caros y en vogue de la ciudad. Este es el mejor barrio si quiere admirar y vivir en la zona noble del fascinante modernismo catalán, residir en una de sus características fincas regias, y convivir en perfecto equilibrio con la vibrante y lujosa vida comercial. Es ideal si desea caminar cada día por sus calles anchas y ordenadas, con fáciles conexiones de transporte, disponer de todo tipo de servicios y equipamientos incluidas escuelas concertadas o privadas, y disfrutar del ambiente más chic, cultural y cosmopolita de Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8118.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98378398', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/af/08/1c/1027086647.jpg', 'externalReference': '3000', 'numPhotos': 22, 'floor': '2', 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 90.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Petritxol', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3822216, 'longitude': 2.1741355, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98378398/', 'distance': '689', 'description': 'Fabulosa propiedad situada en el corazón del Barrio Gótico, en la emblemática Calle Petritxol, a escasos metros de la Plaza del Pi y Las Ramblas. Se trata de un elegante piso exterior de 90 m2 ubicada en una finca regia del año 1780.    La propiedad ha sido completamente renovada manteniendo y respetando elementos originales como las vigas de madera de los techos y los suelos de mosaico originales combinados con parquet de madera y hormigón pulido en la cocina y baños.     El resultado es un hogar elegante, moderno y acogedor. El edificio, que cuenta con un ascensor recientemente instalado, data de 1780. Ha pasado la ITE (inspección técnica del edificio) y ha sido rehabilitado recientemente.    Cocina abierta con electrodomésticos de alta calidad, integrados junto al salón comedor muy agradable que disfruta de dos grandes balcones orientados a la calle Petritxol.    Es un piso ideal tanto para vivir como para invertir, ya que alquilado, tiene una alta rentabilidad.  El piso, gracias a su rehabilitación integral de todo el edificio, combina las ventajas de una construcción nueva con elementos originales, lo que sin duda hacen de está vivienda una pieza única.    Una gran oportunidad de adquirir una vivienda única con amplias estancias y mucha luz en una de las zonas más demandadas del barrio Gótico.    La zona disfruta de todos los servicios, colegios, mercados como La Boquería o Santa Catalina, comercios y locales de ocio. La zona también está muy bien comunicada por transporte público, cercana a las líneas de metro L1 y L3, y líneas de autobús que atraviesan la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5389.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso en Calle de Petritxol'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98378398', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/af/08/1c/1027086647.jpg', 'externalReference': '3000', 'numPhotos': 22, 'floor': '2', 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 90.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Petritxol', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3822216, 'longitude': 2.1741355, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98378398/', 'distance': '689', 'description': 'Fabulosa propiedad situada en el corazón del Barrio Gótico, en la emblemática Calle Petritxol, a escasos metros de la Plaza del Pi y Las Ramblas. Se trata de un elegante piso exterior de 90 m2 ubicada en una finca regia del año 1780.    La propiedad ha sido completamente renovada manteniendo y respetando elementos originales como las vigas de madera de los techos y los suelos de mosaico originales combinados con parquet de madera y hormigón pulido en la cocina y baños.     El resultado es un hogar elegante, moderno y acogedor. El edificio, que cuenta con un ascensor recientemente instalado, data de 1780. Ha pasado la ITE (inspección técnica del edificio) y ha sido rehabilitado recientemente.    Cocina abierta con electrodomésticos de alta calidad, integrados junto al salón comedor muy agradable que disfruta de dos grandes balcones orientados a la calle Petritxol.    Es un piso ideal tanto para vivir como para invertir, ya que alquilado, tiene una alta rentabilidad.  El piso, gracias a su rehabilitación integral de todo el edificio, combina las ventajas de una construcción nueva con elementos originales, lo que sin duda hacen de está vivienda una pieza única.    Una gran oportunidad de adquirir una vivienda única con amplias estancias y mucha luz en una de las zonas más demandadas del barrio Gótico.    La zona disfruta de todos los servicios, colegios, mercados como La Boquería o Santa Catalina, comercios y locales de ocio. La zona también está muy bien comunicada por transporte público, cercana a las líneas de metro L1 y L3, y líneas de autobús que atraviesan la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5389.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso en Calle de Petritxol'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98264311', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b9/b6/8a/1006013108.jpg', 'externalReference': '3855V_6', 'numPhotos': 46, 'floor': '6', 'price': 2650000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 195.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3919731, 'longitude': 2.1693451, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98264311/', 'distance': '501', 'description': 'Este espectacular y exclusivo ático de 101m2 construidos y 94m2 de terraza viene distribuido en un amplio y luminoso salón comedor con salida a la magnifíca terraza con doble altura. El suelo es de madera flotante que proporciona una sensación de relajación gracias a sus zonas ajardinadas. Con posbilidades de amueblar con una zona chill out o un agradable comedor exterior donde disfrutar las tardes de verano. Las increíbles vistas que proporciona no te dejarán indiferente.  La cocina es abierta al comedor con isleta y barra de desayuno. Viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr) y tiene acceso a la zona de aguas independiente. La zona de noche consta de un dormitorio máster suite con salida a un amplio balcón, un vestidor y un baño con bañera ovalada y plato de ducha.  El segundo dormitorio también en suite y con salida al balcón. Ambos dormitorios cuentan con armarios empotrados. Todas las estancias disponen de aire acondicionado y calefacción por conductos, domótica, suelos de parqué, carpintería de aluminio y cristales dobles. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 13590.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Ático en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98264311', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b9/b6/8a/1006013108.jpg', 'externalReference': '3855V_6', 'numPhotos': 46, 'floor': '6', 'price': 2650000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 195.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3919731, 'longitude': 2.1693451, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98264311/', 'distance': '501', 'description': 'Este espectacular y exclusivo ático de 101m2 construidos y 94m2 de terraza viene distribuido en un amplio y luminoso salón comedor con salida a la magnifíca terraza con doble altura. El suelo es de madera flotante que proporciona una sensación de relajación gracias a sus zonas ajardinadas. Con posbilidades de amueblar con una zona chill out o un agradable comedor exterior donde disfrutar las tardes de verano. Las increíbles vistas que proporciona no te dejarán indiferente.  La cocina es abierta al comedor con isleta y barra de desayuno. Viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr) y tiene acceso a la zona de aguas independiente. La zona de noche consta de un dormitorio máster suite con salida a un amplio balcón, un vestidor y un baño con bañera ovalada y plato de ducha.  El segundo dormitorio también en suite y con salida al balcón. Ambos dormitorios cuentan con armarios empotrados. Todas las estancias disponen de aire acondicionado y calefacción por conductos, domótica, suelos de parqué, carpintería de aluminio y cristales dobles. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 13590.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Ático en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98261311', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f2/8a/bd/1005921523.jpg', 'externalReference': '3855V_3', 'numPhotos': 42, 'floor': '1', 'price': 1925000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 168.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3890208, 'longitude': 2.1642732, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98261311/', 'distance': '487', 'description': 'Exclusiva vivienda de 143m2 construidos y 23m2 de terraza, distribuidos en un luminoso salón comedor con salida a dos agradables balcones. La cocina es abierta y viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr). A través del distribuidor accedemos a la zona de noche, donde encontraremos la habitación master suite con salida a la espectacular terraza, este dormitorio dispone de un amplio vestidor y un baño completo con plato de ducha. La segunda habitación también es doble y tiene justo en frente un baño completo con bañera. Ambas habitaciones tienen armarios empotrados y vienen diseñadas con materiales de alta calidad. Todas las estancias disponen de aire acondicionado y calefacción por conductos, domótica, suelos de parqué, carpintería de aluminio y cristales dobles. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Ubicada en el corazón de Barcelona, Paseo de Gracia es la avenida más elegante y señorial de la ciudad, y en una de las ubicaciones más buscadas para los negocios. Una propuesta comercial muy atractiva. Ofrece una vida muy cómoda, con todos los servicios al alcance de su mano. Vivir en esta avenida significa disfrutar de exclusividad en el mismo centro de la ciudad. Disfruta de la exquisita arquitectura de sus edificios modernistas como son la Casa Batlló, la Casa Milá o la Casa Lleó Morera, mezclados con edificios del estilo moderno, clásico y neoclásico.  Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 11458.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98261311', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f2/8a/bd/1005921523.jpg', 'externalReference': '3855V_3', 'numPhotos': 42, 'floor': '1', 'price': 1925000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 168.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3890208, 'longitude': 2.1642732, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98261311/', 'distance': '487', 'description': 'Exclusiva vivienda de 143m2 construidos y 23m2 de terraza, distribuidos en un luminoso salón comedor con salida a dos agradables balcones. La cocina es abierta y viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr). A través del distribuidor accedemos a la zona de noche, donde encontraremos la habitación master suite con salida a la espectacular terraza, este dormitorio dispone de un amplio vestidor y un baño completo con plato de ducha. La segunda habitación también es doble y tiene justo en frente un baño completo con bañera. Ambas habitaciones tienen armarios empotrados y vienen diseñadas con materiales de alta calidad. Todas las estancias disponen de aire acondicionado y calefacción por conductos, domótica, suelos de parqué, carpintería de aluminio y cristales dobles. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Ubicada en el corazón de Barcelona, Paseo de Gracia es la avenida más elegante y señorial de la ciudad, y en una de las ubicaciones más buscadas para los negocios. Una propuesta comercial muy atractiva. Ofrece una vida muy cómoda, con todos los servicios al alcance de su mano. Vivir en esta avenida significa disfrutar de exclusividad en el mismo centro de la ciudad. Disfruta de la exquisita arquitectura de sus edificios modernistas como son la Casa Batlló, la Casa Milá o la Casa Lleó Morera, mezclados con edificios del estilo moderno, clásico y neoclásico.  Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 11458.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98256266', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f3/cf/34/1005719750.jpg', 'externalReference': '3855V_2', 'numPhotos': 43, 'floor': '5', 'price': 2680000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 157.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3924731, 'longitude': 2.1675451, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98256266/', 'distance': '585', 'description': 'Piso a estrenar con Piscina en Paseo de Gracia, Barcelona Exclusiva vivienda de 157m2 construidos, distribuidos en un amplio salón comedor. La cocina es abierta con isleta y barra de desayuno y viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr). La zona de noche dispone de 2 habitaciones; una doble y otra doble en suite con bañera ovalada y plato de ducha. Ambas disponen de armarios empotrado. Otro baño completo con plato de ducha por donde se accede al lavadero. En el recibidor encontramos un cómodo baño de cortesía y un armario empotrado. Todas las estancias disponen de suelo radiante, aire acondicionado y calefacción, domótica, suelos de roble, carpintería de madera y doble acristalamiento. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Ubicada en el corazón de Barcelona, Paseo de Gracia es la avenida más elegante y señorial de la ciudad, y en una de las ubicaciones más buscadas para los negocios. Una propuesta comercial muy atractiva. Ofrece una vida muy cómoda, con todos los servicios al alcance de su mano. Vivir en esta avenida significa disfrutar de exclusividad en el mismo centro de la ciudad. Disfruta de la exquisita arquitectura de sus edificios modernistas como son la Casa Batlló, la Casa Milá o la Casa Lleó Morera, mezclados con edificios del estilo moderno, clásico y neoclásico.  Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas. En total, la finca presenta 21 viviendas únicas, una azotea con piscina y zona chill out, un patio vegetal interior, mirador y zonas comunes. Distribuidos en 5 plantas más ático, viviendas de 1, 2 o 4 dormitorios, algunos con balcón y otros con agradables terrazas. El exclusivo ático, de un dormitorio y salida a una impresionante terraza con vistas inmejorables, el mejor producto para nuestros clientes más exigentes.  Cada tipología de vivienda tiene su personalidad, diferente distribución y distintas superficies, todas construidas con materiales de alta calidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 17070.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98256266', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f3/cf/34/1005719750.jpg', 'externalReference': '3855V_2', 'numPhotos': 43, 'floor': '5', 'price': 2680000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 157.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3924731, 'longitude': 2.1675451, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98256266/', 'distance': '585', 'description': 'Piso a estrenar con Piscina en Paseo de Gracia, Barcelona Exclusiva vivienda de 157m2 construidos, distribuidos en un amplio salón comedor. La cocina es abierta con isleta y barra de desayuno y viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr). La zona de noche dispone de 2 habitaciones; una doble y otra doble en suite con bañera ovalada y plato de ducha. Ambas disponen de armarios empotrado. Otro baño completo con plato de ducha por donde se accede al lavadero. En el recibidor encontramos un cómodo baño de cortesía y un armario empotrado. Todas las estancias disponen de suelo radiante, aire acondicionado y calefacción, domótica, suelos de roble, carpintería de madera y doble acristalamiento. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Ubicada en el corazón de Barcelona, Paseo de Gracia es la avenida más elegante y señorial de la ciudad, y en una de las ubicaciones más buscadas para los negocios. Una propuesta comercial muy atractiva. Ofrece una vida muy cómoda, con todos los servicios al alcance de su mano. Vivir en esta avenida significa disfrutar de exclusividad en el mismo centro de la ciudad. Disfruta de la exquisita arquitectura de sus edificios modernistas como son la Casa Batlló, la Casa Milá o la Casa Lleó Morera, mezclados con edificios del estilo moderno, clásico y neoclásico.  Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas. En total, la finca presenta 21 viviendas únicas, una azotea con piscina y zona chill out, un patio vegetal interior, mirador y zonas comunes. Distribuidos en 5 plantas más ático, viviendas de 1, 2 o 4 dormitorios, algunos con balcón y otros con agradables terrazas. El exclusivo ático, de un dormitorio y salida a una impresionante terraza con vistas inmejorables, el mejor producto para nuestros clientes más exigentes.  Cada tipología de vivienda tiene su personalidad, diferente distribución y distintas superficies, todas construidas con materiales de alta calidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 17070.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98000858', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8b/d9/71/997711176.jpg', 'externalReference': '3835V', 'numPhotos': 36, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 114.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3902528, 'longitude': 2.1608339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98000858/', 'distance': '804', 'description': 'Espectacular y exclusiva vivienda de 114m2, distribuida en un amplio recibidor con paredes de ladrillo visto que conducen a una luminosa habitación doble con armarios empotrados y acceso a una pequeña salida exterior. Un baño completo con plato de ducha. La cocina es abierta y viene completamente equipada con electrodomésticos y placas de inducción. El suelo es hidráulico. Dispone de zona de aguas independiente. Un amplio y luminoso comedor con dos grandes ventanales y vistas al patio del Eixample. El dormitorio principal con baño en suite; con plato de ducha, bañera de hidromasaje y suelos de microcemento. Orientado al exterior y también con armarios empotrados. El piso incluye sistema de ósmosis en la cocina, aire acodicionado, calefacción, suelos de parqué y persianas eléctricas. Ubicado en Rambla Catalunya, una de las calles más exclusivas de la ciudad, en una 5º planta de una magnífica finca regia con servicio de consejería y ascensir. La vivienda goza de mucha tranquilidad a pesar de su ubicación tan céntrica. Con VISITA SEGURA de Walter Haus podrás seguir alquilando y vendiendo tu piso con total seguridad. Nuestras viviendas y las visitas que realizamos están libres de Covid-19 gracias al protocolo que hemos desarrollado: •Visitas Virtuales •Desinfección con ozono •Kit de seguridad •Firma digital Todo para que puedas seguir alquilando y vendiendo tu piso con total normalidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 7719.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98000858', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8b/d9/71/997711176.jpg', 'externalReference': '3835V', 'numPhotos': 36, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 114.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3902528, 'longitude': 2.1608339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98000858/', 'distance': '804', 'description': 'Espectacular y exclusiva vivienda de 114m2, distribuida en un amplio recibidor con paredes de ladrillo visto que conducen a una luminosa habitación doble con armarios empotrados y acceso a una pequeña salida exterior. Un baño completo con plato de ducha. La cocina es abierta y viene completamente equipada con electrodomésticos y placas de inducción. El suelo es hidráulico. Dispone de zona de aguas independiente. Un amplio y luminoso comedor con dos grandes ventanales y vistas al patio del Eixample. El dormitorio principal con baño en suite; con plato de ducha, bañera de hidromasaje y suelos de microcemento. Orientado al exterior y también con armarios empotrados. El piso incluye sistema de ósmosis en la cocina, aire acodicionado, calefacción, suelos de parqué y persianas eléctricas. Ubicado en Rambla Catalunya, una de las calles más exclusivas de la ciudad, en una 5º planta de una magnífica finca regia con servicio de consejería y ascensir. La vivienda goza de mucha tranquilidad a pesar de su ubicación tan céntrica. Con VISITA SEGURA de Walter Haus podrás seguir alquilando y vendiendo tu piso con total seguridad. Nuestras viviendas y las visitas que realizamos están libres de Covid-19 gracias al protocolo que hemos desarrollado: •Visitas Virtuales •Desinfección con ozono •Kit de seguridad •Firma digital Todo para que puedas seguir alquilando y vendiendo tu piso con total normalidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 7719.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98676867', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5d/9f/10/1052038319.jpg', 'externalReference': 'KB1508', 'numPhotos': 25, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 132.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3904528, 'longitude': 2.1637339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98676867/', 'distance': '600', 'description': 'Excelente propiedad en la quinta planta de un edificio histórico de Rambla Catalunya, una de las mejores calles de Barcelona. En una de las zonas más lujosas nos encontramos con esta exclusiva propiedad que ofrece todas las comodidades de un moderno apartamento en un entorno único y con uno acabados interiores excelentes. Exterior a patio de manzana, dispone de grandes ventanales que inundan de luz sus estancias. Su entrada está perfectamente trabajada y nos ofrece calidez mediante sus preciosos ventanales y sus paredes originales. La moderna cocina, abierta al salón conjuga un precioso diseño con una excelente funcionalidad y su ubicación facilita mucho la accesibilidad al salón. El suelo es de madera natural. Una de las habitaciones con armarios empotrados, tiene salida a una terraza y goza de mucha luminosidad. Encontramos un baño completo con ducha y baldosas hidráulicas. La habitación principal es suite con armarios empotrados y dispone también de un enorme y luminoso baño con bañera de hidromasaje con cascada y amplia ducha. La habitación tiene amplios ventanales también que le dan luz y vistas despejadas.  El inmueble ha sido recientemente renovado con acabados de máxima calidad e insonorizado en su totalidad, dispone de persianas eléctricas, aire acondicionado por conductos y calefacción por gas natural. El edificio dispone de conserje a jornada completa y ascensor. La ubicación es excelente, cerca del transporte público, en el cuadrado de oro de Barcelona, en una de las mejores calles y a escasos pasos de Passeig de gràcia o Plaza Catalunya. Un pedazo de la historia de Barcelona en una de las mejore ubicaciones de la ciudad. Estaremos encantados de poder mostrarselo.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6667.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98676867', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5d/9f/10/1052038319.jpg', 'externalReference': 'KB1508', 'numPhotos': 25, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 132.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3904528, 'longitude': 2.1637339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98676867/', 'distance': '600', 'description': 'Excelente propiedad en la quinta planta de un edificio histórico de Rambla Catalunya, una de las mejores calles de Barcelona. En una de las zonas más lujosas nos encontramos con esta exclusiva propiedad que ofrece todas las comodidades de un moderno apartamento en un entorno único y con uno acabados interiores excelentes. Exterior a patio de manzana, dispone de grandes ventanales que inundan de luz sus estancias. Su entrada está perfectamente trabajada y nos ofrece calidez mediante sus preciosos ventanales y sus paredes originales. La moderna cocina, abierta al salón conjuga un precioso diseño con una excelente funcionalidad y su ubicación facilita mucho la accesibilidad al salón. El suelo es de madera natural. Una de las habitaciones con armarios empotrados, tiene salida a una terraza y goza de mucha luminosidad. Encontramos un baño completo con ducha y baldosas hidráulicas. La habitación principal es suite con armarios empotrados y dispone también de un enorme y luminoso baño con bañera de hidromasaje con cascada y amplia ducha. La habitación tiene amplios ventanales también que le dan luz y vistas despejadas.  El inmueble ha sido recientemente renovado con acabados de máxima calidad e insonorizado en su totalidad, dispone de persianas eléctricas, aire acondicionado por conductos y calefacción por gas natural. El edificio dispone de conserje a jornada completa y ascensor. La ubicación es excelente, cerca del transporte público, en el cuadrado de oro de Barcelona, en una de las mejores calles y a escasos pasos de Passeig de gràcia o Plaza Catalunya. Un pedazo de la historia de Barcelona en una de las mejore ubicaciones de la ciudad. Estaremos encantados de poder mostrarselo.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6667.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99119853', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/fd/90/38/1034166911.jpg', 'externalReference': 'PBARDE 39', 'numPhotos': 51, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 170.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3873408, 'longitude': 2.1621522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99119853/', 'distance': '633', 'description': 'Terraza soleada de 40 metros orientada al mar, en una propiedad de obra nueva que da a las 2 fachadas, con acabados de altísima calidad, suelos radiantes, hidrotermia, domótica, reguladores de la intensidad de la luz, y todo el glamour que caracteriza a este barrio del Eixample de Barcelona.  La vivienda está ubicada a 100 metros de Plaza Universidad, en una finca completamente rehabilitada con ascensor.  A la entrada a la izquierda encontramos una elegante y moderna cocina abierta al salón comedor, con salida a un balcón que discurre por la calle Diputació. En esta zona también se halla un aseo de cortesía, el equipo de hidrotermia y el dispositivo táctil para la domótica de la casa.  En la parte posterior del piso se encuentran las dos habitaciones dobles, ambas con baños completos en suite, armarios con iluminación led interior, y mucha luz y sol.  A continuación del dormitorio principal encontramos la joya de la corona, su gran terraza. De la misma solo podemos añadir que, si a la funcionalidad y elegancia de unas magníficas reformas de alto standing, sumamos el hecho de tener este espacio exterior con sol todo el año, en el barrio seguramente con más Flow de Barcelona, podemos considerar que nos encontramos ante una vivienda única, difícilmente superable. Cabe señalar que es un piso con amplias estancias, se trata de 130 metros construidos para tres ambientes principales, salón y dos habitaciones dobles, con lo cual nos ofrece mucha versatilidad: salón comedor en la zona de los balcones que dan a la calle, como está distribuido ahora, o salón comedor hacia la terraza. Como hablamos de un solo piso por rellano, las dimensiones de la estancia trasera y la delantera son idénticas, o sea, que sin demasiado cambio se podría distribuir según nuestras preferencias. El barrio y esa calle en concreto se caracteriza por su encanto, con bares de moda, estilo, buen rollo y ese encanto urbanita de sus comercios y tiendas siempre a la vanguardia. Casi en los bajos del edificio encontramos una estación de Bicing, por si somos de los que prefieren moverse de esta forma por la ciudad.  Le invitamos a visitar este magnífico inmueble con QUATRECASES, y disfrutar de la experiencia.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4988.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '99119853', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/fd/90/38/1034166911.jpg', 'externalReference': 'PBARDE 39', 'numPhotos': 51, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 170.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3873408, 'longitude': 2.1621522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99119853/', 'distance': '633', 'description': 'Terraza soleada de 40 metros orientada al mar, en una propiedad de obra nueva que da a las 2 fachadas, con acabados de altísima calidad, suelos radiantes, hidrotermia, domótica, reguladores de la intensidad de la luz, y todo el glamour que caracteriza a este barrio del Eixample de Barcelona.  La vivienda está ubicada a 100 metros de Plaza Universidad, en una finca completamente rehabilitada con ascensor.  A la entrada a la izquierda encontramos una elegante y moderna cocina abierta al salón comedor, con salida a un balcón que discurre por la calle Diputació. En esta zona también se halla un aseo de cortesía, el equipo de hidrotermia y el dispositivo táctil para la domótica de la casa.  En la parte posterior del piso se encuentran las dos habitaciones dobles, ambas con baños completos en suite, armarios con iluminación led interior, y mucha luz y sol.  A continuación del dormitorio principal encontramos la joya de la corona, su gran terraza. De la misma solo podemos añadir que, si a la funcionalidad y elegancia de unas magníficas reformas de alto standing, sumamos el hecho de tener este espacio exterior con sol todo el año, en el barrio seguramente con más Flow de Barcelona, podemos considerar que nos encontramos ante una vivienda única, difícilmente superable. Cabe señalar que es un piso con amplias estancias, se trata de 130 metros construidos para tres ambientes principales, salón y dos habitaciones dobles, con lo cual nos ofrece mucha versatilidad: salón comedor en la zona de los balcones que dan a la calle, como está distribuido ahora, o salón comedor hacia la terraza. Como hablamos de un solo piso por rellano, las dimensiones de la estancia trasera y la delantera son idénticas, o sea, que sin demasiado cambio se podría distribuir según nuestras preferencias. El barrio y esa calle en concreto se caracteriza por su encanto, con bares de moda, estilo, buen rollo y ese encanto urbanita de sus comercios y tiendas siempre a la vanguardia. Casi en los bajos del edificio encontramos una estación de Bicing, por si somos de los que prefieren moverse de esta forma por la ciudad.  Le invitamos a visitar este magnífico inmueble con QUATRECASES, y disfrutar de la experiencia.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4988.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98192535', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/eb/3a/00/1003587995.jpg', 'externalReference': 'W-02I8M0', 'numPhotos': 31, 'floor': '5', 'price': 1619000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 207.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle del Tenor Viñas', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sarrià-Sant Gervasi', 'country': 'es', 'neighborhood': 'Sant Gervasi - Galvany', 'latitude': 41.3937255, 'longitude': 2.1418776, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98192535/', 'distance': '2426', 'description': 'Espectacular ático con terraza en Turó Parc En una de las mejores fincas de la zona se sitúa este ático con una espectacular terraza de 135 metros. Se trata de un piso de 142 metros cuadrados, reformado, en el que antiguamente tenía 4 dormitorios, y ahora con la reforma tiene 2 grandes suites. El piso tiene un bonito recibidor que nos conduce a la zona de día, una bonita cocina con una zona de lavadero y al esplendido salón comedor con chimenea de mármol y salida directa a la terraza. En el pasillo encontramos un aseo de cortesía y la zona de noche con las 2 magníficas suites también con acceso a la terraza. La terraza tiene forma de L pudiendo crear en ella diferentes ambientes.  Se trata de una finca de lujo, con servicio de portería, 2 ascensores y posibilidad de alquilar parking en la misma finca. El Turó Parc es una de las zonas más demandadas de la ciudad. La elegancia y el prestigio son las características que definen tanto sus edificios como sus habitantes. Se trata de una zona muy segura, con todo tipo de comercios, servicios y ocio. El Turó Parc es la esencia del espíritu más sofisticado de Barcelona, sin perder al mismo tiempo la dimensión más pura y la calidez del barrio.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 7821.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': 'Sant Gervasi - Galvany, Barcelona', 'title': 'Ático en Calle del Tenor Viñas'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98192535', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/eb/3a/00/1003587995.jpg', 'externalReference': 'W-02I8M0', 'numPhotos': 31, 'floor': '5', 'price': 1619000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 207.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle del Tenor Viñas', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sarrià-Sant Gervasi', 'country': 'es', 'neighborhood': 'Sant Gervasi - Galvany', 'latitude': 41.3937255, 'longitude': 2.1418776, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98192535/', 'distance': '2426', 'description': 'Espectacular ático con terraza en Turó Parc En una de las mejores fincas de la zona se sitúa este ático con una espectacular terraza de 135 metros. Se trata de un piso de 142 metros cuadrados, reformado, en el que antiguamente tenía 4 dormitorios, y ahora con la reforma tiene 2 grandes suites. El piso tiene un bonito recibidor que nos conduce a la zona de día, una bonita cocina con una zona de lavadero y al esplendido salón comedor con chimenea de mármol y salida directa a la terraza. En el pasillo encontramos un aseo de cortesía y la zona de noche con las 2 magníficas suites también con acceso a la terraza. La terraza tiene forma de L pudiendo crear en ella diferentes ambientes.  Se trata de una finca de lujo, con servicio de portería, 2 ascensores y posibilidad de alquilar parking en la misma finca. El Turó Parc es una de las zonas más demandadas de la ciudad. La elegancia y el prestigio son las características que definen tanto sus edificios como sus habitantes. Se trata de una zona muy segura, con todo tipo de comercios, servicios y ocio. El Turó Parc es la esencia del espíritu más sofisticado de Barcelona, sin perder al mismo tiempo la dimensión más pura y la calidez del barrio.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 7821.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': 'Sant Gervasi - Galvany, Barcelona', 'title': 'Ático en Calle del Tenor Viñas'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '89103723', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b0/f6/f1/976630614.jpg', 'externalReference': '019264', 'numPhotos': 31, 'price': 768000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 149.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3874885, 'longitude': 2.1594455, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/89103723/', 'distance': '859', 'description': 'Exclusivo piso de diseño y obra nueva a estrenar de 149m² situado en calle Diputació, junto la calle Muntaner. Dispone de un amplio y luminoso salón comedor con cocina independiente, 1 espacioso recibidor, 2 habitaciones dobles suite (25m² y 14m² respectivamente), 2 baños completos y 1 aseo de cortesía. Excelentes acabados. Cuenta con suelos de mármol, aire acondicionado (frío - calor), calefacción a gas y carpintería exterior de aluminio. Exterior y soleado. Ubicado en una finca regia de 1886 rehabilitada que dispone de una gran terraza comunitaria, un espacio de 60m² con zona “chill out” y unas preciosas vistas de Barcelona. En la rehabilitación se han utilizado los mejores materiales con un diseño muy elegante, creando espacios actuales y acogedores. El proyecto de reforma ha sido realizado por Jaime Beriestain Studio, que cuenta con reconocimiento de nivel mundial. Muy bien comunicado con transporte público, autobuses y metro (parada- Universitat). Una magnífica oportunidad para adquirir una lujosa vivienda a estrenar en el corazón de Barcelona. "Contacte con nosotros para solicitar más información o visitar el inmueble".', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5154.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '89103723', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b0/f6/f1/976630614.jpg', 'externalReference': '019264', 'numPhotos': 31, 'price': 768000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 149.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3874885, 'longitude': 2.1594455, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/89103723/', 'distance': '859', 'description': 'Exclusivo piso de diseño y obra nueva a estrenar de 149m² situado en calle Diputació, junto la calle Muntaner. Dispone de un amplio y luminoso salón comedor con cocina independiente, 1 espacioso recibidor, 2 habitaciones dobles suite (25m² y 14m² respectivamente), 2 baños completos y 1 aseo de cortesía. Excelentes acabados. Cuenta con suelos de mármol, aire acondicionado (frío - calor), calefacción a gas y carpintería exterior de aluminio. Exterior y soleado. Ubicado en una finca regia de 1886 rehabilitada que dispone de una gran terraza comunitaria, un espacio de 60m² con zona “chill out” y unas preciosas vistas de Barcelona. En la rehabilitación se han utilizado los mejores materiales con un diseño muy elegante, creando espacios actuales y acogedores. El proyecto de reforma ha sido realizado por Jaime Beriestain Studio, que cuenta con reconocimiento de nivel mundial. Muy bien comunicado con transporte público, autobuses y metro (parada- Universitat). Una magnífica oportunidad para adquirir una lujosa vivienda a estrenar en el corazón de Barcelona. "Contacte con nosotros para solicitar más información o visitar el inmueble".', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5154.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98269623', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a3/9c/10/1006157929.jpg', 'externalReference': 'VB2112040-1', 'numPhotos': 28, 'floor': 'en', 'price': 369000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 70.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "Calle d'Aribau", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3948237, 'longitude': 2.1524215, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98269623/', 'distance': '1660', 'description': 'Piso con terraza en venta en Calle Aribau Esta vivienda está ubicada en la Calle Aribau, cerca de la Diagonal y Enric Granados. Es un entresuelo, de 63m2 construidos, tiene una excelente ubicación en una finca clásica que conserva los elementos originales de la época, con ascensor y terrado comunitario. La zona de día consta de un amplio salón-comedor con salida a una terraza de 14m2, muy disfrutable, soleada y tranquila. Dispone de dos armarios para lavadora y secadora. Cocina equipada independiente, con la posibilidad de poderse abrir al salón-comedor. La zona de noche tiene un dormitorio principal y un baño completo en suite, un segundo dormitorio/despacho adjunto, con salida a la terraza. Tiene también baño completo con ducha. Suelos de parqué, aire acondicionado (frío/calor) calefacción, acumulador de agua, gran equipamiento de armarios, toldo eléctrico. ITE del edificio pasada.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 5271.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': "Piso en Calle d'Aribau"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98269623', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a3/9c/10/1006157929.jpg', 'externalReference': 'VB2112040-1', 'numPhotos': 28, 'floor': 'en', 'price': 369000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 70.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "Calle d'Aribau", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3948237, 'longitude': 2.1524215, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98269623/', 'distance': '1660', 'description': 'Piso con terraza en venta en Calle Aribau Esta vivienda está ubicada en la Calle Aribau, cerca de la Diagonal y Enric Granados. Es un entresuelo, de 63m2 construidos, tiene una excelente ubicación en una finca clásica que conserva los elementos originales de la época, con ascensor y terrado comunitario. La zona de día consta de un amplio salón-comedor con salida a una terraza de 14m2, muy disfrutable, soleada y tranquila. Dispone de dos armarios para lavadora y secadora. Cocina equipada independiente, con la posibilidad de poderse abrir al salón-comedor. La zona de noche tiene un dormitorio principal y un baño completo en suite, un segundo dormitorio/despacho adjunto, con salida a la terraza. Tiene también baño completo con ducha. Suelos de parqué, aire acondicionado (frío/calor) calefacción, acumulador de agua, gran equipamiento de armarios, toldo eléctrico. ITE del edificio pasada.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 5271.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': "Piso en Calle d'Aribau"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99268088', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/1d/34/d4/1038618419.jpg', 'externalReference': 'VB2210039', 'numPhotos': 28, 'floor': '3', 'price': 299000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 62.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de la Riereta', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3778121, 'longitude': 2.1688796, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99268088/', 'distance': '1076', 'description': 'Piso reformado con terraza en venta en la calle Riereta Preciosa vivienda totalmente reformada en 2019 situada a escasos metros de la Rambla del Raval y muy bien ubicada en el centro de Barcelona. La calle Riereta es una calle muy tranquila en la que se combinan edificios clásicos y edificios de recién construcción. El piso se encuentra en una tercera planta real en una finca de 1860 SIN ASCENSOR, rehabilitada y en muy buen estado de conservación, con terrado comunitario practicable con estupendas vistas a la ciudad de Barcelona y a la montaña de Montjuic. Se distribuye de la siguiente forma: dos habitaciones dobles exteriores a calle, baño completo, zona de aguas, cocina abierta al comedor, salón independiente con salida a terraza a nivel que orienta a un tranquilo y amplio patio de manzana. Doble orientación NE y SO. La propiedad se reformó en 2019. Los suelos son de gres imitación madera. Cerramientos de doble cristal en todas las estancias, aire acondicionado y calefacción por splits, puerta blindada, cocina equipada con todos los electrodomésticos, volta catalana y vigas vistas de madera, termo de agua caliente de 100L y alarma de Securitas Direct. Es un piso ideal como piso vacacional o como inversión por su alta rentabilidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 4823.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de la Riereta'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '99268088', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/1d/34/d4/1038618419.jpg', 'externalReference': 'VB2210039', 'numPhotos': 28, 'floor': '3', 'price': 299000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 62.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de la Riereta', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3778121, 'longitude': 2.1688796, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99268088/', 'distance': '1076', 'description': 'Piso reformado con terraza en venta en la calle Riereta Preciosa vivienda totalmente reformada en 2019 situada a escasos metros de la Rambla del Raval y muy bien ubicada en el centro de Barcelona. La calle Riereta es una calle muy tranquila en la que se combinan edificios clásicos y edificios de recién construcción. El piso se encuentra en una tercera planta real en una finca de 1860 SIN ASCENSOR, rehabilitada y en muy buen estado de conservación, con terrado comunitario practicable con estupendas vistas a la ciudad de Barcelona y a la montaña de Montjuic. Se distribuye de la siguiente forma: dos habitaciones dobles exteriores a calle, baño completo, zona de aguas, cocina abierta al comedor, salón independiente con salida a terraza a nivel que orienta a un tranquilo y amplio patio de manzana. Doble orientación NE y SO. La propiedad se reformó en 2019. Los suelos son de gres imitación madera. Cerramientos de doble cristal en todas las estancias, aire acondicionado y calefacción por splits, puerta blindada, cocina equipada con todos los electrodomésticos, volta catalana y vigas vistas de madera, termo de agua caliente de 100L y alarma de Securitas Direct. Es un piso ideal como piso vacacional o como inversión por su alta rentabilidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 4823.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de la Riereta'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98985637', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/2d/73/6b/1030519082.jpg', 'externalReference': 'VB2209039', 'numPhotos': 27, 'floor': 'en', 'price': 325000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 69.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de Ribes', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'El Fort Pienc', 'latitude': 41.4015389, 'longitude': 2.1846789, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98985637/', 'distance': '1999', 'description': 'Piso en venta frente al Auditori y al Teatre Nacional En el barrio de Fortpienc, frente al Teatre Nacional y al Auditori de Barcelona, muy cerca dels Encants nous y de la Plaça de les Glòries, encontramos esta propiedad, situada en una finca clásica de 1890, en muy buen estado de conservación, con ascensor y con doble orientación. El piso se reformó en 2004 y actualmente su estado de conservación es muy bueno. Se vende completamente equipado y amueblado. Consta de 69m2 construidos, 57m2 útiles y dos balcones, el que da a calle de 2m2 y el que está en la habitación de 3,25m2. Se distribuye de la siguiente manera: salón independiente exterior a la calle Ribes, con salida directa a balcón, con orientación sur. Cocina abierta al comedor. Baño completo con ventilación natural. Dormitorio individual amplio con ventana a patio interior de la finca. Dormitorio doble con salida a balcón. La zona de aguas se encuentra en el balcón al lado de la habitación de matrimonio. Termo de agua caliente eléctrico, ventanas de aluminio, splits de aire frío y caliente. Cocina equipada con vitro, campana extractora, horno, lavaplatos y nevera-congelador. La ubicación de esta vivienda es inmejorable, cerca de todos los servicios, bien comunicado, con aparcamiento público frente al edificio, el centro comercial Glòries a 10 minutos caminando, transporte público (bus, metro, tranvía), comercios y restaurantes. ¡No dudes en contactar con nosotros para ver esta magnífica propiedad!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4710.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Fort Pienc, Barcelona', 'title': 'Piso en Calle de Ribes'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98985637', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/2d/73/6b/1030519082.jpg', 'externalReference': 'VB2209039', 'numPhotos': 27, 'floor': 'en', 'price': 325000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 69.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de Ribes', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'El Fort Pienc', 'latitude': 41.4015389, 'longitude': 2.1846789, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98985637/', 'distance': '1999', 'description': 'Piso en venta frente al Auditori y al Teatre Nacional En el barrio de Fortpienc, frente al Teatre Nacional y al Auditori de Barcelona, muy cerca dels Encants nous y de la Plaça de les Glòries, encontramos esta propiedad, situada en una finca clásica de 1890, en muy buen estado de conservación, con ascensor y con doble orientación. El piso se reformó en 2004 y actualmente su estado de conservación es muy bueno. Se vende completamente equipado y amueblado. Consta de 69m2 construidos, 57m2 útiles y dos balcones, el que da a calle de 2m2 y el que está en la habitación de 3,25m2. Se distribuye de la siguiente manera: salón independiente exterior a la calle Ribes, con salida directa a balcón, con orientación sur. Cocina abierta al comedor. Baño completo con ventilación natural. Dormitorio individual amplio con ventana a patio interior de la finca. Dormitorio doble con salida a balcón. La zona de aguas se encuentra en el balcón al lado de la habitación de matrimonio. Termo de agua caliente eléctrico, ventanas de aluminio, splits de aire frío y caliente. Cocina equipada con vitro, campana extractora, horno, lavaplatos y nevera-congelador. La ubicación de esta vivienda es inmejorable, cerca de todos los servicios, bien comunicado, con aparcamiento público frente al edificio, el centro comercial Glòries a 10 minutos caminando, transporte público (bus, metro, tranvía), comercios y restaurantes. ¡No dudes en contactar con nosotros para ver esta magnífica propiedad!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4710.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Fort Pienc, Barcelona', 'title': 'Piso en Calle de Ribes'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98374038', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/4a/c7/58/1009839184.jpg', 'externalReference': 'VB2207045', 'numPhotos': 47, 'floor': '3', 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 77.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Riereta', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3791652, 'longitude': 2.1708504, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98374038/', 'distance': '928', 'description': 'Loft de Obra Nueva con jardín y piscina en el centro histórico de Barcelona  Preciosa vivienda en edificio de obra nueva del 2021 en el centro de Barcelona. Se trata de una rehabilitación integral de una antigua fábrica textil de 1833, creando unas viviendas únicas de estilo neoyorquino con grande ventanales y techos de doble altura con vigas de madera y paredes de ladrillo visto. El piso estilo loft se encuentra en la planta tercera, tiene una superficie de 74 m2, más una terraza cubierta de 6 m2 que da a las zonas comunitarias. Los materiales utilizados son de la más alta calidad y además consta de algunos elementos recuperados. Se compone de cocina totalmente equipada, salón, comedor, un dormitorio doble con baño en suite, y otro baño completo. Además, se ha aprovechado de la altura de los techos para realizar un altillo de 12 m2 donde ahora se ubica otro dormitorio doble. El edificio cuenta con zonas comunes que incluyen piscina y solárium con impresionantes vistas a la ciudad, huertos urbanos, jardines verticales, sistema de climatización por Aerotermia, servicio conserjería, video vigilancia 24h, reciclaje de aguas pluviales, parking para bicicletas y un atrio en medio del complejo lleno de tragaluces y árboles. Una oportunidad única para vivir una nueva experiencia en la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6299.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de la Riereta'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98374038', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/4a/c7/58/1009839184.jpg', 'externalReference': 'VB2207045', 'numPhotos': 47, 'floor': '3', 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 77.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Riereta', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3791652, 'longitude': 2.1708504, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98374038/', 'distance': '928', 'description': 'Loft de Obra Nueva con jardín y piscina en el centro histórico de Barcelona  Preciosa vivienda en edificio de obra nueva del 2021 en el centro de Barcelona. Se trata de una rehabilitación integral de una antigua fábrica textil de 1833, creando unas viviendas únicas de estilo neoyorquino con grande ventanales y techos de doble altura con vigas de madera y paredes de ladrillo visto. El piso estilo loft se encuentra en la planta tercera, tiene una superficie de 74 m2, más una terraza cubierta de 6 m2 que da a las zonas comunitarias. Los materiales utilizados son de la más alta calidad y además consta de algunos elementos recuperados. Se compone de cocina totalmente equipada, salón, comedor, un dormitorio doble con baño en suite, y otro baño completo. Además, se ha aprovechado de la altura de los techos para realizar un altillo de 12 m2 donde ahora se ubica otro dormitorio doble. El edificio cuenta con zonas comunes que incluyen piscina y solárium con impresionantes vistas a la ciudad, huertos urbanos, jardines verticales, sistema de climatización por Aerotermia, servicio conserjería, video vigilancia 24h, reciclaje de aguas pluviales, parking para bicicletas y un atrio en medio del complejo lleno de tragaluces y árboles. Una oportunidad única para vivir una nueva experiencia en la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6299.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de la Riereta'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98272281', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/df/38/a0/1006238408.jpg', 'externalReference': 'VB2206060', 'numPhotos': 29, 'floor': 'en', 'price': 345000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 63.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle d'Enric Granados", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3923655, 'longitude': 2.1573188, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98272281/', 'distance': '1170', 'description': 'Piso reformado de 2 habitaciones en la Calle Enric Granados Situado en una de las calles más emblemáticas de Barcelona i del Eixample Esquerra, rodeado de todo tipo de servicios, restaurantes, cafeterías y muy bien comunicado, se encuentra este bonito, reformado y práctico piso ubicado en una finca Regia con estilo del 1900. La vivienda, de 63 m2, está para entrar a vivir y se encuentra en una planta baja por lo que disfruta de una agradable terraza, muy agradable y tranquila orientada a Noreste de 12 m2. El piso dispone de dos habitaciones dobles, y una de ellas tiene una galería con vistas a la terraza, ideal para ubicar un despacho, por ejemplo. La segunda, interior y con salida a patio de luces, completa Completa este práctico piso la cocina / salón desde donde también se accede a la terraza, que permite disfrutar del sol y el aire libre en un espacio alegre. Ven a visitar este bonito y céntrico piso en Barcelona!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5476.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': "Piso en Calle d'Enric Granados"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98272281', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/df/38/a0/1006238408.jpg', 'externalReference': 'VB2206060', 'numPhotos': 29, 'floor': 'en', 'price': 345000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 63.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle d'Enric Granados", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3923655, 'longitude': 2.1573188, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98272281/', 'distance': '1170', 'description': 'Piso reformado de 2 habitaciones en la Calle Enric Granados Situado en una de las calles más emblemáticas de Barcelona i del Eixample Esquerra, rodeado de todo tipo de servicios, restaurantes, cafeterías y muy bien comunicado, se encuentra este bonito, reformado y práctico piso ubicado en una finca Regia con estilo del 1900. La vivienda, de 63 m2, está para entrar a vivir y se encuentra en una planta baja por lo que disfruta de una agradable terraza, muy agradable y tranquila orientada a Noreste de 12 m2. El piso dispone de dos habitaciones dobles, y una de ellas tiene una galería con vistas a la terraza, ideal para ubicar un despacho, por ejemplo. La segunda, interior y con salida a patio de luces, completa Completa este práctico piso la cocina / salón desde donde también se accede a la terraza, que permite disfrutar del sol y el aire libre en un espacio alegre. Ven a visitar este bonito y céntrico piso en Barcelona!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5476.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': "Piso en Calle d'Enric Granados"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98271905', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/e5/49/6f/1006228158.jpg', 'externalReference': 'VB2206005', 'numPhotos': 41, 'floor': 'bj', 'price': 480000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 139.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "Calle d'en Carabassa", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3811984, 'longitude': 2.1775831, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98271905/', 'distance': '956', 'description': 'Piso en venta reformado con bodega de 47m2 al lado de la Iglesia de la Mercè A escasos pasos de la Basílica de la Mercè y del Moll de la Fusta, en el pleno centro del barrio Gótico con más historia de la ciudad, encontramos este apartamento de 92m2 construidos totalmente rehabilitado, situado en la primera planta de una finca de 1890 con ascensor, orientación Sur. El piso, gracias a su rehabilitación integral de todo el edificio, combina las ventajas de una construcción nueva con elementos originales, lo que sin duda hacen de está vivienda una pieza única. A destacar las zonas comunes con el terrado de uso comunitario con vistas a la ciudad y totalmente acondicionado con barbacoa, baño y sala de reuniones. Zona de parking para bicicletas en la entrada de la vivienda, y un largo etc. Sus 139m2 están compuestos de una bodega en la planta –1 de 47m2 totalmente habilitada y el piso de 92m2 que consta dde un amplio salón comedor con una cocina totalmente integrada y equipada, una suite con baño, una habitación semi doble y un baño completo. La zona de aguas está contigua a la cocina. Las ventanas del piso son de aluminio con rotura de puente térmico y doble cristal, para garantizar un aislamiento térmico y acústico. Sistema de eficiencia energética mediante aerotermia, los suelos están pavimentados con parquet en madera y los baños con gres porcelánico. Terrado de uso comunitario con vistas a la ciudad y totalmente acondicionado con barbacoa, baño y sala de reuniones. Si quiere vivir en el barrio gótico, no dudes en pedirnos visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3453.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': "Piso en Calle d'en Carabassa"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98271905', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/e5/49/6f/1006228158.jpg', 'externalReference': 'VB2206005', 'numPhotos': 41, 'floor': 'bj', 'price': 480000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 139.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "Calle d'en Carabassa", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3811984, 'longitude': 2.1775831, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98271905/', 'distance': '956', 'description': 'Piso en venta reformado con bodega de 47m2 al lado de la Iglesia de la Mercè A escasos pasos de la Basílica de la Mercè y del Moll de la Fusta, en el pleno centro del barrio Gótico con más historia de la ciudad, encontramos este apartamento de 92m2 construidos totalmente rehabilitado, situado en la primera planta de una finca de 1890 con ascensor, orientación Sur. El piso, gracias a su rehabilitación integral de todo el edificio, combina las ventajas de una construcción nueva con elementos originales, lo que sin duda hacen de está vivienda una pieza única. A destacar las zonas comunes con el terrado de uso comunitario con vistas a la ciudad y totalmente acondicionado con barbacoa, baño y sala de reuniones. Zona de parking para bicicletas en la entrada de la vivienda, y un largo etc. Sus 139m2 están compuestos de una bodega en la planta –1 de 47m2 totalmente habilitada y el piso de 92m2 que consta dde un amplio salón comedor con una cocina totalmente integrada y equipada, una suite con baño, una habitación semi doble y un baño completo. La zona de aguas está contigua a la cocina. Las ventanas del piso son de aluminio con rotura de puente térmico y doble cristal, para garantizar un aislamiento térmico y acústico. Sistema de eficiencia energética mediante aerotermia, los suelos están pavimentados con parquet en madera y los baños con gres porcelánico. Terrado de uso comunitario con vistas a la ciudad y totalmente acondicionado con barbacoa, baño y sala de reuniones. Si quiere vivir en el barrio gótico, no dudes en pedirnos visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3453.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': "Piso en Calle d'en Carabassa"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98271257', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f4/c7/a6/1006207841.jpg', 'externalReference': 'VB2203084-1', 'numPhotos': 34, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 110.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3928528, 'longitude': 2.1615339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98271257/', 'distance': '909', 'description': 'Piso de diseño en venta en Rambla Catalunya En la Rambla Catalunya, una de las calles más exclusivas de la ciudad encontramos esta magnífica vivienda en una preciosa finca regia con servicio de conserjería y ascensor. El piso consta de 110m2 y gracias a su altura y orientación, goza de mucha tranquilidad a pesar de su ubicación tan céntrica. Al entrar, un amplio pasillo con pared de ladrillo visto nos conduce a un dormitorio doble con armario empotrado y salida a una pequeña terraza. Sus puertas cristaleras confieren al piso una sensación maravillosa de espacio y luz. En la habitación contigua el lavadero con armario empotrado y en frente un baño completo con ducha. A continuación, la moderna cocina office, equipada con electrodomésticos de primera categoría y con espacio para mesa de 6 comensales. Seguidamente accedemos al amplio salón que gracias a su grandes ventanales y orientación a bonito patio de manzana goza de muchísima luz natural. El segundo dormitorio es el principal, orientado al exterior, con armarios empotrados y con baño completo con ducha y bañera de hidromasaje en suite. El piso dispone de suelos de parquet, calefacción por radiadores, aire acondicionado por conductos y ventanas con doble acristalamiento. ¡Contacta con nosotros hoy para visitar esta propiedad única en la zona más exclusiva de L’Eixample!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8000.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98271257', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f4/c7/a6/1006207841.jpg', 'externalReference': 'VB2203084-1', 'numPhotos': 34, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 110.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3928528, 'longitude': 2.1615339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98271257/', 'distance': '909', 'description': 'Piso de diseño en venta en Rambla Catalunya En la Rambla Catalunya, una de las calles más exclusivas de la ciudad encontramos esta magnífica vivienda en una preciosa finca regia con servicio de conserjería y ascensor. El piso consta de 110m2 y gracias a su altura y orientación, goza de mucha tranquilidad a pesar de su ubicación tan céntrica. Al entrar, un amplio pasillo con pared de ladrillo visto nos conduce a un dormitorio doble con armario empotrado y salida a una pequeña terraza. Sus puertas cristaleras confieren al piso una sensación maravillosa de espacio y luz. En la habitación contigua el lavadero con armario empotrado y en frente un baño completo con ducha. A continuación, la moderna cocina office, equipada con electrodomésticos de primera categoría y con espacio para mesa de 6 comensales. Seguidamente accedemos al amplio salón que gracias a su grandes ventanales y orientación a bonito patio de manzana goza de muchísima luz natural. El segundo dormitorio es el principal, orientado al exterior, con armarios empotrados y con baño completo con ducha y bañera de hidromasaje en suite. El piso dispone de suelos de parquet, calefacción por radiadores, aire acondicionado por conductos y ventanas con doble acristalamiento. ¡Contacta con nosotros hoy para visitar esta propiedad única en la zona más exclusiva de L’Eixample!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8000.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98269646', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/0e/44/3a/1006158045.jpg', 'externalReference': 'VB2112041-1', 'numPhotos': 34, 'floor': '1', 'price': 750000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 140.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de les Jonqueres', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3867007, 'longitude': 2.1744305, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98269646/', 'distance': '400', 'description': 'Piso tipo Loft en venta en la calle Jonqueres Este loft está situado en Born, muy cerca del Palau de la Musica, en un edificio original del 1870 que había sido un antiguo convento y se rehabilitó íntegramente en el año 1997. En la entrada del edificio hay un amplio recibidor que da acceso a la escalera y al ascensor. En el primer piso encontramos una zona comunitaria ajardinada central donde se ubicaba en el antiguo claustro, que da acceso a la propiedad. La vivienda es toda exterior, con amplios ventanales al tranquilo y silencioso espacio central del edificio. El loft se reformó hace unos 13 años y mantiene ese encanto bohemio tan característico de la zona. En la entrada encontramos el recibidor abierto al amplio salón-comedor con cocina abierta. Está rodeado de grandes ventanales con mucha luz. Tiene acceso a una amplia terraza de 40m2, una zona muy tranquila y luminosa. En la misma planta hay un dormitorio doble con baño completo y en la zona del altillo (planta escriturada) se encuentra el segundo dormitorio abierto al espacio del salón, también dispone de un baño completo en suite. El techo mide 4.50mts de alto y tiene bonitas vigas de madera, el suelo es de parque macizo (se pulirá a gusto del comprador). Además, la vivienda dispone de screens, aire acondicionado frío-calor por Split y calefacción individual por radiadores. La propiedad no dispone de parking en finca, pero existe la posibilidad de alquilar una plaza de aparcamiento en la misma manzana..', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5357.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso en Calle de les Jonqueres'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98269646', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/0e/44/3a/1006158045.jpg', 'externalReference': 'VB2112041-1', 'numPhotos': 34, 'floor': '1', 'price': 750000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 140.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de les Jonqueres', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3867007, 'longitude': 2.1744305, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98269646/', 'distance': '400', 'description': 'Piso tipo Loft en venta en la calle Jonqueres Este loft está situado en Born, muy cerca del Palau de la Musica, en un edificio original del 1870 que había sido un antiguo convento y se rehabilitó íntegramente en el año 1997. En la entrada del edificio hay un amplio recibidor que da acceso a la escalera y al ascensor. En el primer piso encontramos una zona comunitaria ajardinada central donde se ubicaba en el antiguo claustro, que da acceso a la propiedad. La vivienda es toda exterior, con amplios ventanales al tranquilo y silencioso espacio central del edificio. El loft se reformó hace unos 13 años y mantiene ese encanto bohemio tan característico de la zona. En la entrada encontramos el recibidor abierto al amplio salón-comedor con cocina abierta. Está rodeado de grandes ventanales con mucha luz. Tiene acceso a una amplia terraza de 40m2, una zona muy tranquila y luminosa. En la misma planta hay un dormitorio doble con baño completo y en la zona del altillo (planta escriturada) se encuentra el segundo dormitorio abierto al espacio del salón, también dispone de un baño completo en suite. El techo mide 4.50mts de alto y tiene bonitas vigas de madera, el suelo es de parque macizo (se pulirá a gusto del comprador). Además, la vivienda dispone de screens, aire acondicionado frío-calor por Split y calefacción individual por radiadores. La propiedad no dispone de parking en finca, pero existe la posibilidad de alquilar una plaza de aparcamiento en la misma manzana..', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5357.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso en Calle de les Jonqueres'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '91592832', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/72/64/da/925378429.jpg', 'externalReference': 'W-02JZPS', 'numPhotos': 40, 'floor': '2', 'price': 818000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 87.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3949048, 'longitude': 2.167361, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/91592832/', 'distance': '850', 'description': 'Finca regia renovada cerca de Paseo de Gracia\r Estamos encantados de ofrecer este impresionante apartamento de 2 dormitorios en un edificio histórico completamente renovado con 10 pisos impecables, ubicado justo al lado de la famosa avenida comercial de Paseo de Gracia de Barcelona.\r Cada hogar ha sido diseñado por expertos en estilo y funcionalidad. Mientras que las características arquitectónicas clásicas de Barcelona se han restaurado para impartir la esencia de la historia del edificio como una "finca regia".\r Un vestíbulo de cristal le da la bienvenida a la casa antes de entrar en la cocina de diseño contemporáneo que se abre a la sala de estar. Con dos balcones, esta casa está bien iluminada y tiene un sentido de conexión con la ciudad, ya que todas las habitaciones dan al exterior.\r Las zonas separadas de día y de noche imparten amplitud y privacidad, y en la parte trasera del apartamento encontramos la suite principal. Los amplios pisos de tablones de madera de roble alargan el espacio. Los armarios están inteligentemente integrados en todas partes. Los amplios baños están equipados con accesorios de primera calidad.\r Los detalles arquitectónicos restaurados incluyen las fachadas del edificio, los techos abovedados catalanes, la entrada y la escalera del edificio, además de integrar pisos hidráulicos originales en los baños.\r La propiedad cuenta con marcas de primera calidad y materiales de construcción para maximizar el confort: electrodomésticos Miele, aerotermia Mitsubishi, cocinas Bulthaup, electrodomésticos Duravit y más. Se han tomado medidas específicas para maximizar la privacidad y el control del sonido, como las nuevas ventanas de doble acristalamiento y los sustratos de piso reforzado.\r El elegante barrio del Eixample se caracteriza por su arquitectura visionaria modernista, tiendas independientes, boutiques elegantes y cultura del café.\r La propiedad está situada en el corazón del Eixample Quadrat d’Or (‘Square Golden Square’), a solo una cuadra de la avenida arbolada del Passeig de Gràcia.\r Barcelona se ha transformado desde los Juegos Olímpicos de 1992, y la capital catalana se ha convertido en la meca de los creativos y emprendedores de todo el mundo gracias a su creciente reputación como un importante centro de nuevas empresas e innovación tecnológica.\r La segunda ciudad de España continúa liderando la cocina internacional de vanguardia y actualmente alberga más de 30 restaurantes con estrellas Michelin. Una de las ciudades "inteligentes" líderes en Europa, sus credenciales incluyen 500 kilómetros de fibra óptica, WiFi gratis a través de su alumbrado público y sensores para monitorear la calidad del aire. La propiedad tiene una gran demanda, particularmente en los barrios principales del casco antiguo de Barcelona y el Eixample, el núcleo cultural y vibrante de la ciudad.\r En la década de 1900, este codiciado barrio fue construido por la burguesía de Barcelona, que compitió para crear las casas más estéticamente refinadas. En los últimos años, esta área ha experimentado un gran renacimiento y se ha convertido en un imán para los compradores internacionales, especialmente con la concentración de una serie de desarrollos de lujo.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 9402.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '91592832', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/72/64/da/925378429.jpg', 'externalReference': 'W-02JZPS', 'numPhotos': 40, 'floor': '2', 'price': 818000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 87.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3949048, 'longitude': 2.167361, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/91592832/', 'distance': '850', 'description': 'Finca regia renovada cerca de Paseo de Gracia\r Estamos encantados de ofrecer este impresionante apartamento de 2 dormitorios en un edificio histórico completamente renovado con 10 pisos impecables, ubicado justo al lado de la famosa avenida comercial de Paseo de Gracia de Barcelona.\r Cada hogar ha sido diseñado por expertos en estilo y funcionalidad. Mientras que las características arquitectónicas clásicas de Barcelona se han restaurado para impartir la esencia de la historia del edificio como una "finca regia".\r Un vestíbulo de cristal le da la bienvenida a la casa antes de entrar en la cocina de diseño contemporáneo que se abre a la sala de estar. Con dos balcones, esta casa está bien iluminada y tiene un sentido de conexión con la ciudad, ya que todas las habitaciones dan al exterior.\r Las zonas separadas de día y de noche imparten amplitud y privacidad, y en la parte trasera del apartamento encontramos la suite principal. Los amplios pisos de tablones de madera de roble alargan el espacio. Los armarios están inteligentemente integrados en todas partes. Los amplios baños están equipados con accesorios de primera calidad.\r Los detalles arquitectónicos restaurados incluyen las fachadas del edificio, los techos abovedados catalanes, la entrada y la escalera del edificio, además de integrar pisos hidráulicos originales en los baños.\r La propiedad cuenta con marcas de primera calidad y materiales de construcción para maximizar el confort: electrodomésticos Miele, aerotermia Mitsubishi, cocinas Bulthaup, electrodomésticos Duravit y más. Se han tomado medidas específicas para maximizar la privacidad y el control del sonido, como las nuevas ventanas de doble acristalamiento y los sustratos de piso reforzado.\r El elegante barrio del Eixample se caracteriza por su arquitectura visionaria modernista, tiendas independientes, boutiques elegantes y cultura del café.\r La propiedad está situada en el corazón del Eixample Quadrat d’Or (‘Square Golden Square’), a solo una cuadra de la avenida arbolada del Passeig de Gràcia.\r Barcelona se ha transformado desde los Juegos Olímpicos de 1992, y la capital catalana se ha convertido en la meca de los creativos y emprendedores de todo el mundo gracias a su creciente reputación como un importante centro de nuevas empresas e innovación tecnológica.\r La segunda ciudad de España continúa liderando la cocina internacional de vanguardia y actualmente alberga más de 30 restaurantes con estrellas Michelin. Una de las ciudades "inteligentes" líderes en Europa, sus credenciales incluyen 500 kilómetros de fibra óptica, WiFi gratis a través de su alumbrado público y sensores para monitorear la calidad del aire. La propiedad tiene una gran demanda, particularmente en los barrios principales del casco antiguo de Barcelona y el Eixample, el núcleo cultural y vibrante de la ciudad.\r En la década de 1900, este codiciado barrio fue construido por la burguesía de Barcelona, que compitió para crear las casas más estéticamente refinadas. En los últimos años, esta área ha experimentado un gran renacimiento y se ha convertido en un imán para los compradores internacionales, especialmente con la concentración de una serie de desarrollos de lujo.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 9402.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '96603203', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/99/69/76/951332285.jpg', 'externalReference': 'BHHS-004107', 'numPhotos': 40, 'floor': '6', 'price': 560000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 62.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3967221, 'longitude': 2.1548047, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96603203/', 'distance': '1615', 'description': 'PISO ALTO Y SOLEADO EN FINCA MODERNA DE LA PARTE ALTA DEL EIXAMPLE EL PISO IDEAL EN FINCA MODERNA BERKSHIRE\xa0HATHAWAY\xa0HomeServices\xa0Barcelona, consultora especializada en la comercialización de propiedades exclusivas en las mejores zonas de Barcelona, les ofrece este fantástico piso, situado en la parte alta del barrio del Eixample de Barcelona, junto a la Rambla Catalunya. Según entramos en el piso, nos encontramos con la barra baja que separa el hall de la\xa0cocina\xa0la izquierda. Al frente\xa0nos dirigimos\xa0al salón comedor con salida al gran ventanal exterior a la calle, con vistas y muy soleado durante todo el día. También tiene un estrecho balcón, por el que se mueven las persianas correderas. El salón está orientado a Sur, y es exterior a la calle\xa0Córsega, que es de poquísimo tránsito en este\xa0tramo, ya que\xa0su acceso se inicia desde la adyacente Rambla de\xa0Catalunya. La cocina está equipada con electrodomésticos y cruzando una puerta se accede al lavadero con espacio para lavadora, secadora y lavabo. Los muebles de diseño, y electrodomésticos que ven en las fotografías, no están incluidos en el precio. Desde el salón, a través de una puerta que separa la zona de día de la zona de noche, accedemos a un distribuidor con un baño completo al frente, con bañera, y las dos habitaciones, una a cada lado, son dobles y tienen armarios empotrados. Una es exterior al pequeño balcón que da a la calle, y la otra da al vestíbulo privado de vecinos de la planta. El piso tiene calefacción por radiadores, caldera y acumulador, aire acondicionado por conductos a todas las estancias, suelos de parquet... \xa0Además, \xa0está muy bien distribuido, con muy buen gusto, y sin espacios perdidos. Esta finca fue construida en el 1967, y en el 2007\xa0Metrovacesa\xa0la adaptó para tener viviendas cómodas y accesibles, además con buen gusto y diseño, como se puede apreciar en las fotografías de la misma. Se completa con un vestíbulo muy acogedor, donde recibe, el que posiblemente sea, el mejor conserje de Barcelona. Para más información no dude en contactar con Berkshire Hathaway\xa0HomeServices\xa0Barcelona, especialistas en inmuebles de alto standing en Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 9032.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '96603203', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/99/69/76/951332285.jpg', 'externalReference': 'BHHS-004107', 'numPhotos': 40, 'floor': '6', 'price': 560000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 62.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3967221, 'longitude': 2.1548047, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96603203/', 'distance': '1615', 'description': 'PISO ALTO Y SOLEADO EN FINCA MODERNA DE LA PARTE ALTA DEL EIXAMPLE EL PISO IDEAL EN FINCA MODERNA BERKSHIRE\xa0HATHAWAY\xa0HomeServices\xa0Barcelona, consultora especializada en la comercialización de propiedades exclusivas en las mejores zonas de Barcelona, les ofrece este fantástico piso, situado en la parte alta del barrio del Eixample de Barcelona, junto a la Rambla Catalunya. Según entramos en el piso, nos encontramos con la barra baja que separa el hall de la\xa0cocina\xa0la izquierda. Al frente\xa0nos dirigimos\xa0al salón comedor con salida al gran ventanal exterior a la calle, con vistas y muy soleado durante todo el día. También tiene un estrecho balcón, por el que se mueven las persianas correderas. El salón está orientado a Sur, y es exterior a la calle\xa0Córsega, que es de poquísimo tránsito en este\xa0tramo, ya que\xa0su acceso se inicia desde la adyacente Rambla de\xa0Catalunya. La cocina está equipada con electrodomésticos y cruzando una puerta se accede al lavadero con espacio para lavadora, secadora y lavabo. Los muebles de diseño, y electrodomésticos que ven en las fotografías, no están incluidos en el precio. Desde el salón, a través de una puerta que separa la zona de día de la zona de noche, accedemos a un distribuidor con un baño completo al frente, con bañera, y las dos habitaciones, una a cada lado, son dobles y tienen armarios empotrados. Una es exterior al pequeño balcón que da a la calle, y la otra da al vestíbulo privado de vecinos de la planta. El piso tiene calefacción por radiadores, caldera y acumulador, aire acondicionado por conductos a todas las estancias, suelos de parquet... \xa0Además, \xa0está muy bien distribuido, con muy buen gusto, y sin espacios perdidos. Esta finca fue construida en el 1967, y en el 2007\xa0Metrovacesa\xa0la adaptó para tener viviendas cómodas y accesibles, además con buen gusto y diseño, como se puede apreciar en las fotografías de la misma. Se completa con un vestíbulo muy acogedor, donde recibe, el que posiblemente sea, el mejor conserje de Barcelona. Para más información no dude en contactar con Berkshire Hathaway\xa0HomeServices\xa0Barcelona, especialistas en inmuebles de alto standing en Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 9032.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99671987', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ef/7d/5e/1050814553.jpg', 'externalReference': 'BCN38016', 'numPhotos': 33, 'price': 500000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 66.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3940703, 'longitude': 2.1510348, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99671987/', 'distance': '1724', 'description': 'Lucas Fox presenta esta propiedad reformada ubicada a pocos pasos de la Avenida Diagonal y de la plaza de Francesc Macià.  Está situada en la planta principal del edificio, por lo que dispone de techos altos.  En la zona de día, encontramos una cocina americana totalmente equipada. \xa0El salón comedor es exterior y tiene un pequeño balcón donde colocar una mesa y dos sillas para disfrutar del sol de tarde. \xa0Además, tiene suelos hidráulicos y una bonita pared de obra vista en uno de sus laterales.  Por otro lado, un pequeño pasillo conduce a la otra parte de la vivienda. Aquí, vemos el dormitorio principal doble equipado con armario y un aseo y un segundo dormitorio también doble y con un armario muy espacioso. Ambos dormitorios son interiores, por lo que son muy tranquilos. Finalmente, entre los dormitorios encontramos el baño principal con ducha. El piso cuenta con unos altillos muy prácticos que se pueden aprovechar para almacenaje, aire acondicionado, calefacción por conductos y suelos de parquet en parte de la casa e hidráulicos en otra. Asimismo, los vecinos del edificio pueden disfrutar de la terraza comunitaria.  Póngase en contacto con nosotros para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 7576.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '99671987', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ef/7d/5e/1050814553.jpg', 'externalReference': 'BCN38016', 'numPhotos': 33, 'price': 500000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 66.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3940703, 'longitude': 2.1510348, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99671987/', 'distance': '1724', 'description': 'Lucas Fox presenta esta propiedad reformada ubicada a pocos pasos de la Avenida Diagonal y de la plaza de Francesc Macià.  Está situada en la planta principal del edificio, por lo que dispone de techos altos.  En la zona de día, encontramos una cocina americana totalmente equipada. \xa0El salón comedor es exterior y tiene un pequeño balcón donde colocar una mesa y dos sillas para disfrutar del sol de tarde. \xa0Además, tiene suelos hidráulicos y una bonita pared de obra vista en uno de sus laterales.  Por otro lado, un pequeño pasillo conduce a la otra parte de la vivienda. Aquí, vemos el dormitorio principal doble equipado con armario y un aseo y un segundo dormitorio también doble y con un armario muy espacioso. Ambos dormitorios son interiores, por lo que son muy tranquilos. Finalmente, entre los dormitorios encontramos el baño principal con ducha. El piso cuenta con unos altillos muy prácticos que se pueden aprovechar para almacenaje, aire acondicionado, calefacción por conductos y suelos de parquet en parte de la casa e hidráulicos en otra. Asimismo, los vecinos del edificio pueden disfrutar de la terraza comunitaria.  Póngase en contacto con nosotros para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 7576.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99602294', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/e5/3c/c0/1048891671.jpg', 'externalReference': 'BCN37037', 'numPhotos': 37, 'price': 649000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 102.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Gòtic', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3858046, 'longitude': 2.1752293, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99602294/', 'distance': '493', 'description': "Situado en el Barrio Gótico, a un paso de Portal de l'Àngel, Plaza de Catalunya y de la Catedral de Barcelona, Lucas Fox presenta este piso recién reformado y totalmente amueblado a estrenar.  La reforma ha terminado recientemente y el piso está listo para entrar a vivir.  Tiene doble orientación y al estar en una planta alta, goza de abundante luz natural que entra por grandes ventanales.  Al entrar en el piso nos encontramos con un amplio hall de entrada, con espacio de almacenamiento adicional, que nos da acceso a la zona de día. A nuestra derecha tenemos el salón-comedor de 32m2 con salida a dos balcones con bonitas vistas a edificios monumentales. A nuestra izquierda tenemos un baño y el cuarto lavadero.  A través de la cocina totalmente equipada, que alberga otro espacio de comedor/zona de trabajo, accedemos a la zona de noche que consta de dos dormitorios dobles con armarios y el segundo baño. \xa0Ambos dormitorios dan a un tranquilo patio interior.  Este excelente piso cuenta con todas las instalaciones nuevas: fontanería, gas, electricidad, ventilación, aire acondicionado por conductos en la zona de día, splits en la zona de noche y calefacción eléctrica independiente en todas partes.  Consta con suelos y baldosas de madera nuevos, una cocina hecha a medida con electrodomésticos de marcas de alta calidad, muebles de diseño, lámparas y fotografías de lugares emblemáticos de Barcelona, como se muestra en las imágenes.  Los residentes del edificio pueden disfrutar de la terraza comunitaria con vistas al casco antiguo.  Póngase en contacto con nosotros para concertar una visita.  Características básicas:  - 102 m² construidos  - 2 dormitorios dobles  - 2 baños  - Terraza  - Armarios  Edificio  - Exterior/interior  -\xa0Construido en 1836  Equipamiento  - Aire acondicionado (conductos/splits)  - Calefacción independiente.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 6363.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '99602294', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/e5/3c/c0/1048891671.jpg', 'externalReference': 'BCN37037', 'numPhotos': 37, 'price': 649000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 102.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Gòtic', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3858046, 'longitude': 2.1752293, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99602294/', 'distance': '493', 'description': "Situado en el Barrio Gótico, a un paso de Portal de l'Àngel, Plaza de Catalunya y de la Catedral de Barcelona, Lucas Fox presenta este piso recién reformado y totalmente amueblado a estrenar.  La reforma ha terminado recientemente y el piso está listo para entrar a vivir.  Tiene doble orientación y al estar en una planta alta, goza de abundante luz natural que entra por grandes ventanales.  Al entrar en el piso nos encontramos con un amplio hall de entrada, con espacio de almacenamiento adicional, que nos da acceso a la zona de día. A nuestra derecha tenemos el salón-comedor de 32m2 con salida a dos balcones con bonitas vistas a edificios monumentales. A nuestra izquierda tenemos un baño y el cuarto lavadero.  A través de la cocina totalmente equipada, que alberga otro espacio de comedor/zona de trabajo, accedemos a la zona de noche que consta de dos dormitorios dobles con armarios y el segundo baño. \xa0Ambos dormitorios dan a un tranquilo patio interior.  Este excelente piso cuenta con todas las instalaciones nuevas: fontanería, gas, electricidad, ventilación, aire acondicionado por conductos en la zona de día, splits en la zona de noche y calefacción eléctrica independiente en todas partes.  Consta con suelos y baldosas de madera nuevos, una cocina hecha a medida con electrodomésticos de marcas de alta calidad, muebles de diseño, lámparas y fotografías de lugares emblemáticos de Barcelona, como se muestra en las imágenes.  Los residentes del edificio pueden disfrutar de la terraza comunitaria con vistas al casco antiguo.  Póngase en contacto con nosotros para concertar una visita.  Características básicas:  - 102 m² construidos  - 2 dormitorios dobles  - 2 baños  - Terraza  - Armarios  Edificio  - Exterior/interior  -\xa0Construido en 1836  Equipamiento  - Aire acondicionado (conductos/splits)  - Calefacción independiente.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 6363.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99484200', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/49/bd/6f/1045894352.jpg', 'externalReference': 'BCNP4955', 'numPhotos': 30, 'price': 990000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 126.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Gòtic', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3837041, 'longitude': 2.1717083, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99484200/', 'distance': '449', 'description': 'Céntrico y alto apartamento con detalles de la época en el barrio Gótico. Los apartamentos esquineros suelen ser los más demandados en el centro de Barcelona. Esta preciosa finca con ascensor en el barrio Gótico, queda a 15 minutos caminando de Paseo de Gracia, haciendo ruta por el Portal de Ángel. Un magnífico paseo a lo largo del barrio histórico de la ciudad condal. Destaca en esta propiedad la reforma integral realizada en el año 2021 preservando el carácter modernista visto en sus suelos hidráulicos, techos altos y el detalle de dar nueva vida a la pared original de la finca del año 1900. El apartamento está distribuido en dos dormitorios dobles y dos baños. Uno de los dormitorios dispone de un walking closet que en el caso de necesidad podría hacer función de un tercer dormitorio. Amplio y luminoso salón comedor y cocina americana con cuatro balcones. Excelentes materiales y acabados. Solo disponible con Sotheby’s International Realty. El Barrio Gótico es el núcleo más antiguo de la ciudad. Está delimitado por Las Ramblas, La Vía Laietana, el Paseo Colón y la Plaza de Catalunya, cada uno de estos puntos por sí solos tiene su propia importancia e historia. De calles angostas y estructura irregular, varios de sus edificios han sido construidos sobre los restos románicos de la ciudad, así que puede hacerse con algún apartamento en el que al menos una pared date de la época romana o medieval. Es el barrio turístico por excelencia por lo que representa una inversión asegurada, sobretodo si está cerca de alguno de sus atractivos como La Catedral, la Plaza Sant Jaume con el Ayuntamiento y el Palacio de la Generalitat, la Plaza Real, Las famosas Rambas, y el Museo de Historia de la ciudad. Este podría ser su barrio si busca hacer una inversión rentable o adquirir un excelente piet-à-terre en un barrio con gran historia, edificaciones particulares, de interés turístico y con todo tipo de negocios a mano, buena gastronomía, y múltiples rincones mágicos para descubrir y recorrer.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 7857.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '99484200', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/49/bd/6f/1045894352.jpg', 'externalReference': 'BCNP4955', 'numPhotos': 30, 'price': 990000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 126.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Gòtic', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3837041, 'longitude': 2.1717083, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99484200/', 'distance': '449', 'description': 'Céntrico y alto apartamento con detalles de la época en el barrio Gótico. Los apartamentos esquineros suelen ser los más demandados en el centro de Barcelona. Esta preciosa finca con ascensor en el barrio Gótico, queda a 15 minutos caminando de Paseo de Gracia, haciendo ruta por el Portal de Ángel. Un magnífico paseo a lo largo del barrio histórico de la ciudad condal. Destaca en esta propiedad la reforma integral realizada en el año 2021 preservando el carácter modernista visto en sus suelos hidráulicos, techos altos y el detalle de dar nueva vida a la pared original de la finca del año 1900. El apartamento está distribuido en dos dormitorios dobles y dos baños. Uno de los dormitorios dispone de un walking closet que en el caso de necesidad podría hacer función de un tercer dormitorio. Amplio y luminoso salón comedor y cocina americana con cuatro balcones. Excelentes materiales y acabados. Solo disponible con Sotheby’s International Realty. El Barrio Gótico es el núcleo más antiguo de la ciudad. Está delimitado por Las Ramblas, La Vía Laietana, el Paseo Colón y la Plaza de Catalunya, cada uno de estos puntos por sí solos tiene su propia importancia e historia. De calles angostas y estructura irregular, varios de sus edificios han sido construidos sobre los restos románicos de la ciudad, así que puede hacerse con algún apartamento en el que al menos una pared date de la época romana o medieval. Es el barrio turístico por excelencia por lo que representa una inversión asegurada, sobretodo si está cerca de alguno de sus atractivos como La Catedral, la Plaza Sant Jaume con el Ayuntamiento y el Palacio de la Generalitat, la Plaza Real, Las famosas Rambas, y el Museo de Historia de la ciudad. Este podría ser su barrio si busca hacer una inversión rentable o adquirir un excelente piet-à-terre en un barrio con gran historia, edificaciones particulares, de interés turístico y con todo tipo de negocios a mano, buena gastronomía, y múltiples rincones mágicos para descubrir y recorrer.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 7857.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97472923', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/9d/de/31/980489261.jpg', 'externalReference': 'B83', 'numPhotos': 32, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 180.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3864408, 'longitude': 2.1600522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97472923/', 'distance': '816', 'description': 'Magnífico piso de lujo reformado a estrenar, con calidades muy altas y grandes espacios, pensado para personas que quieran estar en el centro de la ciudad, sin estar en zona turística. Estas son sus características principales: 2 grandes habitaciones suites. Una de las habitaciones da hacia el patio interior con armarios empotrados e iluminación y maderas nobles, también se encuentra una pequeña zona de estudio y un baño incorporado completo con ducha y sanitario. Master suite con espacio para cama king size con salida a terraza amplia una zona tranquila. Armarios empotrados. Baño completo espacioso y doble lavabo, luz natural que da hacia la terraza y armarios incorporados. Ducha amplia con sanitario separado. Cocina pequeña, pensada para uso básico y disfrutar de la zona gourmet de Barcelona. Enchufes con USB. Maderas nobles. Electrodomésticos integrados, nevera americana de alta calidad. Sistema de domótica para la iluminación. Sistema de calefacción y aire acondicionado última generación. Edificio reformado recientemente.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4711.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '97472923', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/9d/de/31/980489261.jpg', 'externalReference': 'B83', 'numPhotos': 32, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 180.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3864408, 'longitude': 2.1600522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97472923/', 'distance': '816', 'description': 'Magnífico piso de lujo reformado a estrenar, con calidades muy altas y grandes espacios, pensado para personas que quieran estar en el centro de la ciudad, sin estar en zona turística. Estas son sus características principales: 2 grandes habitaciones suites. Una de las habitaciones da hacia el patio interior con armarios empotrados e iluminación y maderas nobles, también se encuentra una pequeña zona de estudio y un baño incorporado completo con ducha y sanitario. Master suite con espacio para cama king size con salida a terraza amplia una zona tranquila. Armarios empotrados. Baño completo espacioso y doble lavabo, luz natural que da hacia la terraza y armarios incorporados. Ducha amplia con sanitario separado. Cocina pequeña, pensada para uso básico y disfrutar de la zona gourmet de Barcelona. Enchufes con USB. Maderas nobles. Electrodomésticos integrados, nevera americana de alta calidad. Sistema de domótica para la iluminación. Sistema de calefacción y aire acondicionado última generación. Edificio reformado recientemente.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4711.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99440277', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/02/5b/41/1044037924.jpg', 'externalReference': '4919', 'numPhotos': 42, 'floor': '5', 'price': 345000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 64.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Mallorca', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3831025, 'longitude': 2.1528715, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99440277/', 'distance': '1488', 'description': 'Excelente vivienda en la Nova Esquerra del Eixample reformado para entrar a vivir ¡ Luminoso y muy tranquilo orientado a patio de manzana, con amplio salón comedor, cocina equipada, 2 habitaciones (1 doble y 1 individual), baño completo con plato de ducha. climatizado mediante aire acondicionado y calefaccion de gas natural, suelos de parquet. Anteriormente distribido en cuatro habitaciones. 5ª planta con ascensor en finca del año 1.964. No cobramos honorarios al comprador. Impuestos, gastos de notaría y gestoría no incluidos en el precio de compra de la vivienda.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5391.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Mallorca'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '99440277', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/02/5b/41/1044037924.jpg', 'externalReference': '4919', 'numPhotos': 42, 'floor': '5', 'price': 345000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 64.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Mallorca', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3831025, 'longitude': 2.1528715, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99440277/', 'distance': '1488', 'description': 'Excelente vivienda en la Nova Esquerra del Eixample reformado para entrar a vivir ¡ Luminoso y muy tranquilo orientado a patio de manzana, con amplio salón comedor, cocina equipada, 2 habitaciones (1 doble y 1 individual), baño completo con plato de ducha. climatizado mediante aire acondicionado y calefaccion de gas natural, suelos de parquet. Anteriormente distribido en cuatro habitaciones. 5ª planta con ascensor en finca del año 1.964. No cobramos honorarios al comprador. Impuestos, gastos de notaría y gestoría no incluidos en el precio de compra de la vivienda.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5391.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Mallorca'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '96745288', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5f/9b/9b/955352422.jpg', 'externalReference': 'BCN23896', 'numPhotos': 42, 'price': 1200000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 187.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3849911, 'longitude': 2.1546049, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96745288/', 'distance': '1292', 'description': 'En un edificio del año 2000, en perfectas condiciones y con ascensor, encontramos este magnífico ático de 160 m², totalmente reformado, muy amplio y con mucha luz gracias a los grandes ventanales de suelo a techo que hay en prácticamente toda la vivienda.  El piso consta de un agradable salón-comedor con cocina abierta con mucha luz y bonitas vistas a la ciudad, dos dormitorios dobles, uno de ellos con vestidor y baño privado, así como un baño completo extra con zona de aguas integrada.  En la planta superior, accesible desde la escalera comunitaria, encontramos un espacio exterior de más de 150 m² escriturado junto con nuestra vivienda.  En este espacio se consolidó una construcción de 69 m² que actualmente alberga un gran salón con la cocina abierta y un baño completo. Un espacio ideal para celebrar reuniones, fiestas o simplemente relajarse. Este espacio tiene salida a una soleada terraza de más de 85 m² con zona de barbacoa y un trastero.  En el precio se incluyen dos plazas de aparcamiento de tamaño grande en la misma finca, donde pueden caber dos coches grandes y una moto.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6417.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Ático'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '96745288', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5f/9b/9b/955352422.jpg', 'externalReference': 'BCN23896', 'numPhotos': 42, 'price': 1200000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 187.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3849911, 'longitude': 2.1546049, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96745288/', 'distance': '1292', 'description': 'En un edificio del año 2000, en perfectas condiciones y con ascensor, encontramos este magnífico ático de 160 m², totalmente reformado, muy amplio y con mucha luz gracias a los grandes ventanales de suelo a techo que hay en prácticamente toda la vivienda.  El piso consta de un agradable salón-comedor con cocina abierta con mucha luz y bonitas vistas a la ciudad, dos dormitorios dobles, uno de ellos con vestidor y baño privado, así como un baño completo extra con zona de aguas integrada.  En la planta superior, accesible desde la escalera comunitaria, encontramos un espacio exterior de más de 150 m² escriturado junto con nuestra vivienda.  En este espacio se consolidó una construcción de 69 m² que actualmente alberga un gran salón con la cocina abierta y un baño completo. Un espacio ideal para celebrar reuniones, fiestas o simplemente relajarse. Este espacio tiene salida a una soleada terraza de más de 85 m² con zona de barbacoa y un trastero.  En el precio se incluyen dos plazas de aparcamiento de tamaño grande en la misma finca, donde pueden caber dos coches grandes y una moto.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6417.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Ático'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '94496557', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ae/e9/5e/890458989.jpg', 'externalReference': 'BCN28118', 'numPhotos': 36, 'floor': '6', 'price': 1500000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 139.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3901548, 'longitude': 2.1655207, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/94496557/', 'distance': '461', 'description': 'Lucas Fox presenta este piso en venta reformado a estrenar y totalmente amueblado en una ubicación Prime de Barcelona, entre Paseo de Gracia y Rambla Catalunya.  Está situado en la última planta de una finca regia del 1.890 con ascensor, que ha pasado favorablemente la Inspección Técnica de Edificios.  Todos los espacios de la vivienda son amplios y gozan de abundante entrada de luz natural. Al entrar en la vivienda, a mano izquierda encontramos la zona de día compuesta por el salón-comedor con balcón exterior a la calle y con una chimenea de bioetanol. A continuación, se dispone la elegante cocina de la firma italiana Modulnova, equipada con vinoteca y electrodomésticos de marca.  A través de un amplio pasillo con armarios empotrados, accedemos a la zona de noche compuesta por dos dormitorios dobles, uno de ellos con baño privado. Ambos dormitorios disponen de amplios armarios empotrados y salida a una terraza orientada a sureste. Esta zona se completa con un baño con ducha.  El piso está equipado por calefacción por radiadores de gas (que se puede controlar mediante Wifi), aire acondicionado por conductos con bomba para frío y calor, suelos de parqué y además dispone de un trastero en el terrado de la finca.  La reforma se ha realizada de la mano de un reconocido estudio de arquitectura de interiores, con grandes calidades y creando ambientes elegantes, cálidos y con carácter.  Póngase en contacto con nosotros para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 10791.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '94496557', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ae/e9/5e/890458989.jpg', 'externalReference': 'BCN28118', 'numPhotos': 36, 'floor': '6', 'price': 1500000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 139.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3901548, 'longitude': 2.1655207, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/94496557/', 'distance': '461', 'description': 'Lucas Fox presenta este piso en venta reformado a estrenar y totalmente amueblado en una ubicación Prime de Barcelona, entre Paseo de Gracia y Rambla Catalunya.  Está situado en la última planta de una finca regia del 1.890 con ascensor, que ha pasado favorablemente la Inspección Técnica de Edificios.  Todos los espacios de la vivienda son amplios y gozan de abundante entrada de luz natural. Al entrar en la vivienda, a mano izquierda encontramos la zona de día compuesta por el salón-comedor con balcón exterior a la calle y con una chimenea de bioetanol. A continuación, se dispone la elegante cocina de la firma italiana Modulnova, equipada con vinoteca y electrodomésticos de marca.  A través de un amplio pasillo con armarios empotrados, accedemos a la zona de noche compuesta por dos dormitorios dobles, uno de ellos con baño privado. Ambos dormitorios disponen de amplios armarios empotrados y salida a una terraza orientada a sureste. Esta zona se completa con un baño con ducha.  El piso está equipado por calefacción por radiadores de gas (que se puede controlar mediante Wifi), aire acondicionado por conductos con bomba para frío y calor, suelos de parqué y además dispone de un trastero en el terrado de la finca.  La reforma se ha realizada de la mano de un reconocido estudio de arquitectura de interiores, con grandes calidades y creando ambientes elegantes, cálidos y con carácter.  Póngase en contacto con nosotros para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 10791.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97637906', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/77/0d/ef/985947670.jpg', 'externalReference': '4392', 'numPhotos': 71, 'floor': 'en', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 190.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3860408, 'longitude': 2.1633522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97637906/', 'distance': '556', 'description': 'Viviendas de Lujo en Ensanche Izquierdo. Viviendas a estrenar en exclusiva finca clásica. Situada en el Ensanche Izquierdo, está ubicada en la calle Diputación cerca de Plaza Universidad y a escasos minutos de la Rambla de Catalunya y el Paseo de Gracia. Terraza privada de 41m2. Ademas podrá disfrutar de una gran terraza comunitaria, un espacio de 60 m² con zona “chill out” y unas preciosas vistas de Barcelona. Exclusiva finca con sólo 4 vecinos, ha sido totalmente rehabilitada teniendo todas las zonas comunes, ascensor y terrado nuevos. El proyecto de esta fantástica vivienda ha sido realizado por Jaime Beriestain Studio, se han utilizado los mejores materiales con un diseño muy elegante creando espacios actuales y acogedores. Vivienda de alto standing con todo tipo de detalles, distribuida en:  - Recibidor. - Salón de unos 26m2 independiente y exterior a la calle. - Cocina independiente cerrada con puertas correderas, lo que nos facilita la sensación de cocina abierta. - Zona de lavado. - Aseo de cortesía. - Zona de noche con dos dormitorios ambos dobles y en suite, uno de ellos de 13m2 con armarios empotrados, estudio y con un baño de 8m2 con plato de ducha. El dormitorio principal tiene una superficie de 25m2, consta de vestidor y de un baño de 13m2 con plato de ducha y bañera, también tiene acceso a la terraza de 42m2. Zona comercial con todo tipo de servicios y muy bien comunicada con transporte público. Oportunidad inmejorable para adquirir una vivienda a estrenar en el corazón de Barcelona. Disponemos de más pisos a la venta en la misma finca: 1° de 130m2 a 768.000€  2° de 130m2 a 816.000€  Local de 165m2 a 576.000€ Posibilidad de comprar edificio completo. Aincasa Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4463.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '97637906', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/77/0d/ef/985947670.jpg', 'externalReference': '4392', 'numPhotos': 71, 'floor': 'en', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 190.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3860408, 'longitude': 2.1633522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97637906/', 'distance': '556', 'description': 'Viviendas de Lujo en Ensanche Izquierdo. Viviendas a estrenar en exclusiva finca clásica. Situada en el Ensanche Izquierdo, está ubicada en la calle Diputación cerca de Plaza Universidad y a escasos minutos de la Rambla de Catalunya y el Paseo de Gracia. Terraza privada de 41m2. Ademas podrá disfrutar de una gran terraza comunitaria, un espacio de 60 m² con zona “chill out” y unas preciosas vistas de Barcelona. Exclusiva finca con sólo 4 vecinos, ha sido totalmente rehabilitada teniendo todas las zonas comunes, ascensor y terrado nuevos. El proyecto de esta fantástica vivienda ha sido realizado por Jaime Beriestain Studio, se han utilizado los mejores materiales con un diseño muy elegante creando espacios actuales y acogedores. Vivienda de alto standing con todo tipo de detalles, distribuida en:  - Recibidor. - Salón de unos 26m2 independiente y exterior a la calle. - Cocina independiente cerrada con puertas correderas, lo que nos facilita la sensación de cocina abierta. - Zona de lavado. - Aseo de cortesía. - Zona de noche con dos dormitorios ambos dobles y en suite, uno de ellos de 13m2 con armarios empotrados, estudio y con un baño de 8m2 con plato de ducha. El dormitorio principal tiene una superficie de 25m2, consta de vestidor y de un baño de 13m2 con plato de ducha y bañera, también tiene acceso a la terraza de 42m2. Zona comercial con todo tipo de servicios y muy bien comunicada con transporte público. Oportunidad inmejorable para adquirir una vivienda a estrenar en el corazón de Barcelona. Disponemos de más pisos a la venta en la misma finca: 1° de 130m2 a 768.000€  2° de 130m2 a 816.000€  Local de 165m2 a 576.000€ Posibilidad de comprar edificio completo. Aincasa Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4463.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99794526', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/14/7c/63/1054779399.jpg', 'externalReference': '2809', 'numPhotos': 26, 'floor': '2', 'price': 490000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 71.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de París', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3887258, 'longitude': 2.1473163, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99794526/', 'distance': '1876', 'description': 'Vivienda de 71m2 en edificio de 2011. En excelente estado, exterior y funcional. Salón comedor esquinero, dos habitaciones dobles. Cocina americana equipada. Un baño completo. Armarios empotrados. Calefacción y aire acondicionado por conductos. Excelentes cerramientos Technal con doble cristal. Persianas mecanizadas. Terraza comunitaria en la cubierta del edificio. Plaza de garaje grande y trastero de 14m2. Garaje con vigilancia 24 horas. Dos ascensores. Gastos e impuestos no incluidos en el precio del anuncio.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': True}, 'priceByArea': 6901.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de París'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '99794526', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/14/7c/63/1054779399.jpg', 'externalReference': '2809', 'numPhotos': 26, 'floor': '2', 'price': 490000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 71.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de París', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3887258, 'longitude': 2.1473163, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99794526/', 'distance': '1876', 'description': 'Vivienda de 71m2 en edificio de 2011. En excelente estado, exterior y funcional. Salón comedor esquinero, dos habitaciones dobles. Cocina americana equipada. Un baño completo. Armarios empotrados. Calefacción y aire acondicionado por conductos. Excelentes cerramientos Technal con doble cristal. Persianas mecanizadas. Terraza comunitaria en la cubierta del edificio. Plaza de garaje grande y trastero de 14m2. Garaje con vigilancia 24 horas. Dos ascensores. Gastos e impuestos no incluidos en el precio del anuncio.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': True}, 'priceByArea': 6901.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de París'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97534780', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/3e/ee/b3/982449385.jpg', 'externalReference': 'BCN-Carrera Bajos2', 'numPhotos': 31, 'floor': 'bj', 'price': 510000.0, 'propertyType': 'duplex', 'operation': 'sale', 'size': 86.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Carrera', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'El Poble Sec - Parc de Montjuïc', 'latitude': 41.372431, 'longitude': 2.1760547, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97534780/', 'distance': '1753', 'description': 'Fabulosa planta baja dúplex de 86 m2, muy luminosa, con soleado patio de 59m2. La vivienda se distribuye en planta baja (recibidor, aseo de cortesía, cocina abierta, salón comedor con salida al patio de 59m2) y planta piso (2 habitaciones a patio de manzana y 2 baños). Finca con ascensor y con una ubicación privilegiada. Disponemos de plazas de parking en la misma finca, así como otros pisos en diferentes alturas. Nuestras viviendas se encuentran en la calle Carrera, justo delante de los Jardines de Walter Benjamin y la Plaça de les Drassanes, frente al Puerto de Barcelona. Justo al lado de la famosa Avda del Paral. lel con sus teatros y todo tipo de comercios. A un paso del Mirador del Poble Sec, disfrute de los paseos por Montjuïc y por sus amplias zonas ajardinadas ideales para hacer deporte al aire libre. Aproveche el buen clima de nuestra ciudad en las playas de alrededor. Muy bien comunicado con toda la ciudad con Lineas de Metro y autobuses. deportes al aire libre. Aproveche el buen clima de nuestra ciudad en las playas de alrededor. Muy bien comunicado con toda la ciudad con Líneas de Metro y autobuses.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': True}, 'priceByArea': 5930.0, 'detailedType': {'typology': 'flat', 'subTypology': 'duplex'}, 'suggestedTexts': {'subtitle': 'El Poble Sec - Parc de Montjuïc, Barcelona', 'title': 'Dúplex en Carrera'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '97534780', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/3e/ee/b3/982449385.jpg', 'externalReference': 'BCN-Carrera Bajos2', 'numPhotos': 31, 'floor': 'bj', 'price': 510000.0, 'propertyType': 'duplex', 'operation': 'sale', 'size': 86.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Carrera', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'El Poble Sec - Parc de Montjuïc', 'latitude': 41.372431, 'longitude': 2.1760547, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97534780/', 'distance': '1753', 'description': 'Fabulosa planta baja dúplex de 86 m2, muy luminosa, con soleado patio de 59m2. La vivienda se distribuye en planta baja (recibidor, aseo de cortesía, cocina abierta, salón comedor con salida al patio de 59m2) y planta piso (2 habitaciones a patio de manzana y 2 baños). Finca con ascensor y con una ubicación privilegiada. Disponemos de plazas de parking en la misma finca, así como otros pisos en diferentes alturas. Nuestras viviendas se encuentran en la calle Carrera, justo delante de los Jardines de Walter Benjamin y la Plaça de les Drassanes, frente al Puerto de Barcelona. Justo al lado de la famosa Avda del Paral. lel con sus teatros y todo tipo de comercios. A un paso del Mirador del Poble Sec, disfrute de los paseos por Montjuïc y por sus amplias zonas ajardinadas ideales para hacer deporte al aire libre. Aproveche el buen clima de nuestra ciudad en las playas de alrededor. Muy bien comunicado con toda la ciudad con Lineas de Metro y autobuses. deportes al aire libre. Aproveche el buen clima de nuestra ciudad en las playas de alrededor. Muy bien comunicado con toda la ciudad con Líneas de Metro y autobuses.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': True}, 'priceByArea': 5930.0, 'detailedType': {'typology': 'flat', 'subTypology': 'duplex'}, 'suggestedTexts': {'subtitle': 'El Poble Sec - Parc de Montjuïc, Barcelona', 'title': 'Dúplex en Carrera'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99348106', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a6/63/11/962649051.jpg', 'externalReference': 'B34', 'numPhotos': 23, 'floor': '2', 'price': 579000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 70.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de París', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3899266, 'longitude': 2.1499647, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99348106/', 'distance': '1672', 'description': 'Un piso único con bóveda catalana 70 m2 1 dormitorio doble en suite con baño abierto con ducha, con armario grande 1 dormitorio individual con sofa-cama y armario 1 sala de estar Cocina con comedor, con isla, totalmente equipada (lavadora, lavaplatos, placa de inducción, campana, nevera, horno, tostadora, hervidor…) 1 baño separado con una bañera y WC  1 Balcón Aire acondicionado split (frio/calor) Caldera de gas nueva Hay plancha, aspiradora, secador de pelo Parquet de madera buena calidad, gres en la cocina Orientación Sur.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8271.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de París'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '99348106', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a6/63/11/962649051.jpg', 'externalReference': 'B34', 'numPhotos': 23, 'floor': '2', 'price': 579000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 70.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de París', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3899266, 'longitude': 2.1499647, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99348106/', 'distance': '1672', 'description': 'Un piso único con bóveda catalana 70 m2 1 dormitorio doble en suite con baño abierto con ducha, con armario grande 1 dormitorio individual con sofa-cama y armario 1 sala de estar Cocina con comedor, con isla, totalmente equipada (lavadora, lavaplatos, placa de inducción, campana, nevera, horno, tostadora, hervidor…) 1 baño separado con una bañera y WC  1 Balcón Aire acondicionado split (frio/calor) Caldera de gas nueva Hay plancha, aspiradora, secador de pelo Parquet de madera buena calidad, gres en la cocina Orientación Sur.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8271.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de París'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '91626925', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8c/85/9a/958647886.jpg', 'externalReference': 'V2084-R', 'numPhotos': 28, 'floor': '3', 'price': 256000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 67.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Princesa', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3879197, 'longitude': 2.1811329, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/91626925/', 'distance': '951', 'description': 'Vivienda de 67 m2 con doble orientación a calle Princesa y Assaonadors, con sol todo el día, que ocupa la tercera planta de un edificio de 1880, sin ascensor.   Distribuye 2 dormitorios, uno doble con balcón a calle Princesa y otro individual (habitación ciega), vestidor, baño completo con bañera, cocina abierta al comedor y salón.   Ventilación cruzada, cerramientos de aluminio, suelos de parquet laminado y de gres en baño, climatización en la estancia con más incidencia solar. El dormitorio individual y vestidor ventilan al actual dormitorio doble.  La distribución actual puede modificarse cambiando el dormitorio doble por el salón, sin obras. No hay posibilidad de instalar ascensor en la finca.   El Born, con comercio de proximidad y servicios, pero también una amplia oferta gastronómica y un envidiable entorno histórico de la evolución de la ciudad.   Los honorarios son a cargo del vendedor. El precio no incluye los impuestos, ni gastos de notaría ni de gestoría de la compraventa.  Eurofincas International Real Estate | Referencia V2084.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 3821.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso en Princesa'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '91626925', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8c/85/9a/958647886.jpg', 'externalReference': 'V2084-R', 'numPhotos': 28, 'floor': '3', 'price': 256000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 67.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Princesa', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3879197, 'longitude': 2.1811329, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/91626925/', 'distance': '951', 'description': 'Vivienda de 67 m2 con doble orientación a calle Princesa y Assaonadors, con sol todo el día, que ocupa la tercera planta de un edificio de 1880, sin ascensor.   Distribuye 2 dormitorios, uno doble con balcón a calle Princesa y otro individual (habitación ciega), vestidor, baño completo con bañera, cocina abierta al comedor y salón.   Ventilación cruzada, cerramientos de aluminio, suelos de parquet laminado y de gres en baño, climatización en la estancia con más incidencia solar. El dormitorio individual y vestidor ventilan al actual dormitorio doble.  La distribución actual puede modificarse cambiando el dormitorio doble por el salón, sin obras. No hay posibilidad de instalar ascensor en la finca.   El Born, con comercio de proximidad y servicios, pero también una amplia oferta gastronómica y un envidiable entorno histórico de la evolución de la ciudad.   Los honorarios son a cargo del vendedor. El precio no incluye los impuestos, ni gastos de notaría ni de gestoría de la compraventa.  Eurofincas International Real Estate | Referencia V2084.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 3821.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso en Princesa'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98124798', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/45/91/16/1001891426.jpg', 'externalReference': '4400', 'numPhotos': 37, 'floor': 'bj', 'price': 350000.0, 'propertyType': 'duplex', 'operation': 'sale', 'size': 147.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle de l'Olivera", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'El Poble Sec - Parc de Montjuïc', 'latitude': 41.3715925, 'longitude': 2.1592743, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98124798/', 'distance': '1969', 'description': 'Planta baja reformada con mucho encanto. En una calle muy tranquila junto a la Plaza de Santa Madrona encontramos esta planta baja con mucho encanto. Se accede al interior por una entrada independiente, encontramos una vez en su interior a un amplio espacio para poder guardar bicicletas así como espacio polivalente para almacenaje, a continuación accedemos a un amplio comedor con cocina abierta, desde ahí podemos acceder a la planta altillo mediante unas escaleras de hierro forjado incrustadas en la pared de piedra natural o al fondo del comedor un pasillo nos daría paso a u baño con ducha seguido de un agradable patio con luz natural seguido de un cuarto de máquinas y al final un amplio espacio que hace de sala y zona polivalente con salida a una pequeña terraza con mucha luminosidad. destacar el microclima que se respira y el silencio que se respira. ! Si lo que realmente buscas es luz y tranquilidad dejaras de seguir buscando ¡ En la planta duplex o altillo encontramos un amplio espacio con zona de armarios actualmente la propiedad lo utiliza como una zona de trabajo con la posibilidad de poder hacer otro dormitorio con otro baño (preparado para ejecutar la obra, se puede ver en el plano adjunto, al fondo un pequeño pasillo nos daría paso a un segundo dormitorio con zona de vestidor con posibilidad de hacer otro baño (preparado para ejecutar la obra, se puede ver en el plano adjunto). Dispone de calefacción de gas, ventilador de techo, cocina equipada con electrodomésticos. Aincasa Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 2381.0, 'detailedType': {'typology': 'flat', 'subTypology': 'duplex'}, 'suggestedTexts': {'subtitle': 'El Poble Sec - Parc de Montjuïc, Barcelona', 'title': "Dúplex en Calle de l'Olivera"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98124798', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/45/91/16/1001891426.jpg', 'externalReference': '4400', 'numPhotos': 37, 'floor': 'bj', 'price': 350000.0, 'propertyType': 'duplex', 'operation': 'sale', 'size': 147.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle de l'Olivera", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'El Poble Sec - Parc de Montjuïc', 'latitude': 41.3715925, 'longitude': 2.1592743, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98124798/', 'distance': '1969', 'description': 'Planta baja reformada con mucho encanto. En una calle muy tranquila junto a la Plaza de Santa Madrona encontramos esta planta baja con mucho encanto. Se accede al interior por una entrada independiente, encontramos una vez en su interior a un amplio espacio para poder guardar bicicletas así como espacio polivalente para almacenaje, a continuación accedemos a un amplio comedor con cocina abierta, desde ahí podemos acceder a la planta altillo mediante unas escaleras de hierro forjado incrustadas en la pared de piedra natural o al fondo del comedor un pasillo nos daría paso a u baño con ducha seguido de un agradable patio con luz natural seguido de un cuarto de máquinas y al final un amplio espacio que hace de sala y zona polivalente con salida a una pequeña terraza con mucha luminosidad. destacar el microclima que se respira y el silencio que se respira. ! Si lo que realmente buscas es luz y tranquilidad dejaras de seguir buscando ¡ En la planta duplex o altillo encontramos un amplio espacio con zona de armarios actualmente la propiedad lo utiliza como una zona de trabajo con la posibilidad de poder hacer otro dormitorio con otro baño (preparado para ejecutar la obra, se puede ver en el plano adjunto, al fondo un pequeño pasillo nos daría paso a un segundo dormitorio con zona de vestidor con posibilidad de hacer otro baño (preparado para ejecutar la obra, se puede ver en el plano adjunto). Dispone de calefacción de gas, ventilador de techo, cocina equipada con electrodomésticos. Aincasa Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 2381.0, 'detailedType': {'typology': 'flat', 'subTypology': 'duplex'}, 'suggestedTexts': {'subtitle': 'El Poble Sec - Parc de Montjuïc, Barcelona', 'title': "Dúplex en Calle de l'Olivera"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AM5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97501131', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/6b/f9/3d/981296577.jpg', 'externalReference': 'V220429', 'numPhotos': 20, 'floor': '1', 'price': 384000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 78.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle Balmes', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3925976, 'longitude': 2.1616804, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97501131/', 'distance': '881', 'description': 'Cafur les presenta, en la céntrica calle Balmes, en el corazón de la Barcelona tradicional, esta maravillosa propiedad en finca regia del año 1909 con ascensor. La vivienda, que destaca por la altura de los techos, la sensación de confort y la luminosidad da al patio de manzana, por lo que no tendrás que sufrir por los ruidos del tráfico rodado. Cuenta con la siguiente distribución: amplio y luminoso salón comedor gracias a su conexión con la galería, ideal para poner una zona de lectura o un pequeño estudio; cocina independiente para actualizar; 2 dormitorios; 1 baño completo de tres piezas con bañera; y pasillo distribuidor. Está ubicado a sólo unos metros de la emblemática Rambla Catalunya y Passeig de Gràcia, donde encontrarás tiendas de primeras marcas. Además estarás rodeado de todos los servicios que puedas necesitar y de una amplia red de transporte público.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4923.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle Balmes'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '97501131', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/6b/f9/3d/981296577.jpg', 'externalReference': 'V220429', 'numPhotos': 20, 'floor': '1', 'price': 384000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 78.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle Balmes', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3925976, 'longitude': 2.1616804, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97501131/', 'distance': '881', 'description': 'Cafur les presenta, en la céntrica calle Balmes, en el corazón de la Barcelona tradicional, esta maravillosa propiedad en finca regia del año 1909 con ascensor. La vivienda, que destaca por la altura de los techos, la sensación de confort y la luminosidad da al patio de manzana, por lo que no tendrás que sufrir por los ruidos del tráfico rodado. Cuenta con la siguiente distribución: amplio y luminoso salón comedor gracias a su conexión con la galería, ideal para poner una zona de lectura o un pequeño estudio; cocina independiente para actualizar; 2 dormitorios; 1 baño completo de tres piezas con bañera; y pasillo distribuidor. Está ubicado a sólo unos metros de la emblemática Rambla Catalunya y Passeig de Gràcia, donde encontrarás tiendas de primeras marcas. Además estarás rodeado de todos los servicios que puedas necesitar y de una amplia red de transporte público.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4923.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle Balmes'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AN5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '96967469', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/21/cc/9b/961770545.jpg', 'externalReference': '4382', 'numPhotos': 39, 'floor': 'bj', 'price': 249000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 80.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de Sant Antoni Abat', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3780021, 'longitude': 2.1625679, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96967469/', 'distance': '1211', 'description': 'A escasos metros del Mercado de Sant Antoni y Ronda Sant Antoni. Reforma de Lujo. Planta baja reformada integralmente, paredes recuperadas de piedra, techos altos con bóveda catalana y vigas de madera, en el acceso nos encontramos con una doble entrada con pared de piedra ideal par dejar bicicleta o moto protegidas. Al acceder al interior tenemos un amplio salón-comedor, cocina independiente totalmente equipada, dos dormitorios dobles, ambos con baño en suite mas un tercer baño con ducha, el dormitorio principal tiene salida a un patio por el que entra luz natural. Dispone de aire acondicionado con bomba de calor. Con mucho encanto, reforma cuidada hasta el ultimo detalle. En los gastos de comunidad está incluido el suministro del agua. Zona con todo tipo de servicios, comercios y restaurantes, a 200 metros del Mercado de Sant Antoni. El precio no incluye los impuestos, ni los gastos de Notaria, Registro y Gestoría. Aincasa Aicat número 2677. Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 3113.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de Sant Antoni Abat'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '96967469', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/21/cc/9b/961770545.jpg', 'externalReference': '4382', 'numPhotos': 39, 'floor': 'bj', 'price': 249000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 80.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de Sant Antoni Abat', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3780021, 'longitude': 2.1625679, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96967469/', 'distance': '1211', 'description': 'A escasos metros del Mercado de Sant Antoni y Ronda Sant Antoni. Reforma de Lujo. Planta baja reformada integralmente, paredes recuperadas de piedra, techos altos con bóveda catalana y vigas de madera, en el acceso nos encontramos con una doble entrada con pared de piedra ideal par dejar bicicleta o moto protegidas. Al acceder al interior tenemos un amplio salón-comedor, cocina independiente totalmente equipada, dos dormitorios dobles, ambos con baño en suite mas un tercer baño con ducha, el dormitorio principal tiene salida a un patio por el que entra luz natural. Dispone de aire acondicionado con bomba de calor. Con mucho encanto, reforma cuidada hasta el ultimo detalle. En los gastos de comunidad está incluido el suministro del agua. Zona con todo tipo de servicios, comercios y restaurantes, a 200 metros del Mercado de Sant Antoni. El precio no incluye los impuestos, ni los gastos de Notaria, Registro y Gestoría. Aincasa Aicat número 2677. Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 3113.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de Sant Antoni Abat'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AO5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '94041284', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/cd/c0/bb/888738711.jpg', 'externalReference': '4340', 'numPhotos': 27, 'floor': '4', 'price': 360000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle de l'Oli", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3833513, 'longitude': 2.1766716, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/94041284/', 'distance': '737', 'description': "A escasos metros de La Catedral de Barcelona y Mercado de Santa Caterina. En el Barrio de La Ribera- Borne se encuentra esta fabulosa vivienda, con mucho encanto, al acceder a la vivienda dos zonas dividen la zona de día y de noche, en la zona de día encontramos un amplio salón-comedor con luz a raudales y bonitas vistas a terrazas ajardinadas, la cocina comunica con una ventana que permite el paso con el comedor para compartir momentos con familia y amigos, en frente se encuentra el baño con ducha, un amplio pasillo nos da paso a los dormitorios (2) dobles y muy soleados, el dormitorio principal tiene salida a un pequeño balcón con vistas a la misma calle de L'Oli, destacar los detalles como las vigas vistas, la contraventanas tienen aislamiento térmico con poco uso, calefacción. La finca dispone de ascensor, se accede subiendo un tramo de escaleras. El edificio cuenta con dos terrazas de uso comunitario con unas vistas únicas para poder disfrutar de las puestas de sol, en el terrado también se encuentra un amplio trastero para uso comunitario. El Born es un barrio a la última caracterizado por sus callejas medievales. De día, es posible disfrutar de cafeterías y boutiques de diseñadores, mientras que las coctelerías y la samba protagonizan sus noches. La basílica de Santa María del Mar exhibe ornamentales vidrieras. En el famoso museo Picasso se exponen muchas de las obras maestras del artista. El Born Centre de Cultura i Memoria es un centro polivalente que ocupa el edificio de un antiguo mercado y conserva en su interior un yacimiento arqueológico. El Born se encuentra entre la Via Laietana y la Barceloneta y tiene un buen servicio de transporte, con las paradas del metro Barceloneta y Jaume 1 en la misma línea. No obstante, a Las Ramblas y al centro de la ciudad puedes llegar caminando en sólo 10 minutos. La playa también está a unos 10 minutos caminando, lo que significa que podrás disfrutar de unas vacaciones en la playa y descansar de la ciudad al mismo tiempo. Además, el Born está bastante cerca del Parque de la Ciutadella: un pulmón de la ciudad condal, un lugar tranquilo para relajarte y pasear. Aincasa Un sueño una realidad.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4337.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': "Piso en Calle de l'Oli"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '94041284', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/cd/c0/bb/888738711.jpg', 'externalReference': '4340', 'numPhotos': 27, 'floor': '4', 'price': 360000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle de l'Oli", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3833513, 'longitude': 2.1766716, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/94041284/', 'distance': '737', 'description': "A escasos metros de La Catedral de Barcelona y Mercado de Santa Caterina. En el Barrio de La Ribera- Borne se encuentra esta fabulosa vivienda, con mucho encanto, al acceder a la vivienda dos zonas dividen la zona de día y de noche, en la zona de día encontramos un amplio salón-comedor con luz a raudales y bonitas vistas a terrazas ajardinadas, la cocina comunica con una ventana que permite el paso con el comedor para compartir momentos con familia y amigos, en frente se encuentra el baño con ducha, un amplio pasillo nos da paso a los dormitorios (2) dobles y muy soleados, el dormitorio principal tiene salida a un pequeño balcón con vistas a la misma calle de L'Oli, destacar los detalles como las vigas vistas, la contraventanas tienen aislamiento térmico con poco uso, calefacción. La finca dispone de ascensor, se accede subiendo un tramo de escaleras. El edificio cuenta con dos terrazas de uso comunitario con unas vistas únicas para poder disfrutar de las puestas de sol, en el terrado también se encuentra un amplio trastero para uso comunitario. El Born es un barrio a la última caracterizado por sus callejas medievales. De día, es posible disfrutar de cafeterías y boutiques de diseñadores, mientras que las coctelerías y la samba protagonizan sus noches. La basílica de Santa María del Mar exhibe ornamentales vidrieras. En el famoso museo Picasso se exponen muchas de las obras maestras del artista. El Born Centre de Cultura i Memoria es un centro polivalente que ocupa el edificio de un antiguo mercado y conserva en su interior un yacimiento arqueológico. El Born se encuentra entre la Via Laietana y la Barceloneta y tiene un buen servicio de transporte, con las paradas del metro Barceloneta y Jaume 1 en la misma línea. No obstante, a Las Ramblas y al centro de la ciudad puedes llegar caminando en sólo 10 minutos. La playa también está a unos 10 minutos caminando, lo que significa que podrás disfrutar de unas vacaciones en la playa y descansar de la ciudad al mismo tiempo. Además, el Born está bastante cerca del Parque de la Ciutadella: un pulmón de la ciudad condal, un lugar tranquilo para relajarte y pasear. Aincasa Un sueño una realidad.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4337.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': "Piso en Calle de l'Oli"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AP5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98793896', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ce/23/f6/1024006628.jpg', 'externalReference': '11650', 'numPhotos': 28, 'floor': '3', 'price': 574000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 86.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio Vila de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'Vila de Gràcia', 'latitude': 41.4110641, 'longitude': 2.1580262, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98793896/', 'distance': '2799', 'description': "Situado en una finca moderna, nos encontramos con este coqueto y acogedor ático dúplex de 86\u202fm construidos más 20\u202fm de trza. Con vistas totalmente despejadas al Icónico Tenis, la Salut y al Tibidabo, muy luminoso y con sol de tarde. La vivienda está muy bien conservado. Se distribuye en un amplio y agradable salón comedor con vistas al tenis, y con cocina americana, práctica y funcional, totalmente equipada y amueblada. En esta planta también nos encontramos con una habitación individual exterior al tenis. Un baño completo con ducha y un armario amplio que nos puede hacer la función de trastero. Accedemos a la primera planta a través de una amplia y cómoda escalera que nos da paso, a la Suite, con un espacioso baño. Y a la agradable terraza. Dicha terraza nos induce a disfrutarla durante el día, al sol para, relajarse, leer o hacer actividades, y a sus atardeceres que se prestan a tomar una copa con la tranquilidad y la calma. Al igual que al anochecer que nos invita al disfrute de cenas y veladas bajo las estrellas y a la luz de la luna. Rodeada de plantas y flores que nos pueden transportar a un pequeño Edén, en la ciudad. Observaciones: plaza de parking opcional por 25.000, calefacción a gas, aire centralizado, armarios empotrados. Suelos de parquet, etc. En definitiva, una excelente calidad de vida. Gracia es un barrio informal con calles estrechas y plazas acogedoras lleno de tiendas de comestibles ecológicos, espacios de trabajo compartido modernos y estudios de artistas. La zona está muy bien comunicada a todos los niveles. Pocos distritos de Barcelona están rodeados de tanta simbología como el de Gràcia. El casco antiguo del barrio que le da nombre no ha dejado nunca de reivindicar con orgullo su pasado como municipio independiente (se agregó a la ciudad en 1897) La urbanización del barrio de la Salut-Gracia Nova, comenzó, en la segunda mitad del siglo XIX, alrededor de la iglesia, que tomo el nombre de Nuestra Señora de la Salut cuyas inmediaciones creció el barrio a lo largo de los años. En sus inicios la actividad más importante de la zona era agrícola, hallándose importantes masías como Can Xipreret, Can Tusquets, Can Muntaner y Ca l'Alegre de Dalt, pero progresivamente fueron convirtiéndose en zona residencial de veraneo de la burguesía barcelonesa y de la antigua villa de Gracia. También se halla en el barrio el reconocidísimo tenis la Salut, la entidad fue constituida como Salud Sport Club el 8 de junio de 1902, por un grupo de deportistas a partir del Club Social La Salud, fundado en 1899. Eusebio Güell, conde de Güell, fue nombrado presidente honorífico. Para construir sus instalaciones lograron unos terrenos de la masía de Can Xipreret. En el ámbito de la raqueta, destaca la creación de la primera escuela de tenis de España, en 1959. En ella se han formado algunos de los principales tenistas españoles de la historia como Manuel Orantes, Beto Martín, Conchita Martínez o Àlex Corretja. La Salut es el único club del mundo con dos campeones de la Copa Másters de Tenis, los citados Orantes y Corretja.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': False, 'parkingSpacePrice': 25000.0}, 'priceByArea': 6674.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': 'Vila de Gràcia, Barcelona', 'title': 'Ático'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98793896', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ce/23/f6/1024006628.jpg', 'externalReference': '11650', 'numPhotos': 28, 'floor': '3', 'price': 574000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 86.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio Vila de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'Vila de Gràcia', 'latitude': 41.4110641, 'longitude': 2.1580262, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98793896/', 'distance': '2799', 'description': "Situado en una finca moderna, nos encontramos con este coqueto y acogedor ático dúplex de 86\u202fm construidos más 20\u202fm de trza. Con vistas totalmente despejadas al Icónico Tenis, la Salut y al Tibidabo, muy luminoso y con sol de tarde. La vivienda está muy bien conservado. Se distribuye en un amplio y agradable salón comedor con vistas al tenis, y con cocina americana, práctica y funcional, totalmente equipada y amueblada. En esta planta también nos encontramos con una habitación individual exterior al tenis. Un baño completo con ducha y un armario amplio que nos puede hacer la función de trastero. Accedemos a la primera planta a través de una amplia y cómoda escalera que nos da paso, a la Suite, con un espacioso baño. Y a la agradable terraza. Dicha terraza nos induce a disfrutarla durante el día, al sol para, relajarse, leer o hacer actividades, y a sus atardeceres que se prestan a tomar una copa con la tranquilidad y la calma. Al igual que al anochecer que nos invita al disfrute de cenas y veladas bajo las estrellas y a la luz de la luna. Rodeada de plantas y flores que nos pueden transportar a un pequeño Edén, en la ciudad. Observaciones: plaza de parking opcional por 25.000, calefacción a gas, aire centralizado, armarios empotrados. Suelos de parquet, etc. En definitiva, una excelente calidad de vida. Gracia es un barrio informal con calles estrechas y plazas acogedoras lleno de tiendas de comestibles ecológicos, espacios de trabajo compartido modernos y estudios de artistas. La zona está muy bien comunicada a todos los niveles. Pocos distritos de Barcelona están rodeados de tanta simbología como el de Gràcia. El casco antiguo del barrio que le da nombre no ha dejado nunca de reivindicar con orgullo su pasado como municipio independiente (se agregó a la ciudad en 1897) La urbanización del barrio de la Salut-Gracia Nova, comenzó, en la segunda mitad del siglo XIX, alrededor de la iglesia, que tomo el nombre de Nuestra Señora de la Salut cuyas inmediaciones creció el barrio a lo largo de los años. En sus inicios la actividad más importante de la zona era agrícola, hallándose importantes masías como Can Xipreret, Can Tusquets, Can Muntaner y Ca l'Alegre de Dalt, pero progresivamente fueron convirtiéndose en zona residencial de veraneo de la burguesía barcelonesa y de la antigua villa de Gracia. También se halla en el barrio el reconocidísimo tenis la Salut, la entidad fue constituida como Salud Sport Club el 8 de junio de 1902, por un grupo de deportistas a partir del Club Social La Salud, fundado en 1899. Eusebio Güell, conde de Güell, fue nombrado presidente honorífico. Para construir sus instalaciones lograron unos terrenos de la masía de Can Xipreret. En el ámbito de la raqueta, destaca la creación de la primera escuela de tenis de España, en 1959. En ella se han formado algunos de los principales tenistas españoles de la historia como Manuel Orantes, Beto Martín, Conchita Martínez o Àlex Corretja. La Salut es el único club del mundo con dos campeones de la Copa Másters de Tenis, los citados Orantes y Corretja.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': False, 'parkingSpacePrice': 25000.0}, 'priceByArea': 6674.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': 'Vila de Gràcia, Barcelona', 'title': 'Ático'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AQ5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98508998', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/19/98/bb/1014756994.jpg', 'externalReference': '4740X', 'numPhotos': 17, 'floor': '5', 'price': 385000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle del Rosselló', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3858287, 'longitude': 2.148551, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98508998/', 'distance': '1777', 'description': "Este piso se encuentra en la zona del La Nova Esquerra de l'Eixample, en la quinta planta.  En el área hay todo tipo de servicios como ocio y restauración, colegios, sanidad, transporte público, etc.  La vivienda tiene dos dormitorios, uno de ellos es doble exterior y el otro es individual con ventana a un patio interior.  Tiene un baño en perfecto estado que es completo con ducha y se ubica en el centro del piso. El piso tiene un amplio y luminosos salón, estilo diáfano, con dos ambientes comunicados para el comedor y otro para el salón. En el mismo hay una salida directa a un perfecto balcón.  La cocina es estilo americana y se encuentra en perfecto estado. Para más información o programar una visita pueden dejar un WhatsApp en el 681 38 77 03 Encuentra más en.", 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4639.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle del Rosselló'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98508998', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/19/98/bb/1014756994.jpg', 'externalReference': '4740X', 'numPhotos': 17, 'floor': '5', 'price': 385000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle del Rosselló', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3858287, 'longitude': 2.148551, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98508998/', 'distance': '1777', 'description': "Este piso se encuentra en la zona del La Nova Esquerra de l'Eixample, en la quinta planta.  En el área hay todo tipo de servicios como ocio y restauración, colegios, sanidad, transporte público, etc.  La vivienda tiene dos dormitorios, uno de ellos es doble exterior y el otro es individual con ventana a un patio interior.  Tiene un baño en perfecto estado que es completo con ducha y se ubica en el centro del piso. El piso tiene un amplio y luminosos salón, estilo diáfano, con dos ambientes comunicados para el comedor y otro para el salón. En el mismo hay una salida directa a un perfecto balcón.  La cocina es estilo americana y se encuentra en perfecto estado. Para más información o programar una visita pueden dejar un WhatsApp en el 681 38 77 03 Encuentra más en.", 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4639.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle del Rosselló'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AR5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98145102', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/94/3e/d6/1002492446.jpg', 'externalReference': '101217', 'numPhotos': 35, 'floor': 'en', 'price': 420000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 101.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Sant Pau', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3776106, 'longitude': 2.172716, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98145102/', 'distance': '1124', 'description': 'PISAZO DE 100M2 + 58M2 DE TERRAZA, EN FINCA DEL AÑO 1850 COMPLETAMENTE REHABILITADA. La propiedad en venta actualmente está dividida físicamente (no segregada) en dos apartamentos completos e independientes, que comparten luz, agua y gas. Cada apartamento tiene su propio acceso independiente con llave, y constan de un dormitorio doble, cocina totalmente equipada, sala de estar/comedor y baño completo. La vivienda está situada en la amplia plaza Salvador Seguí, delante de la Filmoteca, en el Raval, a tres minutos de les Ramblas. La finca es del año 1850, ha sido completamente rehabilitada, cuenta con cámaras de seguridad en la entrada y en cada rellano, tiene la ITE pasada con su correspondiente Certificado de Aptitud del año 2020, y no tiene derramas pendientes. El acceso a la finca es a través de un código numérico, llave física o interfono preparado con videocámara.  La propiedad está en una primera planta real sin ascensor y tiene caja de llaves digital. Al entrar por la puerta principal, tenemos un distribuidor con cámara de vigilancia y los contadores generales del inmueble, desde aquí accedemos a mano derecha al apartamento exterior a la calle, que da a la plaza Salvador Seguí, que consta de un salón comedor exterior con dos ventanas y un gran ventanal con balcón, con orientación noroeste, cocina totalmente equipada, un dormitorio doble que le entra luz por unas ventanas que dan al salón, y un baño completo. Techos altos de unos cuatro metros. Tiene luz todo el día y sol por las tardes.  El otro apartamento consta de un amplio salón comedor que goza de mucha luz natural gracias a su gran ventanal orientado al sudeste por donde entra luz todo el día y sol directo toda la mañana y mediodía, que da a una terraza de 50 metros cuadrados, privada, amueblada, con toldo retraible y de uso exclusivo. La terraza está en un patio interior de manzana absolutamente silencioso. Techos altos a más de cuatro metros con volta catalana. Consta de una habitación doble, baño completo, y cocina totalmente equipada. Ambos apartamentos gozan de carpintería de aluminio con doble cristal acústico, aire acondicionado y bomba de calor por conductos en todas las habitaciones, calefacción de radiadores y agua caliente ilimitada por caldera de gas centralizada. Actualmente, cada apartamento tiene un contrato de alquiler a largo plazo. Por lo tanto, esta propiedad genera dos alquileres que conjuntamente suman 2.150€ brutos al mes, o 25,800€ anuales. En una configuración de alquiler vacacional puro (contratos mensuales, el apartamento no tiene licencia turística) el bruto anual incrementa un 35% hasta los 35,000€, aproximadamente. A pesar de los contratos de largo plazo actuales, los apartamentos están diseñados para alquileres de temporada o vacacionales e incluyen en el precio de venta todo lo necesario para entrar a vivir inmediatamente: cubertería, ropa de cama, etc. Los apartamentos están separados por anchas paredes de piedra y fibra acústica en ambos lados, justamente para que no se molesten acústicamente. Cada apartamento tiene su llave privada y una cámara de seguridad en el pasillo interior que los une. Así, sería posible alquilar un apartamento en régimen vacacional y otro a largo plazo, por ejemplo. La flexibilidad es total. El propietario ha alquilado la propiedad como un solo apartamento y como dos apartamentos independientes. Ha alquilado a largo plazo, por temporada y como apartamentos vacacionales. Los apartamentos se han diseñado como hogares de alto standing. El precio de venta incluye todos los muebles y objetos de decoración tal y como se ven en las fotografías, menos los cuadros. Destaco: dos sofás cama (uno de ellos un Chesterfield original, importado de Inglaterra, de cuero rojo), dos camas dobles, dos mesas y sus sillas de comedor, los muebles de terraza (sofás de exterior, alfombra, plantas y tumbonas de madera). Gracias a los sofás cama, cada apart.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 4158.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de Sant Pau'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '98145102', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/94/3e/d6/1002492446.jpg', 'externalReference': '101217', 'numPhotos': 35, 'floor': 'en', 'price': 420000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 101.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Sant Pau', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3776106, 'longitude': 2.172716, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98145102/', 'distance': '1124', 'description': 'PISAZO DE 100M2 + 58M2 DE TERRAZA, EN FINCA DEL AÑO 1850 COMPLETAMENTE REHABILITADA. La propiedad en venta actualmente está dividida físicamente (no segregada) en dos apartamentos completos e independientes, que comparten luz, agua y gas. Cada apartamento tiene su propio acceso independiente con llave, y constan de un dormitorio doble, cocina totalmente equipada, sala de estar/comedor y baño completo. La vivienda está situada en la amplia plaza Salvador Seguí, delante de la Filmoteca, en el Raval, a tres minutos de les Ramblas. La finca es del año 1850, ha sido completamente rehabilitada, cuenta con cámaras de seguridad en la entrada y en cada rellano, tiene la ITE pasada con su correspondiente Certificado de Aptitud del año 2020, y no tiene derramas pendientes. El acceso a la finca es a través de un código numérico, llave física o interfono preparado con videocámara.  La propiedad está en una primera planta real sin ascensor y tiene caja de llaves digital. Al entrar por la puerta principal, tenemos un distribuidor con cámara de vigilancia y los contadores generales del inmueble, desde aquí accedemos a mano derecha al apartamento exterior a la calle, que da a la plaza Salvador Seguí, que consta de un salón comedor exterior con dos ventanas y un gran ventanal con balcón, con orientación noroeste, cocina totalmente equipada, un dormitorio doble que le entra luz por unas ventanas que dan al salón, y un baño completo. Techos altos de unos cuatro metros. Tiene luz todo el día y sol por las tardes.  El otro apartamento consta de un amplio salón comedor que goza de mucha luz natural gracias a su gran ventanal orientado al sudeste por donde entra luz todo el día y sol directo toda la mañana y mediodía, que da a una terraza de 50 metros cuadrados, privada, amueblada, con toldo retraible y de uso exclusivo. La terraza está en un patio interior de manzana absolutamente silencioso. Techos altos a más de cuatro metros con volta catalana. Consta de una habitación doble, baño completo, y cocina totalmente equipada. Ambos apartamentos gozan de carpintería de aluminio con doble cristal acústico, aire acondicionado y bomba de calor por conductos en todas las habitaciones, calefacción de radiadores y agua caliente ilimitada por caldera de gas centralizada. Actualmente, cada apartamento tiene un contrato de alquiler a largo plazo. Por lo tanto, esta propiedad genera dos alquileres que conjuntamente suman 2.150€ brutos al mes, o 25,800€ anuales. En una configuración de alquiler vacacional puro (contratos mensuales, el apartamento no tiene licencia turística) el bruto anual incrementa un 35% hasta los 35,000€, aproximadamente. A pesar de los contratos de largo plazo actuales, los apartamentos están diseñados para alquileres de temporada o vacacionales e incluyen en el precio de venta todo lo necesario para entrar a vivir inmediatamente: cubertería, ropa de cama, etc. Los apartamentos están separados por anchas paredes de piedra y fibra acústica en ambos lados, justamente para que no se molesten acústicamente. Cada apartamento tiene su llave privada y una cámara de seguridad en el pasillo interior que los une. Así, sería posible alquilar un apartamento en régimen vacacional y otro a largo plazo, por ejemplo. La flexibilidad es total. El propietario ha alquilado la propiedad como un solo apartamento y como dos apartamentos independientes. Ha alquilado a largo plazo, por temporada y como apartamentos vacacionales. Los apartamentos se han diseñado como hogares de alto standing. El precio de venta incluye todos los muebles y objetos de decoración tal y como se ven en las fotografías, menos los cuadros. Destaco: dos sofás cama (uno de ellos un Chesterfield original, importado de Inglaterra, de cuero rojo), dos camas dobles, dos mesas y sus sillas de comedor, los muebles de terraza (sofás de exterior, alfombra, plantas y tumbonas de madera). Gracias a los sofás cama, cada apart.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 4158.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de Sant Pau'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AS5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97933192', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/11/01/9b/995459861.jpg', 'externalReference': '261437', 'numPhotos': 16, 'floor': '1', 'price': 768000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 130.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3858408, 'longitude': 2.1603522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97933192/', 'distance': '804', 'description': 'DIPUTACIO - ARIBAU impresionante piso de diseño nuevo a estrenar en finca regia tiene 148 m² según referencia catastral, dispone de 2 habitaciones tipos suite, gran vestidor. La vivienda muy bien distribuida y bien diferenciada la zona de día de la de noche, al entrar encontramos un gran hall que da acceso a la cómoda cocina completamente equipada con electrodomésticos de alta gama y al magnífico salón comedor exterior a la calle con balcón, dispone de sistema de domótica de luz y persianas, carpintería de aluminio, aire acondicionado en todas las estancias y radiadores. En la zona de noche encontramos los dos dormitorios suitte uno de ellos con vestidor. La finca regia es preciosa, muy elegante, cuidada. Está ubicado en uno de los barrios más elegantes y de mayor comercio de Barcelona y una zona muy demandada debido a su enclave privilegiado. Se encuentra cerca de las principales vías de entrada y salida de la ciudad, cerca del exclusivo Paseo de Gracia y rodeada de transporte publico para acceder a cualquier parte de Barcelona. Este barrio cuenta con todos los servicios y tiendas especializadas que usted necesite. Desde las tiendas más exclusivas de la ciudad y famosas internacionalmente tanto moda y complementos como tiendas gourmet, parques, oficinas etc. Zona prime en pleno centro de Barcelona. Zona Ciutat Vella. ( El PVP indicado no incluye impuestos ni gastos de Escritura ).  PARA PROPIETARIOS:  1. ¿Necesitas vender para comprar? donpiso puede comprar tu casa entregándote el 10% en 48 horas y el resto ante Notario.  2. ¿Problemas económicos? Te ayudamos entregándote una cantidad pactada cada mes mientras vendemos tu casa. Sin gastos de ningún tipo.  3. ¿Vendes un piso con hipoteca? mientras gestionamos la venta, te adelantamos la cuota mensual.  4. ¿Reformas? al mejor precio y te las financiamos dentro de la hipoteca.  5. ¿La mejor hipoteca? en donpiso la encuentras y con condiciones preferentes.  6. ¿Herencias y divorcios? te ayudamos y coordinamos todo.  Infórmate: 93 306 90 90 -.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5908.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': False, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '97933192', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/11/01/9b/995459861.jpg', 'externalReference': '261437', 'numPhotos': 16, 'floor': '1', 'price': 768000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 130.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3858408, 'longitude': 2.1603522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97933192/', 'distance': '804', 'description': 'DIPUTACIO - ARIBAU impresionante piso de diseño nuevo a estrenar en finca regia tiene 148 m² según referencia catastral, dispone de 2 habitaciones tipos suite, gran vestidor. La vivienda muy bien distribuida y bien diferenciada la zona de día de la de noche, al entrar encontramos un gran hall que da acceso a la cómoda cocina completamente equipada con electrodomésticos de alta gama y al magnífico salón comedor exterior a la calle con balcón, dispone de sistema de domótica de luz y persianas, carpintería de aluminio, aire acondicionado en todas las estancias y radiadores. En la zona de noche encontramos los dos dormitorios suitte uno de ellos con vestidor. La finca regia es preciosa, muy elegante, cuidada. Está ubicado en uno de los barrios más elegantes y de mayor comercio de Barcelona y una zona muy demandada debido a su enclave privilegiado. Se encuentra cerca de las principales vías de entrada y salida de la ciudad, cerca del exclusivo Paseo de Gracia y rodeada de transporte publico para acceder a cualquier parte de Barcelona. Este barrio cuenta con todos los servicios y tiendas especializadas que usted necesite. Desde las tiendas más exclusivas de la ciudad y famosas internacionalmente tanto moda y complementos como tiendas gourmet, parques, oficinas etc. Zona prime en pleno centro de Barcelona. Zona Ciutat Vella. ( El PVP indicado no incluye impuestos ni gastos de Escritura ).  PARA PROPIETARIOS:  1. ¿Necesitas vender para comprar? donpiso puede comprar tu casa entregándote el 10% en 48 horas y el resto ante Notario.  2. ¿Problemas económicos? Te ayudamos entregándote una cantidad pactada cada mes mientras vendemos tu casa. Sin gastos de ningún tipo.  3. ¿Vendes un piso con hipoteca? mientras gestionamos la venta, te adelantamos la cuota mensual.  4. ¿Reformas? al mejor precio y te las financiamos dentro de la hipoteca.  5. ¿La mejor hipoteca? en donpiso la encuentras y con condiciones preferentes.  6. ¿Herencias y divorcios? te ayudamos y coordinamos todo.  Infórmate: 93 306 90 90 -.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5908.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': False, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AT5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97661362', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/27/af/fc/1031239714.jpg', 'externalReference': '236620', 'numPhotos': 19, 'floor': 'bj', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 149.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3843408, 'longitude': 2.1626522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97661362/', 'distance': '686', 'description': 'DIPUTACIO - ARIBAU Impresionante piso de diseño con terraza nuevo a estrenar en finca regia tiene 148 m² según referencia catastral, dispone de 2 habitaciones de las cuales dos son suite, gran vestidor. La vivienda muy bien distribuida y bien diferenciada la zona de día de la de noche, al entrar encontramos un gran hall que da acceso a la cómoda cocina completamente equipada con electrodomésticos de alta gama y al magnífico salón comedor exterior a la calle con balcón, dispone de sistema de domótica de luz y persianas, carpintería de aluminio, aire acondicionado en todas las estancias y radiadores. En la zona de noche encontramos los dos dormitorios suitte uno de ellos con vestidor y con salia a la magnífica terraza de 41 m². La finca regia es preciosa, muy elegante, cuidada. Está ubicado en uno de los barrios más elegantes y de mayor comercio de Barcelona y una zona muy demandada debido a su enclave privilegiado. Se encuentra cerca de las principales vías de entrada y salida de la ciudad, cerca del exclusivo Paseo de Gracia y rodeada de transporte publico para acceder a cualquier parte de Barcelona. Este barrio cuenta con todos los servicios y tiendas especializadas que usted necesite. Desde las tiendas más exclusivas de la ciudad y famosas internacionalmente tanto moda y complementos como tiendas gourmet, parques, oficinas etc. Zona prime en pleno centro de Barcelona. Zona Ciutat Vella. ( El PVP indicado no incluye impuestos ni gastos de Escritura ).  PARA PROPIETARIOS:  1. ¿Necesitas vender para comprar? donpiso puede comprar tu casa entregándote el 10% en 48 horas y el resto ante Notario.  2. ¿Problemas económicos? Te ayudamos entregándote una cantidad pactada cada mes mientras vendemos tu casa. Sin gastos de ningún tipo.  3. ¿Vendes un piso con hipoteca? mientras gestionamos la venta, te adelantamos la cuota mensual.  4. ¿Reformas? al mejor precio y te las financiamos dentro de la hipoteca.  5. ¿La mejor hipoteca? en donpiso la encuentras y con condiciones preferentes.  6. ¿Herencias y divorcios? te ayudamos y coordinamos todo.  Infórmate: 93 306 90 90 -.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5691.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': False, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '97661362', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/27/af/fc/1031239714.jpg', 'externalReference': '236620', 'numPhotos': 19, 'floor': 'bj', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 149.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3843408, 'longitude': 2.1626522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97661362/', 'distance': '686', 'description': 'DIPUTACIO - ARIBAU Impresionante piso de diseño con terraza nuevo a estrenar en finca regia tiene 148 m² según referencia catastral, dispone de 2 habitaciones de las cuales dos son suite, gran vestidor. La vivienda muy bien distribuida y bien diferenciada la zona de día de la de noche, al entrar encontramos un gran hall que da acceso a la cómoda cocina completamente equipada con electrodomésticos de alta gama y al magnífico salón comedor exterior a la calle con balcón, dispone de sistema de domótica de luz y persianas, carpintería de aluminio, aire acondicionado en todas las estancias y radiadores. En la zona de noche encontramos los dos dormitorios suitte uno de ellos con vestidor y con salia a la magnífica terraza de 41 m². La finca regia es preciosa, muy elegante, cuidada. Está ubicado en uno de los barrios más elegantes y de mayor comercio de Barcelona y una zona muy demandada debido a su enclave privilegiado. Se encuentra cerca de las principales vías de entrada y salida de la ciudad, cerca del exclusivo Paseo de Gracia y rodeada de transporte publico para acceder a cualquier parte de Barcelona. Este barrio cuenta con todos los servicios y tiendas especializadas que usted necesite. Desde las tiendas más exclusivas de la ciudad y famosas internacionalmente tanto moda y complementos como tiendas gourmet, parques, oficinas etc. Zona prime en pleno centro de Barcelona. Zona Ciutat Vella. ( El PVP indicado no incluye impuestos ni gastos de Escritura ).  PARA PROPIETARIOS:  1. ¿Necesitas vender para comprar? donpiso puede comprar tu casa entregándote el 10% en 48 horas y el resto ante Notario.  2. ¿Problemas económicos? Te ayudamos entregándote una cantidad pactada cada mes mientras vendemos tu casa. Sin gastos de ningún tipo.  3. ¿Vendes un piso con hipoteca? mientras gestionamos la venta, te adelantamos la cuota mensual.  4. ¿Reformas? al mejor precio y te las financiamos dentro de la hipoteca.  5. ¿La mejor hipoteca? en donpiso la encuentras y con condiciones preferentes.  6. ¿Herencias y divorcios? te ayudamos y coordinamos todo.  Infórmate: 93 306 90 90 -.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5691.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': False, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AU5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '95993558', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8a/45/92/933783157.jpg', 'externalReference': 'W-02NAXU', 'numPhotos': 31, 'price': 275000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 88.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle del Moianès', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'Hostafrancs', 'latitude': 41.3748961, 'longitude': 2.1433843, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/95993558/', 'distance': '2605', 'description': 'Pis a reformar con cédula Engel &amp; Völkers presenta una oportunidad de inversión en un amplio piso con vistas despejadas en Carrer de Moianès. Se compone de una vivienda de 88m2 construidos con cédula de habitabilidad, en una finca con ascensor, que hasta el momento se utilizaba como oficina, por tanto, tenemos un gran espacio diáfano con dos habitaciones y un baño que se puede reconvertir al piso que desees. Una quinta planta real. Entrando por la puerta accedemos a un pequeño pasillo con una amplia habitación y cocina a la izquierda y, a la derecha, otra pequeña con el baño. A continuación vemos el gran espacio diáfano con grandes ventanales que dejan entrar muchísima luz. Piso de grandes dimensiones para hacerlo completamente al gusto. La propiedad está estratégicamente ubicada en la mejor zona del barrio de Hostafrancs (Sants). La proximidad de la vivienda a la Plaza España, uno de los centros neurálgicos de Barcelona, así como también a la Estación de Sants, situándose en calle Moianès, representa la comodidad de tenerlo todo a solo dos minutos, supermercados, comercios varios, bancos, gimnasios, escuelas. Contando además con todos los medios de transporte urbano (FGC, Metro Líneas 1 y 3, Aerobús A1 y A2, más de 10 líneas de buses) y el desplazamiento directo a pie de la Fira de Barcelona. Es una ubicación ideal para familias, turistas, y personas que necesiten un "pied a terre" en Barcelona, facilitando los desplazamientos y viajes por trabajo. Sants, La Bordeta y Hostafrancs, son el símbolo de la Barcelona turística y cosmopolita, pero también de las tradiciones de los barrios más céntricos de la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3125.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Hostafrancs, Barcelona', 'title': 'Piso en Calle del Moianès'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': True, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '95993558', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8a/45/92/933783157.jpg', 'externalReference': 'W-02NAXU', 'numPhotos': 31, 'price': 275000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 88.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle del Moianès', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'Hostafrancs', 'latitude': 41.3748961, 'longitude': 2.1433843, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/95993558/', 'distance': '2605', 'description': 'Pis a reformar con cédula Engel &amp; Völkers presenta una oportunidad de inversión en un amplio piso con vistas despejadas en Carrer de Moianès. Se compone de una vivienda de 88m2 construidos con cédula de habitabilidad, en una finca con ascensor, que hasta el momento se utilizaba como oficina, por tanto, tenemos un gran espacio diáfano con dos habitaciones y un baño que se puede reconvertir al piso que desees. Una quinta planta real. Entrando por la puerta accedemos a un pequeño pasillo con una amplia habitación y cocina a la izquierda y, a la derecha, otra pequeña con el baño. A continuación vemos el gran espacio diáfano con grandes ventanales que dejan entrar muchísima luz. Piso de grandes dimensiones para hacerlo completamente al gusto. La propiedad está estratégicamente ubicada en la mejor zona del barrio de Hostafrancs (Sants). La proximidad de la vivienda a la Plaza España, uno de los centros neurálgicos de Barcelona, así como también a la Estación de Sants, situándose en calle Moianès, representa la comodidad de tenerlo todo a solo dos minutos, supermercados, comercios varios, bancos, gimnasios, escuelas. Contando además con todos los medios de transporte urbano (FGC, Metro Líneas 1 y 3, Aerobús A1 y A2, más de 10 líneas de buses) y el desplazamiento directo a pie de la Fira de Barcelona. Es una ubicación ideal para familias, turistas, y personas que necesiten un "pied a terre" en Barcelona, facilitando los desplazamientos y viajes por trabajo. Sants, La Bordeta y Hostafrancs, son el símbolo de la Barcelona turística y cosmopolita, pero también de las tradiciones de los barrios más céntricos de la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3125.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Hostafrancs, Barcelona', 'title': 'Piso en Calle del Moianès'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': True, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AV5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97340498', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/80/e6/98/1046925847.jpg', 'externalReference': 'FloridaFranç', 'numPhotos': 23, 'floor': '2', 'price': 315000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de Floridablanca', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'Sant Antoni', 'latitude': 41.3766483, 'longitude': 2.1541467, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97340498/', 'distance': '1772', 'description': 'Piso totalmente reformado conservando de manera cuidadosa los elementos originales tales como techos de bóveda catalana y puerta originales de madera recuperada, todo combinado con una reforma integral con materiales de muy buena calidad de un gusto excepcional. El piso tiene una superficie construida de 83 metros y una superficie útil de 75 metros, el piso tiene 2 habitaciones, baño completo cocina equipada y salón con balcón. Es una segunda planta real con ASCENSOR, en una finca Regia. No esperes más y ven a visitar este piso con nosotros. Valoramos tu casa Encuentra más en.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3795.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Antoni, Barcelona', 'title': 'Piso en Calle de Floridablanca'}, 'hasPlan': False, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '97340498', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/80/e6/98/1046925847.jpg', 'externalReference': 'FloridaFranç', 'numPhotos': 23, 'floor': '2', 'price': 315000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de Floridablanca', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'Sant Antoni', 'latitude': 41.3766483, 'longitude': 2.1541467, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97340498/', 'distance': '1772', 'description': 'Piso totalmente reformado conservando de manera cuidadosa los elementos originales tales como techos de bóveda catalana y puerta originales de madera recuperada, todo combinado con una reforma integral con materiales de muy buena calidad de un gusto excepcional. El piso tiene una superficie construida de 83 metros y una superficie útil de 75 metros, el piso tiene 2 habitaciones, baño completo cocina equipada y salón con balcón. Es una segunda planta real con ASCENSOR, en una finca Regia. No esperes más y ven a visitar este piso con nosotros. Valoramos tu casa Encuentra más en.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3795.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Antoni, Barcelona', 'title': 'Piso en Calle de Floridablanca'}, 'hasPlan': False, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AW5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99079881', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/9e/74/a7/1032868162.jpg', 'externalReference': 'VB2210011', 'numPhotos': 45, 'floor': 'bj', 'price': 890000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 137.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Fraternitat', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'Vila de Gràcia', 'latitude': 41.3991723, 'longitude': 2.158972, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99079881/', 'distance': '1581', 'description': 'Vivienda exclusiva con jardín en el corazón de Vila de Gràcia \xa0 En pleno corazón de la Vila de Gràcia, cerca de la plaza de la revolución y a cinco minutos caminando del metro Diagonal, encontramos esta vivienda exclusiva reformada en 2018 con todos los materiales de la mejor calidad. Este piso sorprende por sus detalles Arquitectónicos, Al entrar en la vivienda encontramos un recibidor con armarios y ventanas hacia el exterior y detrás de ello un sorprendente doble nivel donde la zona de abajo se convierte en una habitación totalmente cerrada y la parte de arriba puede ser un estudio o una sala de estar. A continuación, encontramos la cocina abierta y la sala de estar con mucha luz natural y vistas hacia el patio / jardín. con los techos altos en bóveda catalana toda la vivienda tiene una gran sensación de amplitud. Y después de la sala encontramos un pasillo con techos ventanas que dejan pasar totalmente la luz del día. Este pasillo puede quedar totalmente abierto en patio ya que la separación con el propio patio es con unos grandes ventanales tipo paneles japoneses y se pueden abrir totalmente para dejar un espacio muy grande donde se puede instalar mesa y sillas para hacer comidas en verano. En este mismo pasillo encontramos una pared entera de armarios para poder almacenar todo lo necesario en la vivienda. En la última parte a continuación del pasillo, encontramos en el antiguo lavadero una habitación doble en suite con su propio baño. Desde el patio interior podemos acceder a través de unas escaleras a un espacio extra, un jardín con vegetación y toldo, ideal para comidas y cenas y disfrutar de un espacio exterior despejado. La vivienda cuenta con una reforma de la mejor calidad, y ha conservado los detalles originales como las bóvedas catalanas, las paredes de piedras, y añadiendo materiales cálidos como los suelos de Madera. La finca tiene pasado la ITE y ha obtenido el certificado de aptitud. Disponemos de planos. No dudes en pedirnos visita en esta vivienda espectacular! \xa0 \xa0.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6496.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Vila de Gràcia, Barcelona', 'title': 'Piso en Calle de la Fraternitat'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': True, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '99079881', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/9e/74/a7/1032868162.jpg', 'externalReference': 'VB2210011', 'numPhotos': 45, 'floor': 'bj', 'price': 890000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 137.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Fraternitat', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'Vila de Gràcia', 'latitude': 41.3991723, 'longitude': 2.158972, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99079881/', 'distance': '1581', 'description': 'Vivienda exclusiva con jardín en el corazón de Vila de Gràcia \xa0 En pleno corazón de la Vila de Gràcia, cerca de la plaza de la revolución y a cinco minutos caminando del metro Diagonal, encontramos esta vivienda exclusiva reformada en 2018 con todos los materiales de la mejor calidad. Este piso sorprende por sus detalles Arquitectónicos, Al entrar en la vivienda encontramos un recibidor con armarios y ventanas hacia el exterior y detrás de ello un sorprendente doble nivel donde la zona de abajo se convierte en una habitación totalmente cerrada y la parte de arriba puede ser un estudio o una sala de estar. A continuación, encontramos la cocina abierta y la sala de estar con mucha luz natural y vistas hacia el patio / jardín. con los techos altos en bóveda catalana toda la vivienda tiene una gran sensación de amplitud. Y después de la sala encontramos un pasillo con techos ventanas que dejan pasar totalmente la luz del día. Este pasillo puede quedar totalmente abierto en patio ya que la separación con el propio patio es con unos grandes ventanales tipo paneles japoneses y se pueden abrir totalmente para dejar un espacio muy grande donde se puede instalar mesa y sillas para hacer comidas en verano. En este mismo pasillo encontramos una pared entera de armarios para poder almacenar todo lo necesario en la vivienda. En la última parte a continuación del pasillo, encontramos en el antiguo lavadero una habitación doble en suite con su propio baño. Desde el patio interior podemos acceder a través de unas escaleras a un espacio extra, un jardín con vegetación y toldo, ideal para comidas y cenas y disfrutar de un espacio exterior despejado. La vivienda cuenta con una reforma de la mejor calidad, y ha conservado los detalles originales como las bóvedas catalanas, las paredes de piedras, y añadiendo materiales cálidos como los suelos de Madera. La finca tiene pasado la ITE y ha obtenido el certificado de aptitud. Disponemos de planos. No dudes en pedirnos visita en esta vivienda espectacular! \xa0 \xa0.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6496.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Vila de Gràcia, Barcelona', 'title': 'Piso en Calle de la Fraternitat'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': True, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AX5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99791140', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/de/1c/b1/1054580932.jpg', 'externalReference': 'BCN38000', 'numPhotos': 32, 'price': 575000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 103.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio La Salut', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'La Salut', 'latitude': 41.4073525, 'longitude': 2.1502985, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99791140/', 'distance': '2741', 'description': 'Propiedad en venta en perfecto estado impecable, con dos dormitorios dobles (uno en suite) y 2 baños con una bonita distribución abierta. Se han utilizado materiales de alta calidad con la renovación, lo que resultó en esta propiedad luminosa y lista para entrar. El estilo es contemporáneo y de buen gusto; el lienzo en blanco perfecto para que el nuevo propietario entre y lo complete con su propio toque personal.  El apartamento se encuentra en el sexto piso real del edificio y cuenta con una terraza soleada con espacio para comer al aire libre. También en el edificio existe la posibilidad de alquilar o comprar una plaza de aparcamiento; un detalle que se agradecerá mucho en un barrio donde escasea el aparcamiento.  La propiedad viene completamente equipada con aire acondicionado central por conductos, y la propiedad cuenta con pisos de madera real, una cocina totalmente equipada y muebles flexibles.  El edificio dispone de servicio de conserjería para mayor comodidad.  La ubicación es en Gracia, al lado del transporte público, restaurantes, etc. pero también cerca de parques para tener un entorno verde.  No dude en ponerse en contacto con nosotros para obtener más información o para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5583.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'La Salut, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '99791140', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/de/1c/b1/1054580932.jpg', 'externalReference': 'BCN38000', 'numPhotos': 32, 'price': 575000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 103.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio La Salut', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'La Salut', 'latitude': 41.4073525, 'longitude': 2.1502985, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99791140/', 'distance': '2741', 'description': 'Propiedad en venta en perfecto estado impecable, con dos dormitorios dobles (uno en suite) y 2 baños con una bonita distribución abierta. Se han utilizado materiales de alta calidad con la renovación, lo que resultó en esta propiedad luminosa y lista para entrar. El estilo es contemporáneo y de buen gusto; el lienzo en blanco perfecto para que el nuevo propietario entre y lo complete con su propio toque personal.  El apartamento se encuentra en el sexto piso real del edificio y cuenta con una terraza soleada con espacio para comer al aire libre. También en el edificio existe la posibilidad de alquilar o comprar una plaza de aparcamiento; un detalle que se agradecerá mucho en un barrio donde escasea el aparcamiento.  La propiedad viene completamente equipada con aire acondicionado central por conductos, y la propiedad cuenta con pisos de madera real, una cocina totalmente equipada y muebles flexibles.  El edificio dispone de servicio de conserjería para mayor comodidad.  La ubicación es en Gracia, al lado del transporte público, restaurantes, etc. pero también cerca de parques para tener un entorno verde.  No dude en ponerse en contacto con nosotros para obtener más información o para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5583.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'La Salut, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
       <c r="AY5" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99766521', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/29/1b/91/1053990542.jpg', 'externalReference': 'BCN37642', 'numPhotos': 27, 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 80.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Raval', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3763632, 'longitude': 2.1674975, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99766521/', 'distance': '1249', 'description': 'Nos encontramos ante una obra nueva a partir de la rehabilitación de una antigua fábrica textil de los años 30. Se han mantenido muchos de sus elementos originales, y se han creado\xa0lofts modernos de estilo industrial y con mucha luz, grandes ventanales y zonas comunes como piscina, sala social, terrazas y jardines.  La propiedad en venta es un apartamento muy diáfano que consta de salón comedor cocina con acceso a una bonita terraza cubierta orientada a las zonas comunes del complejo. También tenemos una habitación doble con baño en suite, otro baño completo y una segunda habitación doble en un mezzanine construido gracias a la altura de los techos.  El apartamento está en perfecto estado y cuenta con vigas vistas de madera, cerramientos de aluminio de suelo a techo de grandes dimensiones, aire acondicionado, bomba de calor por splits, paredes de ladrillo visto y suelos de parquet, entre otros aspectos.  Se trata así de un pequeño oasis en el centro del casco antiguo de Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6063.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
+          <t>{'propertyCode': '99766521', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/29/1b/91/1053990542.jpg', 'externalReference': 'BCN37642', 'numPhotos': 27, 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 80.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Raval', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3763632, 'longitude': 2.1674975, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99766521/', 'distance': '1249', 'description': 'Nos encontramos ante una obra nueva a partir de la rehabilitación de una antigua fábrica textil de los años 30. Se han mantenido muchos de sus elementos originales, y se han creado\xa0lofts modernos de estilo industrial y con mucha luz, grandes ventanales y zonas comunes como piscina, sala social, terrazas y jardines.  La propiedad en venta es un apartamento muy diáfano que consta de salón comedor cocina con acceso a una bonita terraza cubierta orientada a las zonas comunes del complejo. También tenemos una habitación doble con baño en suite, otro baño completo y una segunda habitación doble en un mezzanine construido gracias a la altura de los techos.  El apartamento está en perfecto estado y cuenta con vigas vistas de madera, cerramientos de aluminio de suelo a techo de grandes dimensiones, aire acondicionado, bomba de calor por splits, paredes de ladrillo visto y suelos de parquet, entre otros aspectos.  Se trata así de un pequeño oasis en el centro del casco antiguo de Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6063.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
         </is>
       </c>
     </row>
@@ -1611,252 +1611,252 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '87797664', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5d/ba/ea/1026649594.jpg', 'externalReference': 'BCN05285', 'numPhotos': 52, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 170.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3863885, 'longitude': 2.1622455, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/87797664/', 'distance': '636', 'description': 'Magnífica vivienda de obra nueva con terraza en Eixample Esquerra. Espectacular vivienda de obra nueva en finca modernista rehabilitada con ascensor, situada junto a la histórica Universidad de Barcelona. Se trata de una ubicación perfecta en pleno centro de la ciudad, con los mejores servicios y comunicaciones, a tan solo 3 calles de Plaza Catalunya y el Paseo de Gracia. El piso dispone de 130 m2 construidos interiores más 40 m2 de terraza, que le da un gran valor, un patio de 8 m2 y un balcón de 3 m2. La zona de día consta de salón-comedor con balcón hacia la calle, cocina independiente con electrodomésticos y galería con lavadero. La zona de noche se compone de dos habitaciones en suite con cuarto de baño propio: la principal tiene vestidor y acceso a la terraza, orientada hacia el patio de manzana inrterior; y la otra es interior y tiene acceso a un patio de 8 m2. Además, hay un aseo de cortesía. El edificio tiene además un terrado comunitario para disfrutar del aire libre. El piso goza de una reforma de alta calidad y diseño de la mano del prestigioso interiorista Jaime Beriestain. Está equipado con sistema hibrido de aerotermia de la casa Mintsubishi con integración de Hidrokit, fancoils por conductos y suelo radiante (controlado por domótica), suelos de piedra natural, armarios empotrados y cristales Climalit.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4988.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '87797664', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5d/ba/ea/1026649594.jpg', 'externalReference': 'BCN05285', 'numPhotos': 52, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 170.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3863885, 'longitude': 2.1622455, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/87797664/', 'distance': '636', 'description': 'Magnífica vivienda de obra nueva con terraza en Eixample Esquerra. Espectacular vivienda de obra nueva en finca modernista rehabilitada con ascensor, situada junto a la histórica Universidad de Barcelona. Se trata de una ubicación perfecta en pleno centro de la ciudad, con los mejores servicios y comunicaciones, a tan solo 3 calles de Plaza Catalunya y el Paseo de Gracia. El piso dispone de 130 m2 construidos interiores más 40 m2 de terraza, que le da un gran valor, un patio de 8 m2 y un balcón de 3 m2. La zona de día consta de salón-comedor con balcón hacia la calle, cocina independiente con electrodomésticos y galería con lavadero. La zona de noche se compone de dos habitaciones en suite con cuarto de baño propio: la principal tiene vestidor y acceso a la terraza, orientada hacia el patio de manzana inrterior; y la otra es interior y tiene acceso a un patio de 8 m2. Además, hay un aseo de cortesía. El edificio tiene además un terrado comunitario para disfrutar del aire libre. El piso goza de una reforma de alta calidad y diseño de la mano del prestigioso interiorista Jaime Beriestain. Está equipado con sistema hibrido de aerotermia de la casa Mintsubishi con integración de Hidrokit, fancoils por conductos y suelo radiante (controlado por domótica), suelos de piedra natural, armarios empotrados y cristales Climalit.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4988.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98351591', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/d2/66/bf/1009058214.jpg', 'externalReference': 'VB2207038', 'numPhotos': 29, 'floor': '3', 'price': 359000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 63.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Pi i Margall', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': "El Camp d'En Grassot i Gràcia Nova", 'latitude': 41.4096591, 'longitude': 2.1622433, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98351591/', 'distance': '2545', 'description': 'Piso reformado de dos habitaciones en venta en Gràcia Nova Fantástico piso reformado con dos habitaciones y balcón en Gràcia Nova En plena Gràcia Nova, a pocos metros del Mercat del Estrella, entre las paradas de metro Alfons X y Joanic, en uno de los futuros ejes verdes de la ciudad, encontramos este bonito apartamento totalmente reformado y a estrenar, listo para entrar a vivir. Luminosidad, buen gusto, distribución de espacios muy bien pensada y una reforma de calidad, es lo que describe mejor esta propiedad. la vivienda tiene una superficie de 60 m2 aprox que se distribuyen de forma muy lógica, al entrar en la vivienda encontramos el recibidor y el baño de cortesía, avanzamos en el pasillo y encontramos una primera habitación doble con baño completo en suite, avanzando un poco más llegamos a la habitación individual. Al final del pasillo se encuentra la amplia sala con cocina abierta totalmente equipada y con salida a un agradable balcón con vistas a un patio de manzana muy tranquilo y soleado por la tarde. La vivienda cuenta con aire acondicionado / calefacción por conductos, los suelos de parqué natural dan una calidez ideal a toda la vivienda. El edificio de los años 1963 cuenta con ascensor. ¡Sin duda, hablamos de una excelente oportunidad en la zona!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5698.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "El Camp d'En Grassot i Gràcia Nova, Barcelona", 'title': 'Piso en Calle de Pi i Margall'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98351591', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/d2/66/bf/1009058214.jpg', 'externalReference': 'VB2207038', 'numPhotos': 29, 'floor': '3', 'price': 359000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 63.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Pi i Margall', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': "El Camp d'En Grassot i Gràcia Nova", 'latitude': 41.4096591, 'longitude': 2.1622433, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98351591/', 'distance': '2545', 'description': 'Piso reformado de dos habitaciones en venta en Gràcia Nova Fantástico piso reformado con dos habitaciones y balcón en Gràcia Nova En plena Gràcia Nova, a pocos metros del Mercat del Estrella, entre las paradas de metro Alfons X y Joanic, en uno de los futuros ejes verdes de la ciudad, encontramos este bonito apartamento totalmente reformado y a estrenar, listo para entrar a vivir. Luminosidad, buen gusto, distribución de espacios muy bien pensada y una reforma de calidad, es lo que describe mejor esta propiedad. la vivienda tiene una superficie de 60 m2 aprox que se distribuyen de forma muy lógica, al entrar en la vivienda encontramos el recibidor y el baño de cortesía, avanzamos en el pasillo y encontramos una primera habitación doble con baño completo en suite, avanzando un poco más llegamos a la habitación individual. Al final del pasillo se encuentra la amplia sala con cocina abierta totalmente equipada y con salida a un agradable balcón con vistas a un patio de manzana muy tranquilo y soleado por la tarde. La vivienda cuenta con aire acondicionado / calefacción por conductos, los suelos de parqué natural dan una calidez ideal a toda la vivienda. El edificio de los años 1963 cuenta con ascensor. ¡Sin duda, hablamos de una excelente oportunidad en la zona!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5698.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "El Camp d'En Grassot i Gràcia Nova, Barcelona", 'title': 'Piso en Calle de Pi i Margall'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99349576', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b0/f6/f4/1041061889.jpg', 'externalReference': 'S-35432', 'numPhotos': 36, 'floor': '2', 'price': 229000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 68.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Ronda de Sant Pau', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'Sant Antoni', 'latitude': 41.375152, 'longitude': 2.1633305, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99349576/', 'distance': '1470', 'description': 'PLAÇA JOSEP MARIA FOLCH I TORRES Acogedora vivienda situada en uno de los barrios más emblemáticos de la ciudad condal junto a la Ronda Sant Pau y los Jardines de la Plaça Josep María Floch i Torres. Consta de 2 dormitorios (originalmente 3), luminoso comedor, baño con bañera y cocina con salida a lavadero. Toda la vivienda se encuentra en perfecto estado de conservación, con acabados de calidad. Suelo de mármol, puertas de madera noble, carpintería exterior de aluminio con persianas integradas y puerta de entrada de seguridad. Piso muy luminoso y tranquilo. Edificio de obra vista con ascensor.  En FINCAS Gp somos una empresa especializada en servicios inmobiliarios en la ciudad de Barcelona desde 1993. Los precios indicados no incluyen gastos e impuestos de escrituración ni de financiación. Venta y alquiler de apartamentos y locales comerciales. Encuentre más en nuestro sitio web.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3368.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Antoni, Barcelona', 'title': 'Piso en Ronda de Sant Pau'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99349576', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b0/f6/f4/1041061889.jpg', 'externalReference': 'S-35432', 'numPhotos': 36, 'floor': '2', 'price': 229000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 68.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Ronda de Sant Pau', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'Sant Antoni', 'latitude': 41.375152, 'longitude': 2.1633305, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99349576/', 'distance': '1470', 'description': 'PLAÇA JOSEP MARIA FOLCH I TORRES Acogedora vivienda situada en uno de los barrios más emblemáticos de la ciudad condal junto a la Ronda Sant Pau y los Jardines de la Plaça Josep María Floch i Torres. Consta de 2 dormitorios (originalmente 3), luminoso comedor, baño con bañera y cocina con salida a lavadero. Toda la vivienda se encuentra en perfecto estado de conservación, con acabados de calidad. Suelo de mármol, puertas de madera noble, carpintería exterior de aluminio con persianas integradas y puerta de entrada de seguridad. Piso muy luminoso y tranquilo. Edificio de obra vista con ascensor.  En FINCAS Gp somos una empresa especializada en servicios inmobiliarios en la ciudad de Barcelona desde 1993. Los precios indicados no incluyen gastos e impuestos de escrituración ni de financiación. Venta y alquiler de apartamentos y locales comerciales. Encuentre más en nuestro sitio web.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3368.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Antoni, Barcelona', 'title': 'Piso en Ronda de Sant Pau'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98840562', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/0e/a9/0e/1025701609.jpg', 'externalReference': 'BCNP4881', 'numPhotos': 24, 'price': 1100000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 125.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio Sant Pere - Santa Caterina i la Ribera', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3832064, 'longitude': 2.1829743, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98840562/', 'distance': '1201', 'description': 'El impacto directo de este excepcional apartamento hace que se distinga de otros en el mercado desde el primer momento en que se cruza la puerta. Encontrará techos altos, cinco grandes y originales puertas balconeras de tres orientaciones que ofrecen una inmensa luz natural, y vistas a la terraza privada con un verde jardín vertical. La cocina abierta de alta gama y totalmente equipada en la zona de estar ha sido hecha a medida desde Italia y da una agradable elegancia al apartamento con sus colores oscuros. La carpintería ha sido igualmente hecha a medida desde Italia para el apartamento y equilibra bien un espacio de oficina abierto con el primer dormitorio en suite. También hay un cuarto de baño para invitados justo al lado del segundo dormitorio. El suelo es de parquet natural y el apartamento dispone de radiadores para la calefacción. Pero la joya de la propiedad es sin duda la terraza de 28 m2 que conecta con el salón y el segundo dormitorio. Ofrece un hermoso jardín vertical y el lujo de la tranquilidad en el corazón de El Born. Escondido en el jardín vertical hay un acceso a un trastero que también se utiliza como lavadero. La micro ubicación del apartamento es otro importante punto de venta de la propiedad, ya que está rodeado de algunas de las mejores plazas y restaurantes de la zona. Además, a pocos minutos a pie se encuentra también el Parque de la Ciutadella, el puerto Port-Vell y la playa de la Barceloneta. En definitiva, estamos hablando de una auténtica oportunidad en uno de los barrios más populares de Barcelona. Si hay un lugar de moda tanto para turistas como locales, es el dinámico barrio de El Born con su particular mercado, ahora convertido en museo, tras conseguir unas fantásticas ruinas romanas durante su remodelación. Es hogar de artistas, artesanos y bohemios, con infinidad de tiendas curiosas y únicas. Aún más famosos son sus \xa0variados restaurantes, tantos como para descubrir uno nuevo cada día. El mercado de Santa Caterina con su techo inspirado en la piel del dragón de Sant Jordi es por sí mismo una obra para admirar. La Basílica de Santa María del Mar, El Palau de la Música, y el pulmón verde de La Ciutadella son algunos de los referentes importantes de este barrio. Es un barrio para vivir y conocer. Sus edificios continúan el patrón irregular de El Barrio Gótico, y sus calles aunque por momentos más despejadas, también son angostas. En los bajos de los edificios puede encontrar bares de autor, galerías de arte, talleres de artesanos y un sinfín de pequeños y curiosos negocios. Este barrio le interesará si le gusta el estilo de vida bohemio, convivir con los\xa0 múltiples artesanos, el tapeo y buen comer, y vivir en un barrio que le sorprenda con tiendas y rincones nuevos. Es una buena ubicación para invertir en un pied-à-terre.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 8800.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98840562', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/0e/a9/0e/1025701609.jpg', 'externalReference': 'BCNP4881', 'numPhotos': 24, 'price': 1100000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 125.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio Sant Pere - Santa Caterina i la Ribera', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3832064, 'longitude': 2.1829743, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98840562/', 'distance': '1201', 'description': 'El impacto directo de este excepcional apartamento hace que se distinga de otros en el mercado desde el primer momento en que se cruza la puerta. Encontrará techos altos, cinco grandes y originales puertas balconeras de tres orientaciones que ofrecen una inmensa luz natural, y vistas a la terraza privada con un verde jardín vertical. La cocina abierta de alta gama y totalmente equipada en la zona de estar ha sido hecha a medida desde Italia y da una agradable elegancia al apartamento con sus colores oscuros. La carpintería ha sido igualmente hecha a medida desde Italia para el apartamento y equilibra bien un espacio de oficina abierto con el primer dormitorio en suite. También hay un cuarto de baño para invitados justo al lado del segundo dormitorio. El suelo es de parquet natural y el apartamento dispone de radiadores para la calefacción. Pero la joya de la propiedad es sin duda la terraza de 28 m2 que conecta con el salón y el segundo dormitorio. Ofrece un hermoso jardín vertical y el lujo de la tranquilidad en el corazón de El Born. Escondido en el jardín vertical hay un acceso a un trastero que también se utiliza como lavadero. La micro ubicación del apartamento es otro importante punto de venta de la propiedad, ya que está rodeado de algunas de las mejores plazas y restaurantes de la zona. Además, a pocos minutos a pie se encuentra también el Parque de la Ciutadella, el puerto Port-Vell y la playa de la Barceloneta. En definitiva, estamos hablando de una auténtica oportunidad en uno de los barrios más populares de Barcelona. Si hay un lugar de moda tanto para turistas como locales, es el dinámico barrio de El Born con su particular mercado, ahora convertido en museo, tras conseguir unas fantásticas ruinas romanas durante su remodelación. Es hogar de artistas, artesanos y bohemios, con infinidad de tiendas curiosas y únicas. Aún más famosos son sus \xa0variados restaurantes, tantos como para descubrir uno nuevo cada día. El mercado de Santa Caterina con su techo inspirado en la piel del dragón de Sant Jordi es por sí mismo una obra para admirar. La Basílica de Santa María del Mar, El Palau de la Música, y el pulmón verde de La Ciutadella son algunos de los referentes importantes de este barrio. Es un barrio para vivir y conocer. Sus edificios continúan el patrón irregular de El Barrio Gótico, y sus calles aunque por momentos más despejadas, también son angostas. En los bajos de los edificios puede encontrar bares de autor, galerías de arte, talleres de artesanos y un sinfín de pequeños y curiosos negocios. Este barrio le interesará si le gusta el estilo de vida bohemio, convivir con los\xa0 múltiples artesanos, el tapeo y buen comer, y vivir en un barrio que le sorprenda con tiendas y rincones nuevos. Es una buena ubicación para invertir en un pied-à-terre.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 8800.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98382386', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a8/9e/34/1022400721.jpg', 'externalReference': 'BCNP4798', 'numPhotos': 27, 'price': 690000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 85.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3905269, 'longitude': 2.1644133, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98382386/', 'distance': '559', 'description': 'Maravilloso piso en venta en el corazón del Ensanche Derecho de Barcelona, a la vuelta de la esquina de la elegante Rambla de Catalunya conocida por sus lujosos comercios y conocida aun más por sus restaurantes con terraza ideales para disfrutar del buen tiempo de la ciudad condal. El piso es una auténtica maravilla. Los acabados que se han utilizado en la reforma es de auténtico lujo, como por ejemplo los suelos de madera noble de roble americano, la cocina de muy buena calidad con vinoteca y nevera Liebherr, baños y grifería de diseño, radiadores de alta gamma, armarios empotrados realizados a medida, panelados de madera en las paredes y papel decorativo de alta calidad, además de un sistema de filtro osmosis para mejorar el agua de toda la vivienda. El piso no solo dispone de maravillosos acabados, sino que además dispone de características arquitectónicas de la época, como los techos altos y artesonados, la chimenea original y marcos decorativos. El piso consta de un agradable salón comedor con salida a una terraza muy disfrutable de aproximadamente unos 8m2 orientada hacia el sudeste, una cocina totalmente equipada, un lavadero muy práctico, un dormitorio doble “en suite” también con salida a la terraza, y otro dormitorio individual con su propio baño. La finca es también un espectáculo, ya que se trata de un edificio regio del 1900, completamente reformada y actualizada con acceso directo al ascensor y además un excelente servicio de conserjería. En resumen una propiedad para gozar desde el primer instante que reúne todo lo que se buscaría en la mejor zona de Barcelona. La Dreta de L’Eixample se inicia en Plaça de Catalunya y su eje central gira en torno al Passeig de Gràcia y el Cuadrat d’Or. Se delimita desde la transitada Calle Balmes hasta el renovado Passeig de Sant Joan y desde la comercial Ronda Sant Pere hasta la conveniente Avinguda Diagonal. Es uno de los barrios, junto con Pedralbes y Sarrià-Sant Gervasi, más caros y exclusivos de Barcelona ciudad. Es imposible no hacer referencia al lujo del Paseo de Gràcia, con las boutiques de las marcas más exclusivas del mundo, o a los comercios de La Rambla de Catalunya. Sin embargo, el resto de sus calles son tanto o más interesantes. En ellas residía parte de la burguesía textilera catalana de principios del siglo XX, la cual ha dejado huella en las espectaculares fincas regias y casas modernistas diseñadas por los arquitectos más famosos de la época, como la Pedrera o la Casa Batlló del gran Antoni Gaudí. En consecuencia, las viviendas características de este barrio son apartamentos amplios, de techos elevados, molduras, elaborados pavimentos y balcones. Muchos edificios y pisos conservan esta herencia arquitectónica original artesanal y es posible encontrar apartamentos remodelados recientemente, áticos, lofts e incluso estudios, que reviven estos elementos, así como pisos con mucho potencial para ser reformados. Este lado de L’Eixample está dotado de todo tipo de servicios y comercios, centros educativos -principalmente escuelas concertadas y privadas-. Le resultará muy fácil moverse andando o desplazarse a través de las conexiones de transporte público hasta las tiendas y restaurantes más caros y en vogue de la ciudad. Este es el mejor barrio si quiere admirar y vivir en la zona noble del fascinante modernismo catalán, residir en una de sus características fincas regias, y convivir en perfecto equilibrio con la vibrante y lujosa vida comercial. Es ideal si desea caminar cada día por sus calles anchas y ordenadas, con fáciles conexiones de transporte, disponer de todo tipo de servicios y equipamientos incluidas escuelas concertadas o privadas, y disfrutar del ambiente más chic, cultural y cosmopolita de Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8118.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98382386', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a8/9e/34/1022400721.jpg', 'externalReference': 'BCNP4798', 'numPhotos': 27, 'price': 690000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 85.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3905269, 'longitude': 2.1644133, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98382386/', 'distance': '559', 'description': 'Maravilloso piso en venta en el corazón del Ensanche Derecho de Barcelona, a la vuelta de la esquina de la elegante Rambla de Catalunya conocida por sus lujosos comercios y conocida aun más por sus restaurantes con terraza ideales para disfrutar del buen tiempo de la ciudad condal. El piso es una auténtica maravilla. Los acabados que se han utilizado en la reforma es de auténtico lujo, como por ejemplo los suelos de madera noble de roble americano, la cocina de muy buena calidad con vinoteca y nevera Liebherr, baños y grifería de diseño, radiadores de alta gamma, armarios empotrados realizados a medida, panelados de madera en las paredes y papel decorativo de alta calidad, además de un sistema de filtro osmosis para mejorar el agua de toda la vivienda. El piso no solo dispone de maravillosos acabados, sino que además dispone de características arquitectónicas de la época, como los techos altos y artesonados, la chimenea original y marcos decorativos. El piso consta de un agradable salón comedor con salida a una terraza muy disfrutable de aproximadamente unos 8m2 orientada hacia el sudeste, una cocina totalmente equipada, un lavadero muy práctico, un dormitorio doble “en suite” también con salida a la terraza, y otro dormitorio individual con su propio baño. La finca es también un espectáculo, ya que se trata de un edificio regio del 1900, completamente reformada y actualizada con acceso directo al ascensor y además un excelente servicio de conserjería. En resumen una propiedad para gozar desde el primer instante que reúne todo lo que se buscaría en la mejor zona de Barcelona. La Dreta de L’Eixample se inicia en Plaça de Catalunya y su eje central gira en torno al Passeig de Gràcia y el Cuadrat d’Or. Se delimita desde la transitada Calle Balmes hasta el renovado Passeig de Sant Joan y desde la comercial Ronda Sant Pere hasta la conveniente Avinguda Diagonal. Es uno de los barrios, junto con Pedralbes y Sarrià-Sant Gervasi, más caros y exclusivos de Barcelona ciudad. Es imposible no hacer referencia al lujo del Paseo de Gràcia, con las boutiques de las marcas más exclusivas del mundo, o a los comercios de La Rambla de Catalunya. Sin embargo, el resto de sus calles son tanto o más interesantes. En ellas residía parte de la burguesía textilera catalana de principios del siglo XX, la cual ha dejado huella en las espectaculares fincas regias y casas modernistas diseñadas por los arquitectos más famosos de la época, como la Pedrera o la Casa Batlló del gran Antoni Gaudí. En consecuencia, las viviendas características de este barrio son apartamentos amplios, de techos elevados, molduras, elaborados pavimentos y balcones. Muchos edificios y pisos conservan esta herencia arquitectónica original artesanal y es posible encontrar apartamentos remodelados recientemente, áticos, lofts e incluso estudios, que reviven estos elementos, así como pisos con mucho potencial para ser reformados. Este lado de L’Eixample está dotado de todo tipo de servicios y comercios, centros educativos -principalmente escuelas concertadas y privadas-. Le resultará muy fácil moverse andando o desplazarse a través de las conexiones de transporte público hasta las tiendas y restaurantes más caros y en vogue de la ciudad. Este es el mejor barrio si quiere admirar y vivir en la zona noble del fascinante modernismo catalán, residir en una de sus características fincas regias, y convivir en perfecto equilibrio con la vibrante y lujosa vida comercial. Es ideal si desea caminar cada día por sus calles anchas y ordenadas, con fáciles conexiones de transporte, disponer de todo tipo de servicios y equipamientos incluidas escuelas concertadas o privadas, y disfrutar del ambiente más chic, cultural y cosmopolita de Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8118.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98378398', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/af/08/1c/1027086647.jpg', 'externalReference': '3000', 'numPhotos': 22, 'floor': '2', 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 90.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Petritxol', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3822216, 'longitude': 2.1741355, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98378398/', 'distance': '689', 'description': 'Fabulosa propiedad situada en el corazón del Barrio Gótico, en la emblemática Calle Petritxol, a escasos metros de la Plaza del Pi y Las Ramblas. Se trata de un elegante piso exterior de 90 m2 ubicada en una finca regia del año 1780.    La propiedad ha sido completamente renovada manteniendo y respetando elementos originales como las vigas de madera de los techos y los suelos de mosaico originales combinados con parquet de madera y hormigón pulido en la cocina y baños.     El resultado es un hogar elegante, moderno y acogedor. El edificio, que cuenta con un ascensor recientemente instalado, data de 1780. Ha pasado la ITE (inspección técnica del edificio) y ha sido rehabilitado recientemente.    Cocina abierta con electrodomésticos de alta calidad, integrados junto al salón comedor muy agradable que disfruta de dos grandes balcones orientados a la calle Petritxol.    Es un piso ideal tanto para vivir como para invertir, ya que alquilado, tiene una alta rentabilidad.  El piso, gracias a su rehabilitación integral de todo el edificio, combina las ventajas de una construcción nueva con elementos originales, lo que sin duda hacen de está vivienda una pieza única.    Una gran oportunidad de adquirir una vivienda única con amplias estancias y mucha luz en una de las zonas más demandadas del barrio Gótico.    La zona disfruta de todos los servicios, colegios, mercados como La Boquería o Santa Catalina, comercios y locales de ocio. La zona también está muy bien comunicada por transporte público, cercana a las líneas de metro L1 y L3, y líneas de autobús que atraviesan la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5389.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso en Calle de Petritxol'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98378398', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/af/08/1c/1027086647.jpg', 'externalReference': '3000', 'numPhotos': 22, 'floor': '2', 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 90.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Petritxol', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3822216, 'longitude': 2.1741355, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98378398/', 'distance': '689', 'description': 'Fabulosa propiedad situada en el corazón del Barrio Gótico, en la emblemática Calle Petritxol, a escasos metros de la Plaza del Pi y Las Ramblas. Se trata de un elegante piso exterior de 90 m2 ubicada en una finca regia del año 1780.    La propiedad ha sido completamente renovada manteniendo y respetando elementos originales como las vigas de madera de los techos y los suelos de mosaico originales combinados con parquet de madera y hormigón pulido en la cocina y baños.     El resultado es un hogar elegante, moderno y acogedor. El edificio, que cuenta con un ascensor recientemente instalado, data de 1780. Ha pasado la ITE (inspección técnica del edificio) y ha sido rehabilitado recientemente.    Cocina abierta con electrodomésticos de alta calidad, integrados junto al salón comedor muy agradable que disfruta de dos grandes balcones orientados a la calle Petritxol.    Es un piso ideal tanto para vivir como para invertir, ya que alquilado, tiene una alta rentabilidad.  El piso, gracias a su rehabilitación integral de todo el edificio, combina las ventajas de una construcción nueva con elementos originales, lo que sin duda hacen de está vivienda una pieza única.    Una gran oportunidad de adquirir una vivienda única con amplias estancias y mucha luz en una de las zonas más demandadas del barrio Gótico.    La zona disfruta de todos los servicios, colegios, mercados como La Boquería o Santa Catalina, comercios y locales de ocio. La zona también está muy bien comunicada por transporte público, cercana a las líneas de metro L1 y L3, y líneas de autobús que atraviesan la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5389.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso en Calle de Petritxol'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98264311', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b9/b6/8a/1006013108.jpg', 'externalReference': '3855V_6', 'numPhotos': 46, 'floor': '6', 'price': 2650000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 195.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3919731, 'longitude': 2.1693451, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98264311/', 'distance': '501', 'description': 'Este espectacular y exclusivo ático de 101m2 construidos y 94m2 de terraza viene distribuido en un amplio y luminoso salón comedor con salida a la magnifíca terraza con doble altura. El suelo es de madera flotante que proporciona una sensación de relajación gracias a sus zonas ajardinadas. Con posbilidades de amueblar con una zona chill out o un agradable comedor exterior donde disfrutar las tardes de verano. Las increíbles vistas que proporciona no te dejarán indiferente.  La cocina es abierta al comedor con isleta y barra de desayuno. Viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr) y tiene acceso a la zona de aguas independiente. La zona de noche consta de un dormitorio máster suite con salida a un amplio balcón, un vestidor y un baño con bañera ovalada y plato de ducha.  El segundo dormitorio también en suite y con salida al balcón. Ambos dormitorios cuentan con armarios empotrados. Todas las estancias disponen de aire acondicionado y calefacción por conductos, domótica, suelos de parqué, carpintería de aluminio y cristales dobles. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 13590.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Ático en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98264311', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b9/b6/8a/1006013108.jpg', 'externalReference': '3855V_6', 'numPhotos': 46, 'floor': '6', 'price': 2650000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 195.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3919731, 'longitude': 2.1693451, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98264311/', 'distance': '501', 'description': 'Este espectacular y exclusivo ático de 101m2 construidos y 94m2 de terraza viene distribuido en un amplio y luminoso salón comedor con salida a la magnifíca terraza con doble altura. El suelo es de madera flotante que proporciona una sensación de relajación gracias a sus zonas ajardinadas. Con posbilidades de amueblar con una zona chill out o un agradable comedor exterior donde disfrutar las tardes de verano. Las increíbles vistas que proporciona no te dejarán indiferente.  La cocina es abierta al comedor con isleta y barra de desayuno. Viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr) y tiene acceso a la zona de aguas independiente. La zona de noche consta de un dormitorio máster suite con salida a un amplio balcón, un vestidor y un baño con bañera ovalada y plato de ducha.  El segundo dormitorio también en suite y con salida al balcón. Ambos dormitorios cuentan con armarios empotrados. Todas las estancias disponen de aire acondicionado y calefacción por conductos, domótica, suelos de parqué, carpintería de aluminio y cristales dobles. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 13590.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Ático en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98261311', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f2/8a/bd/1005921523.jpg', 'externalReference': '3855V_3', 'numPhotos': 42, 'floor': '1', 'price': 1925000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 168.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3890208, 'longitude': 2.1642732, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98261311/', 'distance': '487', 'description': 'Exclusiva vivienda de 143m2 construidos y 23m2 de terraza, distribuidos en un luminoso salón comedor con salida a dos agradables balcones. La cocina es abierta y viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr). A través del distribuidor accedemos a la zona de noche, donde encontraremos la habitación master suite con salida a la espectacular terraza, este dormitorio dispone de un amplio vestidor y un baño completo con plato de ducha. La segunda habitación también es doble y tiene justo en frente un baño completo con bañera. Ambas habitaciones tienen armarios empotrados y vienen diseñadas con materiales de alta calidad. Todas las estancias disponen de aire acondicionado y calefacción por conductos, domótica, suelos de parqué, carpintería de aluminio y cristales dobles. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Ubicada en el corazón de Barcelona, Paseo de Gracia es la avenida más elegante y señorial de la ciudad, y en una de las ubicaciones más buscadas para los negocios. Una propuesta comercial muy atractiva. Ofrece una vida muy cómoda, con todos los servicios al alcance de su mano. Vivir en esta avenida significa disfrutar de exclusividad en el mismo centro de la ciudad. Disfruta de la exquisita arquitectura de sus edificios modernistas como son la Casa Batlló, la Casa Milá o la Casa Lleó Morera, mezclados con edificios del estilo moderno, clásico y neoclásico.  Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 11458.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98261311', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f2/8a/bd/1005921523.jpg', 'externalReference': '3855V_3', 'numPhotos': 42, 'floor': '1', 'price': 1925000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 168.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3890208, 'longitude': 2.1642732, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98261311/', 'distance': '487', 'description': 'Exclusiva vivienda de 143m2 construidos y 23m2 de terraza, distribuidos en un luminoso salón comedor con salida a dos agradables balcones. La cocina es abierta y viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr). A través del distribuidor accedemos a la zona de noche, donde encontraremos la habitación master suite con salida a la espectacular terraza, este dormitorio dispone de un amplio vestidor y un baño completo con plato de ducha. La segunda habitación también es doble y tiene justo en frente un baño completo con bañera. Ambas habitaciones tienen armarios empotrados y vienen diseñadas con materiales de alta calidad. Todas las estancias disponen de aire acondicionado y calefacción por conductos, domótica, suelos de parqué, carpintería de aluminio y cristales dobles. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Ubicada en el corazón de Barcelona, Paseo de Gracia es la avenida más elegante y señorial de la ciudad, y en una de las ubicaciones más buscadas para los negocios. Una propuesta comercial muy atractiva. Ofrece una vida muy cómoda, con todos los servicios al alcance de su mano. Vivir en esta avenida significa disfrutar de exclusividad en el mismo centro de la ciudad. Disfruta de la exquisita arquitectura de sus edificios modernistas como son la Casa Batlló, la Casa Milá o la Casa Lleó Morera, mezclados con edificios del estilo moderno, clásico y neoclásico.  Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 11458.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98256266', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f3/cf/34/1005719750.jpg', 'externalReference': '3855V_2', 'numPhotos': 43, 'floor': '5', 'price': 2680000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 157.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3924731, 'longitude': 2.1675451, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98256266/', 'distance': '585', 'description': 'Piso a estrenar con Piscina en Paseo de Gracia, Barcelona Exclusiva vivienda de 157m2 construidos, distribuidos en un amplio salón comedor. La cocina es abierta con isleta y barra de desayuno y viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr). La zona de noche dispone de 2 habitaciones; una doble y otra doble en suite con bañera ovalada y plato de ducha. Ambas disponen de armarios empotrado. Otro baño completo con plato de ducha por donde se accede al lavadero. En el recibidor encontramos un cómodo baño de cortesía y un armario empotrado. Todas las estancias disponen de suelo radiante, aire acondicionado y calefacción, domótica, suelos de roble, carpintería de madera y doble acristalamiento. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Ubicada en el corazón de Barcelona, Paseo de Gracia es la avenida más elegante y señorial de la ciudad, y en una de las ubicaciones más buscadas para los negocios. Una propuesta comercial muy atractiva. Ofrece una vida muy cómoda, con todos los servicios al alcance de su mano. Vivir en esta avenida significa disfrutar de exclusividad en el mismo centro de la ciudad. Disfruta de la exquisita arquitectura de sus edificios modernistas como son la Casa Batlló, la Casa Milá o la Casa Lleó Morera, mezclados con edificios del estilo moderno, clásico y neoclásico.  Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas. En total, la finca presenta 21 viviendas únicas, una azotea con piscina y zona chill out, un patio vegetal interior, mirador y zonas comunes. Distribuidos en 5 plantas más ático, viviendas de 1, 2 o 4 dormitorios, algunos con balcón y otros con agradables terrazas. El exclusivo ático, de un dormitorio y salida a una impresionante terraza con vistas inmejorables, el mejor producto para nuestros clientes más exigentes.  Cada tipología de vivienda tiene su personalidad, diferente distribución y distintas superficies, todas construidas con materiales de alta calidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 17070.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98256266', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f3/cf/34/1005719750.jpg', 'externalReference': '3855V_2', 'numPhotos': 43, 'floor': '5', 'price': 2680000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 157.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Paseo de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3924731, 'longitude': 2.1675451, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98256266/', 'distance': '585', 'description': 'Piso a estrenar con Piscina en Paseo de Gracia, Barcelona Exclusiva vivienda de 157m2 construidos, distribuidos en un amplio salón comedor. La cocina es abierta con isleta y barra de desayuno y viene completamente equipada con electrodomésticos de alta gama (entre ellos una nevera para vinos Liebherr). La zona de noche dispone de 2 habitaciones; una doble y otra doble en suite con bañera ovalada y plato de ducha. Ambas disponen de armarios empotrado. Otro baño completo con plato de ducha por donde se accede al lavadero. En el recibidor encontramos un cómodo baño de cortesía y un armario empotrado. Todas las estancias disponen de suelo radiante, aire acondicionado y calefacción, domótica, suelos de roble, carpintería de madera y doble acristalamiento. La elegante y única azotea ofrece un espacio único, con cantidad de vegetación y una estructura de madera que rodea la increible piscina, ideal para refrescarse en los meses mas calurosos. Ubicada en el corazón de Barcelona, Paseo de Gracia es la avenida más elegante y señorial de la ciudad, y en una de las ubicaciones más buscadas para los negocios. Una propuesta comercial muy atractiva. Ofrece una vida muy cómoda, con todos los servicios al alcance de su mano. Vivir en esta avenida significa disfrutar de exclusividad en el mismo centro de la ciudad. Disfruta de la exquisita arquitectura de sus edificios modernistas como son la Casa Batlló, la Casa Milá o la Casa Lleó Morera, mezclados con edificios del estilo moderno, clásico y neoclásico.  Su situación goza de una comunicación excelente, y la experiencia única de vivir en Paseo de Gracia; rodeada de las mejores tiendas de moda, hoteles, restaurantes de alta categoría y los ejemplos más representativos del modernismo. Un lujo al alcance de pocos.  La obra de rehabilitación de este edificio neoclásico tradicional se ha llevado a cabo con los más altos estándares y detalles. Se ha buscado fusionar lo más distinguido del pasado y lo más funcional del futuro. Su diseño es totalmente vanguardista y cuenta con todas las comodidades de las construcciones más modernas. En total, la finca presenta 21 viviendas únicas, una azotea con piscina y zona chill out, un patio vegetal interior, mirador y zonas comunes. Distribuidos en 5 plantas más ático, viviendas de 1, 2 o 4 dormitorios, algunos con balcón y otros con agradables terrazas. El exclusivo ático, de un dormitorio y salida a una impresionante terraza con vistas inmejorables, el mejor producto para nuestros clientes más exigentes.  Cada tipología de vivienda tiene su personalidad, diferente distribución y distintas superficies, todas construidas con materiales de alta calidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 17070.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Paseo de Gràcia'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98000858', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8b/d9/71/997711176.jpg', 'externalReference': '3835V', 'numPhotos': 36, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 114.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3902528, 'longitude': 2.1608339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98000858/', 'distance': '804', 'description': 'Espectacular y exclusiva vivienda de 114m2, distribuida en un amplio recibidor con paredes de ladrillo visto que conducen a una luminosa habitación doble con armarios empotrados y acceso a una pequeña salida exterior. Un baño completo con plato de ducha. La cocina es abierta y viene completamente equipada con electrodomésticos y placas de inducción. El suelo es hidráulico. Dispone de zona de aguas independiente. Un amplio y luminoso comedor con dos grandes ventanales y vistas al patio del Eixample. El dormitorio principal con baño en suite; con plato de ducha, bañera de hidromasaje y suelos de microcemento. Orientado al exterior y también con armarios empotrados. El piso incluye sistema de ósmosis en la cocina, aire acodicionado, calefacción, suelos de parqué y persianas eléctricas. Ubicado en Rambla Catalunya, una de las calles más exclusivas de la ciudad, en una 5º planta de una magnífica finca regia con servicio de consejería y ascensir. La vivienda goza de mucha tranquilidad a pesar de su ubicación tan céntrica. Con VISITA SEGURA de Walter Haus podrás seguir alquilando y vendiendo tu piso con total seguridad. Nuestras viviendas y las visitas que realizamos están libres de Covid-19 gracias al protocolo que hemos desarrollado: •Visitas Virtuales •Desinfección con ozono •Kit de seguridad •Firma digital Todo para que puedas seguir alquilando y vendiendo tu piso con total normalidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 7719.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98000858', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8b/d9/71/997711176.jpg', 'externalReference': '3835V', 'numPhotos': 36, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 114.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3902528, 'longitude': 2.1608339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98000858/', 'distance': '804', 'description': 'Espectacular y exclusiva vivienda de 114m2, distribuida en un amplio recibidor con paredes de ladrillo visto que conducen a una luminosa habitación doble con armarios empotrados y acceso a una pequeña salida exterior. Un baño completo con plato de ducha. La cocina es abierta y viene completamente equipada con electrodomésticos y placas de inducción. El suelo es hidráulico. Dispone de zona de aguas independiente. Un amplio y luminoso comedor con dos grandes ventanales y vistas al patio del Eixample. El dormitorio principal con baño en suite; con plato de ducha, bañera de hidromasaje y suelos de microcemento. Orientado al exterior y también con armarios empotrados. El piso incluye sistema de ósmosis en la cocina, aire acodicionado, calefacción, suelos de parqué y persianas eléctricas. Ubicado en Rambla Catalunya, una de las calles más exclusivas de la ciudad, en una 5º planta de una magnífica finca regia con servicio de consejería y ascensir. La vivienda goza de mucha tranquilidad a pesar de su ubicación tan céntrica. Con VISITA SEGURA de Walter Haus podrás seguir alquilando y vendiendo tu piso con total seguridad. Nuestras viviendas y las visitas que realizamos están libres de Covid-19 gracias al protocolo que hemos desarrollado: •Visitas Virtuales •Desinfección con ozono •Kit de seguridad •Firma digital Todo para que puedas seguir alquilando y vendiendo tu piso con total normalidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 7719.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98676867', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5d/9f/10/1052038319.jpg', 'externalReference': 'KB1508', 'numPhotos': 25, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 132.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3904528, 'longitude': 2.1637339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98676867/', 'distance': '600', 'description': 'Excelente propiedad en la quinta planta de un edificio histórico de Rambla Catalunya, una de las mejores calles de Barcelona. En una de las zonas más lujosas nos encontramos con esta exclusiva propiedad que ofrece todas las comodidades de un moderno apartamento en un entorno único y con uno acabados interiores excelentes. Exterior a patio de manzana, dispone de grandes ventanales que inundan de luz sus estancias. Su entrada está perfectamente trabajada y nos ofrece calidez mediante sus preciosos ventanales y sus paredes originales. La moderna cocina, abierta al salón conjuga un precioso diseño con una excelente funcionalidad y su ubicación facilita mucho la accesibilidad al salón. El suelo es de madera natural. Una de las habitaciones con armarios empotrados, tiene salida a una terraza y goza de mucha luminosidad. Encontramos un baño completo con ducha y baldosas hidráulicas. La habitación principal es suite con armarios empotrados y dispone también de un enorme y luminoso baño con bañera de hidromasaje con cascada y amplia ducha. La habitación tiene amplios ventanales también que le dan luz y vistas despejadas.  El inmueble ha sido recientemente renovado con acabados de máxima calidad e insonorizado en su totalidad, dispone de persianas eléctricas, aire acondicionado por conductos y calefacción por gas natural. El edificio dispone de conserje a jornada completa y ascensor. La ubicación es excelente, cerca del transporte público, en el cuadrado de oro de Barcelona, en una de las mejores calles y a escasos pasos de Passeig de gràcia o Plaza Catalunya. Un pedazo de la historia de Barcelona en una de las mejore ubicaciones de la ciudad. Estaremos encantados de poder mostrarselo.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6667.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98676867', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5d/9f/10/1052038319.jpg', 'externalReference': 'KB1508', 'numPhotos': 25, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 132.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3904528, 'longitude': 2.1637339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98676867/', 'distance': '600', 'description': 'Excelente propiedad en la quinta planta de un edificio histórico de Rambla Catalunya, una de las mejores calles de Barcelona. En una de las zonas más lujosas nos encontramos con esta exclusiva propiedad que ofrece todas las comodidades de un moderno apartamento en un entorno único y con uno acabados interiores excelentes. Exterior a patio de manzana, dispone de grandes ventanales que inundan de luz sus estancias. Su entrada está perfectamente trabajada y nos ofrece calidez mediante sus preciosos ventanales y sus paredes originales. La moderna cocina, abierta al salón conjuga un precioso diseño con una excelente funcionalidad y su ubicación facilita mucho la accesibilidad al salón. El suelo es de madera natural. Una de las habitaciones con armarios empotrados, tiene salida a una terraza y goza de mucha luminosidad. Encontramos un baño completo con ducha y baldosas hidráulicas. La habitación principal es suite con armarios empotrados y dispone también de un enorme y luminoso baño con bañera de hidromasaje con cascada y amplia ducha. La habitación tiene amplios ventanales también que le dan luz y vistas despejadas.  El inmueble ha sido recientemente renovado con acabados de máxima calidad e insonorizado en su totalidad, dispone de persianas eléctricas, aire acondicionado por conductos y calefacción por gas natural. El edificio dispone de conserje a jornada completa y ascensor. La ubicación es excelente, cerca del transporte público, en el cuadrado de oro de Barcelona, en una de las mejores calles y a escasos pasos de Passeig de gràcia o Plaza Catalunya. Un pedazo de la historia de Barcelona en una de las mejore ubicaciones de la ciudad. Estaremos encantados de poder mostrarselo.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6667.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': True, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99119853', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/fd/90/38/1034166911.jpg', 'externalReference': 'PBARDE 39', 'numPhotos': 51, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 170.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3873408, 'longitude': 2.1621522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99119853/', 'distance': '633', 'description': 'Terraza soleada de 40 metros orientada al mar, en una propiedad de obra nueva que da a las 2 fachadas, con acabados de altísima calidad, suelos radiantes, hidrotermia, domótica, reguladores de la intensidad de la luz, y todo el glamour que caracteriza a este barrio del Eixample de Barcelona.  La vivienda está ubicada a 100 metros de Plaza Universidad, en una finca completamente rehabilitada con ascensor.  A la entrada a la izquierda encontramos una elegante y moderna cocina abierta al salón comedor, con salida a un balcón que discurre por la calle Diputació. En esta zona también se halla un aseo de cortesía, el equipo de hidrotermia y el dispositivo táctil para la domótica de la casa.  En la parte posterior del piso se encuentran las dos habitaciones dobles, ambas con baños completos en suite, armarios con iluminación led interior, y mucha luz y sol.  A continuación del dormitorio principal encontramos la joya de la corona, su gran terraza. De la misma solo podemos añadir que, si a la funcionalidad y elegancia de unas magníficas reformas de alto standing, sumamos el hecho de tener este espacio exterior con sol todo el año, en el barrio seguramente con más Flow de Barcelona, podemos considerar que nos encontramos ante una vivienda única, difícilmente superable. Cabe señalar que es un piso con amplias estancias, se trata de 130 metros construidos para tres ambientes principales, salón y dos habitaciones dobles, con lo cual nos ofrece mucha versatilidad: salón comedor en la zona de los balcones que dan a la calle, como está distribuido ahora, o salón comedor hacia la terraza. Como hablamos de un solo piso por rellano, las dimensiones de la estancia trasera y la delantera son idénticas, o sea, que sin demasiado cambio se podría distribuir según nuestras preferencias. El barrio y esa calle en concreto se caracteriza por su encanto, con bares de moda, estilo, buen rollo y ese encanto urbanita de sus comercios y tiendas siempre a la vanguardia. Casi en los bajos del edificio encontramos una estación de Bicing, por si somos de los que prefieren moverse de esta forma por la ciudad.  Le invitamos a visitar este magnífico inmueble con QUATRECASES, y disfrutar de la experiencia.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4988.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99119853', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/fd/90/38/1034166911.jpg', 'externalReference': 'PBARDE 39', 'numPhotos': 51, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 170.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3873408, 'longitude': 2.1621522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99119853/', 'distance': '633', 'description': 'Terraza soleada de 40 metros orientada al mar, en una propiedad de obra nueva que da a las 2 fachadas, con acabados de altísima calidad, suelos radiantes, hidrotermia, domótica, reguladores de la intensidad de la luz, y todo el glamour que caracteriza a este barrio del Eixample de Barcelona.  La vivienda está ubicada a 100 metros de Plaza Universidad, en una finca completamente rehabilitada con ascensor.  A la entrada a la izquierda encontramos una elegante y moderna cocina abierta al salón comedor, con salida a un balcón que discurre por la calle Diputació. En esta zona también se halla un aseo de cortesía, el equipo de hidrotermia y el dispositivo táctil para la domótica de la casa.  En la parte posterior del piso se encuentran las dos habitaciones dobles, ambas con baños completos en suite, armarios con iluminación led interior, y mucha luz y sol.  A continuación del dormitorio principal encontramos la joya de la corona, su gran terraza. De la misma solo podemos añadir que, si a la funcionalidad y elegancia de unas magníficas reformas de alto standing, sumamos el hecho de tener este espacio exterior con sol todo el año, en el barrio seguramente con más Flow de Barcelona, podemos considerar que nos encontramos ante una vivienda única, difícilmente superable. Cabe señalar que es un piso con amplias estancias, se trata de 130 metros construidos para tres ambientes principales, salón y dos habitaciones dobles, con lo cual nos ofrece mucha versatilidad: salón comedor en la zona de los balcones que dan a la calle, como está distribuido ahora, o salón comedor hacia la terraza. Como hablamos de un solo piso por rellano, las dimensiones de la estancia trasera y la delantera son idénticas, o sea, que sin demasiado cambio se podría distribuir según nuestras preferencias. El barrio y esa calle en concreto se caracteriza por su encanto, con bares de moda, estilo, buen rollo y ese encanto urbanita de sus comercios y tiendas siempre a la vanguardia. Casi en los bajos del edificio encontramos una estación de Bicing, por si somos de los que prefieren moverse de esta forma por la ciudad.  Le invitamos a visitar este magnífico inmueble con QUATRECASES, y disfrutar de la experiencia.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4988.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98192535', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/eb/3a/00/1003587995.jpg', 'externalReference': 'W-02I8M0', 'numPhotos': 31, 'floor': '5', 'price': 1619000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 207.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle del Tenor Viñas', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sarrià-Sant Gervasi', 'country': 'es', 'neighborhood': 'Sant Gervasi - Galvany', 'latitude': 41.3937255, 'longitude': 2.1418776, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98192535/', 'distance': '2426', 'description': 'Espectacular ático con terraza en Turó Parc En una de las mejores fincas de la zona se sitúa este ático con una espectacular terraza de 135 metros. Se trata de un piso de 142 metros cuadrados, reformado, en el que antiguamente tenía 4 dormitorios, y ahora con la reforma tiene 2 grandes suites. El piso tiene un bonito recibidor que nos conduce a la zona de día, una bonita cocina con una zona de lavadero y al esplendido salón comedor con chimenea de mármol y salida directa a la terraza. En el pasillo encontramos un aseo de cortesía y la zona de noche con las 2 magníficas suites también con acceso a la terraza. La terraza tiene forma de L pudiendo crear en ella diferentes ambientes.  Se trata de una finca de lujo, con servicio de portería, 2 ascensores y posibilidad de alquilar parking en la misma finca. El Turó Parc es una de las zonas más demandadas de la ciudad. La elegancia y el prestigio son las características que definen tanto sus edificios como sus habitantes. Se trata de una zona muy segura, con todo tipo de comercios, servicios y ocio. El Turó Parc es la esencia del espíritu más sofisticado de Barcelona, sin perder al mismo tiempo la dimensión más pura y la calidez del barrio.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 7821.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': 'Sant Gervasi - Galvany, Barcelona', 'title': 'Ático en Calle del Tenor Viñas'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98192535', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/eb/3a/00/1003587995.jpg', 'externalReference': 'W-02I8M0', 'numPhotos': 31, 'floor': '5', 'price': 1619000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 207.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle del Tenor Viñas', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sarrià-Sant Gervasi', 'country': 'es', 'neighborhood': 'Sant Gervasi - Galvany', 'latitude': 41.3937255, 'longitude': 2.1418776, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98192535/', 'distance': '2426', 'description': 'Espectacular ático con terraza en Turó Parc En una de las mejores fincas de la zona se sitúa este ático con una espectacular terraza de 135 metros. Se trata de un piso de 142 metros cuadrados, reformado, en el que antiguamente tenía 4 dormitorios, y ahora con la reforma tiene 2 grandes suites. El piso tiene un bonito recibidor que nos conduce a la zona de día, una bonita cocina con una zona de lavadero y al esplendido salón comedor con chimenea de mármol y salida directa a la terraza. En el pasillo encontramos un aseo de cortesía y la zona de noche con las 2 magníficas suites también con acceso a la terraza. La terraza tiene forma de L pudiendo crear en ella diferentes ambientes.  Se trata de una finca de lujo, con servicio de portería, 2 ascensores y posibilidad de alquilar parking en la misma finca. El Turó Parc es una de las zonas más demandadas de la ciudad. La elegancia y el prestigio son las características que definen tanto sus edificios como sus habitantes. Se trata de una zona muy segura, con todo tipo de comercios, servicios y ocio. El Turó Parc es la esencia del espíritu más sofisticado de Barcelona, sin perder al mismo tiempo la dimensión más pura y la calidez del barrio.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 7821.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': 'Sant Gervasi - Galvany, Barcelona', 'title': 'Ático en Calle del Tenor Viñas'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '89103723', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b0/f6/f1/976630614.jpg', 'externalReference': '019264', 'numPhotos': 31, 'price': 768000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 149.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3874885, 'longitude': 2.1594455, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/89103723/', 'distance': '859', 'description': 'Exclusivo piso de diseño y obra nueva a estrenar de 149m² situado en calle Diputació, junto la calle Muntaner. Dispone de un amplio y luminoso salón comedor con cocina independiente, 1 espacioso recibidor, 2 habitaciones dobles suite (25m² y 14m² respectivamente), 2 baños completos y 1 aseo de cortesía. Excelentes acabados. Cuenta con suelos de mármol, aire acondicionado (frío - calor), calefacción a gas y carpintería exterior de aluminio. Exterior y soleado. Ubicado en una finca regia de 1886 rehabilitada que dispone de una gran terraza comunitaria, un espacio de 60m² con zona “chill out” y unas preciosas vistas de Barcelona. En la rehabilitación se han utilizado los mejores materiales con un diseño muy elegante, creando espacios actuales y acogedores. El proyecto de reforma ha sido realizado por Jaime Beriestain Studio, que cuenta con reconocimiento de nivel mundial. Muy bien comunicado con transporte público, autobuses y metro (parada- Universitat). Una magnífica oportunidad para adquirir una lujosa vivienda a estrenar en el corazón de Barcelona. "Contacte con nosotros para solicitar más información o visitar el inmueble".', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5154.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '89103723', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/b0/f6/f1/976630614.jpg', 'externalReference': '019264', 'numPhotos': 31, 'price': 768000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 149.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3874885, 'longitude': 2.1594455, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/89103723/', 'distance': '859', 'description': 'Exclusivo piso de diseño y obra nueva a estrenar de 149m² situado en calle Diputació, junto la calle Muntaner. Dispone de un amplio y luminoso salón comedor con cocina independiente, 1 espacioso recibidor, 2 habitaciones dobles suite (25m² y 14m² respectivamente), 2 baños completos y 1 aseo de cortesía. Excelentes acabados. Cuenta con suelos de mármol, aire acondicionado (frío - calor), calefacción a gas y carpintería exterior de aluminio. Exterior y soleado. Ubicado en una finca regia de 1886 rehabilitada que dispone de una gran terraza comunitaria, un espacio de 60m² con zona “chill out” y unas preciosas vistas de Barcelona. En la rehabilitación se han utilizado los mejores materiales con un diseño muy elegante, creando espacios actuales y acogedores. El proyecto de reforma ha sido realizado por Jaime Beriestain Studio, que cuenta con reconocimiento de nivel mundial. Muy bien comunicado con transporte público, autobuses y metro (parada- Universitat). Una magnífica oportunidad para adquirir una lujosa vivienda a estrenar en el corazón de Barcelona. "Contacte con nosotros para solicitar más información o visitar el inmueble".', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5154.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98269623', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a3/9c/10/1006157929.jpg', 'externalReference': 'VB2112040-1', 'numPhotos': 28, 'floor': 'en', 'price': 369000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 70.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "Calle d'Aribau", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3948237, 'longitude': 2.1524215, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98269623/', 'distance': '1660', 'description': 'Piso con terraza en venta en Calle Aribau Esta vivienda está ubicada en la Calle Aribau, cerca de la Diagonal y Enric Granados. Es un entresuelo, de 63m2 construidos, tiene una excelente ubicación en una finca clásica que conserva los elementos originales de la época, con ascensor y terrado comunitario. La zona de día consta de un amplio salón-comedor con salida a una terraza de 14m2, muy disfrutable, soleada y tranquila. Dispone de dos armarios para lavadora y secadora. Cocina equipada independiente, con la posibilidad de poderse abrir al salón-comedor. La zona de noche tiene un dormitorio principal y un baño completo en suite, un segundo dormitorio/despacho adjunto, con salida a la terraza. Tiene también baño completo con ducha. Suelos de parqué, aire acondicionado (frío/calor) calefacción, acumulador de agua, gran equipamiento de armarios, toldo eléctrico. ITE del edificio pasada.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 5271.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': "Piso en Calle d'Aribau"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98269623', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a3/9c/10/1006157929.jpg', 'externalReference': 'VB2112040-1', 'numPhotos': 28, 'floor': 'en', 'price': 369000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 70.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "Calle d'Aribau", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3948237, 'longitude': 2.1524215, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98269623/', 'distance': '1660', 'description': 'Piso con terraza en venta en Calle Aribau Esta vivienda está ubicada en la Calle Aribau, cerca de la Diagonal y Enric Granados. Es un entresuelo, de 63m2 construidos, tiene una excelente ubicación en una finca clásica que conserva los elementos originales de la época, con ascensor y terrado comunitario. La zona de día consta de un amplio salón-comedor con salida a una terraza de 14m2, muy disfrutable, soleada y tranquila. Dispone de dos armarios para lavadora y secadora. Cocina equipada independiente, con la posibilidad de poderse abrir al salón-comedor. La zona de noche tiene un dormitorio principal y un baño completo en suite, un segundo dormitorio/despacho adjunto, con salida a la terraza. Tiene también baño completo con ducha. Suelos de parqué, aire acondicionado (frío/calor) calefacción, acumulador de agua, gran equipamiento de armarios, toldo eléctrico. ITE del edificio pasada.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 5271.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': "Piso en Calle d'Aribau"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99268088', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/1d/34/d4/1038618419.jpg', 'externalReference': 'VB2210039', 'numPhotos': 28, 'floor': '3', 'price': 299000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 62.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de la Riereta', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3778121, 'longitude': 2.1688796, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99268088/', 'distance': '1076', 'description': 'Piso reformado con terraza en venta en la calle Riereta Preciosa vivienda totalmente reformada en 2019 situada a escasos metros de la Rambla del Raval y muy bien ubicada en el centro de Barcelona. La calle Riereta es una calle muy tranquila en la que se combinan edificios clásicos y edificios de recién construcción. El piso se encuentra en una tercera planta real en una finca de 1860 SIN ASCENSOR, rehabilitada y en muy buen estado de conservación, con terrado comunitario practicable con estupendas vistas a la ciudad de Barcelona y a la montaña de Montjuic. Se distribuye de la siguiente forma: dos habitaciones dobles exteriores a calle, baño completo, zona de aguas, cocina abierta al comedor, salón independiente con salida a terraza a nivel que orienta a un tranquilo y amplio patio de manzana. Doble orientación NE y SO. La propiedad se reformó en 2019. Los suelos son de gres imitación madera. Cerramientos de doble cristal en todas las estancias, aire acondicionado y calefacción por splits, puerta blindada, cocina equipada con todos los electrodomésticos, volta catalana y vigas vistas de madera, termo de agua caliente de 100L y alarma de Securitas Direct. Es un piso ideal como piso vacacional o como inversión por su alta rentabilidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 4823.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de la Riereta'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99268088', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/1d/34/d4/1038618419.jpg', 'externalReference': 'VB2210039', 'numPhotos': 28, 'floor': '3', 'price': 299000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 62.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de la Riereta', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3778121, 'longitude': 2.1688796, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99268088/', 'distance': '1076', 'description': 'Piso reformado con terraza en venta en la calle Riereta Preciosa vivienda totalmente reformada en 2019 situada a escasos metros de la Rambla del Raval y muy bien ubicada en el centro de Barcelona. La calle Riereta es una calle muy tranquila en la que se combinan edificios clásicos y edificios de recién construcción. El piso se encuentra en una tercera planta real en una finca de 1860 SIN ASCENSOR, rehabilitada y en muy buen estado de conservación, con terrado comunitario practicable con estupendas vistas a la ciudad de Barcelona y a la montaña de Montjuic. Se distribuye de la siguiente forma: dos habitaciones dobles exteriores a calle, baño completo, zona de aguas, cocina abierta al comedor, salón independiente con salida a terraza a nivel que orienta a un tranquilo y amplio patio de manzana. Doble orientación NE y SO. La propiedad se reformó en 2019. Los suelos son de gres imitación madera. Cerramientos de doble cristal en todas las estancias, aire acondicionado y calefacción por splits, puerta blindada, cocina equipada con todos los electrodomésticos, volta catalana y vigas vistas de madera, termo de agua caliente de 100L y alarma de Securitas Direct. Es un piso ideal como piso vacacional o como inversión por su alta rentabilidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 4823.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de la Riereta'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98985637', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/2d/73/6b/1030519082.jpg', 'externalReference': 'VB2209039', 'numPhotos': 27, 'floor': 'en', 'price': 325000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 69.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de Ribes', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'El Fort Pienc', 'latitude': 41.4015389, 'longitude': 2.1846789, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98985637/', 'distance': '1999', 'description': 'Piso en venta frente al Auditori y al Teatre Nacional En el barrio de Fortpienc, frente al Teatre Nacional y al Auditori de Barcelona, muy cerca dels Encants nous y de la Plaça de les Glòries, encontramos esta propiedad, situada en una finca clásica de 1890, en muy buen estado de conservación, con ascensor y con doble orientación. El piso se reformó en 2004 y actualmente su estado de conservación es muy bueno. Se vende completamente equipado y amueblado. Consta de 69m2 construidos, 57m2 útiles y dos balcones, el que da a calle de 2m2 y el que está en la habitación de 3,25m2. Se distribuye de la siguiente manera: salón independiente exterior a la calle Ribes, con salida directa a balcón, con orientación sur. Cocina abierta al comedor. Baño completo con ventilación natural. Dormitorio individual amplio con ventana a patio interior de la finca. Dormitorio doble con salida a balcón. La zona de aguas se encuentra en el balcón al lado de la habitación de matrimonio. Termo de agua caliente eléctrico, ventanas de aluminio, splits de aire frío y caliente. Cocina equipada con vitro, campana extractora, horno, lavaplatos y nevera-congelador. La ubicación de esta vivienda es inmejorable, cerca de todos los servicios, bien comunicado, con aparcamiento público frente al edificio, el centro comercial Glòries a 10 minutos caminando, transporte público (bus, metro, tranvía), comercios y restaurantes. ¡No dudes en contactar con nosotros para ver esta magnífica propiedad!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4710.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Fort Pienc, Barcelona', 'title': 'Piso en Calle de Ribes'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98985637', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/2d/73/6b/1030519082.jpg', 'externalReference': 'VB2209039', 'numPhotos': 27, 'floor': 'en', 'price': 325000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 69.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de Ribes', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'El Fort Pienc', 'latitude': 41.4015389, 'longitude': 2.1846789, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98985637/', 'distance': '1999', 'description': 'Piso en venta frente al Auditori y al Teatre Nacional En el barrio de Fortpienc, frente al Teatre Nacional y al Auditori de Barcelona, muy cerca dels Encants nous y de la Plaça de les Glòries, encontramos esta propiedad, situada en una finca clásica de 1890, en muy buen estado de conservación, con ascensor y con doble orientación. El piso se reformó en 2004 y actualmente su estado de conservación es muy bueno. Se vende completamente equipado y amueblado. Consta de 69m2 construidos, 57m2 útiles y dos balcones, el que da a calle de 2m2 y el que está en la habitación de 3,25m2. Se distribuye de la siguiente manera: salón independiente exterior a la calle Ribes, con salida directa a balcón, con orientación sur. Cocina abierta al comedor. Baño completo con ventilación natural. Dormitorio individual amplio con ventana a patio interior de la finca. Dormitorio doble con salida a balcón. La zona de aguas se encuentra en el balcón al lado de la habitación de matrimonio. Termo de agua caliente eléctrico, ventanas de aluminio, splits de aire frío y caliente. Cocina equipada con vitro, campana extractora, horno, lavaplatos y nevera-congelador. La ubicación de esta vivienda es inmejorable, cerca de todos los servicios, bien comunicado, con aparcamiento público frente al edificio, el centro comercial Glòries a 10 minutos caminando, transporte público (bus, metro, tranvía), comercios y restaurantes. ¡No dudes en contactar con nosotros para ver esta magnífica propiedad!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4710.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Fort Pienc, Barcelona', 'title': 'Piso en Calle de Ribes'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98374038', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/4a/c7/58/1009839184.jpg', 'externalReference': 'VB2207045', 'numPhotos': 47, 'floor': '3', 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 77.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Riereta', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3791652, 'longitude': 2.1708504, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98374038/', 'distance': '928', 'description': 'Loft de Obra Nueva con jardín y piscina en el centro histórico de Barcelona  Preciosa vivienda en edificio de obra nueva del 2021 en el centro de Barcelona. Se trata de una rehabilitación integral de una antigua fábrica textil de 1833, creando unas viviendas únicas de estilo neoyorquino con grande ventanales y techos de doble altura con vigas de madera y paredes de ladrillo visto. El piso estilo loft se encuentra en la planta tercera, tiene una superficie de 74 m2, más una terraza cubierta de 6 m2 que da a las zonas comunitarias. Los materiales utilizados son de la más alta calidad y además consta de algunos elementos recuperados. Se compone de cocina totalmente equipada, salón, comedor, un dormitorio doble con baño en suite, y otro baño completo. Además, se ha aprovechado de la altura de los techos para realizar un altillo de 12 m2 donde ahora se ubica otro dormitorio doble. El edificio cuenta con zonas comunes que incluyen piscina y solárium con impresionantes vistas a la ciudad, huertos urbanos, jardines verticales, sistema de climatización por Aerotermia, servicio conserjería, video vigilancia 24h, reciclaje de aguas pluviales, parking para bicicletas y un atrio en medio del complejo lleno de tragaluces y árboles. Una oportunidad única para vivir una nueva experiencia en la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6299.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de la Riereta'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98374038', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/4a/c7/58/1009839184.jpg', 'externalReference': 'VB2207045', 'numPhotos': 47, 'floor': '3', 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 77.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Riereta', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3791652, 'longitude': 2.1708504, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98374038/', 'distance': '928', 'description': 'Loft de Obra Nueva con jardín y piscina en el centro histórico de Barcelona  Preciosa vivienda en edificio de obra nueva del 2021 en el centro de Barcelona. Se trata de una rehabilitación integral de una antigua fábrica textil de 1833, creando unas viviendas únicas de estilo neoyorquino con grande ventanales y techos de doble altura con vigas de madera y paredes de ladrillo visto. El piso estilo loft se encuentra en la planta tercera, tiene una superficie de 74 m2, más una terraza cubierta de 6 m2 que da a las zonas comunitarias. Los materiales utilizados son de la más alta calidad y además consta de algunos elementos recuperados. Se compone de cocina totalmente equipada, salón, comedor, un dormitorio doble con baño en suite, y otro baño completo. Además, se ha aprovechado de la altura de los techos para realizar un altillo de 12 m2 donde ahora se ubica otro dormitorio doble. El edificio cuenta con zonas comunes que incluyen piscina y solárium con impresionantes vistas a la ciudad, huertos urbanos, jardines verticales, sistema de climatización por Aerotermia, servicio conserjería, video vigilancia 24h, reciclaje de aguas pluviales, parking para bicicletas y un atrio en medio del complejo lleno de tragaluces y árboles. Una oportunidad única para vivir una nueva experiencia en la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6299.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de la Riereta'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98272281', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/df/38/a0/1006238408.jpg', 'externalReference': 'VB2206060', 'numPhotos': 29, 'floor': 'en', 'price': 345000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 63.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle d'Enric Granados", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3923655, 'longitude': 2.1573188, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98272281/', 'distance': '1170', 'description': 'Piso reformado de 2 habitaciones en la Calle Enric Granados Situado en una de las calles más emblemáticas de Barcelona i del Eixample Esquerra, rodeado de todo tipo de servicios, restaurantes, cafeterías y muy bien comunicado, se encuentra este bonito, reformado y práctico piso ubicado en una finca Regia con estilo del 1900. La vivienda, de 63 m2, está para entrar a vivir y se encuentra en una planta baja por lo que disfruta de una agradable terraza, muy agradable y tranquila orientada a Noreste de 12 m2. El piso dispone de dos habitaciones dobles, y una de ellas tiene una galería con vistas a la terraza, ideal para ubicar un despacho, por ejemplo. La segunda, interior y con salida a patio de luces, completa Completa este práctico piso la cocina / salón desde donde también se accede a la terraza, que permite disfrutar del sol y el aire libre en un espacio alegre. Ven a visitar este bonito y céntrico piso en Barcelona!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5476.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': "Piso en Calle d'Enric Granados"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98272281', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/df/38/a0/1006238408.jpg', 'externalReference': 'VB2206060', 'numPhotos': 29, 'floor': 'en', 'price': 345000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 63.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle d'Enric Granados", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3923655, 'longitude': 2.1573188, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98272281/', 'distance': '1170', 'description': 'Piso reformado de 2 habitaciones en la Calle Enric Granados Situado en una de las calles más emblemáticas de Barcelona i del Eixample Esquerra, rodeado de todo tipo de servicios, restaurantes, cafeterías y muy bien comunicado, se encuentra este bonito, reformado y práctico piso ubicado en una finca Regia con estilo del 1900. La vivienda, de 63 m2, está para entrar a vivir y se encuentra en una planta baja por lo que disfruta de una agradable terraza, muy agradable y tranquila orientada a Noreste de 12 m2. El piso dispone de dos habitaciones dobles, y una de ellas tiene una galería con vistas a la terraza, ideal para ubicar un despacho, por ejemplo. La segunda, interior y con salida a patio de luces, completa Completa este práctico piso la cocina / salón desde donde también se accede a la terraza, que permite disfrutar del sol y el aire libre en un espacio alegre. Ven a visitar este bonito y céntrico piso en Barcelona!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5476.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': "Piso en Calle d'Enric Granados"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98271905', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/e5/49/6f/1006228158.jpg', 'externalReference': 'VB2206005', 'numPhotos': 41, 'floor': 'bj', 'price': 480000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 139.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "Calle d'en Carabassa", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3811984, 'longitude': 2.1775831, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98271905/', 'distance': '956', 'description': 'Piso en venta reformado con bodega de 47m2 al lado de la Iglesia de la Mercè A escasos pasos de la Basílica de la Mercè y del Moll de la Fusta, en el pleno centro del barrio Gótico con más historia de la ciudad, encontramos este apartamento de 92m2 construidos totalmente rehabilitado, situado en la primera planta de una finca de 1890 con ascensor, orientación Sur. El piso, gracias a su rehabilitación integral de todo el edificio, combina las ventajas de una construcción nueva con elementos originales, lo que sin duda hacen de está vivienda una pieza única. A destacar las zonas comunes con el terrado de uso comunitario con vistas a la ciudad y totalmente acondicionado con barbacoa, baño y sala de reuniones. Zona de parking para bicicletas en la entrada de la vivienda, y un largo etc. Sus 139m2 están compuestos de una bodega en la planta –1 de 47m2 totalmente habilitada y el piso de 92m2 que consta dde un amplio salón comedor con una cocina totalmente integrada y equipada, una suite con baño, una habitación semi doble y un baño completo. La zona de aguas está contigua a la cocina. Las ventanas del piso son de aluminio con rotura de puente térmico y doble cristal, para garantizar un aislamiento térmico y acústico. Sistema de eficiencia energética mediante aerotermia, los suelos están pavimentados con parquet en madera y los baños con gres porcelánico. Terrado de uso comunitario con vistas a la ciudad y totalmente acondicionado con barbacoa, baño y sala de reuniones. Si quiere vivir en el barrio gótico, no dudes en pedirnos visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3453.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': "Piso en Calle d'en Carabassa"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98271905', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/e5/49/6f/1006228158.jpg', 'externalReference': 'VB2206005', 'numPhotos': 41, 'floor': 'bj', 'price': 480000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 139.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "Calle d'en Carabassa", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3811984, 'longitude': 2.1775831, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98271905/', 'distance': '956', 'description': 'Piso en venta reformado con bodega de 47m2 al lado de la Iglesia de la Mercè A escasos pasos de la Basílica de la Mercè y del Moll de la Fusta, en el pleno centro del barrio Gótico con más historia de la ciudad, encontramos este apartamento de 92m2 construidos totalmente rehabilitado, situado en la primera planta de una finca de 1890 con ascensor, orientación Sur. El piso, gracias a su rehabilitación integral de todo el edificio, combina las ventajas de una construcción nueva con elementos originales, lo que sin duda hacen de está vivienda una pieza única. A destacar las zonas comunes con el terrado de uso comunitario con vistas a la ciudad y totalmente acondicionado con barbacoa, baño y sala de reuniones. Zona de parking para bicicletas en la entrada de la vivienda, y un largo etc. Sus 139m2 están compuestos de una bodega en la planta –1 de 47m2 totalmente habilitada y el piso de 92m2 que consta dde un amplio salón comedor con una cocina totalmente integrada y equipada, una suite con baño, una habitación semi doble y un baño completo. La zona de aguas está contigua a la cocina. Las ventanas del piso son de aluminio con rotura de puente térmico y doble cristal, para garantizar un aislamiento térmico y acústico. Sistema de eficiencia energética mediante aerotermia, los suelos están pavimentados con parquet en madera y los baños con gres porcelánico. Terrado de uso comunitario con vistas a la ciudad y totalmente acondicionado con barbacoa, baño y sala de reuniones. Si quiere vivir en el barrio gótico, no dudes en pedirnos visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3453.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': "Piso en Calle d'en Carabassa"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98271257', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f4/c7/a6/1006207841.jpg', 'externalReference': 'VB2203084-1', 'numPhotos': 34, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 110.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3928528, 'longitude': 2.1615339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98271257/', 'distance': '909', 'description': 'Piso de diseño en venta en Rambla Catalunya En la Rambla Catalunya, una de las calles más exclusivas de la ciudad encontramos esta magnífica vivienda en una preciosa finca regia con servicio de conserjería y ascensor. El piso consta de 110m2 y gracias a su altura y orientación, goza de mucha tranquilidad a pesar de su ubicación tan céntrica. Al entrar, un amplio pasillo con pared de ladrillo visto nos conduce a un dormitorio doble con armario empotrado y salida a una pequeña terraza. Sus puertas cristaleras confieren al piso una sensación maravillosa de espacio y luz. En la habitación contigua el lavadero con armario empotrado y en frente un baño completo con ducha. A continuación, la moderna cocina office, equipada con electrodomésticos de primera categoría y con espacio para mesa de 6 comensales. Seguidamente accedemos al amplio salón que gracias a su grandes ventanales y orientación a bonito patio de manzana goza de muchísima luz natural. El segundo dormitorio es el principal, orientado al exterior, con armarios empotrados y con baño completo con ducha y bañera de hidromasaje en suite. El piso dispone de suelos de parquet, calefacción por radiadores, aire acondicionado por conductos y ventanas con doble acristalamiento. ¡Contacta con nosotros hoy para visitar esta propiedad única en la zona más exclusiva de L’Eixample!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8000.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98271257', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/f4/c7/a6/1006207841.jpg', 'externalReference': 'VB2203084-1', 'numPhotos': 34, 'floor': '5', 'price': 880000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 110.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Rambla de Catalunya', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3928528, 'longitude': 2.1615339, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98271257/', 'distance': '909', 'description': 'Piso de diseño en venta en Rambla Catalunya En la Rambla Catalunya, una de las calles más exclusivas de la ciudad encontramos esta magnífica vivienda en una preciosa finca regia con servicio de conserjería y ascensor. El piso consta de 110m2 y gracias a su altura y orientación, goza de mucha tranquilidad a pesar de su ubicación tan céntrica. Al entrar, un amplio pasillo con pared de ladrillo visto nos conduce a un dormitorio doble con armario empotrado y salida a una pequeña terraza. Sus puertas cristaleras confieren al piso una sensación maravillosa de espacio y luz. En la habitación contigua el lavadero con armario empotrado y en frente un baño completo con ducha. A continuación, la moderna cocina office, equipada con electrodomésticos de primera categoría y con espacio para mesa de 6 comensales. Seguidamente accedemos al amplio salón que gracias a su grandes ventanales y orientación a bonito patio de manzana goza de muchísima luz natural. El segundo dormitorio es el principal, orientado al exterior, con armarios empotrados y con baño completo con ducha y bañera de hidromasaje en suite. El piso dispone de suelos de parquet, calefacción por radiadores, aire acondicionado por conductos y ventanas con doble acristalamiento. ¡Contacta con nosotros hoy para visitar esta propiedad única en la zona más exclusiva de L’Eixample!', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8000.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso en Rambla de Catalunya'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98269646', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/0e/44/3a/1006158045.jpg', 'externalReference': 'VB2112041-1', 'numPhotos': 34, 'floor': '1', 'price': 750000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 140.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de les Jonqueres', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3867007, 'longitude': 2.1744305, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98269646/', 'distance': '400', 'description': 'Piso tipo Loft en venta en la calle Jonqueres Este loft está situado en Born, muy cerca del Palau de la Musica, en un edificio original del 1870 que había sido un antiguo convento y se rehabilitó íntegramente en el año 1997. En la entrada del edificio hay un amplio recibidor que da acceso a la escalera y al ascensor. En el primer piso encontramos una zona comunitaria ajardinada central donde se ubicaba en el antiguo claustro, que da acceso a la propiedad. La vivienda es toda exterior, con amplios ventanales al tranquilo y silencioso espacio central del edificio. El loft se reformó hace unos 13 años y mantiene ese encanto bohemio tan característico de la zona. En la entrada encontramos el recibidor abierto al amplio salón-comedor con cocina abierta. Está rodeado de grandes ventanales con mucha luz. Tiene acceso a una amplia terraza de 40m2, una zona muy tranquila y luminosa. En la misma planta hay un dormitorio doble con baño completo y en la zona del altillo (planta escriturada) se encuentra el segundo dormitorio abierto al espacio del salón, también dispone de un baño completo en suite. El techo mide 4.50mts de alto y tiene bonitas vigas de madera, el suelo es de parque macizo (se pulirá a gusto del comprador). Además, la vivienda dispone de screens, aire acondicionado frío-calor por Split y calefacción individual por radiadores. La propiedad no dispone de parking en finca, pero existe la posibilidad de alquilar una plaza de aparcamiento en la misma manzana..', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5357.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso en Calle de les Jonqueres'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98269646', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/0e/44/3a/1006158045.jpg', 'externalReference': 'VB2112041-1', 'numPhotos': 34, 'floor': '1', 'price': 750000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 140.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de les Jonqueres', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3867007, 'longitude': 2.1744305, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98269646/', 'distance': '400', 'description': 'Piso tipo Loft en venta en la calle Jonqueres Este loft está situado en Born, muy cerca del Palau de la Musica, en un edificio original del 1870 que había sido un antiguo convento y se rehabilitó íntegramente en el año 1997. En la entrada del edificio hay un amplio recibidor que da acceso a la escalera y al ascensor. En el primer piso encontramos una zona comunitaria ajardinada central donde se ubicaba en el antiguo claustro, que da acceso a la propiedad. La vivienda es toda exterior, con amplios ventanales al tranquilo y silencioso espacio central del edificio. El loft se reformó hace unos 13 años y mantiene ese encanto bohemio tan característico de la zona. En la entrada encontramos el recibidor abierto al amplio salón-comedor con cocina abierta. Está rodeado de grandes ventanales con mucha luz. Tiene acceso a una amplia terraza de 40m2, una zona muy tranquila y luminosa. En la misma planta hay un dormitorio doble con baño completo y en la zona del altillo (planta escriturada) se encuentra el segundo dormitorio abierto al espacio del salón, también dispone de un baño completo en suite. El techo mide 4.50mts de alto y tiene bonitas vigas de madera, el suelo es de parque macizo (se pulirá a gusto del comprador). Además, la vivienda dispone de screens, aire acondicionado frío-calor por Split y calefacción individual por radiadores. La propiedad no dispone de parking en finca, pero existe la posibilidad de alquilar una plaza de aparcamiento en la misma manzana..', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5357.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso en Calle de les Jonqueres'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '91592832', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/72/64/da/925378429.jpg', 'externalReference': 'W-02JZPS', 'numPhotos': 40, 'floor': '2', 'price': 818000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 87.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3949048, 'longitude': 2.167361, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/91592832/', 'distance': '850', 'description': 'Finca regia renovada cerca de Paseo de Gracia\r Estamos encantados de ofrecer este impresionante apartamento de 2 dormitorios en un edificio histórico completamente renovado con 10 pisos impecables, ubicado justo al lado de la famosa avenida comercial de Paseo de Gracia de Barcelona.\r Cada hogar ha sido diseñado por expertos en estilo y funcionalidad. Mientras que las características arquitectónicas clásicas de Barcelona se han restaurado para impartir la esencia de la historia del edificio como una "finca regia".\r Un vestíbulo de cristal le da la bienvenida a la casa antes de entrar en la cocina de diseño contemporáneo que se abre a la sala de estar. Con dos balcones, esta casa está bien iluminada y tiene un sentido de conexión con la ciudad, ya que todas las habitaciones dan al exterior.\r Las zonas separadas de día y de noche imparten amplitud y privacidad, y en la parte trasera del apartamento encontramos la suite principal. Los amplios pisos de tablones de madera de roble alargan el espacio. Los armarios están inteligentemente integrados en todas partes. Los amplios baños están equipados con accesorios de primera calidad.\r Los detalles arquitectónicos restaurados incluyen las fachadas del edificio, los techos abovedados catalanes, la entrada y la escalera del edificio, además de integrar pisos hidráulicos originales en los baños.\r La propiedad cuenta con marcas de primera calidad y materiales de construcción para maximizar el confort: electrodomésticos Miele, aerotermia Mitsubishi, cocinas Bulthaup, electrodomésticos Duravit y más. Se han tomado medidas específicas para maximizar la privacidad y el control del sonido, como las nuevas ventanas de doble acristalamiento y los sustratos de piso reforzado.\r El elegante barrio del Eixample se caracteriza por su arquitectura visionaria modernista, tiendas independientes, boutiques elegantes y cultura del café.\r La propiedad está situada en el corazón del Eixample Quadrat d’Or (‘Square Golden Square’), a solo una cuadra de la avenida arbolada del Passeig de Gràcia.\r Barcelona se ha transformado desde los Juegos Olímpicos de 1992, y la capital catalana se ha convertido en la meca de los creativos y emprendedores de todo el mundo gracias a su creciente reputación como un importante centro de nuevas empresas e innovación tecnológica.\r La segunda ciudad de España continúa liderando la cocina internacional de vanguardia y actualmente alberga más de 30 restaurantes con estrellas Michelin. Una de las ciudades "inteligentes" líderes en Europa, sus credenciales incluyen 500 kilómetros de fibra óptica, WiFi gratis a través de su alumbrado público y sensores para monitorear la calidad del aire. La propiedad tiene una gran demanda, particularmente en los barrios principales del casco antiguo de Barcelona y el Eixample, el núcleo cultural y vibrante de la ciudad.\r En la década de 1900, este codiciado barrio fue construido por la burguesía de Barcelona, que compitió para crear las casas más estéticamente refinadas. En los últimos años, esta área ha experimentado un gran renacimiento y se ha convertido en un imán para los compradores internacionales, especialmente con la concentración de una serie de desarrollos de lujo.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 9402.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '91592832', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/72/64/da/925378429.jpg', 'externalReference': 'W-02JZPS', 'numPhotos': 40, 'floor': '2', 'price': 818000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 87.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3949048, 'longitude': 2.167361, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/91592832/', 'distance': '850', 'description': 'Finca regia renovada cerca de Paseo de Gracia\r Estamos encantados de ofrecer este impresionante apartamento de 2 dormitorios en un edificio histórico completamente renovado con 10 pisos impecables, ubicado justo al lado de la famosa avenida comercial de Paseo de Gracia de Barcelona.\r Cada hogar ha sido diseñado por expertos en estilo y funcionalidad. Mientras que las características arquitectónicas clásicas de Barcelona se han restaurado para impartir la esencia de la historia del edificio como una "finca regia".\r Un vestíbulo de cristal le da la bienvenida a la casa antes de entrar en la cocina de diseño contemporáneo que se abre a la sala de estar. Con dos balcones, esta casa está bien iluminada y tiene un sentido de conexión con la ciudad, ya que todas las habitaciones dan al exterior.\r Las zonas separadas de día y de noche imparten amplitud y privacidad, y en la parte trasera del apartamento encontramos la suite principal. Los amplios pisos de tablones de madera de roble alargan el espacio. Los armarios están inteligentemente integrados en todas partes. Los amplios baños están equipados con accesorios de primera calidad.\r Los detalles arquitectónicos restaurados incluyen las fachadas del edificio, los techos abovedados catalanes, la entrada y la escalera del edificio, además de integrar pisos hidráulicos originales en los baños.\r La propiedad cuenta con marcas de primera calidad y materiales de construcción para maximizar el confort: electrodomésticos Miele, aerotermia Mitsubishi, cocinas Bulthaup, electrodomésticos Duravit y más. Se han tomado medidas específicas para maximizar la privacidad y el control del sonido, como las nuevas ventanas de doble acristalamiento y los sustratos de piso reforzado.\r El elegante barrio del Eixample se caracteriza por su arquitectura visionaria modernista, tiendas independientes, boutiques elegantes y cultura del café.\r La propiedad está situada en el corazón del Eixample Quadrat d’Or (‘Square Golden Square’), a solo una cuadra de la avenida arbolada del Passeig de Gràcia.\r Barcelona se ha transformado desde los Juegos Olímpicos de 1992, y la capital catalana se ha convertido en la meca de los creativos y emprendedores de todo el mundo gracias a su creciente reputación como un importante centro de nuevas empresas e innovación tecnológica.\r La segunda ciudad de España continúa liderando la cocina internacional de vanguardia y actualmente alberga más de 30 restaurantes con estrellas Michelin. Una de las ciudades "inteligentes" líderes en Europa, sus credenciales incluyen 500 kilómetros de fibra óptica, WiFi gratis a través de su alumbrado público y sensores para monitorear la calidad del aire. La propiedad tiene una gran demanda, particularmente en los barrios principales del casco antiguo de Barcelona y el Eixample, el núcleo cultural y vibrante de la ciudad.\r En la década de 1900, este codiciado barrio fue construido por la burguesía de Barcelona, que compitió para crear las casas más estéticamente refinadas. En los últimos años, esta área ha experimentado un gran renacimiento y se ha convertido en un imán para los compradores internacionales, especialmente con la concentración de una serie de desarrollos de lujo.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 9402.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '96603203', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/99/69/76/951332285.jpg', 'externalReference': 'BHHS-004107', 'numPhotos': 40, 'floor': '6', 'price': 560000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 62.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3967221, 'longitude': 2.1548047, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96603203/', 'distance': '1615', 'description': 'PISO ALTO Y SOLEADO EN FINCA MODERNA DE LA PARTE ALTA DEL EIXAMPLE EL PISO IDEAL EN FINCA MODERNA BERKSHIRE\xa0HATHAWAY\xa0HomeServices\xa0Barcelona, consultora especializada en la comercialización de propiedades exclusivas en las mejores zonas de Barcelona, les ofrece este fantástico piso, situado en la parte alta del barrio del Eixample de Barcelona, junto a la Rambla Catalunya. Según entramos en el piso, nos encontramos con la barra baja que separa el hall de la\xa0cocina\xa0la izquierda. Al frente\xa0nos dirigimos\xa0al salón comedor con salida al gran ventanal exterior a la calle, con vistas y muy soleado durante todo el día. También tiene un estrecho balcón, por el que se mueven las persianas correderas. El salón está orientado a Sur, y es exterior a la calle\xa0Córsega, que es de poquísimo tránsito en este\xa0tramo, ya que\xa0su acceso se inicia desde la adyacente Rambla de\xa0Catalunya. La cocina está equipada con electrodomésticos y cruzando una puerta se accede al lavadero con espacio para lavadora, secadora y lavabo. Los muebles de diseño, y electrodomésticos que ven en las fotografías, no están incluidos en el precio. Desde el salón, a través de una puerta que separa la zona de día de la zona de noche, accedemos a un distribuidor con un baño completo al frente, con bañera, y las dos habitaciones, una a cada lado, son dobles y tienen armarios empotrados. Una es exterior al pequeño balcón que da a la calle, y la otra da al vestíbulo privado de vecinos de la planta. El piso tiene calefacción por radiadores, caldera y acumulador, aire acondicionado por conductos a todas las estancias, suelos de parquet... \xa0Además, \xa0está muy bien distribuido, con muy buen gusto, y sin espacios perdidos. Esta finca fue construida en el 1967, y en el 2007\xa0Metrovacesa\xa0la adaptó para tener viviendas cómodas y accesibles, además con buen gusto y diseño, como se puede apreciar en las fotografías de la misma. Se completa con un vestíbulo muy acogedor, donde recibe, el que posiblemente sea, el mejor conserje de Barcelona. Para más información no dude en contactar con Berkshire Hathaway\xa0HomeServices\xa0Barcelona, especialistas en inmuebles de alto standing en Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 9032.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '96603203', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/99/69/76/951332285.jpg', 'externalReference': 'BHHS-004107', 'numPhotos': 40, 'floor': '6', 'price': 560000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 62.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3967221, 'longitude': 2.1548047, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96603203/', 'distance': '1615', 'description': 'PISO ALTO Y SOLEADO EN FINCA MODERNA DE LA PARTE ALTA DEL EIXAMPLE EL PISO IDEAL EN FINCA MODERNA BERKSHIRE\xa0HATHAWAY\xa0HomeServices\xa0Barcelona, consultora especializada en la comercialización de propiedades exclusivas en las mejores zonas de Barcelona, les ofrece este fantástico piso, situado en la parte alta del barrio del Eixample de Barcelona, junto a la Rambla Catalunya. Según entramos en el piso, nos encontramos con la barra baja que separa el hall de la\xa0cocina\xa0la izquierda. Al frente\xa0nos dirigimos\xa0al salón comedor con salida al gran ventanal exterior a la calle, con vistas y muy soleado durante todo el día. También tiene un estrecho balcón, por el que se mueven las persianas correderas. El salón está orientado a Sur, y es exterior a la calle\xa0Córsega, que es de poquísimo tránsito en este\xa0tramo, ya que\xa0su acceso se inicia desde la adyacente Rambla de\xa0Catalunya. La cocina está equipada con electrodomésticos y cruzando una puerta se accede al lavadero con espacio para lavadora, secadora y lavabo. Los muebles de diseño, y electrodomésticos que ven en las fotografías, no están incluidos en el precio. Desde el salón, a través de una puerta que separa la zona de día de la zona de noche, accedemos a un distribuidor con un baño completo al frente, con bañera, y las dos habitaciones, una a cada lado, son dobles y tienen armarios empotrados. Una es exterior al pequeño balcón que da a la calle, y la otra da al vestíbulo privado de vecinos de la planta. El piso tiene calefacción por radiadores, caldera y acumulador, aire acondicionado por conductos a todas las estancias, suelos de parquet... \xa0Además, \xa0está muy bien distribuido, con muy buen gusto, y sin espacios perdidos. Esta finca fue construida en el 1967, y en el 2007\xa0Metrovacesa\xa0la adaptó para tener viviendas cómodas y accesibles, además con buen gusto y diseño, como se puede apreciar en las fotografías de la misma. Se completa con un vestíbulo muy acogedor, donde recibe, el que posiblemente sea, el mejor conserje de Barcelona. Para más información no dude en contactar con Berkshire Hathaway\xa0HomeServices\xa0Barcelona, especialistas en inmuebles de alto standing en Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 9032.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99671987', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ef/7d/5e/1050814553.jpg', 'externalReference': 'BCN38016', 'numPhotos': 33, 'price': 500000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 66.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3940703, 'longitude': 2.1510348, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99671987/', 'distance': '1724', 'description': 'Lucas Fox presenta esta propiedad reformada ubicada a pocos pasos de la Avenida Diagonal y de la plaza de Francesc Macià.  Está situada en la planta principal del edificio, por lo que dispone de techos altos.  En la zona de día, encontramos una cocina americana totalmente equipada. \xa0El salón comedor es exterior y tiene un pequeño balcón donde colocar una mesa y dos sillas para disfrutar del sol de tarde. \xa0Además, tiene suelos hidráulicos y una bonita pared de obra vista en uno de sus laterales.  Por otro lado, un pequeño pasillo conduce a la otra parte de la vivienda. Aquí, vemos el dormitorio principal doble equipado con armario y un aseo y un segundo dormitorio también doble y con un armario muy espacioso. Ambos dormitorios son interiores, por lo que son muy tranquilos. Finalmente, entre los dormitorios encontramos el baño principal con ducha. El piso cuenta con unos altillos muy prácticos que se pueden aprovechar para almacenaje, aire acondicionado, calefacción por conductos y suelos de parquet en parte de la casa e hidráulicos en otra. Asimismo, los vecinos del edificio pueden disfrutar de la terraza comunitaria.  Póngase en contacto con nosotros para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 7576.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99671987', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ef/7d/5e/1050814553.jpg', 'externalReference': 'BCN38016', 'numPhotos': 33, 'price': 500000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 66.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3940703, 'longitude': 2.1510348, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99671987/', 'distance': '1724', 'description': 'Lucas Fox presenta esta propiedad reformada ubicada a pocos pasos de la Avenida Diagonal y de la plaza de Francesc Macià.  Está situada en la planta principal del edificio, por lo que dispone de techos altos.  En la zona de día, encontramos una cocina americana totalmente equipada. \xa0El salón comedor es exterior y tiene un pequeño balcón donde colocar una mesa y dos sillas para disfrutar del sol de tarde. \xa0Además, tiene suelos hidráulicos y una bonita pared de obra vista en uno de sus laterales.  Por otro lado, un pequeño pasillo conduce a la otra parte de la vivienda. Aquí, vemos el dormitorio principal doble equipado con armario y un aseo y un segundo dormitorio también doble y con un armario muy espacioso. Ambos dormitorios son interiores, por lo que son muy tranquilos. Finalmente, entre los dormitorios encontramos el baño principal con ducha. El piso cuenta con unos altillos muy prácticos que se pueden aprovechar para almacenaje, aire acondicionado, calefacción por conductos y suelos de parquet en parte de la casa e hidráulicos en otra. Asimismo, los vecinos del edificio pueden disfrutar de la terraza comunitaria.  Póngase en contacto con nosotros para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 7576.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99602294', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/e5/3c/c0/1048891671.jpg', 'externalReference': 'BCN37037', 'numPhotos': 37, 'price': 649000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 102.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Gòtic', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3858046, 'longitude': 2.1752293, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99602294/', 'distance': '493', 'description': "Situado en el Barrio Gótico, a un paso de Portal de l'Àngel, Plaza de Catalunya y de la Catedral de Barcelona, Lucas Fox presenta este piso recién reformado y totalmente amueblado a estrenar.  La reforma ha terminado recientemente y el piso está listo para entrar a vivir.  Tiene doble orientación y al estar en una planta alta, goza de abundante luz natural que entra por grandes ventanales.  Al entrar en el piso nos encontramos con un amplio hall de entrada, con espacio de almacenamiento adicional, que nos da acceso a la zona de día. A nuestra derecha tenemos el salón-comedor de 32m2 con salida a dos balcones con bonitas vistas a edificios monumentales. A nuestra izquierda tenemos un baño y el cuarto lavadero.  A través de la cocina totalmente equipada, que alberga otro espacio de comedor/zona de trabajo, accedemos a la zona de noche que consta de dos dormitorios dobles con armarios y el segundo baño. \xa0Ambos dormitorios dan a un tranquilo patio interior.  Este excelente piso cuenta con todas las instalaciones nuevas: fontanería, gas, electricidad, ventilación, aire acondicionado por conductos en la zona de día, splits en la zona de noche y calefacción eléctrica independiente en todas partes.  Consta con suelos y baldosas de madera nuevos, una cocina hecha a medida con electrodomésticos de marcas de alta calidad, muebles de diseño, lámparas y fotografías de lugares emblemáticos de Barcelona, como se muestra en las imágenes.  Los residentes del edificio pueden disfrutar de la terraza comunitaria con vistas al casco antiguo.  Póngase en contacto con nosotros para concertar una visita.  Características básicas:  - 102 m² construidos  - 2 dormitorios dobles  - 2 baños  - Terraza  - Armarios  Edificio  - Exterior/interior  -\xa0Construido en 1836  Equipamiento  - Aire acondicionado (conductos/splits)  - Calefacción independiente.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 6363.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99602294', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/e5/3c/c0/1048891671.jpg', 'externalReference': 'BCN37037', 'numPhotos': 37, 'price': 649000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 102.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Gòtic', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3858046, 'longitude': 2.1752293, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99602294/', 'distance': '493', 'description': "Situado en el Barrio Gótico, a un paso de Portal de l'Àngel, Plaza de Catalunya y de la Catedral de Barcelona, Lucas Fox presenta este piso recién reformado y totalmente amueblado a estrenar.  La reforma ha terminado recientemente y el piso está listo para entrar a vivir.  Tiene doble orientación y al estar en una planta alta, goza de abundante luz natural que entra por grandes ventanales.  Al entrar en el piso nos encontramos con un amplio hall de entrada, con espacio de almacenamiento adicional, que nos da acceso a la zona de día. A nuestra derecha tenemos el salón-comedor de 32m2 con salida a dos balcones con bonitas vistas a edificios monumentales. A nuestra izquierda tenemos un baño y el cuarto lavadero.  A través de la cocina totalmente equipada, que alberga otro espacio de comedor/zona de trabajo, accedemos a la zona de noche que consta de dos dormitorios dobles con armarios y el segundo baño. \xa0Ambos dormitorios dan a un tranquilo patio interior.  Este excelente piso cuenta con todas las instalaciones nuevas: fontanería, gas, electricidad, ventilación, aire acondicionado por conductos en la zona de día, splits en la zona de noche y calefacción eléctrica independiente en todas partes.  Consta con suelos y baldosas de madera nuevos, una cocina hecha a medida con electrodomésticos de marcas de alta calidad, muebles de diseño, lámparas y fotografías de lugares emblemáticos de Barcelona, como se muestra en las imágenes.  Los residentes del edificio pueden disfrutar de la terraza comunitaria con vistas al casco antiguo.  Póngase en contacto con nosotros para concertar una visita.  Características básicas:  - 102 m² construidos  - 2 dormitorios dobles  - 2 baños  - Terraza  - Armarios  Edificio  - Exterior/interior  -\xa0Construido en 1836  Equipamiento  - Aire acondicionado (conductos/splits)  - Calefacción independiente.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 6363.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99484200', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/49/bd/6f/1045894352.jpg', 'externalReference': 'BCNP4955', 'numPhotos': 30, 'price': 990000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 126.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Gòtic', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3837041, 'longitude': 2.1717083, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99484200/', 'distance': '449', 'description': 'Céntrico y alto apartamento con detalles de la época en el barrio Gótico. Los apartamentos esquineros suelen ser los más demandados en el centro de Barcelona. Esta preciosa finca con ascensor en el barrio Gótico, queda a 15 minutos caminando de Paseo de Gracia, haciendo ruta por el Portal de Ángel. Un magnífico paseo a lo largo del barrio histórico de la ciudad condal. Destaca en esta propiedad la reforma integral realizada en el año 2021 preservando el carácter modernista visto en sus suelos hidráulicos, techos altos y el detalle de dar nueva vida a la pared original de la finca del año 1900. El apartamento está distribuido en dos dormitorios dobles y dos baños. Uno de los dormitorios dispone de un walking closet que en el caso de necesidad podría hacer función de un tercer dormitorio. Amplio y luminoso salón comedor y cocina americana con cuatro balcones. Excelentes materiales y acabados. Solo disponible con Sotheby’s International Realty. El Barrio Gótico es el núcleo más antiguo de la ciudad. Está delimitado por Las Ramblas, La Vía Laietana, el Paseo Colón y la Plaza de Catalunya, cada uno de estos puntos por sí solos tiene su propia importancia e historia. De calles angostas y estructura irregular, varios de sus edificios han sido construidos sobre los restos románicos de la ciudad, así que puede hacerse con algún apartamento en el que al menos una pared date de la época romana o medieval. Es el barrio turístico por excelencia por lo que representa una inversión asegurada, sobretodo si está cerca de alguno de sus atractivos como La Catedral, la Plaza Sant Jaume con el Ayuntamiento y el Palacio de la Generalitat, la Plaza Real, Las famosas Rambas, y el Museo de Historia de la ciudad. Este podría ser su barrio si busca hacer una inversión rentable o adquirir un excelente piet-à-terre en un barrio con gran historia, edificaciones particulares, de interés turístico y con todo tipo de negocios a mano, buena gastronomía, y múltiples rincones mágicos para descubrir y recorrer.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 7857.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99484200', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/49/bd/6f/1045894352.jpg', 'externalReference': 'BCNP4955', 'numPhotos': 30, 'price': 990000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 126.0, 'exterior': False, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Gòtic', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Gòtic', 'latitude': 41.3837041, 'longitude': 2.1717083, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99484200/', 'distance': '449', 'description': 'Céntrico y alto apartamento con detalles de la época en el barrio Gótico. Los apartamentos esquineros suelen ser los más demandados en el centro de Barcelona. Esta preciosa finca con ascensor en el barrio Gótico, queda a 15 minutos caminando de Paseo de Gracia, haciendo ruta por el Portal de Ángel. Un magnífico paseo a lo largo del barrio histórico de la ciudad condal. Destaca en esta propiedad la reforma integral realizada en el año 2021 preservando el carácter modernista visto en sus suelos hidráulicos, techos altos y el detalle de dar nueva vida a la pared original de la finca del año 1900. El apartamento está distribuido en dos dormitorios dobles y dos baños. Uno de los dormitorios dispone de un walking closet que en el caso de necesidad podría hacer función de un tercer dormitorio. Amplio y luminoso salón comedor y cocina americana con cuatro balcones. Excelentes materiales y acabados. Solo disponible con Sotheby’s International Realty. El Barrio Gótico es el núcleo más antiguo de la ciudad. Está delimitado por Las Ramblas, La Vía Laietana, el Paseo Colón y la Plaza de Catalunya, cada uno de estos puntos por sí solos tiene su propia importancia e historia. De calles angostas y estructura irregular, varios de sus edificios han sido construidos sobre los restos románicos de la ciudad, así que puede hacerse con algún apartamento en el que al menos una pared date de la época romana o medieval. Es el barrio turístico por excelencia por lo que representa una inversión asegurada, sobretodo si está cerca de alguno de sus atractivos como La Catedral, la Plaza Sant Jaume con el Ayuntamiento y el Palacio de la Generalitat, la Plaza Real, Las famosas Rambas, y el Museo de Historia de la ciudad. Este podría ser su barrio si busca hacer una inversión rentable o adquirir un excelente piet-à-terre en un barrio con gran historia, edificaciones particulares, de interés turístico y con todo tipo de negocios a mano, buena gastronomía, y múltiples rincones mágicos para descubrir y recorrer.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'priceByArea': 7857.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Gòtic, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97472923', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/9d/de/31/980489261.jpg', 'externalReference': 'B83', 'numPhotos': 32, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 180.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3864408, 'longitude': 2.1600522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97472923/', 'distance': '816', 'description': 'Magnífico piso de lujo reformado a estrenar, con calidades muy altas y grandes espacios, pensado para personas que quieran estar en el centro de la ciudad, sin estar en zona turística. Estas son sus características principales: 2 grandes habitaciones suites. Una de las habitaciones da hacia el patio interior con armarios empotrados e iluminación y maderas nobles, también se encuentra una pequeña zona de estudio y un baño incorporado completo con ducha y sanitario. Master suite con espacio para cama king size con salida a terraza amplia una zona tranquila. Armarios empotrados. Baño completo espacioso y doble lavabo, luz natural que da hacia la terraza y armarios incorporados. Ducha amplia con sanitario separado. Cocina pequeña, pensada para uso básico y disfrutar de la zona gourmet de Barcelona. Enchufes con USB. Maderas nobles. Electrodomésticos integrados, nevera americana de alta calidad. Sistema de domótica para la iluminación. Sistema de calefacción y aire acondicionado última generación. Edificio reformado recientemente.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4711.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97472923', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/9d/de/31/980489261.jpg', 'externalReference': 'B83', 'numPhotos': 32, 'floor': '1', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 180.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3864408, 'longitude': 2.1600522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97472923/', 'distance': '816', 'description': 'Magnífico piso de lujo reformado a estrenar, con calidades muy altas y grandes espacios, pensado para personas que quieran estar en el centro de la ciudad, sin estar en zona turística. Estas son sus características principales: 2 grandes habitaciones suites. Una de las habitaciones da hacia el patio interior con armarios empotrados e iluminación y maderas nobles, también se encuentra una pequeña zona de estudio y un baño incorporado completo con ducha y sanitario. Master suite con espacio para cama king size con salida a terraza amplia una zona tranquila. Armarios empotrados. Baño completo espacioso y doble lavabo, luz natural que da hacia la terraza y armarios incorporados. Ducha amplia con sanitario separado. Cocina pequeña, pensada para uso básico y disfrutar de la zona gourmet de Barcelona. Enchufes con USB. Maderas nobles. Electrodomésticos integrados, nevera americana de alta calidad. Sistema de domótica para la iluminación. Sistema de calefacción y aire acondicionado última generación. Edificio reformado recientemente.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4711.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99440277', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/02/5b/41/1044037924.jpg', 'externalReference': '4919', 'numPhotos': 42, 'floor': '5', 'price': 345000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 64.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Mallorca', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3831025, 'longitude': 2.1528715, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99440277/', 'distance': '1488', 'description': 'Excelente vivienda en la Nova Esquerra del Eixample reformado para entrar a vivir ¡ Luminoso y muy tranquilo orientado a patio de manzana, con amplio salón comedor, cocina equipada, 2 habitaciones (1 doble y 1 individual), baño completo con plato de ducha. climatizado mediante aire acondicionado y calefaccion de gas natural, suelos de parquet. Anteriormente distribido en cuatro habitaciones. 5ª planta con ascensor en finca del año 1.964. No cobramos honorarios al comprador. Impuestos, gastos de notaría y gestoría no incluidos en el precio de compra de la vivienda.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5391.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Mallorca'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99440277', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/02/5b/41/1044037924.jpg', 'externalReference': '4919', 'numPhotos': 42, 'floor': '5', 'price': 345000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 64.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Mallorca', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3831025, 'longitude': 2.1528715, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99440277/', 'distance': '1488', 'description': 'Excelente vivienda en la Nova Esquerra del Eixample reformado para entrar a vivir ¡ Luminoso y muy tranquilo orientado a patio de manzana, con amplio salón comedor, cocina equipada, 2 habitaciones (1 doble y 1 individual), baño completo con plato de ducha. climatizado mediante aire acondicionado y calefaccion de gas natural, suelos de parquet. Anteriormente distribido en cuatro habitaciones. 5ª planta con ascensor en finca del año 1.964. No cobramos honorarios al comprador. Impuestos, gastos de notaría y gestoría no incluidos en el precio de compra de la vivienda.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5391.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Mallorca'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '96745288', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5f/9b/9b/955352422.jpg', 'externalReference': 'BCN23896', 'numPhotos': 42, 'price': 1200000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 187.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3849911, 'longitude': 2.1546049, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96745288/', 'distance': '1292', 'description': 'En un edificio del año 2000, en perfectas condiciones y con ascensor, encontramos este magnífico ático de 160 m², totalmente reformado, muy amplio y con mucha luz gracias a los grandes ventanales de suelo a techo que hay en prácticamente toda la vivienda.  El piso consta de un agradable salón-comedor con cocina abierta con mucha luz y bonitas vistas a la ciudad, dos dormitorios dobles, uno de ellos con vestidor y baño privado, así como un baño completo extra con zona de aguas integrada.  En la planta superior, accesible desde la escalera comunitaria, encontramos un espacio exterior de más de 150 m² escriturado junto con nuestra vivienda.  En este espacio se consolidó una construcción de 69 m² que actualmente alberga un gran salón con la cocina abierta y un baño completo. Un espacio ideal para celebrar reuniones, fiestas o simplemente relajarse. Este espacio tiene salida a una soleada terraza de más de 85 m² con zona de barbacoa y un trastero.  En el precio se incluyen dos plazas de aparcamiento de tamaño grande en la misma finca, donde pueden caber dos coches grandes y una moto.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6417.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Ático'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '96745288', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/5f/9b/9b/955352422.jpg', 'externalReference': 'BCN23896', 'numPhotos': 42, 'price': 1200000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 187.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3849911, 'longitude': 2.1546049, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96745288/', 'distance': '1292', 'description': 'En un edificio del año 2000, en perfectas condiciones y con ascensor, encontramos este magnífico ático de 160 m², totalmente reformado, muy amplio y con mucha luz gracias a los grandes ventanales de suelo a techo que hay en prácticamente toda la vivienda.  El piso consta de un agradable salón-comedor con cocina abierta con mucha luz y bonitas vistas a la ciudad, dos dormitorios dobles, uno de ellos con vestidor y baño privado, así como un baño completo extra con zona de aguas integrada.  En la planta superior, accesible desde la escalera comunitaria, encontramos un espacio exterior de más de 150 m² escriturado junto con nuestra vivienda.  En este espacio se consolidó una construcción de 69 m² que actualmente alberga un gran salón con la cocina abierta y un baño completo. Un espacio ideal para celebrar reuniones, fiestas o simplemente relajarse. Este espacio tiene salida a una soleada terraza de más de 85 m² con zona de barbacoa y un trastero.  En el precio se incluyen dos plazas de aparcamiento de tamaño grande en la misma finca, donde pueden caber dos coches grandes y una moto.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6417.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Ático'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '94496557', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ae/e9/5e/890458989.jpg', 'externalReference': 'BCN28118', 'numPhotos': 36, 'floor': '6', 'price': 1500000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 139.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3901548, 'longitude': 2.1655207, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/94496557/', 'distance': '461', 'description': 'Lucas Fox presenta este piso en venta reformado a estrenar y totalmente amueblado en una ubicación Prime de Barcelona, entre Paseo de Gracia y Rambla Catalunya.  Está situado en la última planta de una finca regia del 1.890 con ascensor, que ha pasado favorablemente la Inspección Técnica de Edificios.  Todos los espacios de la vivienda son amplios y gozan de abundante entrada de luz natural. Al entrar en la vivienda, a mano izquierda encontramos la zona de día compuesta por el salón-comedor con balcón exterior a la calle y con una chimenea de bioetanol. A continuación, se dispone la elegante cocina de la firma italiana Modulnova, equipada con vinoteca y electrodomésticos de marca.  A través de un amplio pasillo con armarios empotrados, accedemos a la zona de noche compuesta por dos dormitorios dobles, uno de ellos con baño privado. Ambos dormitorios disponen de amplios armarios empotrados y salida a una terraza orientada a sureste. Esta zona se completa con un baño con ducha.  El piso está equipado por calefacción por radiadores de gas (que se puede controlar mediante Wifi), aire acondicionado por conductos con bomba para frío y calor, suelos de parqué y además dispone de un trastero en el terrado de la finca.  La reforma se ha realizada de la mano de un reconocido estudio de arquitectura de interiores, con grandes calidades y creando ambientes elegantes, cálidos y con carácter.  Póngase en contacto con nosotros para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 10791.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '94496557', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ae/e9/5e/890458989.jpg', 'externalReference': 'BCN28118', 'numPhotos': 36, 'floor': '6', 'price': 1500000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 139.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio La Dreta de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Dreta de l'Eixample", 'latitude': 41.3901548, 'longitude': 2.1655207, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/94496557/', 'distance': '461', 'description': 'Lucas Fox presenta este piso en venta reformado a estrenar y totalmente amueblado en una ubicación Prime de Barcelona, entre Paseo de Gracia y Rambla Catalunya.  Está situado en la última planta de una finca regia del 1.890 con ascensor, que ha pasado favorablemente la Inspección Técnica de Edificios.  Todos los espacios de la vivienda son amplios y gozan de abundante entrada de luz natural. Al entrar en la vivienda, a mano izquierda encontramos la zona de día compuesta por el salón-comedor con balcón exterior a la calle y con una chimenea de bioetanol. A continuación, se dispone la elegante cocina de la firma italiana Modulnova, equipada con vinoteca y electrodomésticos de marca.  A través de un amplio pasillo con armarios empotrados, accedemos a la zona de noche compuesta por dos dormitorios dobles, uno de ellos con baño privado. Ambos dormitorios disponen de amplios armarios empotrados y salida a una terraza orientada a sureste. Esta zona se completa con un baño con ducha.  El piso está equipado por calefacción por radiadores de gas (que se puede controlar mediante Wifi), aire acondicionado por conductos con bomba para frío y calor, suelos de parqué y además dispone de un trastero en el terrado de la finca.  La reforma se ha realizada de la mano de un reconocido estudio de arquitectura de interiores, con grandes calidades y creando ambientes elegantes, cálidos y con carácter.  Póngase en contacto con nosotros para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 10791.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Dreta de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'labels': [{'name': 'luxuryType', 'text': 'Lujo'}], 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97637906', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/77/0d/ef/985947670.jpg', 'externalReference': '4392', 'numPhotos': 71, 'floor': 'en', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 190.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3860408, 'longitude': 2.1633522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97637906/', 'distance': '556', 'description': 'Viviendas de Lujo en Ensanche Izquierdo. Viviendas a estrenar en exclusiva finca clásica. Situada en el Ensanche Izquierdo, está ubicada en la calle Diputación cerca de Plaza Universidad y a escasos minutos de la Rambla de Catalunya y el Paseo de Gracia. Terraza privada de 41m2. Ademas podrá disfrutar de una gran terraza comunitaria, un espacio de 60 m² con zona “chill out” y unas preciosas vistas de Barcelona. Exclusiva finca con sólo 4 vecinos, ha sido totalmente rehabilitada teniendo todas las zonas comunes, ascensor y terrado nuevos. El proyecto de esta fantástica vivienda ha sido realizado por Jaime Beriestain Studio, se han utilizado los mejores materiales con un diseño muy elegante creando espacios actuales y acogedores. Vivienda de alto standing con todo tipo de detalles, distribuida en:  - Recibidor. - Salón de unos 26m2 independiente y exterior a la calle. - Cocina independiente cerrada con puertas correderas, lo que nos facilita la sensación de cocina abierta. - Zona de lavado. - Aseo de cortesía. - Zona de noche con dos dormitorios ambos dobles y en suite, uno de ellos de 13m2 con armarios empotrados, estudio y con un baño de 8m2 con plato de ducha. El dormitorio principal tiene una superficie de 25m2, consta de vestidor y de un baño de 13m2 con plato de ducha y bañera, también tiene acceso a la terraza de 42m2. Zona comercial con todo tipo de servicios y muy bien comunicada con transporte público. Oportunidad inmejorable para adquirir una vivienda a estrenar en el corazón de Barcelona. Disponemos de más pisos a la venta en la misma finca: 1° de 130m2 a 768.000€  2° de 130m2 a 816.000€  Local de 165m2 a 576.000€ Posibilidad de comprar edificio completo. Aincasa Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4463.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97637906', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/77/0d/ef/985947670.jpg', 'externalReference': '4392', 'numPhotos': 71, 'floor': 'en', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 190.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Diputació', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3860408, 'longitude': 2.1633522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97637906/', 'distance': '556', 'description': 'Viviendas de Lujo en Ensanche Izquierdo. Viviendas a estrenar en exclusiva finca clásica. Situada en el Ensanche Izquierdo, está ubicada en la calle Diputación cerca de Plaza Universidad y a escasos minutos de la Rambla de Catalunya y el Paseo de Gracia. Terraza privada de 41m2. Ademas podrá disfrutar de una gran terraza comunitaria, un espacio de 60 m² con zona “chill out” y unas preciosas vistas de Barcelona. Exclusiva finca con sólo 4 vecinos, ha sido totalmente rehabilitada teniendo todas las zonas comunes, ascensor y terrado nuevos. El proyecto de esta fantástica vivienda ha sido realizado por Jaime Beriestain Studio, se han utilizado los mejores materiales con un diseño muy elegante creando espacios actuales y acogedores. Vivienda de alto standing con todo tipo de detalles, distribuida en:  - Recibidor. - Salón de unos 26m2 independiente y exterior a la calle. - Cocina independiente cerrada con puertas correderas, lo que nos facilita la sensación de cocina abierta. - Zona de lavado. - Aseo de cortesía. - Zona de noche con dos dormitorios ambos dobles y en suite, uno de ellos de 13m2 con armarios empotrados, estudio y con un baño de 8m2 con plato de ducha. El dormitorio principal tiene una superficie de 25m2, consta de vestidor y de un baño de 13m2 con plato de ducha y bañera, también tiene acceso a la terraza de 42m2. Zona comercial con todo tipo de servicios y muy bien comunicada con transporte público. Oportunidad inmejorable para adquirir una vivienda a estrenar en el corazón de Barcelona. Disponemos de más pisos a la venta en la misma finca: 1° de 130m2 a 768.000€  2° de 130m2 a 816.000€  Local de 165m2 a 576.000€ Posibilidad de comprar edificio completo. Aincasa Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4463.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de la Diputació'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99794526', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/14/7c/63/1054779399.jpg', 'externalReference': '2809', 'numPhotos': 26, 'floor': '2', 'price': 490000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 71.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de París', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3887258, 'longitude': 2.1473163, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99794526/', 'distance': '1876', 'description': 'Vivienda de 71m2 en edificio de 2011. En excelente estado, exterior y funcional. Salón comedor esquinero, dos habitaciones dobles. Cocina americana equipada. Un baño completo. Armarios empotrados. Calefacción y aire acondicionado por conductos. Excelentes cerramientos Technal con doble cristal. Persianas mecanizadas. Terraza comunitaria en la cubierta del edificio. Plaza de garaje grande y trastero de 14m2. Garaje con vigilancia 24 horas. Dos ascensores. Gastos e impuestos no incluidos en el precio del anuncio.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': True}, 'priceByArea': 6901.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de París'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99794526', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/14/7c/63/1054779399.jpg', 'externalReference': '2809', 'numPhotos': 26, 'floor': '2', 'price': 490000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 71.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de París', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3887258, 'longitude': 2.1473163, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99794526/', 'distance': '1876', 'description': 'Vivienda de 71m2 en edificio de 2011. En excelente estado, exterior y funcional. Salón comedor esquinero, dos habitaciones dobles. Cocina americana equipada. Un baño completo. Armarios empotrados. Calefacción y aire acondicionado por conductos. Excelentes cerramientos Technal con doble cristal. Persianas mecanizadas. Terraza comunitaria en la cubierta del edificio. Plaza de garaje grande y trastero de 14m2. Garaje con vigilancia 24 horas. Dos ascensores. Gastos e impuestos no incluidos en el precio del anuncio.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': True}, 'priceByArea': 6901.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de París'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97534780', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/3e/ee/b3/982449385.jpg', 'externalReference': 'BCN-Carrera Bajos2', 'numPhotos': 31, 'floor': 'bj', 'price': 510000.0, 'propertyType': 'duplex', 'operation': 'sale', 'size': 86.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Carrera', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'El Poble Sec - Parc de Montjuïc', 'latitude': 41.372431, 'longitude': 2.1760547, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97534780/', 'distance': '1753', 'description': 'Fabulosa planta baja dúplex de 86 m2, muy luminosa, con soleado patio de 59m2. La vivienda se distribuye en planta baja (recibidor, aseo de cortesía, cocina abierta, salón comedor con salida al patio de 59m2) y planta piso (2 habitaciones a patio de manzana y 2 baños). Finca con ascensor y con una ubicación privilegiada. Disponemos de plazas de parking en la misma finca, así como otros pisos en diferentes alturas. Nuestras viviendas se encuentran en la calle Carrera, justo delante de los Jardines de Walter Benjamin y la Plaça de les Drassanes, frente al Puerto de Barcelona. Justo al lado de la famosa Avda del Paral. lel con sus teatros y todo tipo de comercios. A un paso del Mirador del Poble Sec, disfrute de los paseos por Montjuïc y por sus amplias zonas ajardinadas ideales para hacer deporte al aire libre. Aproveche el buen clima de nuestra ciudad en las playas de alrededor. Muy bien comunicado con toda la ciudad con Lineas de Metro y autobuses. deportes al aire libre. Aproveche el buen clima de nuestra ciudad en las playas de alrededor. Muy bien comunicado con toda la ciudad con Líneas de Metro y autobuses.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': True}, 'priceByArea': 5930.0, 'detailedType': {'typology': 'flat', 'subTypology': 'duplex'}, 'suggestedTexts': {'subtitle': 'El Poble Sec - Parc de Montjuïc, Barcelona', 'title': 'Dúplex en Carrera'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97534780', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/3e/ee/b3/982449385.jpg', 'externalReference': 'BCN-Carrera Bajos2', 'numPhotos': 31, 'floor': 'bj', 'price': 510000.0, 'propertyType': 'duplex', 'operation': 'sale', 'size': 86.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Carrera', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'El Poble Sec - Parc de Montjuïc', 'latitude': 41.372431, 'longitude': 2.1760547, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97534780/', 'distance': '1753', 'description': 'Fabulosa planta baja dúplex de 86 m2, muy luminosa, con soleado patio de 59m2. La vivienda se distribuye en planta baja (recibidor, aseo de cortesía, cocina abierta, salón comedor con salida al patio de 59m2) y planta piso (2 habitaciones a patio de manzana y 2 baños). Finca con ascensor y con una ubicación privilegiada. Disponemos de plazas de parking en la misma finca, así como otros pisos en diferentes alturas. Nuestras viviendas se encuentran en la calle Carrera, justo delante de los Jardines de Walter Benjamin y la Plaça de les Drassanes, frente al Puerto de Barcelona. Justo al lado de la famosa Avda del Paral. lel con sus teatros y todo tipo de comercios. A un paso del Mirador del Poble Sec, disfrute de los paseos por Montjuïc y por sus amplias zonas ajardinadas ideales para hacer deporte al aire libre. Aproveche el buen clima de nuestra ciudad en las playas de alrededor. Muy bien comunicado con toda la ciudad con Lineas de Metro y autobuses. deportes al aire libre. Aproveche el buen clima de nuestra ciudad en las playas de alrededor. Muy bien comunicado con toda la ciudad con Líneas de Metro y autobuses.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': True}, 'priceByArea': 5930.0, 'detailedType': {'typology': 'flat', 'subTypology': 'duplex'}, 'suggestedTexts': {'subtitle': 'El Poble Sec - Parc de Montjuïc, Barcelona', 'title': 'Dúplex en Carrera'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99348106', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a6/63/11/962649051.jpg', 'externalReference': 'B34', 'numPhotos': 23, 'floor': '2', 'price': 579000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 70.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de París', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3899266, 'longitude': 2.1499647, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99348106/', 'distance': '1672', 'description': 'Un piso único con bóveda catalana 70 m2 1 dormitorio doble en suite con baño abierto con ducha, con armario grande 1 dormitorio individual con sofa-cama y armario 1 sala de estar Cocina con comedor, con isla, totalmente equipada (lavadora, lavaplatos, placa de inducción, campana, nevera, horno, tostadora, hervidor…) 1 baño separado con una bañera y WC  1 Balcón Aire acondicionado split (frio/calor) Caldera de gas nueva Hay plancha, aspiradora, secador de pelo Parquet de madera buena calidad, gres en la cocina Orientación Sur.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8271.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de París'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99348106', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/a6/63/11/962649051.jpg', 'externalReference': 'B34', 'numPhotos': 23, 'floor': '2', 'price': 579000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 70.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de París', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3899266, 'longitude': 2.1499647, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99348106/', 'distance': '1672', 'description': 'Un piso único con bóveda catalana 70 m2 1 dormitorio doble en suite con baño abierto con ducha, con armario grande 1 dormitorio individual con sofa-cama y armario 1 sala de estar Cocina con comedor, con isla, totalmente equipada (lavadora, lavaplatos, placa de inducción, campana, nevera, horno, tostadora, hervidor…) 1 baño separado con una bañera y WC  1 Balcón Aire acondicionado split (frio/calor) Caldera de gas nueva Hay plancha, aspiradora, secador de pelo Parquet de madera buena calidad, gres en la cocina Orientación Sur.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 8271.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle de París'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '91626925', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8c/85/9a/958647886.jpg', 'externalReference': 'V2084-R', 'numPhotos': 28, 'floor': '3', 'price': 256000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 67.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Princesa', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3879197, 'longitude': 2.1811329, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/91626925/', 'distance': '951', 'description': 'Vivienda de 67 m2 con doble orientación a calle Princesa y Assaonadors, con sol todo el día, que ocupa la tercera planta de un edificio de 1880, sin ascensor.   Distribuye 2 dormitorios, uno doble con balcón a calle Princesa y otro individual (habitación ciega), vestidor, baño completo con bañera, cocina abierta al comedor y salón.   Ventilación cruzada, cerramientos de aluminio, suelos de parquet laminado y de gres en baño, climatización en la estancia con más incidencia solar. El dormitorio individual y vestidor ventilan al actual dormitorio doble.  La distribución actual puede modificarse cambiando el dormitorio doble por el salón, sin obras. No hay posibilidad de instalar ascensor en la finca.   El Born, con comercio de proximidad y servicios, pero también una amplia oferta gastronómica y un envidiable entorno histórico de la evolución de la ciudad.   Los honorarios son a cargo del vendedor. El precio no incluye los impuestos, ni gastos de notaría ni de gestoría de la compraventa.  Eurofincas International Real Estate | Referencia V2084.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 3821.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso en Princesa'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '91626925', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8c/85/9a/958647886.jpg', 'externalReference': 'V2084-R', 'numPhotos': 28, 'floor': '3', 'price': 256000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 67.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Princesa', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3879197, 'longitude': 2.1811329, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/91626925/', 'distance': '951', 'description': 'Vivienda de 67 m2 con doble orientación a calle Princesa y Assaonadors, con sol todo el día, que ocupa la tercera planta de un edificio de 1880, sin ascensor.   Distribuye 2 dormitorios, uno doble con balcón a calle Princesa y otro individual (habitación ciega), vestidor, baño completo con bañera, cocina abierta al comedor y salón.   Ventilación cruzada, cerramientos de aluminio, suelos de parquet laminado y de gres en baño, climatización en la estancia con más incidencia solar. El dormitorio individual y vestidor ventilan al actual dormitorio doble.  La distribución actual puede modificarse cambiando el dormitorio doble por el salón, sin obras. No hay posibilidad de instalar ascensor en la finca.   El Born, con comercio de proximidad y servicios, pero también una amplia oferta gastronómica y un envidiable entorno histórico de la evolución de la ciudad.   Los honorarios son a cargo del vendedor. El precio no incluye los impuestos, ni gastos de notaría ni de gestoría de la compraventa.  Eurofincas International Real Estate | Referencia V2084.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 3821.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': 'Piso en Princesa'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98124798', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/45/91/16/1001891426.jpg', 'externalReference': '4400', 'numPhotos': 37, 'floor': 'bj', 'price': 350000.0, 'propertyType': 'duplex', 'operation': 'sale', 'size': 147.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle de l'Olivera", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'El Poble Sec - Parc de Montjuïc', 'latitude': 41.3715925, 'longitude': 2.1592743, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98124798/', 'distance': '1969', 'description': 'Planta baja reformada con mucho encanto. En una calle muy tranquila junto a la Plaza de Santa Madrona encontramos esta planta baja con mucho encanto. Se accede al interior por una entrada independiente, encontramos una vez en su interior a un amplio espacio para poder guardar bicicletas así como espacio polivalente para almacenaje, a continuación accedemos a un amplio comedor con cocina abierta, desde ahí podemos acceder a la planta altillo mediante unas escaleras de hierro forjado incrustadas en la pared de piedra natural o al fondo del comedor un pasillo nos daría paso a u baño con ducha seguido de un agradable patio con luz natural seguido de un cuarto de máquinas y al final un amplio espacio que hace de sala y zona polivalente con salida a una pequeña terraza con mucha luminosidad. destacar el microclima que se respira y el silencio que se respira. ! Si lo que realmente buscas es luz y tranquilidad dejaras de seguir buscando ¡ En la planta duplex o altillo encontramos un amplio espacio con zona de armarios actualmente la propiedad lo utiliza como una zona de trabajo con la posibilidad de poder hacer otro dormitorio con otro baño (preparado para ejecutar la obra, se puede ver en el plano adjunto, al fondo un pequeño pasillo nos daría paso a un segundo dormitorio con zona de vestidor con posibilidad de hacer otro baño (preparado para ejecutar la obra, se puede ver en el plano adjunto). Dispone de calefacción de gas, ventilador de techo, cocina equipada con electrodomésticos. Aincasa Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 2381.0, 'detailedType': {'typology': 'flat', 'subTypology': 'duplex'}, 'suggestedTexts': {'subtitle': 'El Poble Sec - Parc de Montjuïc, Barcelona', 'title': "Dúplex en Calle de l'Olivera"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98124798', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/45/91/16/1001891426.jpg', 'externalReference': '4400', 'numPhotos': 37, 'floor': 'bj', 'price': 350000.0, 'propertyType': 'duplex', 'operation': 'sale', 'size': 147.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle de l'Olivera", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'El Poble Sec - Parc de Montjuïc', 'latitude': 41.3715925, 'longitude': 2.1592743, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98124798/', 'distance': '1969', 'description': 'Planta baja reformada con mucho encanto. En una calle muy tranquila junto a la Plaza de Santa Madrona encontramos esta planta baja con mucho encanto. Se accede al interior por una entrada independiente, encontramos una vez en su interior a un amplio espacio para poder guardar bicicletas así como espacio polivalente para almacenaje, a continuación accedemos a un amplio comedor con cocina abierta, desde ahí podemos acceder a la planta altillo mediante unas escaleras de hierro forjado incrustadas en la pared de piedra natural o al fondo del comedor un pasillo nos daría paso a u baño con ducha seguido de un agradable patio con luz natural seguido de un cuarto de máquinas y al final un amplio espacio que hace de sala y zona polivalente con salida a una pequeña terraza con mucha luminosidad. destacar el microclima que se respira y el silencio que se respira. ! Si lo que realmente buscas es luz y tranquilidad dejaras de seguir buscando ¡ En la planta duplex o altillo encontramos un amplio espacio con zona de armarios actualmente la propiedad lo utiliza como una zona de trabajo con la posibilidad de poder hacer otro dormitorio con otro baño (preparado para ejecutar la obra, se puede ver en el plano adjunto, al fondo un pequeño pasillo nos daría paso a un segundo dormitorio con zona de vestidor con posibilidad de hacer otro baño (preparado para ejecutar la obra, se puede ver en el plano adjunto). Dispone de calefacción de gas, ventilador de techo, cocina equipada con electrodomésticos. Aincasa Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 2381.0, 'detailedType': {'typology': 'flat', 'subTypology': 'duplex'}, 'suggestedTexts': {'subtitle': 'El Poble Sec - Parc de Montjuïc, Barcelona', 'title': "Dúplex en Calle de l'Olivera"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AM6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97501131', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/6b/f9/3d/981296577.jpg', 'externalReference': 'V220429', 'numPhotos': 20, 'floor': '1', 'price': 384000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 78.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle Balmes', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3925976, 'longitude': 2.1616804, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97501131/', 'distance': '881', 'description': 'Cafur les presenta, en la céntrica calle Balmes, en el corazón de la Barcelona tradicional, esta maravillosa propiedad en finca regia del año 1909 con ascensor. La vivienda, que destaca por la altura de los techos, la sensación de confort y la luminosidad da al patio de manzana, por lo que no tendrás que sufrir por los ruidos del tráfico rodado. Cuenta con la siguiente distribución: amplio y luminoso salón comedor gracias a su conexión con la galería, ideal para poner una zona de lectura o un pequeño estudio; cocina independiente para actualizar; 2 dormitorios; 1 baño completo de tres piezas con bañera; y pasillo distribuidor. Está ubicado a sólo unos metros de la emblemática Rambla Catalunya y Passeig de Gràcia, donde encontrarás tiendas de primeras marcas. Además estarás rodeado de todos los servicios que puedas necesitar y de una amplia red de transporte público.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4923.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle Balmes'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97501131', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/6b/f9/3d/981296577.jpg', 'externalReference': 'V220429', 'numPhotos': 20, 'floor': '1', 'price': 384000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 78.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle Balmes', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3925976, 'longitude': 2.1616804, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97501131/', 'distance': '881', 'description': 'Cafur les presenta, en la céntrica calle Balmes, en el corazón de la Barcelona tradicional, esta maravillosa propiedad en finca regia del año 1909 con ascensor. La vivienda, que destaca por la altura de los techos, la sensación de confort y la luminosidad da al patio de manzana, por lo que no tendrás que sufrir por los ruidos del tráfico rodado. Cuenta con la siguiente distribución: amplio y luminoso salón comedor gracias a su conexión con la galería, ideal para poner una zona de lectura o un pequeño estudio; cocina independiente para actualizar; 2 dormitorios; 1 baño completo de tres piezas con bañera; y pasillo distribuidor. Está ubicado a sólo unos metros de la emblemática Rambla Catalunya y Passeig de Gràcia, donde encontrarás tiendas de primeras marcas. Además estarás rodeado de todos los servicios que puedas necesitar y de una amplia red de transporte público.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4923.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle Balmes'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AN6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '96967469', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/21/cc/9b/961770545.jpg', 'externalReference': '4382', 'numPhotos': 39, 'floor': 'bj', 'price': 249000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 80.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de Sant Antoni Abat', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3780021, 'longitude': 2.1625679, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96967469/', 'distance': '1211', 'description': 'A escasos metros del Mercado de Sant Antoni y Ronda Sant Antoni. Reforma de Lujo. Planta baja reformada integralmente, paredes recuperadas de piedra, techos altos con bóveda catalana y vigas de madera, en el acceso nos encontramos con una doble entrada con pared de piedra ideal par dejar bicicleta o moto protegidas. Al acceder al interior tenemos un amplio salón-comedor, cocina independiente totalmente equipada, dos dormitorios dobles, ambos con baño en suite mas un tercer baño con ducha, el dormitorio principal tiene salida a un patio por el que entra luz natural. Dispone de aire acondicionado con bomba de calor. Con mucho encanto, reforma cuidada hasta el ultimo detalle. En los gastos de comunidad está incluido el suministro del agua. Zona con todo tipo de servicios, comercios y restaurantes, a 200 metros del Mercado de Sant Antoni. El precio no incluye los impuestos, ni los gastos de Notaria, Registro y Gestoría. Aincasa Aicat número 2677. Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 3113.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de Sant Antoni Abat'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '96967469', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/21/cc/9b/961770545.jpg', 'externalReference': '4382', 'numPhotos': 39, 'floor': 'bj', 'price': 249000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 80.0, 'exterior': True, 'rooms': 2, 'bathrooms': 3, 'address': 'Calle de Sant Antoni Abat', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3780021, 'longitude': 2.1625679, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/96967469/', 'distance': '1211', 'description': 'A escasos metros del Mercado de Sant Antoni y Ronda Sant Antoni. Reforma de Lujo. Planta baja reformada integralmente, paredes recuperadas de piedra, techos altos con bóveda catalana y vigas de madera, en el acceso nos encontramos con una doble entrada con pared de piedra ideal par dejar bicicleta o moto protegidas. Al acceder al interior tenemos un amplio salón-comedor, cocina independiente totalmente equipada, dos dormitorios dobles, ambos con baño en suite mas un tercer baño con ducha, el dormitorio principal tiene salida a un patio por el que entra luz natural. Dispone de aire acondicionado con bomba de calor. Con mucho encanto, reforma cuidada hasta el ultimo detalle. En los gastos de comunidad está incluido el suministro del agua. Zona con todo tipo de servicios, comercios y restaurantes, a 200 metros del Mercado de Sant Antoni. El precio no incluye los impuestos, ni los gastos de Notaria, Registro y Gestoría. Aincasa Aicat número 2677. Un sueño una realidad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 3113.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de Sant Antoni Abat'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AO6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '94041284', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/cd/c0/bb/888738711.jpg', 'externalReference': '4340', 'numPhotos': 27, 'floor': '4', 'price': 360000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle de l'Oli", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3833513, 'longitude': 2.1766716, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/94041284/', 'distance': '737', 'description': "A escasos metros de La Catedral de Barcelona y Mercado de Santa Caterina. En el Barrio de La Ribera- Borne se encuentra esta fabulosa vivienda, con mucho encanto, al acceder a la vivienda dos zonas dividen la zona de día y de noche, en la zona de día encontramos un amplio salón-comedor con luz a raudales y bonitas vistas a terrazas ajardinadas, la cocina comunica con una ventana que permite el paso con el comedor para compartir momentos con familia y amigos, en frente se encuentra el baño con ducha, un amplio pasillo nos da paso a los dormitorios (2) dobles y muy soleados, el dormitorio principal tiene salida a un pequeño balcón con vistas a la misma calle de L'Oli, destacar los detalles como las vigas vistas, la contraventanas tienen aislamiento térmico con poco uso, calefacción. La finca dispone de ascensor, se accede subiendo un tramo de escaleras. El edificio cuenta con dos terrazas de uso comunitario con unas vistas únicas para poder disfrutar de las puestas de sol, en el terrado también se encuentra un amplio trastero para uso comunitario. El Born es un barrio a la última caracterizado por sus callejas medievales. De día, es posible disfrutar de cafeterías y boutiques de diseñadores, mientras que las coctelerías y la samba protagonizan sus noches. La basílica de Santa María del Mar exhibe ornamentales vidrieras. En el famoso museo Picasso se exponen muchas de las obras maestras del artista. El Born Centre de Cultura i Memoria es un centro polivalente que ocupa el edificio de un antiguo mercado y conserva en su interior un yacimiento arqueológico. El Born se encuentra entre la Via Laietana y la Barceloneta y tiene un buen servicio de transporte, con las paradas del metro Barceloneta y Jaume 1 en la misma línea. No obstante, a Las Ramblas y al centro de la ciudad puedes llegar caminando en sólo 10 minutos. La playa también está a unos 10 minutos caminando, lo que significa que podrás disfrutar de unas vacaciones en la playa y descansar de la ciudad al mismo tiempo. Además, el Born está bastante cerca del Parque de la Ciutadella: un pulmón de la ciudad condal, un lugar tranquilo para relajarte y pasear. Aincasa Un sueño una realidad.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4337.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': "Piso en Calle de l'Oli"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '94041284', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/cd/c0/bb/888738711.jpg', 'externalReference': '4340', 'numPhotos': 27, 'floor': '4', 'price': 360000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': "Calle de l'Oli", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'Sant Pere - Santa Caterina i la Ribera', 'latitude': 41.3833513, 'longitude': 2.1766716, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/94041284/', 'distance': '737', 'description': "A escasos metros de La Catedral de Barcelona y Mercado de Santa Caterina. En el Barrio de La Ribera- Borne se encuentra esta fabulosa vivienda, con mucho encanto, al acceder a la vivienda dos zonas dividen la zona de día y de noche, en la zona de día encontramos un amplio salón-comedor con luz a raudales y bonitas vistas a terrazas ajardinadas, la cocina comunica con una ventana que permite el paso con el comedor para compartir momentos con familia y amigos, en frente se encuentra el baño con ducha, un amplio pasillo nos da paso a los dormitorios (2) dobles y muy soleados, el dormitorio principal tiene salida a un pequeño balcón con vistas a la misma calle de L'Oli, destacar los detalles como las vigas vistas, la contraventanas tienen aislamiento térmico con poco uso, calefacción. La finca dispone de ascensor, se accede subiendo un tramo de escaleras. El edificio cuenta con dos terrazas de uso comunitario con unas vistas únicas para poder disfrutar de las puestas de sol, en el terrado también se encuentra un amplio trastero para uso comunitario. El Born es un barrio a la última caracterizado por sus callejas medievales. De día, es posible disfrutar de cafeterías y boutiques de diseñadores, mientras que las coctelerías y la samba protagonizan sus noches. La basílica de Santa María del Mar exhibe ornamentales vidrieras. En el famoso museo Picasso se exponen muchas de las obras maestras del artista. El Born Centre de Cultura i Memoria es un centro polivalente que ocupa el edificio de un antiguo mercado y conserva en su interior un yacimiento arqueológico. El Born se encuentra entre la Via Laietana y la Barceloneta y tiene un buen servicio de transporte, con las paradas del metro Barceloneta y Jaume 1 en la misma línea. No obstante, a Las Ramblas y al centro de la ciudad puedes llegar caminando en sólo 10 minutos. La playa también está a unos 10 minutos caminando, lo que significa que podrás disfrutar de unas vacaciones en la playa y descansar de la ciudad al mismo tiempo. Además, el Born está bastante cerca del Parque de la Ciutadella: un pulmón de la ciudad condal, un lugar tranquilo para relajarte y pasear. Aincasa Un sueño una realidad.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4337.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Pere - Santa Caterina i la Ribera, Barcelona', 'title': "Piso en Calle de l'Oli"}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AP6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98793896', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ce/23/f6/1024006628.jpg', 'externalReference': '11650', 'numPhotos': 28, 'floor': '3', 'price': 574000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 86.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio Vila de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'Vila de Gràcia', 'latitude': 41.4110641, 'longitude': 2.1580262, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98793896/', 'distance': '2799', 'description': "Situado en una finca moderna, nos encontramos con este coqueto y acogedor ático dúplex de 86\u202fm construidos más 20\u202fm de trza. Con vistas totalmente despejadas al Icónico Tenis, la Salut y al Tibidabo, muy luminoso y con sol de tarde. La vivienda está muy bien conservado. Se distribuye en un amplio y agradable salón comedor con vistas al tenis, y con cocina americana, práctica y funcional, totalmente equipada y amueblada. En esta planta también nos encontramos con una habitación individual exterior al tenis. Un baño completo con ducha y un armario amplio que nos puede hacer la función de trastero. Accedemos a la primera planta a través de una amplia y cómoda escalera que nos da paso, a la Suite, con un espacioso baño. Y a la agradable terraza. Dicha terraza nos induce a disfrutarla durante el día, al sol para, relajarse, leer o hacer actividades, y a sus atardeceres que se prestan a tomar una copa con la tranquilidad y la calma. Al igual que al anochecer que nos invita al disfrute de cenas y veladas bajo las estrellas y a la luz de la luna. Rodeada de plantas y flores que nos pueden transportar a un pequeño Edén, en la ciudad. Observaciones: plaza de parking opcional por 25.000, calefacción a gas, aire centralizado, armarios empotrados. Suelos de parquet, etc. En definitiva, una excelente calidad de vida. Gracia es un barrio informal con calles estrechas y plazas acogedoras lleno de tiendas de comestibles ecológicos, espacios de trabajo compartido modernos y estudios de artistas. La zona está muy bien comunicada a todos los niveles. Pocos distritos de Barcelona están rodeados de tanta simbología como el de Gràcia. El casco antiguo del barrio que le da nombre no ha dejado nunca de reivindicar con orgullo su pasado como municipio independiente (se agregó a la ciudad en 1897) La urbanización del barrio de la Salut-Gracia Nova, comenzó, en la segunda mitad del siglo XIX, alrededor de la iglesia, que tomo el nombre de Nuestra Señora de la Salut cuyas inmediaciones creció el barrio a lo largo de los años. En sus inicios la actividad más importante de la zona era agrícola, hallándose importantes masías como Can Xipreret, Can Tusquets, Can Muntaner y Ca l'Alegre de Dalt, pero progresivamente fueron convirtiéndose en zona residencial de veraneo de la burguesía barcelonesa y de la antigua villa de Gracia. También se halla en el barrio el reconocidísimo tenis la Salut, la entidad fue constituida como Salud Sport Club el 8 de junio de 1902, por un grupo de deportistas a partir del Club Social La Salud, fundado en 1899. Eusebio Güell, conde de Güell, fue nombrado presidente honorífico. Para construir sus instalaciones lograron unos terrenos de la masía de Can Xipreret. En el ámbito de la raqueta, destaca la creación de la primera escuela de tenis de España, en 1959. En ella se han formado algunos de los principales tenistas españoles de la historia como Manuel Orantes, Beto Martín, Conchita Martínez o Àlex Corretja. La Salut es el único club del mundo con dos campeones de la Copa Másters de Tenis, los citados Orantes y Corretja.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': False, 'parkingSpacePrice': 25000.0}, 'priceByArea': 6674.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': 'Vila de Gràcia, Barcelona', 'title': 'Ático'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98793896', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/ce/23/f6/1024006628.jpg', 'externalReference': '11650', 'numPhotos': 28, 'floor': '3', 'price': 574000.0, 'propertyType': 'penthouse', 'operation': 'sale', 'size': 86.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio Vila de Gràcia', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'Vila de Gràcia', 'latitude': 41.4110641, 'longitude': 2.1580262, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98793896/', 'distance': '2799', 'description': "Situado en una finca moderna, nos encontramos con este coqueto y acogedor ático dúplex de 86\u202fm construidos más 20\u202fm de trza. Con vistas totalmente despejadas al Icónico Tenis, la Salut y al Tibidabo, muy luminoso y con sol de tarde. La vivienda está muy bien conservado. Se distribuye en un amplio y agradable salón comedor con vistas al tenis, y con cocina americana, práctica y funcional, totalmente equipada y amueblada. En esta planta también nos encontramos con una habitación individual exterior al tenis. Un baño completo con ducha y un armario amplio que nos puede hacer la función de trastero. Accedemos a la primera planta a través de una amplia y cómoda escalera que nos da paso, a la Suite, con un espacioso baño. Y a la agradable terraza. Dicha terraza nos induce a disfrutarla durante el día, al sol para, relajarse, leer o hacer actividades, y a sus atardeceres que se prestan a tomar una copa con la tranquilidad y la calma. Al igual que al anochecer que nos invita al disfrute de cenas y veladas bajo las estrellas y a la luz de la luna. Rodeada de plantas y flores que nos pueden transportar a un pequeño Edén, en la ciudad. Observaciones: plaza de parking opcional por 25.000, calefacción a gas, aire centralizado, armarios empotrados. Suelos de parquet, etc. En definitiva, una excelente calidad de vida. Gracia es un barrio informal con calles estrechas y plazas acogedoras lleno de tiendas de comestibles ecológicos, espacios de trabajo compartido modernos y estudios de artistas. La zona está muy bien comunicada a todos los niveles. Pocos distritos de Barcelona están rodeados de tanta simbología como el de Gràcia. El casco antiguo del barrio que le da nombre no ha dejado nunca de reivindicar con orgullo su pasado como municipio independiente (se agregó a la ciudad en 1897) La urbanización del barrio de la Salut-Gracia Nova, comenzó, en la segunda mitad del siglo XIX, alrededor de la iglesia, que tomo el nombre de Nuestra Señora de la Salut cuyas inmediaciones creció el barrio a lo largo de los años. En sus inicios la actividad más importante de la zona era agrícola, hallándose importantes masías como Can Xipreret, Can Tusquets, Can Muntaner y Ca l'Alegre de Dalt, pero progresivamente fueron convirtiéndose en zona residencial de veraneo de la burguesía barcelonesa y de la antigua villa de Gracia. También se halla en el barrio el reconocidísimo tenis la Salut, la entidad fue constituida como Salud Sport Club el 8 de junio de 1902, por un grupo de deportistas a partir del Club Social La Salud, fundado en 1899. Eusebio Güell, conde de Güell, fue nombrado presidente honorífico. Para construir sus instalaciones lograron unos terrenos de la masía de Can Xipreret. En el ámbito de la raqueta, destaca la creación de la primera escuela de tenis de España, en 1959. En ella se han formado algunos de los principales tenistas españoles de la historia como Manuel Orantes, Beto Martín, Conchita Martínez o Àlex Corretja. La Salut es el único club del mundo con dos campeones de la Copa Másters de Tenis, los citados Orantes y Corretja.", 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'parkingSpace': {'hasParkingSpace': True, 'isParkingSpaceIncludedInPrice': False, 'parkingSpacePrice': 25000.0}, 'priceByArea': 6674.0, 'detailedType': {'typology': 'flat', 'subTypology': 'penthouse'}, 'suggestedTexts': {'subtitle': 'Vila de Gràcia, Barcelona', 'title': 'Ático'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AQ6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98508998', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/19/98/bb/1014756994.jpg', 'externalReference': '4740X', 'numPhotos': 17, 'floor': '5', 'price': 385000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle del Rosselló', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3858287, 'longitude': 2.148551, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98508998/', 'distance': '1777', 'description': "Este piso se encuentra en la zona del La Nova Esquerra de l'Eixample, en la quinta planta.  En el área hay todo tipo de servicios como ocio y restauración, colegios, sanidad, transporte público, etc.  La vivienda tiene dos dormitorios, uno de ellos es doble exterior y el otro es individual con ventana a un patio interior.  Tiene un baño en perfecto estado que es completo con ducha y se ubica en el centro del piso. El piso tiene un amplio y luminosos salón, estilo diáfano, con dos ambientes comunicados para el comedor y otro para el salón. En el mismo hay una salida directa a un perfecto balcón.  La cocina es estilo americana y se encuentra en perfecto estado. Para más información o programar una visita pueden dejar un WhatsApp en el 681 38 77 03 Encuentra más en.", 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4639.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle del Rosselló'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98508998', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/19/98/bb/1014756994.jpg', 'externalReference': '4740X', 'numPhotos': 17, 'floor': '5', 'price': 385000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle del Rosselló', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "La Nova Esquerra de l'Eixample", 'latitude': 41.3858287, 'longitude': 2.148551, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98508998/', 'distance': '1777', 'description': "Este piso se encuentra en la zona del La Nova Esquerra de l'Eixample, en la quinta planta.  En el área hay todo tipo de servicios como ocio y restauración, colegios, sanidad, transporte público, etc.  La vivienda tiene dos dormitorios, uno de ellos es doble exterior y el otro es individual con ventana a un patio interior.  Tiene un baño en perfecto estado que es completo con ducha y se ubica en el centro del piso. El piso tiene un amplio y luminosos salón, estilo diáfano, con dos ambientes comunicados para el comedor y otro para el salón. En el mismo hay una salida directa a un perfecto balcón.  La cocina es estilo americana y se encuentra en perfecto estado. Para más información o programar una visita pueden dejar un WhatsApp en el 681 38 77 03 Encuentra más en.", 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 4639.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "La Nova Esquerra de l'Eixample, Barcelona", 'title': 'Piso en Calle del Rosselló'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AR6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '98145102', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/94/3e/d6/1002492446.jpg', 'externalReference': '101217', 'numPhotos': 35, 'floor': 'en', 'price': 420000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 101.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Sant Pau', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3776106, 'longitude': 2.172716, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98145102/', 'distance': '1124', 'description': 'PISAZO DE 100M2 + 58M2 DE TERRAZA, EN FINCA DEL AÑO 1850 COMPLETAMENTE REHABILITADA. La propiedad en venta actualmente está dividida físicamente (no segregada) en dos apartamentos completos e independientes, que comparten luz, agua y gas. Cada apartamento tiene su propio acceso independiente con llave, y constan de un dormitorio doble, cocina totalmente equipada, sala de estar/comedor y baño completo. La vivienda está situada en la amplia plaza Salvador Seguí, delante de la Filmoteca, en el Raval, a tres minutos de les Ramblas. La finca es del año 1850, ha sido completamente rehabilitada, cuenta con cámaras de seguridad en la entrada y en cada rellano, tiene la ITE pasada con su correspondiente Certificado de Aptitud del año 2020, y no tiene derramas pendientes. El acceso a la finca es a través de un código numérico, llave física o interfono preparado con videocámara.  La propiedad está en una primera planta real sin ascensor y tiene caja de llaves digital. Al entrar por la puerta principal, tenemos un distribuidor con cámara de vigilancia y los contadores generales del inmueble, desde aquí accedemos a mano derecha al apartamento exterior a la calle, que da a la plaza Salvador Seguí, que consta de un salón comedor exterior con dos ventanas y un gran ventanal con balcón, con orientación noroeste, cocina totalmente equipada, un dormitorio doble que le entra luz por unas ventanas que dan al salón, y un baño completo. Techos altos de unos cuatro metros. Tiene luz todo el día y sol por las tardes.  El otro apartamento consta de un amplio salón comedor que goza de mucha luz natural gracias a su gran ventanal orientado al sudeste por donde entra luz todo el día y sol directo toda la mañana y mediodía, que da a una terraza de 50 metros cuadrados, privada, amueblada, con toldo retraible y de uso exclusivo. La terraza está en un patio interior de manzana absolutamente silencioso. Techos altos a más de cuatro metros con volta catalana. Consta de una habitación doble, baño completo, y cocina totalmente equipada. Ambos apartamentos gozan de carpintería de aluminio con doble cristal acústico, aire acondicionado y bomba de calor por conductos en todas las habitaciones, calefacción de radiadores y agua caliente ilimitada por caldera de gas centralizada. Actualmente, cada apartamento tiene un contrato de alquiler a largo plazo. Por lo tanto, esta propiedad genera dos alquileres que conjuntamente suman 2.150€ brutos al mes, o 25,800€ anuales. En una configuración de alquiler vacacional puro (contratos mensuales, el apartamento no tiene licencia turística) el bruto anual incrementa un 35% hasta los 35,000€, aproximadamente. A pesar de los contratos de largo plazo actuales, los apartamentos están diseñados para alquileres de temporada o vacacionales e incluyen en el precio de venta todo lo necesario para entrar a vivir inmediatamente: cubertería, ropa de cama, etc. Los apartamentos están separados por anchas paredes de piedra y fibra acústica en ambos lados, justamente para que no se molesten acústicamente. Cada apartamento tiene su llave privada y una cámara de seguridad en el pasillo interior que los une. Así, sería posible alquilar un apartamento en régimen vacacional y otro a largo plazo, por ejemplo. La flexibilidad es total. El propietario ha alquilado la propiedad como un solo apartamento y como dos apartamentos independientes. Ha alquilado a largo plazo, por temporada y como apartamentos vacacionales. Los apartamentos se han diseñado como hogares de alto standing. El precio de venta incluye todos los muebles y objetos de decoración tal y como se ven en las fotografías, menos los cuadros. Destaco: dos sofás cama (uno de ellos un Chesterfield original, importado de Inglaterra, de cuero rojo), dos camas dobles, dos mesas y sus sillas de comedor, los muebles de terraza (sofás de exterior, alfombra, plantas y tumbonas de madera). Gracias a los sofás cama, cada apart.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 4158.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de Sant Pau'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '98145102', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/94/3e/d6/1002492446.jpg', 'externalReference': '101217', 'numPhotos': 35, 'floor': 'en', 'price': 420000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 101.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de Sant Pau', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3776106, 'longitude': 2.172716, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/98145102/', 'distance': '1124', 'description': 'PISAZO DE 100M2 + 58M2 DE TERRAZA, EN FINCA DEL AÑO 1850 COMPLETAMENTE REHABILITADA. La propiedad en venta actualmente está dividida físicamente (no segregada) en dos apartamentos completos e independientes, que comparten luz, agua y gas. Cada apartamento tiene su propio acceso independiente con llave, y constan de un dormitorio doble, cocina totalmente equipada, sala de estar/comedor y baño completo. La vivienda está situada en la amplia plaza Salvador Seguí, delante de la Filmoteca, en el Raval, a tres minutos de les Ramblas. La finca es del año 1850, ha sido completamente rehabilitada, cuenta con cámaras de seguridad en la entrada y en cada rellano, tiene la ITE pasada con su correspondiente Certificado de Aptitud del año 2020, y no tiene derramas pendientes. El acceso a la finca es a través de un código numérico, llave física o interfono preparado con videocámara.  La propiedad está en una primera planta real sin ascensor y tiene caja de llaves digital. Al entrar por la puerta principal, tenemos un distribuidor con cámara de vigilancia y los contadores generales del inmueble, desde aquí accedemos a mano derecha al apartamento exterior a la calle, que da a la plaza Salvador Seguí, que consta de un salón comedor exterior con dos ventanas y un gran ventanal con balcón, con orientación noroeste, cocina totalmente equipada, un dormitorio doble que le entra luz por unas ventanas que dan al salón, y un baño completo. Techos altos de unos cuatro metros. Tiene luz todo el día y sol por las tardes.  El otro apartamento consta de un amplio salón comedor que goza de mucha luz natural gracias a su gran ventanal orientado al sudeste por donde entra luz todo el día y sol directo toda la mañana y mediodía, que da a una terraza de 50 metros cuadrados, privada, amueblada, con toldo retraible y de uso exclusivo. La terraza está en un patio interior de manzana absolutamente silencioso. Techos altos a más de cuatro metros con volta catalana. Consta de una habitación doble, baño completo, y cocina totalmente equipada. Ambos apartamentos gozan de carpintería de aluminio con doble cristal acústico, aire acondicionado y bomba de calor por conductos en todas las habitaciones, calefacción de radiadores y agua caliente ilimitada por caldera de gas centralizada. Actualmente, cada apartamento tiene un contrato de alquiler a largo plazo. Por lo tanto, esta propiedad genera dos alquileres que conjuntamente suman 2.150€ brutos al mes, o 25,800€ anuales. En una configuración de alquiler vacacional puro (contratos mensuales, el apartamento no tiene licencia turística) el bruto anual incrementa un 35% hasta los 35,000€, aproximadamente. A pesar de los contratos de largo plazo actuales, los apartamentos están diseñados para alquileres de temporada o vacacionales e incluyen en el precio de venta todo lo necesario para entrar a vivir inmediatamente: cubertería, ropa de cama, etc. Los apartamentos están separados por anchas paredes de piedra y fibra acústica en ambos lados, justamente para que no se molesten acústicamente. Cada apartamento tiene su llave privada y una cámara de seguridad en el pasillo interior que los une. Así, sería posible alquilar un apartamento en régimen vacacional y otro a largo plazo, por ejemplo. La flexibilidad es total. El propietario ha alquilado la propiedad como un solo apartamento y como dos apartamentos independientes. Ha alquilado a largo plazo, por temporada y como apartamentos vacacionales. Los apartamentos se han diseñado como hogares de alto standing. El precio de venta incluye todos los muebles y objetos de decoración tal y como se ven en las fotografías, menos los cuadros. Destaco: dos sofás cama (uno de ellos un Chesterfield original, importado de Inglaterra, de cuero rojo), dos camas dobles, dos mesas y sus sillas de comedor, los muebles de terraza (sofás de exterior, alfombra, plantas y tumbonas de madera). Gracias a los sofás cama, cada apart.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': False, 'priceByArea': 4158.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso en Calle de Sant Pau'}, 'hasPlan': True, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AS6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97933192', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/11/01/9b/995459861.jpg', 'externalReference': '261437', 'numPhotos': 16, 'floor': '1', 'price': 768000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 130.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3858408, 'longitude': 2.1603522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97933192/', 'distance': '804', 'description': 'DIPUTACIO - ARIBAU impresionante piso de diseño nuevo a estrenar en finca regia tiene 148 m² según referencia catastral, dispone de 2 habitaciones tipos suite, gran vestidor. La vivienda muy bien distribuida y bien diferenciada la zona de día de la de noche, al entrar encontramos un gran hall que da acceso a la cómoda cocina completamente equipada con electrodomésticos de alta gama y al magnífico salón comedor exterior a la calle con balcón, dispone de sistema de domótica de luz y persianas, carpintería de aluminio, aire acondicionado en todas las estancias y radiadores. En la zona de noche encontramos los dos dormitorios suitte uno de ellos con vestidor. La finca regia es preciosa, muy elegante, cuidada. Está ubicado en uno de los barrios más elegantes y de mayor comercio de Barcelona y una zona muy demandada debido a su enclave privilegiado. Se encuentra cerca de las principales vías de entrada y salida de la ciudad, cerca del exclusivo Paseo de Gracia y rodeada de transporte publico para acceder a cualquier parte de Barcelona. Este barrio cuenta con todos los servicios y tiendas especializadas que usted necesite. Desde las tiendas más exclusivas de la ciudad y famosas internacionalmente tanto moda y complementos como tiendas gourmet, parques, oficinas etc. Zona prime en pleno centro de Barcelona. Zona Ciutat Vella. ( El PVP indicado no incluye impuestos ni gastos de Escritura ).  PARA PROPIETARIOS:  1. ¿Necesitas vender para comprar? donpiso puede comprar tu casa entregándote el 10% en 48 horas y el resto ante Notario.  2. ¿Problemas económicos? Te ayudamos entregándote una cantidad pactada cada mes mientras vendemos tu casa. Sin gastos de ningún tipo.  3. ¿Vendes un piso con hipoteca? mientras gestionamos la venta, te adelantamos la cuota mensual.  4. ¿Reformas? al mejor precio y te las financiamos dentro de la hipoteca.  5. ¿La mejor hipoteca? en donpiso la encuentras y con condiciones preferentes.  6. ¿Herencias y divorcios? te ayudamos y coordinamos todo.  Infórmate: 93 306 90 90 -.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5908.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': False, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97933192', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/11/01/9b/995459861.jpg', 'externalReference': '261437', 'numPhotos': 16, 'floor': '1', 'price': 768000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 130.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3858408, 'longitude': 2.1603522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97933192/', 'distance': '804', 'description': 'DIPUTACIO - ARIBAU impresionante piso de diseño nuevo a estrenar en finca regia tiene 148 m² según referencia catastral, dispone de 2 habitaciones tipos suite, gran vestidor. La vivienda muy bien distribuida y bien diferenciada la zona de día de la de noche, al entrar encontramos un gran hall que da acceso a la cómoda cocina completamente equipada con electrodomésticos de alta gama y al magnífico salón comedor exterior a la calle con balcón, dispone de sistema de domótica de luz y persianas, carpintería de aluminio, aire acondicionado en todas las estancias y radiadores. En la zona de noche encontramos los dos dormitorios suitte uno de ellos con vestidor. La finca regia es preciosa, muy elegante, cuidada. Está ubicado en uno de los barrios más elegantes y de mayor comercio de Barcelona y una zona muy demandada debido a su enclave privilegiado. Se encuentra cerca de las principales vías de entrada y salida de la ciudad, cerca del exclusivo Paseo de Gracia y rodeada de transporte publico para acceder a cualquier parte de Barcelona. Este barrio cuenta con todos los servicios y tiendas especializadas que usted necesite. Desde las tiendas más exclusivas de la ciudad y famosas internacionalmente tanto moda y complementos como tiendas gourmet, parques, oficinas etc. Zona prime en pleno centro de Barcelona. Zona Ciutat Vella. ( El PVP indicado no incluye impuestos ni gastos de Escritura ).  PARA PROPIETARIOS:  1. ¿Necesitas vender para comprar? donpiso puede comprar tu casa entregándote el 10% en 48 horas y el resto ante Notario.  2. ¿Problemas económicos? Te ayudamos entregándote una cantidad pactada cada mes mientras vendemos tu casa. Sin gastos de ningún tipo.  3. ¿Vendes un piso con hipoteca? mientras gestionamos la venta, te adelantamos la cuota mensual.  4. ¿Reformas? al mejor precio y te las financiamos dentro de la hipoteca.  5. ¿La mejor hipoteca? en donpiso la encuentras y con condiciones preferentes.  6. ¿Herencias y divorcios? te ayudamos y coordinamos todo.  Infórmate: 93 306 90 90 -.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5908.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': False, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AT6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97661362', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/27/af/fc/1031239714.jpg', 'externalReference': '236620', 'numPhotos': 19, 'floor': 'bj', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 149.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3843408, 'longitude': 2.1626522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97661362/', 'distance': '686', 'description': 'DIPUTACIO - ARIBAU Impresionante piso de diseño con terraza nuevo a estrenar en finca regia tiene 148 m² según referencia catastral, dispone de 2 habitaciones de las cuales dos son suite, gran vestidor. La vivienda muy bien distribuida y bien diferenciada la zona de día de la de noche, al entrar encontramos un gran hall que da acceso a la cómoda cocina completamente equipada con electrodomésticos de alta gama y al magnífico salón comedor exterior a la calle con balcón, dispone de sistema de domótica de luz y persianas, carpintería de aluminio, aire acondicionado en todas las estancias y radiadores. En la zona de noche encontramos los dos dormitorios suitte uno de ellos con vestidor y con salia a la magnífica terraza de 41 m². La finca regia es preciosa, muy elegante, cuidada. Está ubicado en uno de los barrios más elegantes y de mayor comercio de Barcelona y una zona muy demandada debido a su enclave privilegiado. Se encuentra cerca de las principales vías de entrada y salida de la ciudad, cerca del exclusivo Paseo de Gracia y rodeada de transporte publico para acceder a cualquier parte de Barcelona. Este barrio cuenta con todos los servicios y tiendas especializadas que usted necesite. Desde las tiendas más exclusivas de la ciudad y famosas internacionalmente tanto moda y complementos como tiendas gourmet, parques, oficinas etc. Zona prime en pleno centro de Barcelona. Zona Ciutat Vella. ( El PVP indicado no incluye impuestos ni gastos de Escritura ).  PARA PROPIETARIOS:  1. ¿Necesitas vender para comprar? donpiso puede comprar tu casa entregándote el 10% en 48 horas y el resto ante Notario.  2. ¿Problemas económicos? Te ayudamos entregándote una cantidad pactada cada mes mientras vendemos tu casa. Sin gastos de ningún tipo.  3. ¿Vendes un piso con hipoteca? mientras gestionamos la venta, te adelantamos la cuota mensual.  4. ¿Reformas? al mejor precio y te las financiamos dentro de la hipoteca.  5. ¿La mejor hipoteca? en donpiso la encuentras y con condiciones preferentes.  6. ¿Herencias y divorcios? te ayudamos y coordinamos todo.  Infórmate: 93 306 90 90 -.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5691.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': False, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97661362', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/27/af/fc/1031239714.jpg', 'externalReference': '236620', 'numPhotos': 19, 'floor': 'bj', 'price': 848000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 149.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': "barrio L'Antiga Esquerra de l'Eixample", 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': "L'Antiga Esquerra de l'Eixample", 'latitude': 41.3843408, 'longitude': 2.1626522, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97661362/', 'distance': '686', 'description': 'DIPUTACIO - ARIBAU Impresionante piso de diseño con terraza nuevo a estrenar en finca regia tiene 148 m² según referencia catastral, dispone de 2 habitaciones de las cuales dos son suite, gran vestidor. La vivienda muy bien distribuida y bien diferenciada la zona de día de la de noche, al entrar encontramos un gran hall que da acceso a la cómoda cocina completamente equipada con electrodomésticos de alta gama y al magnífico salón comedor exterior a la calle con balcón, dispone de sistema de domótica de luz y persianas, carpintería de aluminio, aire acondicionado en todas las estancias y radiadores. En la zona de noche encontramos los dos dormitorios suitte uno de ellos con vestidor y con salia a la magnífica terraza de 41 m². La finca regia es preciosa, muy elegante, cuidada. Está ubicado en uno de los barrios más elegantes y de mayor comercio de Barcelona y una zona muy demandada debido a su enclave privilegiado. Se encuentra cerca de las principales vías de entrada y salida de la ciudad, cerca del exclusivo Paseo de Gracia y rodeada de transporte publico para acceder a cualquier parte de Barcelona. Este barrio cuenta con todos los servicios y tiendas especializadas que usted necesite. Desde las tiendas más exclusivas de la ciudad y famosas internacionalmente tanto moda y complementos como tiendas gourmet, parques, oficinas etc. Zona prime en pleno centro de Barcelona. Zona Ciutat Vella. ( El PVP indicado no incluye impuestos ni gastos de Escritura ).  PARA PROPIETARIOS:  1. ¿Necesitas vender para comprar? donpiso puede comprar tu casa entregándote el 10% en 48 horas y el resto ante Notario.  2. ¿Problemas económicos? Te ayudamos entregándote una cantidad pactada cada mes mientras vendemos tu casa. Sin gastos de ningún tipo.  3. ¿Vendes un piso con hipoteca? mientras gestionamos la venta, te adelantamos la cuota mensual.  4. ¿Reformas? al mejor precio y te las financiamos dentro de la hipoteca.  5. ¿La mejor hipoteca? en donpiso la encuentras y con condiciones preferentes.  6. ¿Herencias y divorcios? te ayudamos y coordinamos todo.  Infórmate: 93 306 90 90 -.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5691.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': "L'Antiga Esquerra de l'Eixample, Barcelona", 'title': 'Piso'}, 'hasPlan': False, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AU6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '95993558', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8a/45/92/933783157.jpg', 'externalReference': 'W-02NAXU', 'numPhotos': 31, 'price': 275000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 88.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle del Moianès', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'Hostafrancs', 'latitude': 41.3748961, 'longitude': 2.1433843, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/95993558/', 'distance': '2605', 'description': 'Pis a reformar con cédula Engel &amp; Völkers presenta una oportunidad de inversión en un amplio piso con vistas despejadas en Carrer de Moianès. Se compone de una vivienda de 88m2 construidos con cédula de habitabilidad, en una finca con ascensor, que hasta el momento se utilizaba como oficina, por tanto, tenemos un gran espacio diáfano con dos habitaciones y un baño que se puede reconvertir al piso que desees. Una quinta planta real. Entrando por la puerta accedemos a un pequeño pasillo con una amplia habitación y cocina a la izquierda y, a la derecha, otra pequeña con el baño. A continuación vemos el gran espacio diáfano con grandes ventanales que dejan entrar muchísima luz. Piso de grandes dimensiones para hacerlo completamente al gusto. La propiedad está estratégicamente ubicada en la mejor zona del barrio de Hostafrancs (Sants). La proximidad de la vivienda a la Plaza España, uno de los centros neurálgicos de Barcelona, así como también a la Estación de Sants, situándose en calle Moianès, representa la comodidad de tenerlo todo a solo dos minutos, supermercados, comercios varios, bancos, gimnasios, escuelas. Contando además con todos los medios de transporte urbano (FGC, Metro Líneas 1 y 3, Aerobús A1 y A2, más de 10 líneas de buses) y el desplazamiento directo a pie de la Fira de Barcelona. Es una ubicación ideal para familias, turistas, y personas que necesiten un "pied a terre" en Barcelona, facilitando los desplazamientos y viajes por trabajo. Sants, La Bordeta y Hostafrancs, son el símbolo de la Barcelona turística y cosmopolita, pero también de las tradiciones de los barrios más céntricos de la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3125.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Hostafrancs, Barcelona', 'title': 'Piso en Calle del Moianès'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': True, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '95993558', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/8a/45/92/933783157.jpg', 'externalReference': 'W-02NAXU', 'numPhotos': 31, 'price': 275000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 88.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle del Moianès', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Sants-Montjuïc', 'country': 'es', 'neighborhood': 'Hostafrancs', 'latitude': 41.3748961, 'longitude': 2.1433843, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/95993558/', 'distance': '2605', 'description': 'Pis a reformar con cédula Engel &amp; Völkers presenta una oportunidad de inversión en un amplio piso con vistas despejadas en Carrer de Moianès. Se compone de una vivienda de 88m2 construidos con cédula de habitabilidad, en una finca con ascensor, que hasta el momento se utilizaba como oficina, por tanto, tenemos un gran espacio diáfano con dos habitaciones y un baño que se puede reconvertir al piso que desees. Una quinta planta real. Entrando por la puerta accedemos a un pequeño pasillo con una amplia habitación y cocina a la izquierda y, a la derecha, otra pequeña con el baño. A continuación vemos el gran espacio diáfano con grandes ventanales que dejan entrar muchísima luz. Piso de grandes dimensiones para hacerlo completamente al gusto. La propiedad está estratégicamente ubicada en la mejor zona del barrio de Hostafrancs (Sants). La proximidad de la vivienda a la Plaza España, uno de los centros neurálgicos de Barcelona, así como también a la Estación de Sants, situándose en calle Moianès, representa la comodidad de tenerlo todo a solo dos minutos, supermercados, comercios varios, bancos, gimnasios, escuelas. Contando además con todos los medios de transporte urbano (FGC, Metro Líneas 1 y 3, Aerobús A1 y A2, más de 10 líneas de buses) y el desplazamiento directo a pie de la Fira de Barcelona. Es una ubicación ideal para familias, turistas, y personas que necesiten un "pied a terre" en Barcelona, facilitando los desplazamientos y viajes por trabajo. Sants, La Bordeta y Hostafrancs, son el símbolo de la Barcelona turística y cosmopolita, pero también de las tradiciones de los barrios más céntricos de la ciudad.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3125.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Hostafrancs, Barcelona', 'title': 'Piso en Calle del Moianès'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': True, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AV6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '97340498', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/80/e6/98/1046925847.jpg', 'externalReference': 'FloridaFranç', 'numPhotos': 23, 'floor': '2', 'price': 315000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de Floridablanca', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'Sant Antoni', 'latitude': 41.3766483, 'longitude': 2.1541467, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97340498/', 'distance': '1772', 'description': 'Piso totalmente reformado conservando de manera cuidadosa los elementos originales tales como techos de bóveda catalana y puerta originales de madera recuperada, todo combinado con una reforma integral con materiales de muy buena calidad de un gusto excepcional. El piso tiene una superficie construida de 83 metros y una superficie útil de 75 metros, el piso tiene 2 habitaciones, baño completo cocina equipada y salón con balcón. Es una segunda planta real con ASCENSOR, en una finca Regia. No esperes más y ven a visitar este piso con nosotros. Valoramos tu casa Encuentra más en.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3795.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Antoni, Barcelona', 'title': 'Piso en Calle de Floridablanca'}, 'hasPlan': False, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '97340498', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/80/e6/98/1046925847.jpg', 'externalReference': 'FloridaFranç', 'numPhotos': 23, 'floor': '2', 'price': 315000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 83.0, 'exterior': True, 'rooms': 2, 'bathrooms': 1, 'address': 'Calle de Floridablanca', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Eixample', 'country': 'es', 'neighborhood': 'Sant Antoni', 'latitude': 41.3766483, 'longitude': 2.1541467, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/97340498/', 'distance': '1772', 'description': 'Piso totalmente reformado conservando de manera cuidadosa los elementos originales tales como techos de bóveda catalana y puerta originales de madera recuperada, todo combinado con una reforma integral con materiales de muy buena calidad de un gusto excepcional. El piso tiene una superficie construida de 83 metros y una superficie útil de 75 metros, el piso tiene 2 habitaciones, baño completo cocina equipada y salón con balcón. Es una segunda planta real con ASCENSOR, en una finca Regia. No esperes más y ven a visitar este piso con nosotros. Valoramos tu casa Encuentra más en.', 'hasVideo': False, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 3795.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Sant Antoni, Barcelona', 'title': 'Piso en Calle de Floridablanca'}, 'hasPlan': False, 'has3DTour': False, 'has360': True, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AW6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99079881', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/9e/74/a7/1032868162.jpg', 'externalReference': 'VB2210011', 'numPhotos': 45, 'floor': 'bj', 'price': 890000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 137.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Fraternitat', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'Vila de Gràcia', 'latitude': 41.3991723, 'longitude': 2.158972, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99079881/', 'distance': '1581', 'description': 'Vivienda exclusiva con jardín en el corazón de Vila de Gràcia \xa0 En pleno corazón de la Vila de Gràcia, cerca de la plaza de la revolución y a cinco minutos caminando del metro Diagonal, encontramos esta vivienda exclusiva reformada en 2018 con todos los materiales de la mejor calidad. Este piso sorprende por sus detalles Arquitectónicos, Al entrar en la vivienda encontramos un recibidor con armarios y ventanas hacia el exterior y detrás de ello un sorprendente doble nivel donde la zona de abajo se convierte en una habitación totalmente cerrada y la parte de arriba puede ser un estudio o una sala de estar. A continuación, encontramos la cocina abierta y la sala de estar con mucha luz natural y vistas hacia el patio / jardín. con los techos altos en bóveda catalana toda la vivienda tiene una gran sensación de amplitud. Y después de la sala encontramos un pasillo con techos ventanas que dejan pasar totalmente la luz del día. Este pasillo puede quedar totalmente abierto en patio ya que la separación con el propio patio es con unos grandes ventanales tipo paneles japoneses y se pueden abrir totalmente para dejar un espacio muy grande donde se puede instalar mesa y sillas para hacer comidas en verano. En este mismo pasillo encontramos una pared entera de armarios para poder almacenar todo lo necesario en la vivienda. En la última parte a continuación del pasillo, encontramos en el antiguo lavadero una habitación doble en suite con su propio baño. Desde el patio interior podemos acceder a través de unas escaleras a un espacio extra, un jardín con vegetación y toldo, ideal para comidas y cenas y disfrutar de un espacio exterior despejado. La vivienda cuenta con una reforma de la mejor calidad, y ha conservado los detalles originales como las bóvedas catalanas, las paredes de piedras, y añadiendo materiales cálidos como los suelos de Madera. La finca tiene pasado la ITE y ha obtenido el certificado de aptitud. Disponemos de planos. No dudes en pedirnos visita en esta vivienda espectacular! \xa0 \xa0.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6496.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Vila de Gràcia, Barcelona', 'title': 'Piso en Calle de la Fraternitat'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': True, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99079881', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/9e/74/a7/1032868162.jpg', 'externalReference': 'VB2210011', 'numPhotos': 45, 'floor': 'bj', 'price': 890000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 137.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'Calle de la Fraternitat', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'Vila de Gràcia', 'latitude': 41.3991723, 'longitude': 2.158972, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99079881/', 'distance': '1581', 'description': 'Vivienda exclusiva con jardín en el corazón de Vila de Gràcia \xa0 En pleno corazón de la Vila de Gràcia, cerca de la plaza de la revolución y a cinco minutos caminando del metro Diagonal, encontramos esta vivienda exclusiva reformada en 2018 con todos los materiales de la mejor calidad. Este piso sorprende por sus detalles Arquitectónicos, Al entrar en la vivienda encontramos un recibidor con armarios y ventanas hacia el exterior y detrás de ello un sorprendente doble nivel donde la zona de abajo se convierte en una habitación totalmente cerrada y la parte de arriba puede ser un estudio o una sala de estar. A continuación, encontramos la cocina abierta y la sala de estar con mucha luz natural y vistas hacia el patio / jardín. con los techos altos en bóveda catalana toda la vivienda tiene una gran sensación de amplitud. Y después de la sala encontramos un pasillo con techos ventanas que dejan pasar totalmente la luz del día. Este pasillo puede quedar totalmente abierto en patio ya que la separación con el propio patio es con unos grandes ventanales tipo paneles japoneses y se pueden abrir totalmente para dejar un espacio muy grande donde se puede instalar mesa y sillas para hacer comidas en verano. En este mismo pasillo encontramos una pared entera de armarios para poder almacenar todo lo necesario en la vivienda. En la última parte a continuación del pasillo, encontramos en el antiguo lavadero una habitación doble en suite con su propio baño. Desde el patio interior podemos acceder a través de unas escaleras a un espacio extra, un jardín con vegetación y toldo, ideal para comidas y cenas y disfrutar de un espacio exterior despejado. La vivienda cuenta con una reforma de la mejor calidad, y ha conservado los detalles originales como las bóvedas catalanas, las paredes de piedras, y añadiendo materiales cálidos como los suelos de Madera. La finca tiene pasado la ITE y ha obtenido el certificado de aptitud. Disponemos de planos. No dudes en pedirnos visita en esta vivienda espectacular! \xa0 \xa0.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6496.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'Vila de Gràcia, Barcelona', 'title': 'Piso en Calle de la Fraternitat'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': True, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AX6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99791140', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/de/1c/b1/1054580932.jpg', 'externalReference': 'BCN38000', 'numPhotos': 32, 'price': 575000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 103.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio La Salut', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'La Salut', 'latitude': 41.4073525, 'longitude': 2.1502985, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99791140/', 'distance': '2741', 'description': 'Propiedad en venta en perfecto estado impecable, con dos dormitorios dobles (uno en suite) y 2 baños con una bonita distribución abierta. Se han utilizado materiales de alta calidad con la renovación, lo que resultó en esta propiedad luminosa y lista para entrar. El estilo es contemporáneo y de buen gusto; el lienzo en blanco perfecto para que el nuevo propietario entre y lo complete con su propio toque personal.  El apartamento se encuentra en el sexto piso real del edificio y cuenta con una terraza soleada con espacio para comer al aire libre. También en el edificio existe la posibilidad de alquilar o comprar una plaza de aparcamiento; un detalle que se agradecerá mucho en un barrio donde escasea el aparcamiento.  La propiedad viene completamente equipada con aire acondicionado central por conductos, y la propiedad cuenta con pisos de madera real, una cocina totalmente equipada y muebles flexibles.  El edificio dispone de servicio de conserjería para mayor comodidad.  La ubicación es en Gracia, al lado del transporte público, restaurantes, etc. pero también cerca de parques para tener un entorno verde.  No dude en ponerse en contacto con nosotros para obtener más información o para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5583.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'La Salut, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99791140', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/de/1c/b1/1054580932.jpg', 'externalReference': 'BCN38000', 'numPhotos': 32, 'price': 575000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 103.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio La Salut', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Gràcia', 'country': 'es', 'neighborhood': 'La Salut', 'latitude': 41.4073525, 'longitude': 2.1502985, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99791140/', 'distance': '2741', 'description': 'Propiedad en venta en perfecto estado impecable, con dos dormitorios dobles (uno en suite) y 2 baños con una bonita distribución abierta. Se han utilizado materiales de alta calidad con la renovación, lo que resultó en esta propiedad luminosa y lista para entrar. El estilo es contemporáneo y de buen gusto; el lienzo en blanco perfecto para que el nuevo propietario entre y lo complete con su propio toque personal.  El apartamento se encuentra en el sexto piso real del edificio y cuenta con una terraza soleada con espacio para comer al aire libre. También en el edificio existe la posibilidad de alquilar o comprar una plaza de aparcamiento; un detalle que se agradecerá mucho en un barrio donde escasea el aparcamiento.  La propiedad viene completamente equipada con aire acondicionado central por conductos, y la propiedad cuenta con pisos de madera real, una cocina totalmente equipada y muebles flexibles.  El edificio dispone de servicio de conserjería para mayor comodidad.  La ubicación es en Gracia, al lado del transporte público, restaurantes, etc. pero también cerca de parques para tener un entorno verde.  No dude en ponerse en contacto con nosotros para obtener más información o para concertar una visita.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 5583.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'La Salut, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
       <c r="AY6" t="inlineStr">
         <is>
-          <t>{'propertyCode': '99766521', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/29/1b/91/1053990542.jpg', 'externalReference': 'BCN37642', 'numPhotos': 27, 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 80.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Raval', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3763632, 'longitude': 2.1674975, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99766521/', 'distance': '1249', 'description': 'Nos encontramos ante una obra nueva a partir de la rehabilitación de una antigua fábrica textil de los años 30. Se han mantenido muchos de sus elementos originales, y se han creado\xa0lofts modernos de estilo industrial y con mucha luz, grandes ventanales y zonas comunes como piscina, sala social, terrazas y jardines.  La propiedad en venta es un apartamento muy diáfano que consta de salón comedor cocina con acceso a una bonita terraza cubierta orientada a las zonas comunes del complejo. También tenemos una habitación doble con baño en suite, otro baño completo y una segunda habitación doble en un mezzanine construido gracias a la altura de los techos.  El apartamento está en perfecto estado y cuenta con vigas vistas de madera, cerramientos de aluminio de suelo a techo de grandes dimensiones, aire acondicionado, bomba de calor por splits, paredes de ladrillo visto y suelos de parquet, entre otros aspectos.  Se trata así de un pequeño oasis en el centro del casco antiguo de Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6063.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'topNewDevelopment': False, 'superTopHighlight': False}</t>
+          <t>{'propertyCode': '99766521', 'thumbnail': 'https://img3.idealista.com/blur/WEB_LISTING/0/id.pro.es.image.master/29/1b/91/1053990542.jpg', 'externalReference': 'BCN37642', 'numPhotos': 27, 'price': 485000.0, 'propertyType': 'flat', 'operation': 'sale', 'size': 80.0, 'exterior': True, 'rooms': 2, 'bathrooms': 2, 'address': 'barrio El Raval', 'province': 'Barcelona', 'municipality': 'Barcelona', 'district': 'Ciutat Vella', 'country': 'es', 'neighborhood': 'El Raval', 'latitude': 41.3763632, 'longitude': 2.1674975, 'showAddress': False, 'url': 'https://www.idealista.com/inmueble/99766521/', 'distance': '1249', 'description': 'Nos encontramos ante una obra nueva a partir de la rehabilitación de una antigua fábrica textil de los años 30. Se han mantenido muchos de sus elementos originales, y se han creado\xa0lofts modernos de estilo industrial y con mucha luz, grandes ventanales y zonas comunes como piscina, sala social, terrazas y jardines.  La propiedad en venta es un apartamento muy diáfano que consta de salón comedor cocina con acceso a una bonita terraza cubierta orientada a las zonas comunes del complejo. También tenemos una habitación doble con baño en suite, otro baño completo y una segunda habitación doble en un mezzanine construido gracias a la altura de los techos.  El apartamento está en perfecto estado y cuenta con vigas vistas de madera, cerramientos de aluminio de suelo a techo de grandes dimensiones, aire acondicionado, bomba de calor por splits, paredes de ladrillo visto y suelos de parquet, entre otros aspectos.  Se trata así de un pequeño oasis en el centro del casco antiguo de Barcelona.', 'hasVideo': True, 'status': 'good', 'newDevelopment': False, 'hasLift': True, 'priceByArea': 6063.0, 'detailedType': {'typology': 'flat'}, 'suggestedTexts': {'subtitle': 'El Raval, Barcelona', 'title': 'Piso'}, 'hasPlan': True, 'has3DTour': False, 'has360': False, 'hasStaging': False, 'superTopHighlight': False, 'topNewDevelopment': False}</t>
         </is>
       </c>
     </row>

</xml_diff>